<commit_message>
Update for multiple institutions
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesb/Documents/Work/NEXT/NEXTAuthorList/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58055277-3AEC-0A4B-B1D7-0A3D6D8E523A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3252EC60-D375-6845-AE1A-17C41342679A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="9180" windowWidth="25120" windowHeight="9940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="3980" windowWidth="25120" windowHeight="9940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="254">
   <si>
     <t>LastName</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Footnote</t>
   </si>
   <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t xml:space="preserve">\'Alvarez                    </t>
   </si>
   <si>
@@ -768,9 +762,6 @@
     <t xml:space="preserve">Deceased. </t>
   </si>
   <si>
-    <t>Corresponding Author</t>
-  </si>
-  <si>
     <t>II. Physikalisches Institut, Justus-Liebig-Universitat Giessen</t>
   </si>
   <si>
@@ -784,6 +775,24 @@
   </si>
   <si>
     <t>Donostia-San Sebastian, Spain</t>
+  </si>
+  <si>
+    <t>Institution1</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Institution2</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Institution3</t>
+  </si>
+  <si>
+    <t>Address3</t>
   </si>
 </sst>
 </file>
@@ -842,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -852,6 +861,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1154,17 +1166,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1176,644 +1188,664 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>248</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <f t="shared" si="0"/>
+      <c r="F18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <f t="shared" si="0"/>
+      <c r="F30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="D32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1822,17 +1854,17 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1841,19 +1873,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1862,17 +1894,17 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1881,19 +1913,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1902,19 +1934,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1923,19 +1955,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1944,17 +1976,17 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1963,19 +1995,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1984,19 +2016,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2005,19 +2037,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2026,19 +2058,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2047,19 +2079,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2068,19 +2100,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2089,19 +2121,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2110,19 +2142,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2131,19 +2163,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2152,19 +2184,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="D49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2173,17 +2205,17 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2192,19 +2224,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2213,19 +2245,17 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>245</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2234,19 +2264,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2255,19 +2285,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2276,19 +2306,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2297,19 +2327,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2318,17 +2348,17 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2337,19 +2367,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2358,19 +2388,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2379,19 +2409,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2400,19 +2430,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2421,19 +2451,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2442,19 +2472,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2463,19 +2493,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2484,19 +2514,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="E65" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2505,19 +2535,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2526,17 +2556,17 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2545,19 +2575,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2566,19 +2596,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2587,19 +2617,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2608,19 +2638,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2629,17 +2659,17 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2648,19 +2678,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2669,17 +2699,17 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2688,19 +2718,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2709,19 +2739,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2730,19 +2760,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2751,19 +2781,19 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2772,19 +2802,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2793,17 +2823,17 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2812,19 +2842,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2833,19 +2863,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2854,19 +2884,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2875,17 +2905,17 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2894,19 +2924,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2915,19 +2945,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2936,17 +2966,17 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2955,19 +2985,19 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2976,19 +3006,19 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2997,19 +3027,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -3018,19 +3048,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -3039,19 +3069,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="D92" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -3060,19 +3090,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -3081,19 +3111,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -3102,17 +3132,17 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -3121,17 +3151,17 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -3140,17 +3170,17 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -3159,19 +3189,19 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -3180,19 +3210,19 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -3201,19 +3231,19 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -3222,19 +3252,19 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -3243,17 +3273,17 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -3262,19 +3292,19 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -3283,19 +3313,19 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -3304,19 +3334,19 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -3325,19 +3355,17 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>245</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -3346,19 +3374,19 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove A. Martinez, remove 2nd affliation for B. Palmeiro
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesb/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74432D57-C442-E94F-B975-D61D6B4B6C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0899679-D3B5-CF42-83F9-C9660E45D446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="460" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2120" yWindow="500" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="257">
   <si>
     <t>LastName</t>
   </si>
@@ -389,9 +389,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Paterna, E-46980, Spain </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mart\'inez                  </t>
   </si>
   <si>
     <t xml:space="preserve">Mart\'inez-Lema             </t>
@@ -1186,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1205,28 +1202,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1235,17 +1232,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1260,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1268,30 +1265,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" t="s">
         <v>227</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>228</v>
       </c>
-      <c r="D5" t="s">
-        <v>229</v>
-      </c>
       <c r="E5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" t="s">
         <v>230</v>
       </c>
-      <c r="B6" t="s">
-        <v>231</v>
-      </c>
       <c r="D6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1305,7 +1302,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1322,7 +1319,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1330,16 +1327,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" t="s">
         <v>206</v>
       </c>
-      <c r="B9" t="s">
-        <v>207</v>
-      </c>
       <c r="D9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" t="s">
         <v>215</v>
-      </c>
-      <c r="E9" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1347,13 +1344,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1404,10 +1401,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1429,16 +1426,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15" t="s">
         <v>249</v>
-      </c>
-      <c r="E15" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1562,33 +1559,33 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23" t="s">
         <v>225</v>
       </c>
-      <c r="B23" t="s">
-        <v>226</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1596,13 +1593,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -1644,16 +1641,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" t="s">
         <v>204</v>
       </c>
-      <c r="B28" t="s">
-        <v>205</v>
-      </c>
       <c r="D28" t="s">
+        <v>214</v>
+      </c>
+      <c r="E28" t="s">
         <v>215</v>
-      </c>
-      <c r="E28" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1692,16 +1689,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1715,7 +1712,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E32" t="s">
         <v>63</v>
@@ -1749,16 +1746,16 @@
         <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -1780,13 +1777,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" t="s">
         <v>178</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>179</v>
-      </c>
-      <c r="D36" t="s">
-        <v>180</v>
       </c>
       <c r="E36" t="s">
         <v>33</v>
@@ -1811,22 +1808,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J38" s="4"/>
     </row>
@@ -1841,10 +1838,10 @@
         <v>5</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -1875,44 +1872,44 @@
         <v>81</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" t="s">
         <v>190</v>
       </c>
-      <c r="B42" t="s">
-        <v>191</v>
-      </c>
       <c r="D42" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>250</v>
+      </c>
+      <c r="B43" t="s">
         <v>251</v>
       </c>
-      <c r="B43" t="s">
-        <v>252</v>
-      </c>
       <c r="D43" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -1926,10 +1923,10 @@
         <v>5</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -1994,7 +1991,7 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E48" t="s">
         <v>91</v>
@@ -2036,7 +2033,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B51" t="s">
         <v>97</v>
@@ -2045,16 +2042,16 @@
         <v>5</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -2076,27 +2073,27 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" t="s">
         <v>192</v>
       </c>
-      <c r="B53" t="s">
-        <v>193</v>
-      </c>
       <c r="D53" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E54" t="s">
         <v>33</v>
@@ -2113,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E55" t="s">
         <v>63</v>
@@ -2169,16 +2166,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59" t="s">
         <v>245</v>
       </c>
-      <c r="B59" t="s">
-        <v>246</v>
-      </c>
       <c r="D59" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2200,16 +2197,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" t="s">
         <v>211</v>
       </c>
-      <c r="B61" t="s">
-        <v>212</v>
-      </c>
       <c r="D61" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2248,13 +2245,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E64" t="s">
         <v>33</v>
@@ -2299,81 +2296,78 @@
         <v>120</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
-      </c>
-      <c r="C67" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="D67" t="s">
-        <v>36</v>
+        <v>246</v>
       </c>
       <c r="E67" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
-      </c>
-      <c r="D68" t="s">
-        <v>247</v>
+        <v>104</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>239</v>
+      </c>
+      <c r="F68" t="s">
+        <v>36</v>
+      </c>
+      <c r="G68" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>217</v>
+      <c r="D69" t="s">
+        <v>20</v>
       </c>
       <c r="E69" t="s">
-        <v>240</v>
-      </c>
-      <c r="F69" t="s">
-        <v>36</v>
-      </c>
-      <c r="G69" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>254</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
-      </c>
-      <c r="C70" t="s">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="D70" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="E70" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="B71" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D71" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="E71" t="s">
         <v>33</v>
@@ -2381,203 +2375,200 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>208</v>
+        <v>126</v>
       </c>
       <c r="B72" t="s">
-        <v>183</v>
-      </c>
-      <c r="D72" t="s">
-        <v>32</v>
+        <v>127</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="E72" t="s">
-        <v>33</v>
+        <v>239</v>
+      </c>
+      <c r="F72" t="s">
+        <v>202</v>
+      </c>
+      <c r="G72" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>217</v>
+      <c r="D73" t="s">
+        <v>65</v>
       </c>
       <c r="E73" t="s">
-        <v>240</v>
-      </c>
-      <c r="F73" t="s">
-        <v>203</v>
-      </c>
-      <c r="G73" t="s">
-        <v>235</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B74" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E74" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E75" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="B76" t="s">
-        <v>118</v>
-      </c>
-      <c r="C76" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="D76" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E76" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>182</v>
+        <v>247</v>
       </c>
       <c r="B77" t="s">
-        <v>183</v>
-      </c>
-      <c r="D77" t="s">
-        <v>32</v>
+        <v>185</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="E77" t="s">
-        <v>33</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>248</v>
+        <v>134</v>
       </c>
       <c r="B78" t="s">
-        <v>186</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>217</v>
+        <v>135</v>
+      </c>
+      <c r="C78" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" t="s">
+        <v>36</v>
       </c>
       <c r="E78" t="s">
-        <v>240</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B79" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="D79" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E79" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="B80" t="s">
+        <v>194</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E80" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B81" t="s">
+        <v>232</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E81" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>138</v>
       </c>
-      <c r="C80" t="s">
-        <v>81</v>
-      </c>
-      <c r="D80" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>194</v>
-      </c>
-      <c r="B81" t="s">
-        <v>195</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E81" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="B82" t="s">
-        <v>233</v>
+        <v>139</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E82" t="s">
-        <v>240</v>
+        <v>248</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B83" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F83" t="s">
-        <v>36</v>
-      </c>
-      <c r="G83" t="s">
-        <v>119</v>
+      <c r="D83" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -2585,33 +2576,33 @@
         <v>141</v>
       </c>
       <c r="B84" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="E84" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B85" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="E85" t="s">
-        <v>144</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -2619,33 +2610,33 @@
         <v>145</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="C86" t="s">
         <v>5</v>
       </c>
       <c r="D86" t="s">
-        <v>36</v>
+        <v>246</v>
       </c>
       <c r="E86" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B87" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
       </c>
       <c r="D87" t="s">
-        <v>247</v>
+        <v>56</v>
       </c>
       <c r="E87" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2653,101 +2644,101 @@
         <v>148</v>
       </c>
       <c r="B88" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="E88" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
-      </c>
-      <c r="C89" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" t="s">
-        <v>150</v>
+        <v>196</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="E89" t="s">
-        <v>151</v>
+        <v>239</v>
+      </c>
+      <c r="F89" t="s">
+        <v>202</v>
+      </c>
+      <c r="G89" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="B90" t="s">
-        <v>197</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>217</v>
+        <v>100</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>86</v>
       </c>
       <c r="E90" t="s">
-        <v>240</v>
-      </c>
-      <c r="F90" t="s">
-        <v>203</v>
-      </c>
-      <c r="G90" t="s">
-        <v>235</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
       <c r="E91" t="s">
-        <v>153</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>197</v>
       </c>
       <c r="B92" t="s">
-        <v>118</v>
-      </c>
-      <c r="C92" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="D92" t="s">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="E92" t="s">
-        <v>7</v>
+        <v>239</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="B93" t="s">
-        <v>188</v>
+        <v>106</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="E93" t="s">
-        <v>240</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -2755,16 +2746,22 @@
         <v>155</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
       </c>
-      <c r="D94" t="s">
-        <v>224</v>
+      <c r="D94" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="E94" t="s">
-        <v>21</v>
+        <v>239</v>
+      </c>
+      <c r="F94" t="s">
+        <v>142</v>
+      </c>
+      <c r="G94" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -2772,44 +2769,38 @@
         <v>156</v>
       </c>
       <c r="B95" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="C95" t="s">
         <v>5</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>217</v>
+      <c r="D95" t="s">
+        <v>36</v>
       </c>
       <c r="E95" t="s">
-        <v>240</v>
-      </c>
-      <c r="F95" t="s">
-        <v>143</v>
-      </c>
-      <c r="G95" t="s">
-        <v>144</v>
+        <v>37</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B96" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E96" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B97" t="s">
         <v>160</v>
@@ -2818,7 +2809,7 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E97" t="s">
         <v>47</v>
@@ -2826,53 +2817,50 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B98" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C98" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="D98" t="s">
-        <v>65</v>
+        <v>246</v>
       </c>
       <c r="E98" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B99" t="s">
-        <v>163</v>
+        <v>104</v>
       </c>
       <c r="C99" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>247</v>
+        <v>36</v>
       </c>
       <c r="E99" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
-      </c>
-      <c r="C100" t="s">
-        <v>5</v>
-      </c>
-      <c r="D100" t="s">
-        <v>36</v>
-      </c>
-      <c r="E100" t="s">
-        <v>37</v>
+        <v>187</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -2880,44 +2868,47 @@
         <v>199</v>
       </c>
       <c r="B101" t="s">
-        <v>188</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>250</v>
+        <v>200</v>
+      </c>
+      <c r="D101" t="s">
+        <v>65</v>
+      </c>
+      <c r="E101" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="B102" t="s">
-        <v>201</v>
+        <v>167</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E102" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B103" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
       </c>
-      <c r="D103" t="s">
-        <v>6</v>
+      <c r="D103" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="E103" t="s">
-        <v>7</v>
+        <v>239</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -2925,16 +2916,16 @@
         <v>169</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C104" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>217</v>
+      <c r="D104" t="s">
+        <v>36</v>
       </c>
       <c r="E104" t="s">
-        <v>240</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -2942,111 +2933,94 @@
         <v>170</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="C105" t="s">
         <v>5</v>
       </c>
       <c r="D105" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E105" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="B106" t="s">
-        <v>172</v>
-      </c>
-      <c r="C106" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="D106" t="s">
-        <v>16</v>
+        <v>179</v>
       </c>
       <c r="E106" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>184</v>
+        <v>252</v>
       </c>
       <c r="B107" t="s">
-        <v>185</v>
-      </c>
-      <c r="D107" t="s">
-        <v>180</v>
-      </c>
-      <c r="E107" t="s">
-        <v>33</v>
+        <v>253</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>253</v>
+        <v>172</v>
       </c>
       <c r="B108" t="s">
-        <v>254</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>250</v>
+        <v>173</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>163</v>
+      </c>
+      <c r="E108" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B109" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C109" t="s">
-        <v>5</v>
+        <v>213</v>
       </c>
       <c r="D109" t="s">
+        <v>163</v>
+      </c>
+      <c r="E109" t="s">
         <v>164</v>
-      </c>
-      <c r="E109" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>214</v>
+        <v>5</v>
       </c>
       <c r="D110" t="s">
-        <v>164</v>
+        <v>36</v>
       </c>
       <c r="E110" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>177</v>
-      </c>
-      <c r="B111" t="s">
-        <v>112</v>
-      </c>
-      <c r="C111" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" t="s">
-        <v>36</v>
-      </c>
-      <c r="E111" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove J. Diaz, R.M. Gutierrez, M. Losada, J. Perez, L. Ripoll, N. Yahlali; fix typo for A. Nu\~{n}ez
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0899679-D3B5-CF42-83F9-C9660E45D446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6B4B0A-2156-2743-9B2D-53588C0BF6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="500" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7620" yWindow="2220" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="250">
   <si>
     <t>LastName</t>
   </si>
@@ -283,18 +283,9 @@
     <t xml:space="preserve">Guenette                    </t>
   </si>
   <si>
-    <t xml:space="preserve">Guti\'errez                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> R.M.       </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Centro de Investigaci\'on en Ciencias B\'asicas y Aplicadas, Universidad Antonio Nari\~no, Sede Circunvalar, Carretera 3 Este No.\ 47 A-15 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Bogot\'a, Colombia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Haefner                     </t>
   </si>
   <si>
@@ -373,9 +364,6 @@
     <t xml:space="preserve"> Valencia, E-46022, Spain </t>
   </si>
   <si>
-    <t xml:space="preserve">Losada                      </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mano                        </t>
   </si>
   <si>
@@ -454,9 +442,6 @@
     <t xml:space="preserve">Para                        </t>
   </si>
   <si>
-    <t xml:space="preserve">P\'erez                     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Laboratorio Subterr\'aneo de Canfranc, Paseo de los Ayerbe s/n </t>
   </si>
   <si>
@@ -475,9 +460,6 @@
     <t xml:space="preserve">Renner                      </t>
   </si>
   <si>
-    <t xml:space="preserve">Ripoll                      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Escola Polit\`ecnica Superior, Universitat de Girona, Av.~Montilivi, s/n </t>
   </si>
   <si>
@@ -559,9 +541,6 @@
     <t xml:space="preserve"> J.T.      </t>
   </si>
   <si>
-    <t xml:space="preserve">Yahlali                     </t>
-  </si>
-  <si>
     <t>Foss</t>
   </si>
   <si>
@@ -772,9 +751,6 @@
     <t>Unit of Nuclear Engineering, Faculty of Engineering Sciences, Ben-Gurion University of the Negev, P.O.B. 653</t>
   </si>
   <si>
-    <t>Nun\ñez</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Department of Physics and Astronomy, Manchester University </t>
   </si>
   <si>
@@ -800,6 +776,9 @@
   </si>
   <si>
     <t>Dey</t>
+  </si>
+  <si>
+    <t>Nu\~{n}ez</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105:XFD105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1202,28 +1181,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1232,17 +1211,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1257,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1265,30 +1244,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D5" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E5" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E6" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1302,7 +1281,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1319,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1327,16 +1306,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D9" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1344,13 +1323,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1401,10 +1380,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E13" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1426,16 +1405,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B15" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D15" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E15" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1559,33 +1538,33 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B23" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F23" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="G23" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1593,13 +1572,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B25" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -1624,331 +1603,331 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>203</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>204</v>
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>214</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>215</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
+        <v>178</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>209</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>249</v>
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>239</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>246</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
-      <c r="D33" t="s">
-        <v>65</v>
+      <c r="D33" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>232</v>
+      </c>
+      <c r="F33" t="s">
+        <v>195</v>
+      </c>
+      <c r="G33" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>216</v>
+      <c r="D34" t="s">
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>239</v>
-      </c>
-      <c r="F34" t="s">
-        <v>202</v>
-      </c>
-      <c r="G34" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>177</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>178</v>
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
+        <v>236</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>234</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="F37" t="s">
+        <v>195</v>
+      </c>
+      <c r="G37" t="s">
+        <v>227</v>
+      </c>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>243</v>
-      </c>
-      <c r="D38" t="s">
-        <v>241</v>
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E38" t="s">
-        <v>239</v>
-      </c>
-      <c r="F38" t="s">
-        <v>202</v>
-      </c>
-      <c r="G38" t="s">
-        <v>234</v>
-      </c>
-      <c r="J38" s="4"/>
+        <v>232</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>216</v>
+      <c r="D39" t="s">
+        <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>239</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>232</v>
+      </c>
+      <c r="F40" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E41" t="s">
-        <v>239</v>
-      </c>
-      <c r="F41" t="s">
-        <v>202</v>
-      </c>
-      <c r="G41" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>189</v>
+        <v>242</v>
       </c>
       <c r="B42" t="s">
-        <v>190</v>
+        <v>243</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E42" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>250</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>251</v>
+        <v>61</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>249</v>
+      <c r="D44" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
         <v>58</v>
@@ -1957,10 +1936,10 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>233</v>
       </c>
       <c r="E46" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -1968,55 +1947,61 @@
         <v>89</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="E47" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>240</v>
+        <v>56</v>
       </c>
       <c r="E48" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
-      <c r="D49" t="s">
-        <v>65</v>
+      <c r="D49" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E49" t="s">
-        <v>47</v>
+        <v>232</v>
+      </c>
+      <c r="F49" t="s">
+        <v>226</v>
+      </c>
+      <c r="G49" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
         <v>95</v>
@@ -2025,75 +2010,66 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>242</v>
+        <v>184</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" t="s">
-        <v>5</v>
+        <v>185</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E51" t="s">
-        <v>239</v>
-      </c>
-      <c r="F51" t="s">
-        <v>233</v>
-      </c>
-      <c r="G51" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>184</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
+        <v>194</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>191</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>192</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>249</v>
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>239</v>
+      </c>
+      <c r="E53" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>201</v>
+        <v>99</v>
       </c>
       <c r="D54" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="E54" t="s">
         <v>33</v>
@@ -2101,112 +2077,112 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>246</v>
+        <v>56</v>
       </c>
       <c r="E55" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>237</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>56</v>
+        <v>238</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E57" t="s">
-        <v>57</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="E58" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="B59" t="s">
-        <v>245</v>
+        <v>204</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E59" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
         <v>110</v>
-      </c>
-      <c r="B60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" t="s">
-        <v>52</v>
-      </c>
-      <c r="E60" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>210</v>
+        <v>247</v>
       </c>
       <c r="B61" t="s">
-        <v>211</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>249</v>
+        <v>183</v>
+      </c>
+      <c r="D61" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2220,197 +2196,197 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" t="s">
         <v>114</v>
       </c>
-      <c r="B63" t="s">
-        <v>104</v>
-      </c>
       <c r="C63" t="s">
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="E63" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>255</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
       <c r="D64" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="E64" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E65" t="s">
+        <v>232</v>
+      </c>
+      <c r="F65" t="s">
+        <v>36</v>
+      </c>
+      <c r="G65" t="s">
         <v>115</v>
-      </c>
-      <c r="B65" t="s">
-        <v>116</v>
-      </c>
-      <c r="C65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" t="s">
-        <v>65</v>
-      </c>
-      <c r="E65" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B66" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E66" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>246</v>
       </c>
       <c r="B67" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
       <c r="D67" t="s">
-        <v>246</v>
+        <v>172</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="B68" t="s">
-        <v>104</v>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>216</v>
+        <v>175</v>
+      </c>
+      <c r="D68" t="s">
+        <v>32</v>
       </c>
       <c r="E68" t="s">
-        <v>239</v>
-      </c>
-      <c r="F68" t="s">
-        <v>36</v>
-      </c>
-      <c r="G68" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
-      <c r="D69" t="s">
-        <v>20</v>
+      <c r="D69" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E69" t="s">
-        <v>21</v>
+        <v>232</v>
+      </c>
+      <c r="F69" t="s">
+        <v>195</v>
+      </c>
+      <c r="G69" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>254</v>
+        <v>124</v>
       </c>
       <c r="B70" t="s">
-        <v>190</v>
+        <v>125</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>179</v>
+        <v>65</v>
       </c>
       <c r="E70" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>207</v>
+        <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>182</v>
+        <v>127</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E71" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>216</v>
+      <c r="D72" t="s">
+        <v>36</v>
       </c>
       <c r="E72" t="s">
-        <v>239</v>
-      </c>
-      <c r="F72" t="s">
-        <v>202</v>
-      </c>
-      <c r="G72" t="s">
-        <v>234</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="D73" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E73" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2421,38 +2397,38 @@
         <v>131</v>
       </c>
       <c r="C74" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E74" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>132</v>
+        <v>249</v>
       </c>
       <c r="B75" t="s">
-        <v>118</v>
-      </c>
-      <c r="C75" t="s">
-        <v>5</v>
-      </c>
-      <c r="D75" t="s">
-        <v>36</v>
+        <v>178</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E75" t="s">
-        <v>133</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B76" t="s">
-        <v>182</v>
+        <v>133</v>
+      </c>
+      <c r="C76" t="s">
+        <v>81</v>
       </c>
       <c r="D76" t="s">
         <v>32</v>
@@ -2463,180 +2439,183 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>247</v>
+        <v>186</v>
       </c>
       <c r="B77" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E77" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>134</v>
+      <c r="A78" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
-      </c>
-      <c r="C78" t="s">
-        <v>123</v>
-      </c>
-      <c r="D78" t="s">
-        <v>36</v>
+        <v>225</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E78" t="s">
-        <v>37</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C79" t="s">
-        <v>81</v>
-      </c>
-      <c r="D79" t="s">
-        <v>32</v>
-      </c>
-      <c r="E79" t="s">
-        <v>33</v>
+        <v>5</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>194</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>216</v>
+        <v>106</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>52</v>
       </c>
       <c r="E80" t="s">
-        <v>239</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>231</v>
+      <c r="A81" t="s">
+        <v>139</v>
       </c>
       <c r="B81" t="s">
-        <v>232</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>216</v>
+        <v>101</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>36</v>
       </c>
       <c r="E81" t="s">
-        <v>239</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B82" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>249</v>
+      <c r="D82" t="s">
+        <v>239</v>
+      </c>
+      <c r="E82" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E83" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
-      </c>
-      <c r="C84" t="s">
-        <v>5</v>
-      </c>
-      <c r="D84" t="s">
-        <v>142</v>
+        <v>189</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E84" t="s">
-        <v>143</v>
+        <v>232</v>
+      </c>
+      <c r="F84" t="s">
+        <v>195</v>
+      </c>
+      <c r="G84" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="E85" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B86" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="C86" t="s">
         <v>5</v>
       </c>
       <c r="D86" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E86" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="B87" t="s">
-        <v>118</v>
-      </c>
-      <c r="C87" t="s">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="D87" t="s">
-        <v>56</v>
+        <v>226</v>
       </c>
       <c r="E87" t="s">
-        <v>57</v>
+        <v>232</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2644,200 +2623,200 @@
         <v>148</v>
       </c>
       <c r="B88" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
       <c r="E88" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>195</v>
+        <v>149</v>
       </c>
       <c r="B89" t="s">
-        <v>196</v>
+        <v>135</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E89" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F89" t="s">
-        <v>202</v>
+        <v>137</v>
       </c>
       <c r="G89" t="s">
-        <v>234</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>150</v>
+      </c>
+      <c r="B90" t="s">
         <v>151</v>
       </c>
-      <c r="B90" t="s">
-        <v>100</v>
-      </c>
       <c r="C90" t="s">
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="E90" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>152</v>
+      </c>
+      <c r="B91" t="s">
         <v>153</v>
       </c>
-      <c r="B91" t="s">
-        <v>118</v>
-      </c>
       <c r="C91" t="s">
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E91" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="B92" t="s">
-        <v>187</v>
+        <v>154</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>233</v>
+        <v>65</v>
       </c>
       <c r="E92" t="s">
-        <v>239</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B93" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="C93" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="D93" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="E93" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B94" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>216</v>
+      <c r="D94" t="s">
+        <v>36</v>
       </c>
       <c r="E94" t="s">
-        <v>239</v>
-      </c>
-      <c r="F94" t="s">
-        <v>142</v>
-      </c>
-      <c r="G94" t="s">
-        <v>143</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>157</v>
-      </c>
-      <c r="C95" t="s">
-        <v>5</v>
-      </c>
-      <c r="D95" t="s">
-        <v>36</v>
-      </c>
-      <c r="E95" t="s">
-        <v>37</v>
+        <v>180</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="B96" t="s">
-        <v>159</v>
-      </c>
-      <c r="C96" t="s">
-        <v>5</v>
+        <v>193</v>
       </c>
       <c r="D96" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E96" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B97" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E97" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B98" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
       <c r="C98" t="s">
-        <v>123</v>
-      </c>
-      <c r="D98" t="s">
-        <v>246</v>
+        <v>5</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+      <c r="F98" t="s">
+        <v>143</v>
+      </c>
+      <c r="G98" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B99" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
@@ -2849,179 +2828,83 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>187</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E100" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="D101" t="s">
-        <v>65</v>
+        <v>172</v>
       </c>
       <c r="E101" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>244</v>
+      </c>
+      <c r="B102" t="s">
+        <v>245</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>166</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>167</v>
       </c>
-      <c r="C102" t="s">
-        <v>5</v>
-      </c>
-      <c r="D102" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" t="s">
+        <v>157</v>
+      </c>
+      <c r="E103" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>168</v>
       </c>
-      <c r="B103" t="s">
-        <v>118</v>
-      </c>
-      <c r="C103" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E103" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
         <v>169</v>
       </c>
-      <c r="B104" t="s">
-        <v>109</v>
-      </c>
       <c r="C104" t="s">
-        <v>5</v>
+        <v>206</v>
       </c>
       <c r="D104" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="E104" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>170</v>
-      </c>
-      <c r="B105" t="s">
-        <v>171</v>
-      </c>
-      <c r="C105" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" t="s">
-        <v>16</v>
-      </c>
-      <c r="E105" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>183</v>
-      </c>
-      <c r="B106" t="s">
-        <v>184</v>
-      </c>
-      <c r="D106" t="s">
-        <v>179</v>
-      </c>
-      <c r="E106" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>252</v>
-      </c>
-      <c r="B107" t="s">
-        <v>253</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>172</v>
-      </c>
-      <c r="B108" t="s">
-        <v>173</v>
-      </c>
-      <c r="C108" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" t="s">
-        <v>163</v>
-      </c>
-      <c r="E108" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>174</v>
-      </c>
-      <c r="B109" t="s">
-        <v>175</v>
-      </c>
-      <c r="C109" t="s">
-        <v>213</v>
-      </c>
-      <c r="D109" t="s">
-        <v>163</v>
-      </c>
-      <c r="E109" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>176</v>
-      </c>
-      <c r="B110" t="s">
-        <v>112</v>
-      </c>
-      <c r="C110" t="s">
-        <v>5</v>
-      </c>
-      <c r="D110" t="s">
-        <v>36</v>
-      </c>
-      <c r="E110" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove Rodriguez Garcia and Webb
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6B4B0A-2156-2743-9B2D-53588C0BF6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590B1FF5-40A7-D640-B2C3-1CC2CB295FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="2220" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="2220" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="245">
   <si>
     <t>LastName</t>
   </si>
@@ -283,9 +283,6 @@
     <t xml:space="preserve">Guenette                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> Centro de Investigaci\'on en Ciencias B\'asicas y Aplicadas, Universidad Antonio Nari\~no, Sede Circunvalar, Carretera 3 Este No.\ 47 A-15 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Haefner                     </t>
   </si>
   <si>
@@ -466,12 +463,6 @@
     <t xml:space="preserve"> Girona, E-17071, Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">Rodr\'iguez Garc\'ia        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bogot\'a, Colombia </t>
-  </si>
-  <si>
     <t xml:space="preserve">Rodr\'iguez                 </t>
   </si>
   <si>
@@ -527,12 +518,6 @@
   </si>
   <si>
     <t xml:space="preserve"> J.F.C.A.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Webb                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> R.        </t>
   </si>
   <si>
     <t xml:space="preserve">White                       </t>
@@ -1162,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105:XFD105"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1181,28 +1166,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1211,17 +1196,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1236,7 +1221,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1244,30 +1229,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1281,7 +1266,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1298,7 +1283,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1306,16 +1291,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1323,13 +1308,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1380,10 +1365,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E13" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1405,16 +1390,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E15" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1538,33 +1523,33 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G23" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1572,13 +1557,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B25" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D25" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -1603,16 +1588,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D27" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E27" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1651,16 +1636,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1674,7 +1659,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E31" t="s">
         <v>63</v>
@@ -1708,16 +1693,16 @@
         <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E33" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F33" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G33" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -1739,13 +1724,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E35" t="s">
         <v>33</v>
@@ -1770,22 +1755,22 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B37" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D37" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E37" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F37" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G37" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J37" s="4"/>
     </row>
@@ -1800,10 +1785,10 @@
         <v>5</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E38" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1834,44 +1819,44 @@
         <v>81</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E40" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F40" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G40" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E41" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B42" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -1885,15 +1870,15 @@
         <v>5</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
         <v>58</v>
@@ -1910,7 +1895,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -1927,7 +1912,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
         <v>58</v>
@@ -1936,18 +1921,18 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
         <v>89</v>
-      </c>
-      <c r="B47" t="s">
-        <v>90</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1961,10 +1946,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
         <v>91</v>
-      </c>
-      <c r="B48" t="s">
-        <v>92</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1978,33 +1963,33 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E49" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F49" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G49" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -2018,27 +2003,27 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B51" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B52" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D52" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E52" t="s">
         <v>33</v>
@@ -2046,16 +2031,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" t="s">
         <v>96</v>
       </c>
-      <c r="B53" t="s">
-        <v>97</v>
-      </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E53" t="s">
         <v>63</v>
@@ -2063,10 +2048,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" t="s">
         <v>98</v>
-      </c>
-      <c r="B54" t="s">
-        <v>99</v>
       </c>
       <c r="D54" t="s">
         <v>32</v>
@@ -2077,10 +2062,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
         <v>100</v>
-      </c>
-      <c r="B55" t="s">
-        <v>101</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -2094,41 +2079,41 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" t="s">
         <v>102</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
         <v>103</v>
       </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>104</v>
-      </c>
-      <c r="E56" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B57" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E57" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -2142,24 +2127,24 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B59" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" t="s">
         <v>108</v>
-      </c>
-      <c r="B60" t="s">
-        <v>109</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -2168,18 +2153,18 @@
         <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E61" t="s">
         <v>33</v>
@@ -2187,10 +2172,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" t="s">
         <v>111</v>
-      </c>
-      <c r="B62" t="s">
-        <v>112</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -2204,10 +2189,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" t="s">
         <v>113</v>
-      </c>
-      <c r="B63" t="s">
-        <v>114</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -2216,18 +2201,18 @@
         <v>36</v>
       </c>
       <c r="E63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
         <v>116</v>
       </c>
-      <c r="B64" t="s">
-        <v>117</v>
-      </c>
       <c r="D64" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2235,33 +2220,33 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E65" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F65" t="s">
         <v>36</v>
       </c>
       <c r="G65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" t="s">
         <v>120</v>
-      </c>
-      <c r="B66" t="s">
-        <v>121</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -2275,13 +2260,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B67" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D67" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E67" t="s">
         <v>33</v>
@@ -2289,10 +2274,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B68" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D68" t="s">
         <v>32</v>
@@ -2303,33 +2288,33 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" t="s">
         <v>122</v>
       </c>
-      <c r="B69" t="s">
-        <v>123</v>
-      </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E69" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F69" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G69" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" t="s">
         <v>124</v>
-      </c>
-      <c r="B70" t="s">
-        <v>125</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2343,10 +2328,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>125</v>
+      </c>
+      <c r="B71" t="s">
         <v>126</v>
-      </c>
-      <c r="B71" t="s">
-        <v>127</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2360,10 +2345,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2372,15 +2357,15 @@
         <v>36</v>
       </c>
       <c r="E72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B73" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D73" t="s">
         <v>32</v>
@@ -2391,13 +2376,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" t="s">
         <v>130</v>
       </c>
-      <c r="B74" t="s">
-        <v>131</v>
-      </c>
       <c r="C74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D74" t="s">
         <v>36</v>
@@ -2408,24 +2393,24 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B75" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E75" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>131</v>
+      </c>
+      <c r="B76" t="s">
         <v>132</v>
-      </c>
-      <c r="B76" t="s">
-        <v>133</v>
       </c>
       <c r="C76" t="s">
         <v>81</v>
@@ -2439,55 +2424,55 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E77" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B78" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E78" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" t="s">
         <v>134</v>
       </c>
-      <c r="B79" t="s">
-        <v>135</v>
-      </c>
       <c r="C79" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -2501,10 +2486,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
@@ -2518,16 +2503,16 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" t="s">
         <v>140</v>
       </c>
-      <c r="B82" t="s">
-        <v>141</v>
-      </c>
       <c r="C82" t="s">
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
@@ -2535,10 +2520,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B83" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
@@ -2552,141 +2537,141 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B84" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E84" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F84" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G84" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="E85" t="s">
-        <v>146</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
-        <v>114</v>
-      </c>
-      <c r="C86" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="D86" t="s">
-        <v>6</v>
+        <v>221</v>
       </c>
       <c r="E86" t="s">
-        <v>7</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
       <c r="B87" t="s">
-        <v>180</v>
+        <v>102</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
       </c>
       <c r="D87" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="E87" t="s">
-        <v>232</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B88" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
       </c>
-      <c r="D88" t="s">
-        <v>216</v>
+      <c r="D88" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="E88" t="s">
-        <v>21</v>
+        <v>227</v>
+      </c>
+      <c r="F88" t="s">
+        <v>136</v>
+      </c>
+      <c r="G88" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>209</v>
+      <c r="D89" t="s">
+        <v>36</v>
       </c>
       <c r="E89" t="s">
-        <v>232</v>
-      </c>
-      <c r="F89" t="s">
-        <v>137</v>
-      </c>
-      <c r="G89" t="s">
-        <v>138</v>
+        <v>37</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>149</v>
+      </c>
+      <c r="B90" t="s">
         <v>150</v>
       </c>
-      <c r="B90" t="s">
-        <v>151</v>
-      </c>
       <c r="C90" t="s">
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E90" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B91" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E91" t="s">
         <v>47</v>
@@ -2697,214 +2682,180 @@
         <v>152</v>
       </c>
       <c r="B92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C92" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="D92" t="s">
-        <v>65</v>
+        <v>234</v>
       </c>
       <c r="E92" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B93" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="C93" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>239</v>
+        <v>36</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="B94" t="s">
-        <v>101</v>
-      </c>
-      <c r="C94" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" t="s">
-        <v>36</v>
-      </c>
-      <c r="E94" t="s">
-        <v>37</v>
+        <v>175</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B95" t="s">
-        <v>180</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>241</v>
+        <v>188</v>
+      </c>
+      <c r="D95" t="s">
+        <v>65</v>
+      </c>
+      <c r="E95" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="B96" t="s">
-        <v>193</v>
+        <v>158</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E96" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B97" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
       </c>
-      <c r="D97" t="s">
-        <v>6</v>
+      <c r="D97" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="E97" t="s">
-        <v>7</v>
+        <v>227</v>
+      </c>
+      <c r="F97" t="s">
+        <v>142</v>
+      </c>
+      <c r="G97" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B98" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>209</v>
+      <c r="D98" t="s">
+        <v>36</v>
       </c>
       <c r="E98" t="s">
-        <v>232</v>
-      </c>
-      <c r="F98" t="s">
-        <v>143</v>
-      </c>
-      <c r="G98" t="s">
-        <v>144</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B99" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E99" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B100" t="s">
-        <v>165</v>
-      </c>
-      <c r="C100" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
       <c r="D100" t="s">
-        <v>16</v>
+        <v>167</v>
       </c>
       <c r="E100" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>239</v>
       </c>
       <c r="B101" t="s">
-        <v>177</v>
-      </c>
-      <c r="D101" t="s">
-        <v>172</v>
-      </c>
-      <c r="E101" t="s">
-        <v>33</v>
+        <v>240</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>244</v>
+        <v>163</v>
       </c>
       <c r="B102" t="s">
-        <v>245</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>166</v>
-      </c>
-      <c r="B103" t="s">
-        <v>167</v>
-      </c>
-      <c r="C103" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" t="s">
-        <v>157</v>
-      </c>
-      <c r="E103" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>168</v>
-      </c>
-      <c r="B104" t="s">
-        <v>169</v>
-      </c>
-      <c r="C104" t="s">
-        <v>206</v>
-      </c>
-      <c r="D104" t="s">
-        <v>157</v>
-      </c>
-      <c r="E104" t="s">
-        <v>158</v>
+        <v>164</v>
+      </c>
+      <c r="C102" t="s">
+        <v>201</v>
+      </c>
+      <c r="D102" t="s">
+        <v>154</v>
+      </c>
+      <c r="E102" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove NEXT Co-spokesperson footnote to D. Nygren
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590B1FF5-40A7-D640-B2C3-1CC2CB295FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4401811-F9CB-5F47-B850-DBE1EB476F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="2220" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="245">
   <si>
     <t>LastName</t>
   </si>
@@ -274,9 +274,6 @@
     <t xml:space="preserve"> J.J.       </t>
   </si>
   <si>
-    <t xml:space="preserve"> NEXT Co-spokesperson. </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Santiago de Compostela, E-15782, Spain</t>
   </si>
   <si>
@@ -764,6 +761,9 @@
   </si>
   <si>
     <t>Nu\~{n}ez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEXT Spokesperson. </t>
   </si>
 </sst>
 </file>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85:XFD85"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1166,28 +1166,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1196,17 +1196,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1221,7 +1221,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1229,30 +1229,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" t="s">
         <v>214</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>215</v>
       </c>
-      <c r="D5" t="s">
-        <v>216</v>
-      </c>
       <c r="E5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" t="s">
         <v>217</v>
       </c>
-      <c r="B6" t="s">
-        <v>218</v>
-      </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1266,7 +1266,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1283,7 +1283,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1291,16 +1291,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" t="s">
         <v>193</v>
       </c>
-      <c r="B9" t="s">
-        <v>194</v>
-      </c>
       <c r="D9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" t="s">
         <v>202</v>
-      </c>
-      <c r="E9" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1308,13 +1308,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1365,10 +1365,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1390,16 +1390,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E15" t="s">
         <v>235</v>
-      </c>
-      <c r="E15" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1523,33 +1523,33 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23" t="s">
         <v>212</v>
       </c>
-      <c r="B23" t="s">
-        <v>213</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -1588,16 +1588,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" t="s">
         <v>191</v>
       </c>
-      <c r="B27" t="s">
-        <v>192</v>
-      </c>
       <c r="D27" t="s">
+        <v>201</v>
+      </c>
+      <c r="E27" t="s">
         <v>202</v>
-      </c>
-      <c r="E27" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1636,16 +1636,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1659,7 +1659,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E31" t="s">
         <v>63</v>
@@ -1693,16 +1693,16 @@
         <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -1724,13 +1724,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" t="s">
         <v>165</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>166</v>
-      </c>
-      <c r="D35" t="s">
-        <v>167</v>
       </c>
       <c r="E35" t="s">
         <v>33</v>
@@ -1755,22 +1755,22 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J37" s="4"/>
     </row>
@@ -1785,10 +1785,10 @@
         <v>5</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1816,52 +1816,52 @@
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>244</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>176</v>
+      </c>
+      <c r="B41" t="s">
         <v>177</v>
       </c>
-      <c r="B41" t="s">
-        <v>178</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>236</v>
+      </c>
+      <c r="B42" t="s">
         <v>237</v>
       </c>
-      <c r="B42" t="s">
-        <v>238</v>
-      </c>
       <c r="D42" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
         <v>61</v>
@@ -1870,15 +1870,15 @@
         <v>5</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
         <v>58</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
         <v>58</v>
@@ -1921,18 +1921,18 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" t="s">
         <v>88</v>
-      </c>
-      <c r="B47" t="s">
-        <v>89</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" t="s">
         <v>90</v>
-      </c>
-      <c r="B48" t="s">
-        <v>91</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1958,38 +1958,38 @@
         <v>56</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -2003,27 +2003,27 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51" t="s">
         <v>179</v>
       </c>
-      <c r="B51" t="s">
-        <v>180</v>
-      </c>
       <c r="D51" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E52" t="s">
         <v>33</v>
@@ -2031,16 +2031,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" t="s">
         <v>95</v>
       </c>
-      <c r="B53" t="s">
-        <v>96</v>
-      </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E53" t="s">
         <v>63</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
         <v>97</v>
-      </c>
-      <c r="B54" t="s">
-        <v>98</v>
       </c>
       <c r="D54" t="s">
         <v>32</v>
@@ -2062,10 +2062,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" t="s">
         <v>99</v>
-      </c>
-      <c r="B55" t="s">
-        <v>100</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -2079,41 +2079,41 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
         <v>101</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
         <v>102</v>
       </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>103</v>
-      </c>
-      <c r="E56" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>231</v>
+      </c>
+      <c r="B57" t="s">
         <v>232</v>
       </c>
-      <c r="B57" t="s">
-        <v>233</v>
-      </c>
       <c r="D57" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -2127,24 +2127,24 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>197</v>
+      </c>
+      <c r="B59" t="s">
         <v>198</v>
       </c>
-      <c r="B59" t="s">
-        <v>199</v>
-      </c>
       <c r="D59" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" t="s">
         <v>107</v>
-      </c>
-      <c r="B60" t="s">
-        <v>108</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -2153,18 +2153,18 @@
         <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E61" t="s">
         <v>33</v>
@@ -2172,10 +2172,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
         <v>110</v>
-      </c>
-      <c r="B62" t="s">
-        <v>111</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -2189,10 +2189,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
         <v>112</v>
-      </c>
-      <c r="B63" t="s">
-        <v>113</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -2201,18 +2201,18 @@
         <v>36</v>
       </c>
       <c r="E63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" t="s">
         <v>115</v>
       </c>
-      <c r="B64" t="s">
-        <v>116</v>
-      </c>
       <c r="D64" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2220,33 +2220,33 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B65" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F65" t="s">
         <v>36</v>
       </c>
       <c r="G65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" t="s">
         <v>119</v>
-      </c>
-      <c r="B66" t="s">
-        <v>120</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E67" t="s">
         <v>33</v>
@@ -2274,10 +2274,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D68" t="s">
         <v>32</v>
@@ -2288,33 +2288,33 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" t="s">
         <v>121</v>
       </c>
-      <c r="B69" t="s">
-        <v>122</v>
-      </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E69" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" t="s">
         <v>123</v>
-      </c>
-      <c r="B70" t="s">
-        <v>124</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" t="s">
         <v>125</v>
-      </c>
-      <c r="B71" t="s">
-        <v>126</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2345,10 +2345,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2357,15 +2357,15 @@
         <v>36</v>
       </c>
       <c r="E72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" t="s">
         <v>169</v>
-      </c>
-      <c r="B73" t="s">
-        <v>170</v>
       </c>
       <c r="D73" t="s">
         <v>32</v>
@@ -2376,13 +2376,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" t="s">
         <v>129</v>
       </c>
-      <c r="B74" t="s">
-        <v>130</v>
-      </c>
       <c r="C74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D74" t="s">
         <v>36</v>
@@ -2393,27 +2393,24 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B75" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>130</v>
+      </c>
+      <c r="B76" t="s">
         <v>131</v>
-      </c>
-      <c r="B76" t="s">
-        <v>132</v>
-      </c>
-      <c r="C76" t="s">
-        <v>81</v>
       </c>
       <c r="D76" t="s">
         <v>32</v>
@@ -2424,55 +2421,55 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" t="s">
         <v>181</v>
       </c>
-      <c r="B77" t="s">
-        <v>182</v>
-      </c>
       <c r="D77" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B78" t="s">
         <v>219</v>
       </c>
-      <c r="B78" t="s">
-        <v>220</v>
-      </c>
       <c r="D78" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E78" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>132</v>
+      </c>
+      <c r="B79" t="s">
         <v>133</v>
       </c>
-      <c r="B79" t="s">
-        <v>134</v>
-      </c>
       <c r="C79" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -2486,10 +2483,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
@@ -2503,16 +2500,16 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>138</v>
+      </c>
+      <c r="B82" t="s">
         <v>139</v>
       </c>
-      <c r="B82" t="s">
-        <v>140</v>
-      </c>
       <c r="C82" t="s">
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
@@ -2520,10 +2517,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
@@ -2537,30 +2534,30 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" t="s">
         <v>183</v>
       </c>
-      <c r="B84" t="s">
-        <v>184</v>
-      </c>
       <c r="D84" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E84" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G84" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
@@ -2574,30 +2571,30 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D86" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E86" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
       </c>
       <c r="D87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E87" t="s">
         <v>21</v>
@@ -2605,33 +2602,33 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B88" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F88" t="s">
+        <v>135</v>
+      </c>
+      <c r="G88" t="s">
         <v>136</v>
-      </c>
-      <c r="G88" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89" t="s">
         <v>147</v>
-      </c>
-      <c r="B89" t="s">
-        <v>148</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -2645,10 +2642,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>148</v>
+      </c>
+      <c r="B90" t="s">
         <v>149</v>
-      </c>
-      <c r="B90" t="s">
-        <v>150</v>
       </c>
       <c r="C90" t="s">
         <v>5</v>
@@ -2662,10 +2659,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
@@ -2679,16 +2676,16 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>151</v>
+      </c>
+      <c r="B92" t="s">
         <v>152</v>
       </c>
-      <c r="B92" t="s">
-        <v>153</v>
-      </c>
       <c r="C92" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D92" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E92" t="s">
         <v>10</v>
@@ -2696,10 +2693,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C93" t="s">
         <v>5</v>
@@ -2713,24 +2710,24 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B94" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D94" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" t="s">
         <v>187</v>
-      </c>
-      <c r="B95" t="s">
-        <v>188</v>
       </c>
       <c r="D95" t="s">
         <v>65</v>
@@ -2741,10 +2738,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>156</v>
+      </c>
+      <c r="B96" t="s">
         <v>157</v>
-      </c>
-      <c r="B96" t="s">
-        <v>158</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -2758,33 +2755,33 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E97" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F97" t="s">
+        <v>141</v>
+      </c>
+      <c r="G97" t="s">
         <v>142</v>
-      </c>
-      <c r="G97" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B98" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
@@ -2798,10 +2795,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" t="s">
         <v>161</v>
-      </c>
-      <c r="B99" t="s">
-        <v>162</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
@@ -2815,13 +2812,13 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>170</v>
+      </c>
+      <c r="B100" t="s">
         <v>171</v>
       </c>
-      <c r="B100" t="s">
-        <v>172</v>
-      </c>
       <c r="D100" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E100" t="s">
         <v>33</v>
@@ -2829,33 +2826,33 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>238</v>
+      </c>
+      <c r="B101" t="s">
         <v>239</v>
       </c>
-      <c r="B101" t="s">
-        <v>240</v>
-      </c>
       <c r="D101" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E101" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>162</v>
+      </c>
+      <c r="B102" t="s">
         <v>163</v>
       </c>
-      <c r="B102" t="s">
-        <v>164</v>
-      </c>
       <c r="C102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D102" t="s">
+        <v>153</v>
+      </c>
+      <c r="E102" t="s">
         <v>154</v>
-      </c>
-      <c r="E102" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates in santiago: kekic out, herves and perez in
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4401811-F9CB-5F47-B850-DBE1EB476F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B42EA30-C1AA-384E-8EEB-11B61603492E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="2220" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="246">
   <si>
     <t>LastName</t>
   </si>
@@ -325,9 +325,6 @@
     <t xml:space="preserve"> B.J.P.    </t>
   </si>
   <si>
-    <t xml:space="preserve">Kekic                       </t>
-  </si>
-  <si>
     <t xml:space="preserve"> M.        </t>
   </si>
   <si>
@@ -764,6 +761,12 @@
   </si>
   <si>
     <t xml:space="preserve">NEXT Spokesperson. </t>
+  </si>
+  <si>
+    <t>Herv\'es Carrete</t>
+  </si>
+  <si>
+    <t>P\'erez Maneiro</t>
   </si>
 </sst>
 </file>
@@ -1147,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1166,28 +1169,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1196,17 +1199,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1221,7 +1224,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1229,30 +1232,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
         <v>213</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>214</v>
       </c>
-      <c r="D5" t="s">
-        <v>215</v>
-      </c>
       <c r="E5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
         <v>216</v>
       </c>
-      <c r="B6" t="s">
-        <v>217</v>
-      </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1266,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1283,7 +1286,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1291,16 +1294,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" t="s">
         <v>192</v>
       </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
       <c r="D9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" t="s">
         <v>201</v>
-      </c>
-      <c r="E9" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1308,13 +1311,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1365,10 +1368,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1390,16 +1393,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
+        <v>233</v>
+      </c>
+      <c r="E15" t="s">
         <v>234</v>
-      </c>
-      <c r="E15" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1523,33 +1526,33 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23" t="s">
         <v>211</v>
       </c>
-      <c r="B23" t="s">
-        <v>212</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1557,13 +1560,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -1588,16 +1591,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" t="s">
         <v>190</v>
       </c>
-      <c r="B27" t="s">
-        <v>191</v>
-      </c>
       <c r="D27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E27" t="s">
         <v>201</v>
-      </c>
-      <c r="E27" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1636,16 +1639,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1659,7 +1662,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E31" t="s">
         <v>63</v>
@@ -1693,16 +1696,16 @@
         <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -1724,13 +1727,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" t="s">
         <v>164</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>165</v>
-      </c>
-      <c r="D35" t="s">
-        <v>166</v>
       </c>
       <c r="E35" t="s">
         <v>33</v>
@@ -1755,22 +1758,22 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F37" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J37" s="4"/>
     </row>
@@ -1785,10 +1788,10 @@
         <v>5</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1816,47 +1819,47 @@
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>175</v>
+      </c>
+      <c r="B41" t="s">
         <v>176</v>
       </c>
-      <c r="B41" t="s">
-        <v>177</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>235</v>
+      </c>
+      <c r="B42" t="s">
         <v>236</v>
       </c>
-      <c r="B42" t="s">
-        <v>237</v>
-      </c>
       <c r="D42" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -1870,10 +1873,10 @@
         <v>5</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -1921,7 +1924,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E46" t="s">
         <v>86</v>
@@ -1963,7 +1966,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B49" t="s">
         <v>92</v>
@@ -1972,16 +1975,16 @@
         <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2003,114 +2006,111 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>244</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>235</v>
+        <v>173</v>
+      </c>
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>177</v>
+      </c>
+      <c r="B52" t="s">
         <v>178</v>
       </c>
-      <c r="B52" t="s">
-        <v>188</v>
-      </c>
-      <c r="D52" t="s">
-        <v>166</v>
-      </c>
-      <c r="E52" t="s">
-        <v>33</v>
+      <c r="D52" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
-      </c>
-      <c r="C53" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="D53" t="s">
-        <v>233</v>
+        <v>165</v>
       </c>
       <c r="E53" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>32</v>
+        <v>232</v>
       </c>
       <c r="E54" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="E55" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" t="s">
         <v>100</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
         <v>101</v>
       </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>102</v>
-      </c>
-      <c r="E56" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>230</v>
+      </c>
+      <c r="B57" t="s">
         <v>231</v>
       </c>
-      <c r="B57" t="s">
-        <v>232</v>
-      </c>
       <c r="D57" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" t="s">
         <v>92</v>
@@ -2127,24 +2127,24 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59" t="s">
         <v>197</v>
       </c>
-      <c r="B59" t="s">
-        <v>198</v>
-      </c>
       <c r="D59" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s">
         <v>106</v>
-      </c>
-      <c r="B60" t="s">
-        <v>107</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -2153,18 +2153,18 @@
         <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E61" t="s">
         <v>33</v>
@@ -2172,10 +2172,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>108</v>
+      </c>
+      <c r="B62" t="s">
         <v>109</v>
-      </c>
-      <c r="B62" t="s">
-        <v>110</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -2189,10 +2189,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
         <v>111</v>
-      </c>
-      <c r="B63" t="s">
-        <v>112</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -2201,18 +2201,18 @@
         <v>36</v>
       </c>
       <c r="E63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" t="s">
         <v>114</v>
       </c>
-      <c r="B64" t="s">
-        <v>115</v>
-      </c>
       <c r="D64" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2220,33 +2220,33 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E65" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F65" t="s">
         <v>36</v>
       </c>
       <c r="G65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" t="s">
         <v>118</v>
-      </c>
-      <c r="B66" t="s">
-        <v>119</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E67" t="s">
         <v>33</v>
@@ -2274,10 +2274,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
         <v>32</v>
@@ -2288,33 +2288,33 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>119</v>
+      </c>
+      <c r="B69" t="s">
         <v>120</v>
       </c>
-      <c r="B69" t="s">
-        <v>121</v>
-      </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F69" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G69" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" t="s">
         <v>122</v>
-      </c>
-      <c r="B70" t="s">
-        <v>123</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" t="s">
         <v>124</v>
-      </c>
-      <c r="B71" t="s">
-        <v>125</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2345,10 +2345,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2357,15 +2357,15 @@
         <v>36</v>
       </c>
       <c r="E72" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" t="s">
         <v>168</v>
-      </c>
-      <c r="B73" t="s">
-        <v>169</v>
       </c>
       <c r="D73" t="s">
         <v>32</v>
@@ -2376,13 +2376,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" t="s">
         <v>128</v>
       </c>
-      <c r="B74" t="s">
-        <v>129</v>
-      </c>
       <c r="C74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D74" t="s">
         <v>36</v>
@@ -2393,24 +2393,24 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B75" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" t="s">
         <v>130</v>
-      </c>
-      <c r="B76" t="s">
-        <v>131</v>
       </c>
       <c r="D76" t="s">
         <v>32</v>
@@ -2421,55 +2421,55 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" t="s">
         <v>180</v>
       </c>
-      <c r="B77" t="s">
-        <v>181</v>
-      </c>
       <c r="D77" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B78" t="s">
         <v>218</v>
       </c>
-      <c r="B78" t="s">
-        <v>219</v>
-      </c>
       <c r="D78" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E78" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>131</v>
+      </c>
+      <c r="B79" t="s">
         <v>132</v>
       </c>
-      <c r="B79" t="s">
-        <v>133</v>
-      </c>
       <c r="C79" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -2483,192 +2483,189 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>137</v>
+        <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" t="s">
-        <v>5</v>
+        <v>218</v>
       </c>
       <c r="D81" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E81" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B82" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>233</v>
+        <v>36</v>
       </c>
       <c r="E82" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B83" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>56</v>
+        <v>232</v>
       </c>
       <c r="E83" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>182</v>
+        <v>139</v>
       </c>
       <c r="B84" t="s">
-        <v>183</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>203</v>
+        <v>111</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>56</v>
       </c>
       <c r="E84" t="s">
-        <v>226</v>
-      </c>
-      <c r="F84" t="s">
-        <v>189</v>
-      </c>
-      <c r="G84" t="s">
-        <v>221</v>
+        <v>57</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="B85" t="s">
-        <v>112</v>
-      </c>
-      <c r="C85" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" t="s">
-        <v>6</v>
+        <v>182</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="E85" t="s">
-        <v>7</v>
+        <v>225</v>
+      </c>
+      <c r="F85" t="s">
+        <v>188</v>
+      </c>
+      <c r="G85" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
       <c r="B86" t="s">
-        <v>174</v>
+        <v>111</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
       </c>
       <c r="D86" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
       <c r="E86" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="B87" t="s">
-        <v>101</v>
-      </c>
-      <c r="C87" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="D87" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="E87" t="s">
-        <v>21</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B88" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>203</v>
+      <c r="D88" t="s">
+        <v>209</v>
       </c>
       <c r="E88" t="s">
-        <v>226</v>
-      </c>
-      <c r="F88" t="s">
-        <v>135</v>
-      </c>
-      <c r="G88" t="s">
-        <v>136</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B89" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
       </c>
-      <c r="D89" t="s">
-        <v>36</v>
+      <c r="D89" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="E89" t="s">
-        <v>37</v>
+        <v>225</v>
+      </c>
+      <c r="F89" t="s">
+        <v>134</v>
+      </c>
+      <c r="G89" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B90" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C90" t="s">
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E90" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>147</v>
+      </c>
+      <c r="B91" t="s">
         <v>148</v>
       </c>
-      <c r="B91" t="s">
-        <v>150</v>
-      </c>
       <c r="C91" t="s">
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="E91" t="s">
         <v>47</v>
@@ -2676,183 +2673,200 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B92" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C92" t="s">
-        <v>117</v>
+        <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>233</v>
+        <v>65</v>
       </c>
       <c r="E92" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C93" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="D93" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
       <c r="E93" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
       <c r="B94" t="s">
-        <v>174</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>235</v>
+        <v>98</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
-      </c>
-      <c r="D95" t="s">
-        <v>65</v>
-      </c>
-      <c r="E95" t="s">
-        <v>47</v>
+        <v>173</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>157</v>
-      </c>
-      <c r="C96" t="s">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="D96" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="E96" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B97" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>203</v>
+      <c r="D97" t="s">
+        <v>6</v>
       </c>
       <c r="E97" t="s">
-        <v>226</v>
-      </c>
-      <c r="F97" t="s">
-        <v>141</v>
-      </c>
-      <c r="G97" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B98" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
       </c>
-      <c r="D98" t="s">
-        <v>36</v>
+      <c r="D98" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="E98" t="s">
-        <v>37</v>
+        <v>225</v>
+      </c>
+      <c r="F98" t="s">
+        <v>140</v>
+      </c>
+      <c r="G98" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B99" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E99" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B100" t="s">
-        <v>171</v>
+        <v>160</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>166</v>
+        <v>16</v>
       </c>
       <c r="E100" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="B101" t="s">
-        <v>239</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>235</v>
+        <v>170</v>
+      </c>
+      <c r="D101" t="s">
+        <v>165</v>
+      </c>
+      <c r="E101" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>237</v>
+      </c>
+      <c r="B102" t="s">
+        <v>238</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>161</v>
+      </c>
+      <c r="B103" t="s">
         <v>162</v>
       </c>
-      <c r="B102" t="s">
-        <v>163</v>
-      </c>
-      <c r="C102" t="s">
-        <v>200</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="C103" t="s">
+        <v>199</v>
+      </c>
+      <c r="D103" t="s">
+        <v>152</v>
+      </c>
+      <c r="E103" t="s">
         <v>153</v>
-      </c>
-      <c r="E102" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add weizmann footnote for r. felkai, add s.r. soleti at dipc
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B42EA30-C1AA-384E-8EEB-11B61603492E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3495019-B473-4046-ACE0-6D9395658E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="5400" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="249">
   <si>
     <t>LastName</t>
   </si>
@@ -767,6 +767,15 @@
   </si>
   <si>
     <t>P\'erez Maneiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Now at Weizmann Institute of Science, Israel.</t>
+  </si>
+  <si>
+    <t>Soleti</t>
+  </si>
+  <si>
+    <t>S.R.</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K84" sqref="K84"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1659,7 +1668,7 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>246</v>
       </c>
       <c r="D31" t="s">
         <v>232</v>
@@ -2707,165 +2716,179 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>247</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
-      </c>
-      <c r="C94" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" t="s">
-        <v>36</v>
+        <v>248</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="E94" t="s">
-        <v>37</v>
+        <v>225</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B95" t="s">
-        <v>173</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>234</v>
+        <v>98</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E95" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B96" t="s">
-        <v>186</v>
-      </c>
-      <c r="D96" t="s">
-        <v>65</v>
-      </c>
-      <c r="E96" t="s">
-        <v>47</v>
+        <v>173</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="B97" t="s">
-        <v>156</v>
-      </c>
-      <c r="C97" t="s">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="D97" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="E97" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>202</v>
+      <c r="D98" t="s">
+        <v>6</v>
       </c>
       <c r="E98" t="s">
-        <v>225</v>
-      </c>
-      <c r="F98" t="s">
-        <v>140</v>
-      </c>
-      <c r="G98" t="s">
-        <v>141</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
       </c>
-      <c r="D99" t="s">
-        <v>36</v>
+      <c r="D99" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="E99" t="s">
-        <v>37</v>
+        <v>225</v>
+      </c>
+      <c r="F99" t="s">
+        <v>140</v>
+      </c>
+      <c r="G99" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B100" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E100" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B101" t="s">
-        <v>170</v>
+        <v>160</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>165</v>
+        <v>16</v>
       </c>
       <c r="E101" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>237</v>
+        <v>169</v>
       </c>
       <c r="B102" t="s">
-        <v>238</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>234</v>
+        <v>170</v>
+      </c>
+      <c r="D102" t="s">
+        <v>165</v>
+      </c>
+      <c r="E102" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>237</v>
+      </c>
+      <c r="B103" t="s">
+        <v>238</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>161</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>162</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>199</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>152</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E104" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change affiliation for ander simon
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11607FFB-2E24-8740-9D18-B5B1D7624817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D3C6C5-C07D-BD46-8D85-651CAF454DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="2360" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2727,11 +2727,11 @@
       <c r="C94" t="s">
         <v>116</v>
       </c>
-      <c r="D94" t="s">
-        <v>232</v>
+      <c r="D94" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="E94" t="s">
-        <v>10</v>
+        <v>225</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
change affiliation for neus lopez
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D3C6C5-C07D-BD46-8D85-651CAF454DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB539C19-3AFF-7443-B0CB-A5D06E7FDF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="2360" windowWidth="31480" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="250">
   <si>
     <t>LastName</t>
   </si>
@@ -350,9 +350,6 @@
   </si>
   <si>
     <t xml:space="preserve"> N.        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Valencia, E-46022, Spain </t>
   </si>
   <si>
     <t xml:space="preserve">Mano                        </t>
@@ -1167,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1184,28 +1181,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1214,17 +1211,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1239,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1247,30 +1244,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
         <v>212</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>213</v>
       </c>
-      <c r="D5" t="s">
-        <v>214</v>
-      </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" t="s">
         <v>215</v>
       </c>
-      <c r="B6" t="s">
-        <v>216</v>
-      </c>
       <c r="D6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1284,7 +1281,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1301,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1309,16 +1306,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
         <v>191</v>
       </c>
-      <c r="B9" t="s">
-        <v>192</v>
-      </c>
       <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" t="s">
         <v>200</v>
-      </c>
-      <c r="E9" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1326,13 +1323,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1383,10 +1380,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1408,16 +1405,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
+        <v>232</v>
+      </c>
+      <c r="E15" t="s">
         <v>233</v>
-      </c>
-      <c r="E15" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1541,33 +1538,33 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>209</v>
+      </c>
+      <c r="B23" t="s">
         <v>210</v>
       </c>
-      <c r="B23" t="s">
-        <v>211</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1575,13 +1572,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -1606,16 +1603,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B27" t="s">
         <v>189</v>
       </c>
-      <c r="B27" t="s">
-        <v>190</v>
-      </c>
       <c r="D27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E27" t="s">
         <v>200</v>
-      </c>
-      <c r="E27" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1654,16 +1651,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1674,10 +1671,10 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E31" t="s">
         <v>63</v>
@@ -1711,16 +1708,16 @@
         <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -1742,13 +1739,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" t="s">
         <v>163</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>164</v>
-      </c>
-      <c r="D35" t="s">
-        <v>165</v>
       </c>
       <c r="E35" t="s">
         <v>33</v>
@@ -1773,22 +1770,22 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J37" s="4"/>
     </row>
@@ -1803,10 +1800,10 @@
         <v>5</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1834,47 +1831,47 @@
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" t="s">
         <v>175</v>
       </c>
-      <c r="B41" t="s">
-        <v>176</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" t="s">
         <v>235</v>
       </c>
-      <c r="B42" t="s">
-        <v>236</v>
-      </c>
       <c r="D42" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -1888,10 +1885,10 @@
         <v>5</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -1939,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E46" t="s">
         <v>86</v>
@@ -1981,7 +1978,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B49" t="s">
         <v>92</v>
@@ -1990,16 +1987,16 @@
         <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2021,10 +2018,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
         <v>56</v>
@@ -2035,27 +2032,27 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" t="s">
         <v>177</v>
       </c>
-      <c r="B52" t="s">
-        <v>178</v>
-      </c>
       <c r="D52" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E53" t="s">
         <v>33</v>
@@ -2072,7 +2069,7 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E54" t="s">
         <v>63</v>
@@ -2111,16 +2108,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" t="s">
         <v>230</v>
       </c>
-      <c r="B57" t="s">
-        <v>231</v>
-      </c>
       <c r="D57" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2142,16 +2139,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" t="s">
         <v>196</v>
       </c>
-      <c r="B59" t="s">
-        <v>197</v>
-      </c>
       <c r="D59" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2165,21 +2162,21 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E60" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E61" t="s">
         <v>33</v>
@@ -2187,10 +2184,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" t="s">
         <v>108</v>
-      </c>
-      <c r="B62" t="s">
-        <v>109</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -2204,10 +2201,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>248</v>
+      </c>
+      <c r="B63" t="s">
         <v>249</v>
-      </c>
-      <c r="B63" t="s">
-        <v>250</v>
       </c>
       <c r="D63" t="s">
         <v>28</v>
@@ -2218,10 +2215,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" t="s">
         <v>110</v>
-      </c>
-      <c r="B64" t="s">
-        <v>111</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -2230,18 +2227,18 @@
         <v>36</v>
       </c>
       <c r="E64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" t="s">
         <v>113</v>
       </c>
-      <c r="B65" t="s">
-        <v>114</v>
-      </c>
       <c r="D65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E65" t="s">
         <v>10</v>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B66" t="s">
         <v>98</v>
@@ -2258,24 +2255,24 @@
         <v>5</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E66" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F66" t="s">
         <v>36</v>
       </c>
       <c r="G66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" t="s">
         <v>117</v>
-      </c>
-      <c r="B67" t="s">
-        <v>118</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -2289,13 +2286,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D68" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E68" t="s">
         <v>33</v>
@@ -2303,10 +2300,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D69" t="s">
         <v>32</v>
@@ -2317,33 +2314,33 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" t="s">
         <v>119</v>
       </c>
-      <c r="B70" t="s">
-        <v>120</v>
-      </c>
       <c r="C70" t="s">
         <v>5</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G70" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" t="s">
         <v>121</v>
-      </c>
-      <c r="B71" t="s">
-        <v>122</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -2357,10 +2354,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" t="s">
         <v>123</v>
-      </c>
-      <c r="B72" t="s">
-        <v>124</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2374,10 +2371,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
@@ -2386,15 +2383,15 @@
         <v>36</v>
       </c>
       <c r="E73" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>166</v>
+      </c>
+      <c r="B74" t="s">
         <v>167</v>
-      </c>
-      <c r="B74" t="s">
-        <v>168</v>
       </c>
       <c r="D74" t="s">
         <v>32</v>
@@ -2405,13 +2402,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>126</v>
+      </c>
+      <c r="B75" t="s">
         <v>127</v>
       </c>
-      <c r="B75" t="s">
-        <v>128</v>
-      </c>
       <c r="C75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D75" t="s">
         <v>36</v>
@@ -2422,24 +2419,24 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B77" t="s">
         <v>129</v>
-      </c>
-      <c r="B77" t="s">
-        <v>130</v>
       </c>
       <c r="D77" t="s">
         <v>32</v>
@@ -2450,52 +2447,52 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>178</v>
+      </c>
+      <c r="B78" t="s">
         <v>179</v>
       </c>
-      <c r="B78" t="s">
-        <v>180</v>
-      </c>
       <c r="D78" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B79" t="s">
         <v>217</v>
       </c>
-      <c r="B79" t="s">
-        <v>218</v>
-      </c>
       <c r="D79" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E79" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>130</v>
+      </c>
+      <c r="B80" t="s">
         <v>131</v>
       </c>
-      <c r="B80" t="s">
-        <v>132</v>
-      </c>
       <c r="C80" t="s">
         <v>5</v>
       </c>
       <c r="D80" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B81" t="s">
         <v>103</v>
@@ -2512,10 +2509,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D82" t="s">
         <v>56</v>
@@ -2526,7 +2523,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B83" t="s">
         <v>98</v>
@@ -2543,16 +2540,16 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" t="s">
         <v>137</v>
       </c>
-      <c r="B84" t="s">
-        <v>138</v>
-      </c>
       <c r="C84" t="s">
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E84" t="s">
         <v>10</v>
@@ -2560,10 +2557,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
@@ -2577,30 +2574,30 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>180</v>
+      </c>
+      <c r="B86" t="s">
         <v>181</v>
       </c>
-      <c r="B86" t="s">
-        <v>182</v>
-      </c>
       <c r="D86" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E86" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F86" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G86" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
@@ -2614,21 +2611,21 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D88" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B89" t="s">
         <v>100</v>
@@ -2637,7 +2634,7 @@
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E89" t="s">
         <v>21</v>
@@ -2645,33 +2642,33 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B90" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C90" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F90" t="s">
+        <v>133</v>
+      </c>
+      <c r="G90" t="s">
         <v>134</v>
-      </c>
-      <c r="G90" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>144</v>
+      </c>
+      <c r="B91" t="s">
         <v>145</v>
-      </c>
-      <c r="B91" t="s">
-        <v>146</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
@@ -2685,10 +2682,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" t="s">
         <v>147</v>
-      </c>
-      <c r="B92" t="s">
-        <v>148</v>
       </c>
       <c r="C92" t="s">
         <v>5</v>
@@ -2702,10 +2699,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B93" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C93" t="s">
         <v>5</v>
@@ -2719,38 +2716,38 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>149</v>
+      </c>
+      <c r="B94" t="s">
         <v>150</v>
       </c>
-      <c r="B94" t="s">
-        <v>151</v>
-      </c>
       <c r="C94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E94" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>246</v>
+      </c>
+      <c r="B95" t="s">
         <v>247</v>
       </c>
-      <c r="B95" t="s">
-        <v>248</v>
-      </c>
       <c r="D95" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E95" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B96" t="s">
         <v>98</v>
@@ -2767,24 +2764,24 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B97" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D97" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E97" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>184</v>
+      </c>
+      <c r="B98" t="s">
         <v>185</v>
-      </c>
-      <c r="B98" t="s">
-        <v>186</v>
       </c>
       <c r="D98" t="s">
         <v>65</v>
@@ -2795,10 +2792,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>154</v>
+      </c>
+      <c r="B99" t="s">
         <v>155</v>
-      </c>
-      <c r="B99" t="s">
-        <v>156</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
@@ -2812,30 +2809,30 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B100" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E100" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F100" t="s">
+        <v>139</v>
+      </c>
+      <c r="G100" t="s">
         <v>140</v>
-      </c>
-      <c r="G100" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B101" t="s">
         <v>103</v>
@@ -2852,10 +2849,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>158</v>
+      </c>
+      <c r="B102" t="s">
         <v>159</v>
-      </c>
-      <c r="B102" t="s">
-        <v>160</v>
       </c>
       <c r="C102" t="s">
         <v>5</v>
@@ -2869,13 +2866,13 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>168</v>
+      </c>
+      <c r="B103" t="s">
         <v>169</v>
       </c>
-      <c r="B103" t="s">
-        <v>170</v>
-      </c>
       <c r="D103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E103" t="s">
         <v>33</v>
@@ -2883,33 +2880,33 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>236</v>
+      </c>
+      <c r="B104" t="s">
         <v>237</v>
       </c>
-      <c r="B104" t="s">
-        <v>238</v>
-      </c>
       <c r="D104" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>160</v>
+      </c>
+      <c r="B105" t="s">
         <v>161</v>
       </c>
-      <c r="B105" t="s">
-        <v>162</v>
-      </c>
       <c r="C105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D105" t="s">
+        <v>151</v>
+      </c>
+      <c r="E105" t="s">
         <v>152</v>
-      </c>
-      <c r="E105" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update LSC authors and reinstate csv file
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesb/Documents/Work/NEXT/NEXTAuthorList/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581B4B5B-5E1F-3346-85BD-371748426A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A554677-FA08-E542-9055-15688633182A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11620" yWindow="1700" windowWidth="21980" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,20 +16,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="260">
   <si>
     <t>LastName</t>
   </si>
@@ -800,6 +791,15 @@
   </si>
   <si>
     <t>ListOrder</t>
+  </si>
+  <si>
+    <t>Cid</t>
+  </si>
+  <si>
+    <t>Bayo</t>
+  </si>
+  <si>
+    <t>Palacio</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1411,92 +1411,89 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>258</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>200</v>
+        <v>169</v>
+      </c>
+      <c r="E14" t="s">
+        <v>133</v>
       </c>
       <c r="F14" t="s">
-        <v>222</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="E15" t="s">
-        <v>28</v>
+      <c r="E15" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>190</v>
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>230</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>231</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>230</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1510,368 +1507,365 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>257</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
+        <v>228</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>209</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>200</v>
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
       </c>
       <c r="F24" t="s">
-        <v>222</v>
-      </c>
-      <c r="G24" t="s">
-        <v>186</v>
-      </c>
-      <c r="H24" t="s">
-        <v>218</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>238</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
+        <v>209</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>222</v>
+      </c>
+      <c r="G26" t="s">
+        <v>186</v>
+      </c>
+      <c r="H26" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>238</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E27" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="F27" t="s">
-        <v>199</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>200</v>
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>222</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
+        <v>188</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>198</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>252</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>6</v>
+        <v>216</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>193</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>231</v>
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>243</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>229</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>193</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" t="s">
-        <v>47</v>
+        <v>169</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>200</v>
+        <v>243</v>
+      </c>
+      <c r="E34" t="s">
+        <v>229</v>
       </c>
       <c r="F34" t="s">
-        <v>222</v>
-      </c>
-      <c r="G34" t="s">
-        <v>186</v>
-      </c>
-      <c r="H34" t="s">
-        <v>218</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>162</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>163</v>
-      </c>
-      <c r="E36" t="s">
-        <v>164</v>
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F36" t="s">
-        <v>33</v>
+        <v>222</v>
+      </c>
+      <c r="G36" t="s">
+        <v>186</v>
+      </c>
+      <c r="H36" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B38" t="s">
-        <v>226</v>
+        <v>163</v>
       </c>
       <c r="E38" t="s">
-        <v>224</v>
+        <v>164</v>
       </c>
       <c r="F38" t="s">
-        <v>222</v>
-      </c>
-      <c r="G38" t="s">
-        <v>186</v>
-      </c>
-      <c r="H38" t="s">
-        <v>218</v>
-      </c>
-      <c r="K38" s="4"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>200</v>
+      <c r="E39" t="s">
+        <v>65</v>
       </c>
       <c r="F39" t="s">
-        <v>222</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>172</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
       <c r="E40" t="s">
-        <v>77</v>
+        <v>224</v>
       </c>
       <c r="F40" t="s">
-        <v>78</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G40" t="s">
+        <v>186</v>
+      </c>
+      <c r="H40" t="s">
+        <v>218</v>
+      </c>
+      <c r="K40" s="4"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>240</v>
+        <v>5</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>200</v>
@@ -1879,95 +1873,95 @@
       <c r="F41" t="s">
         <v>222</v>
       </c>
-      <c r="G41" t="s">
-        <v>186</v>
-      </c>
-      <c r="H41" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>200</v>
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>77</v>
       </c>
       <c r="F42" t="s">
-        <v>222</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>232</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>240</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>231</v>
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
+        <v>222</v>
+      </c>
+      <c r="G43" t="s">
+        <v>186</v>
+      </c>
+      <c r="H43" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>231</v>
+        <v>200</v>
+      </c>
+      <c r="F44" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" t="s">
-        <v>51</v>
+        <v>233</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
       </c>
-      <c r="E46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" t="s">
-        <v>21</v>
+      <c r="E46" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
         <v>58</v>
@@ -1976,154 +1970,157 @@
         <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>223</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="F48" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>56</v>
+        <v>223</v>
       </c>
       <c r="F49" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>200</v>
+      <c r="E50" t="s">
+        <v>65</v>
       </c>
       <c r="F50" t="s">
-        <v>222</v>
-      </c>
-      <c r="G50" t="s">
-        <v>217</v>
-      </c>
-      <c r="H50" t="s">
-        <v>222</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="F51" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
-      </c>
-      <c r="E52" t="s">
-        <v>56</v>
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F52" t="s">
-        <v>81</v>
+        <v>222</v>
+      </c>
+      <c r="G52" t="s">
+        <v>217</v>
+      </c>
+      <c r="H52" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>176</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>231</v>
+        <v>93</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>241</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="E54" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="F54" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" t="s">
-        <v>229</v>
-      </c>
-      <c r="F55" t="s">
-        <v>63</v>
+        <v>176</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>175</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
       <c r="E56" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="F56" t="s">
         <v>33</v>
@@ -2131,58 +2128,58 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
       </c>
       <c r="E57" t="s">
-        <v>101</v>
+        <v>229</v>
       </c>
       <c r="F57" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>227</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>228</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>200</v>
+        <v>97</v>
+      </c>
+      <c r="E58" t="s">
+        <v>32</v>
       </c>
       <c r="F58" t="s">
-        <v>222</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="F59" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B60" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>200</v>
@@ -2190,804 +2187,846 @@
       <c r="F60" t="s">
         <v>222</v>
       </c>
-      <c r="G60" t="s">
-        <v>36</v>
-      </c>
-      <c r="H60" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>194</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>195</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>231</v>
+        <v>92</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>52</v>
+      </c>
+      <c r="F61" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>248</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" t="s">
+        <v>249</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F62" t="s">
+        <v>222</v>
+      </c>
+      <c r="G62" t="s">
         <v>36</v>
       </c>
-      <c r="F62" t="s">
-        <v>37</v>
+      <c r="H62" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>174</v>
-      </c>
-      <c r="E63" t="s">
-        <v>164</v>
-      </c>
-      <c r="F63" t="s">
-        <v>33</v>
+        <v>195</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="F64" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B65" t="s">
-        <v>247</v>
+        <v>174</v>
       </c>
       <c r="E65" t="s">
-        <v>28</v>
+        <v>164</v>
       </c>
       <c r="F65" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F66" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>112</v>
+        <v>246</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>247</v>
       </c>
       <c r="E67" t="s">
-        <v>229</v>
+        <v>28</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>200</v>
+      <c r="E68" t="s">
+        <v>36</v>
       </c>
       <c r="F68" t="s">
-        <v>222</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="E69" t="s">
-        <v>20</v>
+        <v>229</v>
       </c>
       <c r="F69" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>236</v>
+        <v>114</v>
       </c>
       <c r="B70" t="s">
-        <v>254</v>
-      </c>
-      <c r="E70" t="s">
-        <v>164</v>
+        <v>98</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F70" t="s">
-        <v>33</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>191</v>
+        <v>116</v>
       </c>
       <c r="B71" t="s">
-        <v>166</v>
+        <v>117</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>236</v>
       </c>
       <c r="B72" t="s">
-        <v>119</v>
-      </c>
-      <c r="C72" t="s">
-        <v>5</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>200</v>
+        <v>254</v>
+      </c>
+      <c r="E72" t="s">
+        <v>164</v>
       </c>
       <c r="F72" t="s">
-        <v>222</v>
-      </c>
-      <c r="G72" t="s">
-        <v>186</v>
-      </c>
-      <c r="H72" t="s">
-        <v>218</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="B73" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="E73" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F73" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B74" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
       </c>
-      <c r="E74" t="s">
-        <v>6</v>
+      <c r="E74" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F74" t="s">
-        <v>7</v>
+        <v>222</v>
+      </c>
+      <c r="G74" t="s">
+        <v>186</v>
+      </c>
+      <c r="H74" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
       </c>
       <c r="E75" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F75" t="s">
-        <v>125</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
       <c r="B76" t="s">
-        <v>166</v>
+        <v>123</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
       </c>
       <c r="E76" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="F76" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="E77" t="s">
         <v>36</v>
       </c>
       <c r="F77" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
       <c r="B78" t="s">
-        <v>169</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>200</v>
+        <v>166</v>
+      </c>
+      <c r="E78" t="s">
+        <v>32</v>
       </c>
       <c r="F78" t="s">
-        <v>222</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B79" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="C79" t="s">
+        <v>115</v>
       </c>
       <c r="E79" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F79" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>239</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>200</v>
+        <v>169</v>
+      </c>
+      <c r="E80" t="s">
+        <v>133</v>
       </c>
       <c r="F80" t="s">
-        <v>222</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>215</v>
+      <c r="A81" t="s">
+        <v>128</v>
       </c>
       <c r="B81" t="s">
-        <v>216</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>200</v>
+        <v>129</v>
+      </c>
+      <c r="E81" t="s">
+        <v>32</v>
       </c>
       <c r="F81" t="s">
-        <v>222</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="B82" t="s">
-        <v>131</v>
-      </c>
-      <c r="C82" t="s">
-        <v>5</v>
+        <v>178</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>231</v>
+        <v>200</v>
+      </c>
+      <c r="F82" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>132</v>
+      <c r="A83" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="B83" t="s">
-        <v>103</v>
-      </c>
-      <c r="C83" t="s">
-        <v>5</v>
-      </c>
-      <c r="E83" t="s">
-        <v>52</v>
+        <v>216</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F83" t="s">
-        <v>53</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>255</v>
+      <c r="A84" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="B84" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E84" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="F84" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>250</v>
+        <v>130</v>
       </c>
       <c r="B85" t="s">
-        <v>251</v>
+        <v>131</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F85" t="s">
-        <v>222</v>
+        <v>230</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>242</v>
+        <v>132</v>
       </c>
       <c r="B86" t="s">
-        <v>216</v>
+        <v>103</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
       </c>
       <c r="E86" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F86" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>255</v>
       </c>
       <c r="B87" t="s">
-        <v>98</v>
-      </c>
-      <c r="C87" t="s">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="E87" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F87" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>136</v>
+        <v>250</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
-      </c>
-      <c r="C88" t="s">
-        <v>5</v>
-      </c>
-      <c r="E88" t="s">
-        <v>229</v>
+        <v>251</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F88" t="s">
-        <v>10</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>242</v>
       </c>
       <c r="B89" t="s">
-        <v>110</v>
-      </c>
-      <c r="C89" t="s">
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="E89" t="s">
         <v>56</v>
       </c>
       <c r="F89" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="B90" t="s">
-        <v>180</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>200</v>
+        <v>98</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" t="s">
+        <v>36</v>
       </c>
       <c r="F90" t="s">
-        <v>222</v>
-      </c>
-      <c r="G90" t="s">
-        <v>186</v>
-      </c>
-      <c r="H90" t="s">
-        <v>218</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B91" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>6</v>
+        <v>229</v>
       </c>
       <c r="F91" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="B92" t="s">
-        <v>171</v>
+        <v>110</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
       </c>
       <c r="E92" t="s">
-        <v>217</v>
+        <v>56</v>
       </c>
       <c r="F92" t="s">
-        <v>222</v>
+        <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
-      </c>
-      <c r="C93" t="s">
-        <v>5</v>
-      </c>
-      <c r="E93" t="s">
-        <v>207</v>
+        <v>180</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F93" t="s">
-        <v>21</v>
+        <v>222</v>
+      </c>
+      <c r="G93" t="s">
+        <v>186</v>
+      </c>
+      <c r="H93" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B94" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
       </c>
-      <c r="E94" s="3" t="s">
-        <v>200</v>
+      <c r="E94" t="s">
+        <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>222</v>
-      </c>
-      <c r="G94" t="s">
-        <v>133</v>
-      </c>
-      <c r="H94" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="B95" t="s">
-        <v>145</v>
-      </c>
-      <c r="C95" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="E95" t="s">
-        <v>36</v>
+        <v>217</v>
       </c>
       <c r="F95" t="s">
-        <v>37</v>
+        <v>222</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B96" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
       </c>
       <c r="E96" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="F96" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B97" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
       </c>
-      <c r="E97" t="s">
-        <v>65</v>
+      <c r="E97" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F97" t="s">
-        <v>47</v>
+        <v>222</v>
+      </c>
+      <c r="H97" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B98" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C98" t="s">
-        <v>115</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>200</v>
+        <v>5</v>
+      </c>
+      <c r="E98" t="s">
+        <v>36</v>
       </c>
       <c r="F98" t="s">
-        <v>222</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>244</v>
+        <v>146</v>
       </c>
       <c r="B99" t="s">
-        <v>245</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>200</v>
+        <v>147</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+      <c r="E99" t="s">
+        <v>28</v>
       </c>
       <c r="F99" t="s">
-        <v>222</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B100" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
       </c>
       <c r="E100" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F100" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="B101" t="s">
-        <v>171</v>
+        <v>150</v>
+      </c>
+      <c r="C101" t="s">
+        <v>115</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>231</v>
+        <v>200</v>
+      </c>
+      <c r="F101" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="B102" t="s">
-        <v>184</v>
-      </c>
-      <c r="E102" t="s">
-        <v>65</v>
+        <v>245</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F102" t="s">
-        <v>47</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B103" t="s">
-        <v>155</v>
+        <v>98</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
       </c>
       <c r="E103" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F103" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="B104" t="s">
-        <v>110</v>
-      </c>
-      <c r="C104" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F104" t="s">
-        <v>222</v>
-      </c>
-      <c r="G104" t="s">
-        <v>139</v>
-      </c>
-      <c r="H104" t="s">
-        <v>140</v>
+        <v>230</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
-      </c>
-      <c r="C105" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="E105" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B106" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C106" t="s">
         <v>5</v>
       </c>
       <c r="E106" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F106" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B107" t="s">
-        <v>168</v>
-      </c>
-      <c r="E107" t="s">
-        <v>164</v>
+        <v>110</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="F107" t="s">
-        <v>33</v>
+        <v>222</v>
+      </c>
+      <c r="G107" t="s">
+        <v>139</v>
+      </c>
+      <c r="H107" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="B108" t="s">
-        <v>235</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>231</v>
+        <v>103</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="E108" t="s">
+        <v>36</v>
+      </c>
+      <c r="F108" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>158</v>
+      </c>
+      <c r="B109" t="s">
+        <v>159</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+      <c r="E109" t="s">
+        <v>16</v>
+      </c>
+      <c r="F109" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>167</v>
+      </c>
+      <c r="B110" t="s">
+        <v>168</v>
+      </c>
+      <c r="E110" t="s">
+        <v>164</v>
+      </c>
+      <c r="F110" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>234</v>
+      </c>
+      <c r="B111" t="s">
+        <v>235</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>160</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B112" t="s">
         <v>161</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C112" t="s">
         <v>197</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E112" t="s">
         <v>151</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F112" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small author list fix
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesb/Documents/Work/NEXT/NEXTAuthorList/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDF4EBD-7F9B-C042-A1E7-13E944558D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8845D23D-E4AF-9D4F-A845-305243237A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11620" yWindow="1700" windowWidth="21980" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1188,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1635,7 +1635,7 @@
         <v>178</v>
       </c>
       <c r="E27" t="s">
-        <v>164</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Fix some missing dots
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesb/Documents/Work/NEXT/NEXTAuthorList/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8845D23D-E4AF-9D4F-A845-305243237A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727919F0-5370-6841-9276-55BD6933E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11620" yWindow="1700" windowWidth="21980" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="260">
   <si>
     <t>LastName</t>
   </si>
@@ -769,15 +769,9 @@
     <t>Lopez</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>Pelegrin</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>Elorza</t>
   </si>
   <si>
@@ -803,6 +797,9 @@
   </si>
   <si>
     <t>K.E.</t>
+  </si>
+  <si>
+    <t>F.</t>
   </si>
 </sst>
 </file>
@@ -1188,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1205,7 +1202,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>220</v>
@@ -1400,7 +1397,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B13" t="s">
         <v>216</v>
@@ -1414,7 +1411,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B14" t="s">
         <v>169</v>
@@ -1561,7 +1558,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s">
         <v>228</v>
@@ -1674,7 +1671,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B30" t="s">
         <v>216</v>
@@ -2213,7 +2210,7 @@
         <v>248</v>
       </c>
       <c r="B62" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>200</v>
@@ -2374,7 +2371,7 @@
         <v>236</v>
       </c>
       <c r="B72" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E72" t="s">
         <v>164</v>
@@ -2476,7 +2473,7 @@
         <v>165</v>
       </c>
       <c r="B78" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E78" t="s">
         <v>32</v>
@@ -2560,7 +2557,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B84" t="s">
         <v>176</v>
@@ -2608,7 +2605,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B87" t="s">
         <v>180</v>
@@ -2622,10 +2619,10 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B88" t="s">
-        <v>251</v>
+        <v>176</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>200</v>

</xml_diff>

<commit_message>
fix f. lopez affiliations
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesb/Documents/Work/NEXT/NEXTAuthorList/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727919F0-5370-6841-9276-55BD6933E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B004BD4-A739-EC45-B739-1E4E4A6AA077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11620" yWindow="1700" windowWidth="21980" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="260">
   <si>
     <t>LastName</t>
   </si>
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2218,12 +2218,6 @@
       <c r="F62" t="s">
         <v>222</v>
       </c>
-      <c r="G62" t="s">
-        <v>36</v>
-      </c>
-      <c r="H62" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">

</xml_diff>

<commit_message>
upates in U. Basque Country list, from May 2023: 3 new authors in, 1 old author out, Fernandos instituitons updated
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B004BD4-A739-EC45-B739-1E4E4A6AA077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89486EE0-2FAF-F842-8A4F-023A0055C4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11620" yWindow="1700" windowWidth="21980" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="500" windowWidth="21980" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="259">
   <si>
     <t>LastName</t>
   </si>
@@ -40,9 +40,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> Instituto de Instrumentaci\'on para Imagen Molecular (I3M), Centro Mixto CSIC - Universitat Polit\`ecnica de Val\`encia, Camino de Vera s/n </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Valencia, E-46022, Spain</t>
   </si>
   <si>
@@ -61,18 +58,12 @@
     <t xml:space="preserve"> I.J.       </t>
   </si>
   <si>
-    <t xml:space="preserve"> Pacific Northwest National Laboratory (PNNL) </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Richland, WA 99352, USA</t>
   </si>
   <si>
     <t xml:space="preserve">Azevedo                      </t>
   </si>
   <si>
-    <t xml:space="preserve"> Institute of Nanostructures, Nanomodelling and Nanofabrication (i3N), Universidade de Aveiro, Campus de Santiago </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Aveiro, 3810-193, Portugal             </t>
   </si>
   <si>
@@ -82,9 +73,6 @@
     <t xml:space="preserve"> K.         </t>
   </si>
   <si>
-    <t xml:space="preserve"> Argonne National Laboratory </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Argonne, IL 60439, USA</t>
   </si>
   <si>
@@ -106,9 +94,6 @@
     <t xml:space="preserve"> F.I.G.M.   </t>
   </si>
   <si>
-    <t xml:space="preserve"> LIP, Department of Physics, University of Coimbra </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Coimbra, 3004-516, Portugal </t>
   </si>
   <si>
@@ -118,9 +103,6 @@
     <t xml:space="preserve"> N.         </t>
   </si>
   <si>
-    <t xml:space="preserve"> Department of Physics, University of Texas at Arlington </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Arlington, TX 76019, USA</t>
   </si>
   <si>
@@ -130,9 +112,6 @@
     <t xml:space="preserve"> S.         </t>
   </si>
   <si>
-    <t xml:space="preserve"> Instituto de F\'isica Corpuscular (IFIC), CSIC \&amp; Universitat de Val\`encia, Calle Catedr\'atico Jos\'e Beltr\'an, 2 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Paterna, E-46980, Spain</t>
   </si>
   <si>
@@ -145,9 +124,6 @@
     <t xml:space="preserve">Cebri\'an                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> Centro de Astropart\'iculas y F\'isica de Altas Energ\'ias (CAPA), Universidad de Zaragoza, Calle Pedro Cerbuna, 12 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Zaragoza, E-50009, Spain</t>
   </si>
   <si>
@@ -172,15 +148,9 @@
     <t xml:space="preserve"> T.         </t>
   </si>
   <si>
-    <t xml:space="preserve"> Department of Physics, Harvard University </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Cambridge, MA 02138, USA</t>
   </si>
   <si>
-    <t xml:space="preserve"> Fermi National Accelerator Laboratory </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Batavia, IL 60510, USA</t>
   </si>
   <si>
@@ -190,9 +160,6 @@
     <t xml:space="preserve"> G.         </t>
   </si>
   <si>
-    <t xml:space="preserve"> Instituto Gallego de F\'isica de Altas Energ\'ias, Univ.\ de Santiago de Compostela, Campus sur, R\'ua Xos\'e Mar\'ia Su\'arez N\'u\~nez, s/n </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Santiago de Compostela, E-15782, Spain </t>
   </si>
   <si>
@@ -217,9 +184,6 @@
     <t xml:space="preserve">Fernandes                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> LIBPhys, Physics Department, University of Coimbra, Rua Larga </t>
-  </si>
-  <si>
     <t xml:space="preserve"> L.M.P.     </t>
   </si>
   <si>
@@ -253,9 +217,6 @@
     <t xml:space="preserve"> A.          </t>
   </si>
   <si>
-    <t xml:space="preserve"> Lawrence Berkeley National Laboratory (LBNL), 1 Cyclotron Road </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Berkeley, CA 94720, USA</t>
   </si>
   <si>
@@ -325,9 +286,6 @@
     <t xml:space="preserve"> L.        </t>
   </si>
   <si>
-    <t xml:space="preserve"> Departamento de F\'isica Te\'orica, Universidad Aut\'onoma de Madrid, Campus de Cantoblanco </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Madrid, E-28049, Spain</t>
   </si>
   <si>
@@ -421,9 +379,6 @@
     <t xml:space="preserve">Para                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> Laboratorio Subterr\'aneo de Canfranc, Paseo de los Ayerbe s/n </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Canfranc Estaci\'on, E-22880, Spain</t>
   </si>
   <si>
@@ -475,9 +430,6 @@
     <t xml:space="preserve"> A.       </t>
   </si>
   <si>
-    <t xml:space="preserve"> Department of Physics and Astronomy, Texas A\&amp;M University </t>
-  </si>
-  <si>
     <t xml:space="preserve"> College Station, TX 77843-4242, USA</t>
   </si>
   <si>
@@ -514,9 +466,6 @@
     <t>F.W.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Department of Chemistry and Biochemistry, University of Texas at Arlington </t>
-  </si>
-  <si>
     <t>Navarro</t>
   </si>
   <si>
@@ -667,9 +616,6 @@
     <t>A.I.</t>
   </si>
   <si>
-    <t>Odriozola-Gimeno</t>
-  </si>
-  <si>
     <t>M.</t>
   </si>
   <si>
@@ -691,9 +637,6 @@
     <t>San Sebasti\'an / Donostia, E-20018, Spain</t>
   </si>
   <si>
-    <t xml:space="preserve"> Department of Physics and Astronomy, Iowa State University</t>
-  </si>
-  <si>
     <t>Department of Applied Chemistry, Universidad del Pais Vasco (UPV/EHU), Manuel de Lardizabal 3</t>
   </si>
   <si>
@@ -712,9 +655,6 @@
     <t>Unit of Nuclear Engineering, Faculty of Engineering Sciences, Ben-Gurion University of the Negev, P.O.B. 653</t>
   </si>
   <si>
-    <t xml:space="preserve"> Department of Physics and Astronomy, Manchester University </t>
-  </si>
-  <si>
     <t>Manchester. M13 9PL, United Kingdom</t>
   </si>
   <si>
@@ -800,6 +740,63 @@
   </si>
   <si>
     <t>F.</t>
+  </si>
+  <si>
+    <t>Molina-Canteras</t>
+  </si>
+  <si>
+    <t>Auria-Luna</t>
+  </si>
+  <si>
+    <t>Larumbe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Physics and Astronomy, Manchester University </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratorio Subterr\'aneo de Canfranc, Paseo de los Ayerbe s/n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIP, Department of Physics, University of Coimbra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Physics, University of Texas at Arlington </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instituto de F\'isica Corpuscular (IFIC), CSIC \&amp; Universitat de Val\`encia, Calle Catedr\'atico Jos\'e Beltr\'an, 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centro de Astropart\'iculas y F\'isica de Altas Energ\'ias (CAPA), Universidad de Zaragoza, Calle Pedro Cerbuna, 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Physics, Harvard University </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instituto Gallego de F\'isica de Altas Energ\'ias, Univ.\ de Santiago de Compostela, Campus sur, R\'ua Xos\'e Mar\'ia Su\'arez N\'u\~nez, s/n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIBPhys, Physics Department, University of Coimbra, Rua Larga </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Chemistry and Biochemistry, University of Texas at Arlington </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lawrence Berkeley National Laboratory (LBNL), 1 Cyclotron Road </t>
+  </si>
+  <si>
+    <t>Department of Physics and Astronomy, Iowa State University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Departamento de F\'isica Te\'orica, Universidad Aut\'onoma de Madrid, Campus de Cantoblanco </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fermi National Accelerator Laboratory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Physics and Astronomy, Texas A\&amp;M University </t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1202,52 +1199,52 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -1262,1766 +1259,1794 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="E5" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="F5" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="F6" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>229</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>241</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>239</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F9" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>187</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>190</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>251</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>216</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>200</v>
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>189</v>
       </c>
       <c r="F13" t="s">
-        <v>222</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E14" t="s">
-        <v>133</v>
+        <v>198</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F14" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>200</v>
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
+        <v>245</v>
       </c>
       <c r="F15" t="s">
-        <v>222</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="E16" t="s">
-        <v>28</v>
+      <c r="E16" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>190</v>
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="F17" t="s">
-        <v>231</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>244</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>248</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>248</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
       <c r="F23" t="s">
-        <v>134</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>235</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
+        <v>209</v>
       </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>245</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>246</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>209</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>200</v>
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>250</v>
       </c>
       <c r="F26" t="s">
-        <v>222</v>
-      </c>
-      <c r="G26" t="s">
-        <v>186</v>
-      </c>
-      <c r="H26" t="s">
-        <v>218</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>238</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E27" t="s">
-        <v>32</v>
+        <v>192</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F27" t="s">
-        <v>33</v>
+        <v>204</v>
+      </c>
+      <c r="G27" t="s">
+        <v>205</v>
+      </c>
+      <c r="H27" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>218</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>247</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>187</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>198</v>
+        <v>251</v>
       </c>
       <c r="F29" t="s">
-        <v>199</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>200</v>
+        <v>171</v>
+      </c>
+      <c r="E30" t="s">
+        <v>181</v>
       </c>
       <c r="F30" t="s">
-        <v>222</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>230</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" t="s">
-        <v>28</v>
+        <v>198</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F31" t="s">
-        <v>47</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>231</v>
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>176</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" t="s">
-        <v>243</v>
-      </c>
-      <c r="E34" t="s">
-        <v>229</v>
-      </c>
-      <c r="F34" t="s">
-        <v>63</v>
+        <v>152</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>210</v>
       </c>
       <c r="F35" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>200</v>
+      <c r="E36" t="s">
+        <v>252</v>
       </c>
       <c r="F36" t="s">
-        <v>222</v>
-      </c>
-      <c r="G36" t="s">
-        <v>186</v>
-      </c>
-      <c r="H36" t="s">
-        <v>218</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
-      <c r="E37" t="s">
-        <v>16</v>
+      <c r="E37" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F37" t="s">
-        <v>71</v>
+        <v>204</v>
+      </c>
+      <c r="G37" t="s">
+        <v>169</v>
+      </c>
+      <c r="H37" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="F38" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>253</v>
       </c>
       <c r="F39" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>226</v>
+        <v>61</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="F40" t="s">
-        <v>222</v>
-      </c>
-      <c r="G40" t="s">
-        <v>186</v>
-      </c>
-      <c r="H40" t="s">
-        <v>218</v>
-      </c>
-      <c r="K40" s="4"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>155</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" t="s">
+        <v>205</v>
+      </c>
+      <c r="F41" t="s">
+        <v>204</v>
+      </c>
+      <c r="G41" t="s">
+        <v>169</v>
+      </c>
+      <c r="H41" t="s">
         <v>200</v>
       </c>
-      <c r="F41" t="s">
-        <v>222</v>
-      </c>
+      <c r="K41" s="4"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
       </c>
-      <c r="E42" t="s">
-        <v>77</v>
+      <c r="E42" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F42" t="s">
-        <v>78</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>240</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>200</v>
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>254</v>
       </c>
       <c r="F43" t="s">
-        <v>222</v>
-      </c>
-      <c r="G43" t="s">
-        <v>186</v>
-      </c>
-      <c r="H43" t="s">
-        <v>218</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>173</v>
+        <v>66</v>
       </c>
       <c r="B44" t="s">
-        <v>174</v>
+        <v>67</v>
+      </c>
+      <c r="C44" t="s">
+        <v>220</v>
       </c>
       <c r="E44" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F44" t="s">
+        <v>204</v>
+      </c>
+      <c r="G44" t="s">
+        <v>169</v>
+      </c>
+      <c r="H44" t="s">
         <v>200</v>
-      </c>
-      <c r="F44" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>232</v>
+        <v>156</v>
       </c>
       <c r="B45" t="s">
-        <v>233</v>
+        <v>157</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>231</v>
+        <v>183</v>
+      </c>
+      <c r="F45" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>212</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
+        <v>213</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
-      <c r="E47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47" t="s">
-        <v>51</v>
+      <c r="E47" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="F48" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="F49" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>65</v>
+        <v>255</v>
       </c>
       <c r="F50" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>56</v>
+        <v>252</v>
       </c>
       <c r="F51" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>225</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>200</v>
+      <c r="E52" t="s">
+        <v>251</v>
       </c>
       <c r="F52" t="s">
-        <v>222</v>
-      </c>
-      <c r="G52" t="s">
-        <v>217</v>
-      </c>
-      <c r="H52" t="s">
-        <v>222</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>206</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
-      <c r="E53" t="s">
-        <v>6</v>
+      <c r="E53" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F53" t="s">
-        <v>7</v>
+        <v>204</v>
+      </c>
+      <c r="G53" t="s">
+        <v>199</v>
+      </c>
+      <c r="H53" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>241</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>80</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="F54" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>176</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>231</v>
+        <v>154</v>
+      </c>
+      <c r="E55" t="s">
+        <v>251</v>
+      </c>
+      <c r="F55" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B56" t="s">
-        <v>185</v>
-      </c>
-      <c r="E56" t="s">
-        <v>164</v>
-      </c>
-      <c r="F56" t="s">
-        <v>33</v>
+        <v>159</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="E57" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="F57" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>97</v>
+        <v>82</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>32</v>
+        <v>210</v>
       </c>
       <c r="F58" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="E59" t="s">
-        <v>101</v>
+        <v>247</v>
       </c>
       <c r="F59" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>227</v>
+        <v>86</v>
       </c>
       <c r="B60" t="s">
-        <v>228</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>200</v>
+        <v>87</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>256</v>
       </c>
       <c r="F60" t="s">
-        <v>222</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" t="s">
-        <v>52</v>
+        <v>209</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F61" t="s">
-        <v>53</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>200</v>
+        <v>152</v>
+      </c>
+      <c r="E62" t="s">
+        <v>195</v>
       </c>
       <c r="F62" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>231</v>
+        <v>243</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>257</v>
+      </c>
+      <c r="F63" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>228</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" t="s">
-        <v>36</v>
+        <v>239</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F64" t="s">
-        <v>37</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>237</v>
+        <v>177</v>
       </c>
       <c r="B65" t="s">
-        <v>174</v>
-      </c>
-      <c r="E65" t="s">
-        <v>164</v>
-      </c>
-      <c r="F65" t="s">
-        <v>33</v>
+        <v>178</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>65</v>
+        <v>248</v>
       </c>
       <c r="F66" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="B67" t="s">
-        <v>247</v>
+        <v>157</v>
       </c>
       <c r="E67" t="s">
-        <v>28</v>
+        <v>253</v>
       </c>
       <c r="F67" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>36</v>
+        <v>252</v>
       </c>
       <c r="F68" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>226</v>
       </c>
       <c r="B69" t="s">
-        <v>113</v>
+        <v>227</v>
       </c>
       <c r="E69" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>200</v>
+      <c r="E70" t="s">
+        <v>248</v>
       </c>
       <c r="F70" t="s">
-        <v>222</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
-      </c>
-      <c r="C71" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="E71" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="F71" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>236</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>252</v>
-      </c>
-      <c r="E72" t="s">
-        <v>164</v>
+        <v>85</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F72" t="s">
-        <v>33</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>191</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>166</v>
+        <v>103</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
       </c>
       <c r="E73" t="s">
-        <v>32</v>
+        <v>190</v>
       </c>
       <c r="F73" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>216</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
-      </c>
-      <c r="C74" t="s">
-        <v>5</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>200</v>
+        <v>232</v>
+      </c>
+      <c r="E74" t="s">
+        <v>253</v>
       </c>
       <c r="F74" t="s">
-        <v>222</v>
-      </c>
-      <c r="G74" t="s">
-        <v>186</v>
-      </c>
-      <c r="H74" t="s">
-        <v>218</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="E75" t="s">
-        <v>65</v>
+        <v>247</v>
       </c>
       <c r="F75" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="B76" t="s">
-        <v>123</v>
-      </c>
-      <c r="C76" t="s">
-        <v>5</v>
+        <v>159</v>
       </c>
       <c r="E76" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="F76" t="s">
-        <v>7</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
       </c>
-      <c r="E77" t="s">
-        <v>36</v>
+      <c r="E77" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F77" t="s">
-        <v>125</v>
+        <v>204</v>
+      </c>
+      <c r="G77" t="s">
+        <v>169</v>
+      </c>
+      <c r="H77" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>165</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>258</v>
+        <v>107</v>
+      </c>
+      <c r="C78" t="s">
+        <v>5</v>
       </c>
       <c r="E78" t="s">
-        <v>32</v>
+        <v>252</v>
       </c>
       <c r="F78" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B79" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C79" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="F79" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>239</v>
+        <v>110</v>
       </c>
       <c r="B80" t="s">
-        <v>169</v>
+        <v>96</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
       </c>
       <c r="E80" t="s">
-        <v>133</v>
+        <v>248</v>
       </c>
       <c r="F80" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
       <c r="E81" t="s">
-        <v>32</v>
+        <v>247</v>
       </c>
       <c r="F81" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>112</v>
       </c>
       <c r="B82" t="s">
-        <v>178</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="C82" t="s">
+        <v>101</v>
+      </c>
+      <c r="E82" t="s">
+        <v>248</v>
       </c>
       <c r="F82" t="s">
-        <v>222</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>215</v>
+      <c r="A83" t="s">
+        <v>219</v>
       </c>
       <c r="B83" t="s">
-        <v>216</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>200</v>
+        <v>152</v>
+      </c>
+      <c r="E83" t="s">
+        <v>245</v>
       </c>
       <c r="F83" t="s">
-        <v>222</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>257</v>
+      <c r="A84" t="s">
+        <v>114</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
+        <v>115</v>
       </c>
       <c r="E84" t="s">
-        <v>133</v>
+        <v>247</v>
       </c>
       <c r="F84" t="s">
-        <v>134</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="B85" t="s">
-        <v>131</v>
-      </c>
-      <c r="C85" t="s">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>231</v>
+        <v>183</v>
+      </c>
+      <c r="F85" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>132</v>
+      <c r="A86" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
-      </c>
-      <c r="C86" t="s">
-        <v>5</v>
+        <v>159</v>
       </c>
       <c r="E86" t="s">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="F86" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>253</v>
+        <v>116</v>
       </c>
       <c r="B87" t="s">
-        <v>180</v>
-      </c>
-      <c r="E87" t="s">
-        <v>32</v>
-      </c>
-      <c r="F87" t="s">
-        <v>33</v>
+        <v>117</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>249</v>
+        <v>118</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>200</v>
+        <v>89</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" t="s">
+        <v>257</v>
       </c>
       <c r="F88" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="E89" t="s">
-        <v>56</v>
+        <v>247</v>
       </c>
       <c r="F89" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>229</v>
       </c>
       <c r="B90" t="s">
-        <v>98</v>
-      </c>
-      <c r="C90" t="s">
-        <v>5</v>
-      </c>
-      <c r="E90" t="s">
-        <v>36</v>
+        <v>159</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F90" t="s">
-        <v>37</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="B91" t="s">
-        <v>137</v>
-      </c>
-      <c r="C91" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="E91" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="B92" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="C92" t="s">
         <v>5</v>
       </c>
       <c r="E92" t="s">
-        <v>56</v>
+        <v>248</v>
       </c>
       <c r="F92" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
       <c r="B93" t="s">
-        <v>180</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>200</v>
+        <v>122</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93" t="s">
+        <v>210</v>
       </c>
       <c r="F93" t="s">
-        <v>222</v>
-      </c>
-      <c r="G93" t="s">
-        <v>186</v>
-      </c>
-      <c r="H93" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
       </c>
       <c r="E94" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
       <c r="F94" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B95" t="s">
-        <v>171</v>
-      </c>
-      <c r="E95" t="s">
-        <v>217</v>
+        <v>163</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F95" t="s">
-        <v>222</v>
+        <v>204</v>
+      </c>
+      <c r="G95" t="s">
+        <v>169</v>
+      </c>
+      <c r="H95" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
       </c>
       <c r="E96" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="F96" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
-      </c>
-      <c r="C97" t="s">
-        <v>5</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>200</v>
+        <v>154</v>
+      </c>
+      <c r="E97" t="s">
+        <v>199</v>
       </c>
       <c r="F97" t="s">
-        <v>222</v>
-      </c>
-      <c r="H97" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B98" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
       </c>
       <c r="E98" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B99" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
       </c>
-      <c r="E99" t="s">
-        <v>28</v>
+      <c r="E99" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F99" t="s">
-        <v>47</v>
+        <v>204</v>
+      </c>
+      <c r="H99" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B100" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
       </c>
       <c r="E100" t="s">
-        <v>65</v>
+        <v>248</v>
       </c>
       <c r="F100" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B101" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C101" t="s">
-        <v>115</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>200</v>
+        <v>5</v>
+      </c>
+      <c r="E101" t="s">
+        <v>246</v>
       </c>
       <c r="F101" t="s">
-        <v>222</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>244</v>
+        <v>131</v>
       </c>
       <c r="B102" t="s">
-        <v>245</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>200</v>
+        <v>133</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+      <c r="E102" t="s">
+        <v>252</v>
       </c>
       <c r="F102" t="s">
-        <v>222</v>
+        <v>39</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="B103" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="C103" t="s">
-        <v>5</v>
-      </c>
-      <c r="E103" t="s">
-        <v>36</v>
+        <v>101</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F103" t="s">
-        <v>37</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="B104" t="s">
-        <v>171</v>
+        <v>225</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>231</v>
+        <v>183</v>
+      </c>
+      <c r="F104" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="B105" t="s">
-        <v>184</v>
+        <v>85</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
       </c>
       <c r="E105" t="s">
-        <v>65</v>
+        <v>248</v>
       </c>
       <c r="F105" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>165</v>
+      </c>
+      <c r="B106" t="s">
         <v>154</v>
       </c>
-      <c r="B106" t="s">
-        <v>155</v>
-      </c>
-      <c r="C106" t="s">
-        <v>5</v>
-      </c>
-      <c r="E106" t="s">
-        <v>6</v>
-      </c>
-      <c r="F106" t="s">
-        <v>7</v>
+      <c r="E106" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B107" t="s">
-        <v>110</v>
-      </c>
-      <c r="C107" t="s">
-        <v>5</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>200</v>
+        <v>167</v>
+      </c>
+      <c r="E107" t="s">
+        <v>252</v>
       </c>
       <c r="F107" t="s">
-        <v>222</v>
-      </c>
-      <c r="G107" t="s">
-        <v>139</v>
-      </c>
-      <c r="H107" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="C108" t="s">
         <v>5</v>
       </c>
       <c r="E108" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="F108" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="B109" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
       </c>
-      <c r="E109" t="s">
-        <v>16</v>
+      <c r="E109" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F109" t="s">
-        <v>71</v>
+        <v>204</v>
+      </c>
+      <c r="G109" t="s">
+        <v>124</v>
+      </c>
+      <c r="H109" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B110" t="s">
-        <v>168</v>
+        <v>89</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
       </c>
       <c r="E110" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="F110" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>234</v>
+        <v>142</v>
       </c>
       <c r="B111" t="s">
-        <v>235</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>231</v>
+        <v>143</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+      <c r="E111" t="s">
+        <v>187</v>
+      </c>
+      <c r="F111" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B112" t="s">
-        <v>161</v>
-      </c>
-      <c r="C112" t="s">
-        <v>197</v>
+        <v>151</v>
       </c>
       <c r="E112" t="s">
-        <v>151</v>
+        <v>253</v>
       </c>
       <c r="F112" t="s">
-        <v>152</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>214</v>
+      </c>
+      <c r="B113" t="s">
+        <v>215</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>144</v>
+      </c>
+      <c r="B114" t="s">
+        <v>145</v>
+      </c>
+      <c r="C114" t="s">
+        <v>180</v>
+      </c>
+      <c r="E114" t="s">
+        <v>258</v>
+      </c>
+      <c r="F114" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add J. Soto-Oton at IFIC
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/IB/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89486EE0-2FAF-F842-8A4F-023A0055C4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C75DED-DE01-F14B-876A-CEF00B54112D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="500" windowWidth="21980" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="260">
   <si>
     <t>LastName</t>
   </si>
@@ -797,6 +797,9 @@
   </si>
   <si>
     <t xml:space="preserve">Department of Physics and Astronomy, Texas A\&amp;M University </t>
+  </si>
+  <si>
+    <t>Soto-Oton</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K114"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2904,148 +2907,162 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="B106" t="s">
-        <v>154</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>211</v>
+        <v>159</v>
+      </c>
+      <c r="E106" t="s">
+        <v>248</v>
+      </c>
+      <c r="F106" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B107" t="s">
-        <v>167</v>
-      </c>
-      <c r="E107" t="s">
-        <v>252</v>
-      </c>
-      <c r="F107" t="s">
-        <v>39</v>
+        <v>154</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="B108" t="s">
-        <v>139</v>
-      </c>
-      <c r="C108" t="s">
-        <v>5</v>
+        <v>167</v>
       </c>
       <c r="E108" t="s">
-        <v>189</v>
+        <v>252</v>
       </c>
       <c r="F108" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B109" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
       </c>
-      <c r="E109" s="3" t="s">
-        <v>183</v>
+      <c r="E109" t="s">
+        <v>189</v>
       </c>
       <c r="F109" t="s">
-        <v>204</v>
-      </c>
-      <c r="G109" t="s">
-        <v>124</v>
-      </c>
-      <c r="H109" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B110" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C110" t="s">
         <v>5</v>
       </c>
-      <c r="E110" t="s">
-        <v>248</v>
+      <c r="E110" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="F110" t="s">
-        <v>30</v>
+        <v>204</v>
+      </c>
+      <c r="G110" t="s">
+        <v>124</v>
+      </c>
+      <c r="H110" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B111" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="C111" t="s">
         <v>5</v>
       </c>
       <c r="E111" t="s">
-        <v>187</v>
+        <v>248</v>
       </c>
       <c r="F111" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B112" t="s">
-        <v>151</v>
+        <v>143</v>
+      </c>
+      <c r="C112" t="s">
+        <v>5</v>
       </c>
       <c r="E112" t="s">
-        <v>253</v>
+        <v>187</v>
       </c>
       <c r="F112" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="B113" t="s">
-        <v>215</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>211</v>
+        <v>151</v>
+      </c>
+      <c r="E113" t="s">
+        <v>253</v>
+      </c>
+      <c r="F113" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>214</v>
+      </c>
+      <c r="B114" t="s">
+        <v>215</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>144</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>145</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>180</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E115" t="s">
         <v>258</v>
       </c>
-      <c r="F114" t="s">
+      <c r="F115" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove spaces before first name initials
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben.jones/Library/Mobile Documents/com~apple~CloudDocs/Work/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745D03D6-513E-D144-B351-B4F0C45E7DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE19F1A8-603B-2847-9490-B424B304CFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="251">
   <si>
     <t>LastName</t>
   </si>
@@ -73,9 +73,6 @@
     <t xml:space="preserve">\'Alvarez                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> V.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Instituto de Instrumentaci\'on para Imagen Molecular (I3M), Centro Mixto CSIC - Universitat Polit\`ecnica de Val\`encia, Camino de Vera s/n </t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t xml:space="preserve">Arazi                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> L.         </t>
-  </si>
-  <si>
     <t>Unit of Nuclear Engineering, Faculty of Engineering Sciences, Ben-Gurion University of the Negev, P.O.B. 653</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t xml:space="preserve">Arnquist                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> I.J.       </t>
-  </si>
-  <si>
     <t xml:space="preserve">Pacific Northwest National Laboratory (PNNL) </t>
   </si>
   <si>
@@ -148,9 +139,6 @@
     <t xml:space="preserve">Azevedo                      </t>
   </si>
   <si>
-    <t xml:space="preserve"> C.D.R.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Institute of Nanostructures, Nanomodelling and Nanofabrication (i3N), Universidade de Aveiro, Campus de Santiago </t>
   </si>
   <si>
@@ -160,15 +148,9 @@
     <t xml:space="preserve">Bailey                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> K.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ballester                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> F.         </t>
-  </si>
-  <si>
     <t>del Barrio-Torregrosa</t>
   </si>
   <si>
@@ -199,9 +181,6 @@
     <t xml:space="preserve">Borges                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> F.I.G.M.   </t>
-  </si>
-  <si>
     <t xml:space="preserve">LIP, Department of Physics, University of Coimbra </t>
   </si>
   <si>
@@ -217,9 +196,6 @@
     <t xml:space="preserve">Byrnes                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> N.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Department of Physics, University of Texas at Arlington </t>
   </si>
   <si>
@@ -229,9 +205,6 @@
     <t xml:space="preserve">C\'arcel                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> S.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Instituto de F\'isica Corpuscular (IFIC), CSIC \&amp; Universitat de Val\`encia, Calle Catedr\'atico Jos\'e Beltr\'an, 2 </t>
   </si>
   <si>
@@ -241,9 +214,6 @@
     <t xml:space="preserve">Carri\'on                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.V.       </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cebri\'an                    </t>
   </si>
   <si>
@@ -256,9 +226,6 @@
     <t xml:space="preserve">Church                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> E.         </t>
-  </si>
-  <si>
     <t>Cid</t>
   </si>
   <si>
@@ -268,18 +235,12 @@
     <t xml:space="preserve">Conde                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> C.A.N.     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Coimbra, 3004-516, Portugal</t>
   </si>
   <si>
     <t xml:space="preserve">Contreras                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> T.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Department of Physics, Harvard University </t>
   </si>
   <si>
@@ -301,9 +262,6 @@
     <t xml:space="preserve">D\'iaz                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> G.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Instituto Gallego de F\'isica de Altas Energ\'ias, Univ.\ de Santiago de Compostela, Campus sur, R\'ua Xos\'e Mar\'ia Su\'arez N\'u\~nez, s/n </t>
   </si>
   <si>
@@ -322,15 +280,9 @@
     <t xml:space="preserve">Escada                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Esteve                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> R.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Felkai                       </t>
   </si>
   <si>
@@ -343,18 +295,12 @@
     <t xml:space="preserve">Fernandes                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> L.M.P.     </t>
-  </si>
-  <si>
     <t xml:space="preserve">LIBPhys, Physics Department, University of Coimbra, Rua Larga </t>
   </si>
   <si>
     <t xml:space="preserve">Ferrario                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> P.         </t>
-  </si>
-  <si>
     <t>Ikerbasque (Basque Foundation for Science)</t>
   </si>
   <si>
@@ -364,9 +310,6 @@
     <t xml:space="preserve">Ferreira                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> A.L.       </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Aveiro, 3810-193, Portugal</t>
   </si>
   <si>
@@ -382,9 +325,6 @@
     <t xml:space="preserve">Freitas                      </t>
   </si>
   <si>
-    <t xml:space="preserve"> E.D.C.     </t>
-  </si>
-  <si>
     <t>Freixa</t>
   </si>
   <si>
@@ -397,9 +337,6 @@
     <t xml:space="preserve">Goldschmidt                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> A.          </t>
-  </si>
-  <si>
     <t xml:space="preserve">Lawrence Berkeley National Laboratory (LBNL), 1 Cyclotron Road </t>
   </si>
   <si>
@@ -424,9 +361,6 @@
     <t>Grocott</t>
   </si>
   <si>
-    <t xml:space="preserve"> J.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Guenette                    </t>
   </si>
   <si>
@@ -445,24 +379,15 @@
     <t xml:space="preserve">Henriques                   </t>
   </si>
   <si>
-    <t xml:space="preserve"> C.A.O.     </t>
-  </si>
-  <si>
     <t xml:space="preserve">Hernando~Morata             </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.A.       </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Santiago de Compostela, E-15782, Spain</t>
   </si>
   <si>
     <t>Herrero-G\'omez</t>
   </si>
   <si>
-    <t xml:space="preserve"> P.        </t>
-  </si>
-  <si>
     <t>Hebrew University</t>
   </si>
   <si>
@@ -472,30 +397,18 @@
     <t xml:space="preserve">Herrero                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> V.        </t>
-  </si>
-  <si>
     <t>Herv\'es Carrete</t>
   </si>
   <si>
     <t xml:space="preserve">Ifergan                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> Y.        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Jones                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> B.J.P.    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Labarga                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> L.        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Departamento de F\'isica Te\'orica, Universidad Aut\'onoma de Madrid, Campus de Cantoblanco </t>
   </si>
   <si>
@@ -526,18 +439,12 @@
     <t xml:space="preserve">L\'opez-March               </t>
   </si>
   <si>
-    <t xml:space="preserve"> N.        </t>
-  </si>
-  <si>
     <t>Madigan</t>
   </si>
   <si>
     <t xml:space="preserve">Mano                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> R.D.P.     </t>
-  </si>
-  <si>
     <t>Marques</t>
   </si>
   <si>
@@ -547,30 +454,18 @@
     <t xml:space="preserve">Mart\'in-Albo               </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.        </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Paterna, E-46980, Spain </t>
   </si>
   <si>
     <t xml:space="preserve">Mart\'inez-Lema             </t>
   </si>
   <si>
-    <t xml:space="preserve"> G.        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mart\'inez-Vara             </t>
   </si>
   <si>
-    <t xml:space="preserve"> M.        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Meziani                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> Z.E.      </t>
-  </si>
-  <si>
     <t>Miller</t>
   </si>
   <si>
@@ -592,21 +487,12 @@
     <t xml:space="preserve">Monrabal                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> F.        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Monteiro                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> C.M.B.    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mora                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> F.J.      </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mu\~noz Vidal               </t>
   </si>
   <si>
@@ -622,18 +508,12 @@
     <t xml:space="preserve">Novella                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> P.       </t>
-  </si>
-  <si>
     <t>Nu\~{n}ez</t>
   </si>
   <si>
     <t xml:space="preserve">Nygren                      </t>
   </si>
   <si>
-    <t xml:space="preserve"> D.R.      </t>
-  </si>
-  <si>
     <t>Oblak</t>
   </si>
   <si>
@@ -643,15 +523,9 @@
     <t xml:space="preserve">Palmeiro                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> B.        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Para                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> A.        </t>
-  </si>
-  <si>
     <t>Parmaksiz</t>
   </si>
   <si>
@@ -670,9 +544,6 @@
     <t xml:space="preserve">Redwine                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> A.B.      </t>
-  </si>
-  <si>
     <t xml:space="preserve">Renner                      </t>
   </si>
   <si>
@@ -694,27 +565,15 @@
     <t xml:space="preserve">Romo-Luque                  </t>
   </si>
   <si>
-    <t xml:space="preserve"> C.        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Santos                      </t>
   </si>
   <si>
-    <t xml:space="preserve"> F.P.      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> J.M.F. dos </t>
-  </si>
-  <si>
     <t>Shomroni</t>
   </si>
   <si>
     <t xml:space="preserve">Sim\'on                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> A.       </t>
-  </si>
-  <si>
     <t>Soleti</t>
   </si>
   <si>
@@ -736,9 +595,6 @@
     <t xml:space="preserve">Toledo                      </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.F.      </t>
-  </si>
-  <si>
     <t xml:space="preserve">Torrent                     </t>
   </si>
   <si>
@@ -757,9 +613,6 @@
     <t xml:space="preserve">Veloso                      </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.F.C.A.  </t>
-  </si>
-  <si>
     <t>Waiton</t>
   </si>
   <si>
@@ -769,9 +622,6 @@
     <t xml:space="preserve">White                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.T.      </t>
-  </si>
-  <si>
     <t xml:space="preserve">Deceased. </t>
   </si>
   <si>
@@ -779,6 +629,150 @@
   </si>
   <si>
     <t xml:space="preserve"> College Station, TX 77843-4242, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.A.N.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I.J.       </t>
+  </si>
+  <si>
+    <t>C.D.R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F.I.G.M.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.V.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L.M.P.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.L.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.D.C.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.A.O.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.A.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.J.P.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R.D.P.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z.E.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.M.B.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F.J.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.R.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.B.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F.P.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.M.F. dos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.F.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.F.C.A.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.T.      </t>
   </si>
 </sst>
 </file>
@@ -1621,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1686,119 +1680,119 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>209</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1809,494 +1803,494 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>211</v>
       </c>
       <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
         <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>212</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>213</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>214</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>213</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>215</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>204</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F26" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>218</v>
       </c>
       <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
         <v>18</v>
-      </c>
-      <c r="F33" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>218</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="E35" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F35" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H36" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>221</v>
       </c>
       <c r="E37" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F37" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="F38" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>222</v>
       </c>
       <c r="E39" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F39" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="E40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G40" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H40" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="E41" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>223</v>
       </c>
       <c r="E42" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E43" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H43" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="E44" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="E45" t="s">
         <v>14</v>
@@ -2307,10 +2301,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>218</v>
       </c>
       <c r="E46" t="s">
         <v>14</v>
@@ -2321,10 +2315,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -2335,290 +2329,290 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="E48" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="F48" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>224</v>
       </c>
       <c r="E49" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F49" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="E50" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F50" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E51" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="F51" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>226</v>
       </c>
       <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" t="s">
         <v>18</v>
-      </c>
-      <c r="F52" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F53" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="E54" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>228</v>
       </c>
       <c r="E55" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F55" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B56" t="s">
-        <v>157</v>
+        <v>229</v>
       </c>
       <c r="E56" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="F56" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E57" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" t="s">
         <v>22</v>
-      </c>
-      <c r="F58" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="E59" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="F59" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E60" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>230</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F61" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="E62" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="F62" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="B63" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="E63" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F63" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="B64" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="E64" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F64" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="E65" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F65" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="B66" t="s">
-        <v>178</v>
+        <v>233</v>
       </c>
       <c r="E66" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
-        <v>180</v>
+        <v>234</v>
       </c>
       <c r="E67" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>235</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -2629,198 +2623,198 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="B69" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="E69" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="F69" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="E70" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F70" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="B71" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="E71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71" t="s">
         <v>22</v>
-      </c>
-      <c r="F71" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="B72" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="E72" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G72" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H72" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="B73" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
       <c r="E73" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F73" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="B74" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="E74" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74" t="s">
         <v>18</v>
-      </c>
-      <c r="F74" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="E75" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F75" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="B76" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="E76" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F76" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="B77" t="s">
-        <v>200</v>
+        <v>239</v>
       </c>
       <c r="E77" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F77" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F78" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
+        <v>240</v>
       </c>
       <c r="E79" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F79" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="B80" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E80" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="E81" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F81" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="B82" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2831,156 +2825,156 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="B83" t="s">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="E83" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="F83" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>210</v>
+        <v>168</v>
       </c>
       <c r="B84" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
       <c r="E84" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F84" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="B85" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="E85" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="B86" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E86" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F86" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
       <c r="B87" t="s">
-        <v>180</v>
+        <v>234</v>
       </c>
       <c r="E87" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F87" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>215</v>
+        <v>173</v>
       </c>
       <c r="B88" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
       <c r="E88" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F88" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="B89" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="E89" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F89" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="B90" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
       <c r="E90" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G90" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H90" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>219</v>
+        <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="E91" t="s">
+        <v>17</v>
+      </c>
+      <c r="F91" t="s">
         <v>18</v>
-      </c>
-      <c r="F91" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
       </c>
       <c r="E92" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F92" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="B93" t="s">
-        <v>157</v>
+        <v>229</v>
       </c>
       <c r="E93" t="s">
         <v>10</v>
@@ -2991,187 +2985,187 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
       <c r="B94" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="E94" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F94" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H94" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="E95" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F95" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="B96" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="E96" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F96" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="B97" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="E97" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F97" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>228</v>
+        <v>182</v>
       </c>
       <c r="B98" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
       <c r="E98" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="F98" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>229</v>
+        <v>183</v>
       </c>
       <c r="B99" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="E99" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F99" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="B100" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="E100" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F100" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>233</v>
+        <v>186</v>
       </c>
       <c r="B101" t="s">
-        <v>180</v>
+        <v>234</v>
       </c>
       <c r="E101" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F101" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>234</v>
+        <v>187</v>
       </c>
       <c r="B102" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="E102" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F102" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>235</v>
+        <v>188</v>
       </c>
       <c r="B103" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="E103" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F103" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>237</v>
+        <v>190</v>
       </c>
       <c r="B104" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="E104" t="s">
+        <v>17</v>
+      </c>
+      <c r="F104" t="s">
         <v>18</v>
-      </c>
-      <c r="F104" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>239</v>
+        <v>191</v>
       </c>
       <c r="B105" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="E105" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F105" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G105" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="H105" t="s">
-        <v>241</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>242</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E106" t="s">
         <v>14</v>
@@ -3182,38 +3176,38 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>243</v>
+        <v>195</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="E107" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F107" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="B108" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E108" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F108" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="B109" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
@@ -3224,19 +3218,19 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="B110" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C110" t="s">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="E110" t="s">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="F110" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DIPC updates: add A. Castillo, C. Echevarria, M. Seeman, A. Yubero; A.I. Aranburu from CFM to DIPC
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE19F1A8-603B-2847-9490-B424B304CFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C495876-E5A3-9F41-B991-E2C7488BEAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13480" yWindow="3220" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="255">
   <si>
     <t>LastName</t>
   </si>
@@ -773,6 +773,18 @@
   </si>
   <si>
     <t xml:space="preserve">J.T.      </t>
+  </si>
+  <si>
+    <t>Castillo</t>
+  </si>
+  <si>
+    <t>Echevarria</t>
+  </si>
+  <si>
+    <t>Seeman</t>
+  </si>
+  <si>
+    <t>Yubero</t>
   </si>
 </sst>
 </file>
@@ -1613,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1711,7 +1723,7 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
@@ -1935,328 +1947,325 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>251</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>204</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>216</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>203</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>252</v>
       </c>
       <c r="B32" t="s">
-        <v>217</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>218</v>
+        <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>218</v>
-      </c>
-      <c r="C34" t="s">
-        <v>88</v>
+        <v>217</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E35" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" t="s">
-        <v>93</v>
-      </c>
-      <c r="H36" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>220</v>
       </c>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>59</v>
+        <v>22</v>
+      </c>
+      <c r="G38" t="s">
+        <v>93</v>
+      </c>
+      <c r="H38" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E39" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="F39" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" t="s">
-        <v>93</v>
-      </c>
-      <c r="H40" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E41" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="F41" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>223</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>106</v>
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>93</v>
+      </c>
+      <c r="H42" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C43" t="s">
-        <v>109</v>
+        <v>217</v>
       </c>
       <c r="E43" t="s">
         <v>45</v>
@@ -2264,246 +2273,249 @@
       <c r="F43" t="s">
         <v>22</v>
       </c>
-      <c r="G43" t="s">
-        <v>93</v>
-      </c>
-      <c r="H43" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>223</v>
       </c>
       <c r="E44" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>153</v>
+        <v>108</v>
+      </c>
+      <c r="C45" t="s">
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
+        <v>93</v>
+      </c>
+      <c r="H45" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>111</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B47" t="s">
-        <v>210</v>
+        <v>153</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E48" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="F48" t="s">
-        <v>117</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E49" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E50" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F50" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>224</v>
       </c>
       <c r="E51" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="F51" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E52" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="F52" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="E53" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="F53" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E54" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F54" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>228</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="F55" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B56" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E56" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>228</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>229</v>
       </c>
       <c r="E58" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
       <c r="E59" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E60" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F60" t="s">
         <v>22</v>
@@ -2511,571 +2523,571 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B61" t="s">
-        <v>230</v>
+        <v>134</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
       <c r="F61" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="E62" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E63" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="E64" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="F64" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E65" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="F65" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B66" t="s">
-        <v>233</v>
+        <v>142</v>
       </c>
       <c r="E66" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B67" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E67" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F67" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B68" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F68" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>234</v>
       </c>
       <c r="E69" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B70" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="E70" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="F70" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B71" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E71" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="F71" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E72" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F72" t="s">
-        <v>22</v>
-      </c>
-      <c r="G72" t="s">
-        <v>93</v>
-      </c>
-      <c r="H72" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B73" t="s">
-        <v>237</v>
+        <v>153</v>
       </c>
       <c r="E73" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="F73" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B74" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E74" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="F74" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="G74" t="s">
+        <v>93</v>
+      </c>
+      <c r="H74" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E75" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="F75" t="s">
-        <v>158</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B76" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="E76" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F76" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B77" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E77" t="s">
         <v>61</v>
       </c>
       <c r="F77" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>160</v>
       </c>
       <c r="E78" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F78" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B79" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F79" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="E80" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F80" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s">
-        <v>153</v>
+        <v>240</v>
       </c>
       <c r="E81" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F81" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B82" t="s">
-        <v>241</v>
+        <v>78</v>
       </c>
       <c r="E82" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F82" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
       <c r="E83" t="s">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="F83" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>241</v>
       </c>
       <c r="E84" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="F84" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B85" t="s">
-        <v>153</v>
+        <v>242</v>
       </c>
       <c r="E85" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="F85" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B86" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="E86" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="F86" t="s">
-        <v>120</v>
+        <v>59</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B87" t="s">
-        <v>234</v>
+        <v>153</v>
       </c>
       <c r="E87" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F87" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B88" t="s">
-        <v>243</v>
+        <v>44</v>
       </c>
       <c r="E88" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="F88" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B89" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E89" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="F89" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>243</v>
       </c>
       <c r="E90" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F90" t="s">
-        <v>22</v>
-      </c>
-      <c r="G90" t="s">
-        <v>93</v>
-      </c>
-      <c r="H90" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B91" t="s">
         <v>232</v>
       </c>
       <c r="E91" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="F91" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="E92" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F92" t="s">
         <v>22</v>
       </c>
+      <c r="G92" t="s">
+        <v>93</v>
+      </c>
+      <c r="H92" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F93" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B94" t="s">
-        <v>241</v>
+        <v>9</v>
       </c>
       <c r="E94" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F94" t="s">
         <v>22</v>
       </c>
-      <c r="H94" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B95" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="E95" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F95" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B96" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E96" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F96" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="H96" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B97" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E97" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F97" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B98" t="s">
-        <v>169</v>
+        <v>245</v>
       </c>
       <c r="E98" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="F98" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B99" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E99" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="F99" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>184</v>
+        <v>253</v>
       </c>
       <c r="B100" t="s">
-        <v>185</v>
+        <v>44</v>
       </c>
       <c r="E100" t="s">
         <v>45</v>
@@ -3086,128 +3098,128 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B101" t="s">
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="E101" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="F101" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B102" t="s">
-        <v>153</v>
+        <v>247</v>
       </c>
       <c r="E102" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F102" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B103" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E103" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F103" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B104" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="E104" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F104" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B105" t="s">
-        <v>232</v>
+        <v>153</v>
       </c>
       <c r="E105" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F105" t="s">
-        <v>22</v>
-      </c>
-      <c r="G105" t="s">
-        <v>192</v>
-      </c>
-      <c r="H105" t="s">
-        <v>193</v>
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B106" t="s">
-        <v>47</v>
+        <v>189</v>
       </c>
       <c r="E106" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="F106" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B107" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E107" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="F107" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B108" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="E108" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F108" t="s">
-        <v>96</v>
+        <v>22</v>
+      </c>
+      <c r="G108" t="s">
+        <v>192</v>
+      </c>
+      <c r="H108" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B109" t="s">
-        <v>198</v>
+        <v>47</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
@@ -3218,19 +3230,75 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>195</v>
+      </c>
+      <c r="B110" t="s">
+        <v>242</v>
+      </c>
+      <c r="E110" t="s">
+        <v>61</v>
+      </c>
+      <c r="F110" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>196</v>
+      </c>
+      <c r="B111" t="s">
+        <v>249</v>
+      </c>
+      <c r="E111" t="s">
+        <v>39</v>
+      </c>
+      <c r="F111" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>197</v>
+      </c>
+      <c r="B112" t="s">
+        <v>198</v>
+      </c>
+      <c r="E112" t="s">
+        <v>14</v>
+      </c>
+      <c r="F112" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>199</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B113" t="s">
         <v>250</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C113" t="s">
         <v>200</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E113" t="s">
         <v>201</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F113" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>254</v>
+      </c>
+      <c r="B114" t="s">
+        <v>47</v>
+      </c>
+      <c r="E114" t="s">
+        <v>45</v>
+      </c>
+      <c r="F114" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove goldschmidt, labarga, white
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben.jones/Library/Mobile Documents/com~apple~CloudDocs/Work/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F033F28-9634-A144-81BF-E4E7393DECE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF53442-8447-8D4B-AA49-7D50CE8E5C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3220" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="244">
   <si>
     <t>LastName</t>
   </si>
@@ -334,15 +334,6 @@
     <t xml:space="preserve">Generowicz                   </t>
   </si>
   <si>
-    <t xml:space="preserve">Goldschmidt                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence Berkeley National Laboratory (LBNL), 1 Cyclotron Road </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Berkeley, CA 94720, USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">G\'omez-Cadenas             </t>
   </si>
   <si>
@@ -406,15 +397,6 @@
     <t xml:space="preserve">Jones                       </t>
   </si>
   <si>
-    <t xml:space="preserve">Labarga                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Departamento de F\'isica Te\'orica, Universidad Aut\'onoma de Madrid, Campus de Cantoblanco </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Madrid, E-28049, Spain</t>
-  </si>
-  <si>
     <t>Larizgoitia</t>
   </si>
   <si>
@@ -619,18 +601,6 @@
     <t xml:space="preserve">J. </t>
   </si>
   <si>
-    <t xml:space="preserve">White                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deceased. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Department of Physics and Astronomy, Texas A\&amp;M University </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> College Station, TX 77843-4242, USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">G.         </t>
   </si>
   <si>
@@ -691,9 +661,6 @@
     <t xml:space="preserve">E.D.C.     </t>
   </si>
   <si>
-    <t xml:space="preserve">A.          </t>
-  </si>
-  <si>
     <t xml:space="preserve">C.A.O.     </t>
   </si>
   <si>
@@ -770,9 +737,6 @@
   </si>
   <si>
     <t xml:space="preserve">J.F.C.A.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.T.      </t>
   </si>
   <si>
     <t>Castillo</t>
@@ -1628,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1695,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -1737,7 +1701,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -1751,7 +1715,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1793,7 +1757,7 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1807,7 +1771,7 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1821,7 +1785,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
@@ -1877,7 +1841,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
@@ -1911,7 +1875,7 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="E19" t="s">
         <v>58</v>
@@ -1925,7 +1889,7 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -1939,7 +1903,7 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E21" t="s">
         <v>61</v>
@@ -1950,10 +1914,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B22" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E22" t="s">
         <v>45</v>
@@ -1967,7 +1931,7 @@
         <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E23" t="s">
         <v>65</v>
@@ -1981,7 +1945,7 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>
@@ -2009,7 +1973,7 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
@@ -2023,7 +1987,7 @@
         <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E27" t="s">
         <v>73</v>
@@ -2071,7 +2035,7 @@
         <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E30" t="s">
         <v>80</v>
@@ -2096,7 +2060,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
@@ -2127,7 +2091,7 @@
         <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E34" t="s">
         <v>53</v>
@@ -2141,7 +2105,7 @@
         <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="E35" t="s">
         <v>17</v>
@@ -2155,7 +2119,7 @@
         <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C36" t="s">
         <v>88</v>
@@ -2172,7 +2136,7 @@
         <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E37" t="s">
         <v>91</v>
@@ -2186,7 +2150,7 @@
         <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E38" t="s">
         <v>45</v>
@@ -2206,7 +2170,7 @@
         <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E39" t="s">
         <v>39</v>
@@ -2234,7 +2198,7 @@
         <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E41" t="s">
         <v>91</v>
@@ -2268,7 +2232,7 @@
         <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E43" t="s">
         <v>45</v>
@@ -2282,13 +2246,22 @@
         <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>223</v>
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
+        <v>106</v>
       </c>
       <c r="E44" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>106</v>
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2298,42 +2271,33 @@
       <c r="B45" t="s">
         <v>108</v>
       </c>
-      <c r="C45" t="s">
-        <v>109</v>
-      </c>
       <c r="E45" t="s">
         <v>45</v>
       </c>
       <c r="F45" t="s">
         <v>22</v>
       </c>
-      <c r="G45" t="s">
-        <v>93</v>
-      </c>
-      <c r="H45" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>243</v>
       </c>
       <c r="E46" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>255</v>
+        <v>208</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
@@ -2344,30 +2308,30 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" t="s">
         <v>114</v>
-      </c>
-      <c r="B49" t="s">
-        <v>210</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2375,38 +2339,38 @@
         <v>115</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E50" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F50" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B51" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E51" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F51" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" t="s">
         <v>119</v>
-      </c>
-      <c r="B52" t="s">
-        <v>225</v>
-      </c>
-      <c r="E52" t="s">
-        <v>80</v>
       </c>
       <c r="F52" t="s">
         <v>120</v>
@@ -2417,108 +2381,108 @@
         <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>215</v>
       </c>
       <c r="E53" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="F53" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B54" t="s">
-        <v>226</v>
+        <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="F54" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E55" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E56" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F56" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>228</v>
+        <v>69</v>
       </c>
       <c r="E57" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>229</v>
+        <v>47</v>
       </c>
       <c r="E58" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="F58" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="E59" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="F59" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E60" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F60" t="s">
         <v>22</v>
@@ -2526,571 +2490,571 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="E61" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="F61" t="s">
-        <v>136</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B62" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="E62" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="F62" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B63" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="F63" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B64" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="E64" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="F64" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B65" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E65" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F65" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B66" t="s">
-        <v>142</v>
+        <v>222</v>
       </c>
       <c r="E66" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F66" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B67" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E67" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F67" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E68" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F68" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="E69" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="F69" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>235</v>
+        <v>145</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="F70" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B71" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E71" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="F71" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B72" t="s">
-        <v>151</v>
+        <v>225</v>
       </c>
       <c r="E72" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F72" t="s">
-        <v>59</v>
+        <v>22</v>
+      </c>
+      <c r="G72" t="s">
+        <v>93</v>
+      </c>
+      <c r="H72" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B73" t="s">
-        <v>153</v>
+        <v>226</v>
       </c>
       <c r="E73" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F73" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E74" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F74" t="s">
-        <v>22</v>
-      </c>
-      <c r="G74" t="s">
-        <v>93</v>
-      </c>
-      <c r="H74" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="E75" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F75" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B76" t="s">
-        <v>238</v>
+        <v>154</v>
       </c>
       <c r="E76" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="F76" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B77" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E77" t="s">
         <v>61</v>
       </c>
       <c r="F77" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B78" t="s">
-        <v>160</v>
+        <v>47</v>
       </c>
       <c r="E78" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F78" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E79" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F79" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="E80" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F80" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B81" t="s">
-        <v>240</v>
+        <v>147</v>
       </c>
       <c r="E81" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F81" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B82" t="s">
-        <v>78</v>
+        <v>230</v>
       </c>
       <c r="E82" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="E83" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="F83" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
-        <v>241</v>
+        <v>163</v>
       </c>
       <c r="E84" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="F84" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B85" t="s">
-        <v>242</v>
+        <v>147</v>
       </c>
       <c r="E85" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="F85" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="E86" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="F86" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B87" t="s">
-        <v>153</v>
+        <v>223</v>
       </c>
       <c r="E87" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F87" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="E88" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="F88" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="E89" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="F89" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>243</v>
+        <v>163</v>
       </c>
       <c r="E90" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="F90" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="G90" t="s">
+        <v>93</v>
+      </c>
+      <c r="H90" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B91" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="E91" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="F91" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B92" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="E92" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F92" t="s">
         <v>22</v>
       </c>
-      <c r="G92" t="s">
-        <v>93</v>
-      </c>
-      <c r="H92" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B93" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="E93" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F93" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E94" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F94" t="s">
         <v>22</v>
       </c>
+      <c r="H94" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="F95" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E96" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F96" t="s">
-        <v>22</v>
-      </c>
-      <c r="H96" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E97" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="F97" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>241</v>
       </c>
       <c r="B98" t="s">
-        <v>245</v>
+        <v>44</v>
       </c>
       <c r="E98" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F98" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B99" t="s">
-        <v>246</v>
+        <v>163</v>
       </c>
       <c r="E99" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="F99" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>253</v>
+        <v>177</v>
       </c>
       <c r="B100" t="s">
-        <v>44</v>
+        <v>236</v>
       </c>
       <c r="E100" t="s">
         <v>45</v>
@@ -3101,206 +3065,161 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B101" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E101" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="F101" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B102" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="E102" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F102" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B103" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="E103" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F103" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B104" t="s">
-        <v>234</v>
+        <v>183</v>
       </c>
       <c r="E104" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="F104" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B105" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="E105" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="F105" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B106" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="E106" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F106" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="G106" t="s">
+        <v>186</v>
+      </c>
+      <c r="H106" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B107" t="s">
-        <v>248</v>
+        <v>47</v>
       </c>
       <c r="E107" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F107" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B108" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E108" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F108" t="s">
-        <v>22</v>
-      </c>
-      <c r="G108" t="s">
-        <v>192</v>
-      </c>
-      <c r="H108" t="s">
-        <v>193</v>
+        <v>62</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B109" t="s">
-        <v>47</v>
+        <v>238</v>
       </c>
       <c r="E109" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F109" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B110" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
       <c r="E110" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F110" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="B111" t="s">
-        <v>249</v>
+        <v>47</v>
       </c>
       <c r="E111" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F111" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>197</v>
-      </c>
-      <c r="B112" t="s">
-        <v>198</v>
-      </c>
-      <c r="E112" t="s">
-        <v>14</v>
-      </c>
-      <c r="F112" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>199</v>
-      </c>
-      <c r="B113" t="s">
-        <v>250</v>
-      </c>
-      <c r="C113" t="s">
-        <v>200</v>
-      </c>
-      <c r="E113" t="s">
-        <v>201</v>
-      </c>
-      <c r="F113" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>254</v>
-      </c>
-      <c r="B114" t="s">
-        <v>47</v>
-      </c>
-      <c r="E114" t="s">
-        <v>45</v>
-      </c>
-      <c r="F114" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove JV Carrion, J Generowicz, J Munoz Vidal, J Rodriguez
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF53442-8447-8D4B-AA49-7D50CE8E5C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779B3E40-974F-6245-A26C-FADC9F252D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="3220" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="2240" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="238">
   <si>
     <t>LastName</t>
   </si>
@@ -211,9 +211,6 @@
     <t xml:space="preserve"> Paterna, E-46980, Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">Carri\'on                    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cebri\'an                    </t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>Z.</t>
   </si>
   <si>
-    <t xml:space="preserve">Generowicz                   </t>
-  </si>
-  <si>
     <t xml:space="preserve">G\'omez-Cadenas             </t>
   </si>
   <si>
@@ -475,12 +469,6 @@
     <t xml:space="preserve">Mora                        </t>
   </si>
   <si>
-    <t xml:space="preserve">Mu\~noz Vidal               </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paterna, E-46980, Spain  </t>
-  </si>
-  <si>
     <t>Navarro</t>
   </si>
   <si>
@@ -532,9 +520,6 @@
     <t>Rivilla</t>
   </si>
   <si>
-    <t xml:space="preserve">Rodr\'iguez                 </t>
-  </si>
-  <si>
     <t>Rogero</t>
   </si>
   <si>
@@ -632,9 +617,6 @@
   </si>
   <si>
     <t xml:space="preserve">S.         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.V.       </t>
   </si>
   <si>
     <t xml:space="preserve">E.         </t>
@@ -1592,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1659,7 +1641,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -1701,7 +1683,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -1715,7 +1697,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1757,7 +1739,7 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1771,7 +1753,7 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1785,7 +1767,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
@@ -1841,7 +1823,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
@@ -1875,7 +1857,7 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E19" t="s">
         <v>58</v>
@@ -1889,7 +1871,7 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -1900,44 +1882,44 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>233</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>239</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1945,125 +1927,125 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>189</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>206</v>
+        <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>193</v>
+        <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>234</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>240</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
         <v>45</v>
@@ -2077,13 +2059,13 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -2091,13 +2073,13 @@
         <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="F34" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -2105,92 +2087,92 @@
         <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>202</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
-      </c>
-      <c r="C36" t="s">
-        <v>88</v>
+        <v>203</v>
       </c>
       <c r="E36" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="F36" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E37" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F37" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>92</v>
+      </c>
+      <c r="H37" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E38" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" t="s">
-        <v>93</v>
-      </c>
-      <c r="H38" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="F39" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -2198,41 +2180,50 @@
         <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>101</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
       </c>
       <c r="G42" t="s">
+        <v>92</v>
+      </c>
+      <c r="H42" t="s">
         <v>93</v>
-      </c>
-      <c r="H42" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="E43" t="s">
         <v>45</v>
@@ -2243,39 +2234,30 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" t="s">
-        <v>106</v>
+        <v>237</v>
       </c>
       <c r="E44" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" t="s">
-        <v>93</v>
-      </c>
-      <c r="H44" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="E45" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F45" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -2283,13 +2265,13 @@
         <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>243</v>
+        <v>195</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2297,83 +2279,83 @@
         <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="F47" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E49" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="F49" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>213</v>
+        <v>126</v>
       </c>
       <c r="E50" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="F50" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E51" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="F51" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="F52" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2381,13 +2363,13 @@
         <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E53" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2395,13 +2377,13 @@
         <v>122</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="E54" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="F54" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2409,13 +2391,13 @@
         <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>216</v>
+        <v>68</v>
       </c>
       <c r="E55" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="F55" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2423,13 +2405,13 @@
         <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>217</v>
+        <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2437,24 +2419,24 @@
         <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E58" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F58" t="s">
         <v>22</v>
@@ -2462,16 +2444,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="E59" t="s">
-        <v>129</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2479,13 +2461,13 @@
         <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="E60" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="F60" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2493,13 +2475,13 @@
         <v>132</v>
       </c>
       <c r="B61" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="F61" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2507,55 +2489,55 @@
         <v>133</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="E62" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="F62" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E63" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B64" t="s">
-        <v>136</v>
+        <v>216</v>
       </c>
       <c r="E64" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F64" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E65" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>138</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2563,13 +2545,13 @@
         <v>139</v>
       </c>
       <c r="B66" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E66" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2577,69 +2559,75 @@
         <v>140</v>
       </c>
       <c r="B67" t="s">
-        <v>223</v>
+        <v>141</v>
       </c>
       <c r="E67" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="F67" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>224</v>
+        <v>143</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="F68" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E69" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="F69" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>219</v>
       </c>
       <c r="E70" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F70" t="s">
-        <v>59</v>
+        <v>22</v>
+      </c>
+      <c r="G70" t="s">
+        <v>92</v>
+      </c>
+      <c r="H70" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>220</v>
       </c>
       <c r="E71" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="F71" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2647,19 +2635,13 @@
         <v>148</v>
       </c>
       <c r="B72" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E72" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F72" t="s">
-        <v>22</v>
-      </c>
-      <c r="G72" t="s">
-        <v>93</v>
-      </c>
-      <c r="H72" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2667,41 +2649,41 @@
         <v>149</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="F73" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B74" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E74" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F74" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B75" t="s">
-        <v>221</v>
+        <v>47</v>
       </c>
       <c r="E75" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F75" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2709,7 +2691,7 @@
         <v>153</v>
       </c>
       <c r="B76" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="E76" t="s">
         <v>58</v>
@@ -2720,24 +2702,24 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B77" t="s">
-        <v>228</v>
+        <v>77</v>
       </c>
       <c r="E77" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="E78" t="s">
         <v>48</v>
@@ -2748,44 +2730,44 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B79" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>225</v>
       </c>
       <c r="E80" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="F80" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
         <v>159</v>
       </c>
-      <c r="B81" t="s">
-        <v>147</v>
-      </c>
       <c r="E81" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F81" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2793,13 +2775,13 @@
         <v>160</v>
       </c>
       <c r="B82" t="s">
-        <v>230</v>
+        <v>145</v>
       </c>
       <c r="E82" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F82" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2807,13 +2789,13 @@
         <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>231</v>
+        <v>44</v>
       </c>
       <c r="E83" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="F83" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2821,91 +2803,97 @@
         <v>162</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="E84" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F84" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>147</v>
+        <v>226</v>
       </c>
       <c r="E85" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F85" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="E86" t="s">
+        <v>79</v>
+      </c>
+      <c r="F86" t="s">
         <v>80</v>
-      </c>
-      <c r="F86" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B87" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="E87" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F87" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="G87" t="s">
+        <v>92</v>
+      </c>
+      <c r="H87" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>9</v>
       </c>
       <c r="E88" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="F88" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E89" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F89" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B90" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
       <c r="E90" t="s">
         <v>45</v>
@@ -2913,61 +2901,58 @@
       <c r="F90" t="s">
         <v>22</v>
       </c>
-      <c r="G90" t="s">
-        <v>93</v>
-      </c>
       <c r="H90" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B91" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="E91" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F91" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>228</v>
       </c>
       <c r="E92" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F92" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B93" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="F93" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>173</v>
+        <v>235</v>
       </c>
       <c r="B94" t="s">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="E94" t="s">
         <v>45</v>
@@ -2975,64 +2960,61 @@
       <c r="F94" t="s">
         <v>22</v>
       </c>
-      <c r="H94" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B95" t="s">
-        <v>233</v>
+        <v>159</v>
       </c>
       <c r="E95" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="F95" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B96" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E96" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F96" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B97" t="s">
-        <v>235</v>
+        <v>174</v>
       </c>
       <c r="E97" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F97" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>241</v>
+        <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>44</v>
+        <v>217</v>
       </c>
       <c r="E98" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F98" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3040,13 +3022,13 @@
         <v>176</v>
       </c>
       <c r="B99" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E99" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="F99" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3054,27 +3036,27 @@
         <v>177</v>
       </c>
       <c r="B100" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="E100" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F100" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B101" t="s">
-        <v>179</v>
+        <v>231</v>
       </c>
       <c r="E101" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F101" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3082,144 +3064,88 @@
         <v>180</v>
       </c>
       <c r="B102" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E102" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F102" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="G102" t="s">
+        <v>181</v>
+      </c>
+      <c r="H102" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B103" t="s">
-        <v>147</v>
+        <v>47</v>
       </c>
       <c r="E103" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F103" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B104" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="E104" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F104" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B105" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E105" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="F105" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B106" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="E106" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F106" t="s">
-        <v>22</v>
-      </c>
-      <c r="G106" t="s">
-        <v>186</v>
-      </c>
-      <c r="H106" t="s">
-        <v>187</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
       <c r="B107" t="s">
         <v>47</v>
       </c>
       <c r="E107" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F107" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>189</v>
-      </c>
-      <c r="B108" t="s">
-        <v>231</v>
-      </c>
-      <c r="E108" t="s">
-        <v>61</v>
-      </c>
-      <c r="F108" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>190</v>
-      </c>
-      <c r="B109" t="s">
-        <v>238</v>
-      </c>
-      <c r="E109" t="s">
-        <v>39</v>
-      </c>
-      <c r="F109" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>191</v>
-      </c>
-      <c r="B110" t="s">
-        <v>192</v>
-      </c>
-      <c r="E110" t="s">
-        <v>14</v>
-      </c>
-      <c r="F110" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>242</v>
-      </c>
-      <c r="B111" t="s">
-        <v>47</v>
-      </c>
-      <c r="E111" t="s">
-        <v>45</v>
-      </c>
-      <c r="F111" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix typo in seemann
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779B3E40-974F-6245-A26C-FADC9F252D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A2D67F-286E-CC41-BEF0-2428FE27E9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="2240" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -727,13 +727,13 @@
     <t>Echevarria</t>
   </si>
   <si>
-    <t>Seeman</t>
-  </si>
-  <si>
     <t>Yubero</t>
   </si>
   <si>
     <t>J.W.R.</t>
+  </si>
+  <si>
+    <t>Seemann</t>
   </si>
 </sst>
 </file>
@@ -1576,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:XFD73"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2237,7 +2237,7 @@
         <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
@@ -2949,7 +2949,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B94" t="s">
         <v>44</v>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B107" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
add fabian kellerer at ific
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2F847D-40C2-124F-BAA0-AF55F50CF11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C0DE2C98-29FB-8F42-BADF-4AA13984C223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="8860" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6940" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="242">
   <si>
     <t>LastName</t>
   </si>
@@ -743,6 +755,9 @@
   </si>
   <si>
     <t>Pazos</t>
+  </si>
+  <si>
+    <t>Kellerer</t>
   </si>
 </sst>
 </file>
@@ -1583,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2397,27 +2412,27 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>241</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="E55" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F55" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="E56" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F56" t="s">
         <v>22</v>
@@ -2425,83 +2440,83 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="E57" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="F57" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="E58" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>213</v>
+        <v>33</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>213</v>
       </c>
       <c r="E60" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="F60" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>214</v>
+        <v>106</v>
       </c>
       <c r="E61" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F61" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B62" t="s">
-        <v>134</v>
+        <v>214</v>
       </c>
       <c r="E62" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="F62" t="s">
         <v>70</v>
@@ -2509,83 +2524,83 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B63" t="s">
-        <v>215</v>
+        <v>134</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F63" t="s">
-        <v>136</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B64" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E64" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B65" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E65" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F65" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="F66" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>218</v>
       </c>
       <c r="E67" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="F68" t="s">
         <v>59</v>
@@ -2593,215 +2608,215 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E69" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="F69" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>145</v>
       </c>
       <c r="E70" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F70" t="s">
         <v>22</v>
-      </c>
-      <c r="G70" t="s">
-        <v>92</v>
-      </c>
-      <c r="H70" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B71" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E71" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>70</v>
+        <v>22</v>
+      </c>
+      <c r="G71" t="s">
+        <v>92</v>
+      </c>
+      <c r="H71" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E72" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="F72" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
       <c r="E73" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F73" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="E74" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F74" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>47</v>
+        <v>222</v>
       </c>
       <c r="E75" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F75" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>47</v>
       </c>
       <c r="E76" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F76" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>223</v>
       </c>
       <c r="E77" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F77" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="E78" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F78" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F79" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B80" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E80" t="s">
-        <v>127</v>
+        <v>14</v>
       </c>
       <c r="F80" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" t="s">
-        <v>159</v>
+        <v>225</v>
       </c>
       <c r="E81" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="F81" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="E82" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="B83" t="s">
-        <v>145</v>
+        <v>47</v>
       </c>
       <c r="E83" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F83" t="s">
         <v>22</v>
@@ -2809,151 +2824,151 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B84" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="E84" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="F84" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B85" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="E85" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F85" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E86" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="F86" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="E87" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F87" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B88" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="E88" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F88" t="s">
-        <v>22</v>
-      </c>
-      <c r="G88" t="s">
-        <v>92</v>
-      </c>
-      <c r="H88" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="E89" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F89" t="s">
         <v>22</v>
+      </c>
+      <c r="G89" t="s">
+        <v>92</v>
+      </c>
+      <c r="H89" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B90" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="E90" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="F90" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="E91" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F91" t="s">
-        <v>22</v>
-      </c>
-      <c r="H91" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B92" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E92" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F92" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="H92" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E93" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F93" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2961,10 +2976,10 @@
         <v>170</v>
       </c>
       <c r="B94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E94" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F94" t="s">
         <v>70</v>
@@ -2972,52 +2987,52 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>237</v>
+        <v>170</v>
       </c>
       <c r="B95" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="E95" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F95" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B96" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="E96" t="s">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="F96" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B97" t="s">
-        <v>230</v>
+        <v>159</v>
       </c>
       <c r="E97" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="F97" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B98" t="s">
-        <v>174</v>
+        <v>230</v>
       </c>
       <c r="E98" t="s">
         <v>45</v>
@@ -3028,24 +3043,24 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B99" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="E99" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F99" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B100" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="E100" t="s">
         <v>61</v>
@@ -3056,139 +3071,153 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="E101" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="F101" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B102" t="s">
-        <v>231</v>
+        <v>178</v>
       </c>
       <c r="E102" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="F102" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B103" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="E103" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F103" t="s">
-        <v>22</v>
-      </c>
-      <c r="G103" t="s">
-        <v>181</v>
-      </c>
-      <c r="H103" t="s">
-        <v>182</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B104" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="E104" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F104" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="G104" t="s">
+        <v>181</v>
+      </c>
+      <c r="H104" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
-        <v>225</v>
+        <v>47</v>
       </c>
       <c r="E105" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F105" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>184</v>
       </c>
       <c r="B106" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="E106" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F106" t="s">
-        <v>22</v>
-      </c>
-      <c r="G106" t="s">
-        <v>25</v>
-      </c>
-      <c r="H106" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>185</v>
+        <v>238</v>
       </c>
       <c r="B107" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E107" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F107" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="G107" t="s">
+        <v>25</v>
+      </c>
+      <c r="H107" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B108" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="E108" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F108" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>186</v>
+      </c>
+      <c r="B109" t="s">
+        <v>187</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>235</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>47</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E110" t="s">
         <v>45</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F110" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add c. tonnele (dipc)
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C0DE2C98-29FB-8F42-BADF-4AA13984C223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D228AF-F5E1-0742-B8C1-9BBBCD9498A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="243">
   <si>
     <t>LastName</t>
   </si>
@@ -758,6 +758,9 @@
   </si>
   <si>
     <t>Kellerer</t>
+  </si>
+  <si>
+    <t>Tonnel\'e</t>
   </si>
 </sst>
 </file>
@@ -1598,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3113,10 +3116,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="B104" t="s">
-        <v>215</v>
+        <v>9</v>
       </c>
       <c r="E104" t="s">
         <v>45</v>
@@ -3124,100 +3127,114 @@
       <c r="F104" t="s">
         <v>22</v>
       </c>
-      <c r="G104" t="s">
-        <v>181</v>
-      </c>
-      <c r="H104" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B105" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="E105" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F105" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="G105" t="s">
+        <v>181</v>
+      </c>
+      <c r="H105" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B106" t="s">
-        <v>225</v>
+        <v>47</v>
       </c>
       <c r="E106" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F106" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>238</v>
+        <v>184</v>
       </c>
       <c r="B107" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="E107" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F107" t="s">
-        <v>22</v>
-      </c>
-      <c r="G107" t="s">
-        <v>25</v>
-      </c>
-      <c r="H107" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>185</v>
+        <v>238</v>
       </c>
       <c r="B108" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E108" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F108" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="G108" t="s">
+        <v>25</v>
+      </c>
+      <c r="H108" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B109" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="E109" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F109" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>186</v>
+      </c>
+      <c r="B110" t="s">
+        <v>187</v>
+      </c>
+      <c r="E110" t="s">
+        <v>14</v>
+      </c>
+      <c r="F110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>235</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>47</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E111" t="s">
         <v>45</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F111" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LIBPhys changes: Freitas out, Silva in
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D228AF-F5E1-0742-B8C1-9BBBCD9498A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DCE871-3D81-D74F-8764-8215C98CAF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,9 +331,6 @@
     <t xml:space="preserve">Department of Chemistry and Biochemistry, University of Texas at Arlington </t>
   </si>
   <si>
-    <t xml:space="preserve">Freitas                      </t>
-  </si>
-  <si>
     <t>Freixa</t>
   </si>
   <si>
@@ -652,9 +649,6 @@
     <t xml:space="preserve">A.L.       </t>
   </si>
   <si>
-    <t xml:space="preserve">E.D.C.     </t>
-  </si>
-  <si>
     <t xml:space="preserve">C.A.O.     </t>
   </si>
   <si>
@@ -761,6 +755,12 @@
   </si>
   <si>
     <t>Tonnel\'e</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>P.A.O.C.</t>
   </si>
 </sst>
 </file>
@@ -1603,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1668,7 +1668,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -1710,7 +1710,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -1724,7 +1724,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1766,7 +1766,7 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1780,7 +1780,7 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1794,7 +1794,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
@@ -1850,7 +1850,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
@@ -1884,7 +1884,7 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s">
         <v>58</v>
@@ -1898,7 +1898,7 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
@@ -1926,7 +1926,7 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -1940,7 +1940,7 @@
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E23" t="s">
         <v>30</v>
@@ -1968,7 +1968,7 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
@@ -1982,7 +1982,7 @@
         <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E26" t="s">
         <v>72</v>
@@ -2030,7 +2030,7 @@
         <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E29" t="s">
         <v>79</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
@@ -2086,7 +2086,7 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E33" t="s">
         <v>53</v>
@@ -2100,7 +2100,7 @@
         <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
@@ -2114,7 +2114,7 @@
         <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C35" t="s">
         <v>87</v>
@@ -2131,7 +2131,7 @@
         <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E36" t="s">
         <v>90</v>
@@ -2145,7 +2145,7 @@
         <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E37" t="s">
         <v>45</v>
@@ -2165,7 +2165,7 @@
         <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E38" t="s">
         <v>39</v>
@@ -2193,24 +2193,33 @@
         <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>100</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>70</v>
+        <v>22</v>
+      </c>
+      <c r="G40" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
       </c>
       <c r="E41" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F41" t="s">
         <v>22</v>
@@ -2224,13 +2233,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E42" t="s">
         <v>45</v>
@@ -2238,25 +2244,19 @@
       <c r="F42" t="s">
         <v>22</v>
       </c>
-      <c r="G42" t="s">
-        <v>92</v>
-      </c>
-      <c r="H42" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>234</v>
       </c>
       <c r="E43" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -2264,7 +2264,7 @@
         <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
@@ -2278,13 +2278,13 @@
         <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -2292,27 +2292,27 @@
         <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B47" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E47" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="F47" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2320,41 +2320,41 @@
         <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E48" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F48" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>125</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="F49" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>207</v>
       </c>
       <c r="E50" t="s">
-        <v>117</v>
+        <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2362,13 +2362,13 @@
         <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="F51" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2376,13 +2376,13 @@
         <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>208</v>
       </c>
       <c r="E52" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2390,41 +2390,41 @@
         <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E53" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F53" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>239</v>
       </c>
       <c r="B54" t="s">
-        <v>211</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F54" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>241</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="E55" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F55" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2432,10 +2432,10 @@
         <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
         <v>22</v>
@@ -2446,27 +2446,27 @@
         <v>124</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="E57" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>126</v>
+        <v>33</v>
       </c>
       <c r="E58" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2474,13 +2474,13 @@
         <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>33</v>
+        <v>211</v>
       </c>
       <c r="E59" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,13 +2488,13 @@
         <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>213</v>
+        <v>105</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="F60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2502,13 +2502,13 @@
         <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>212</v>
       </c>
       <c r="E61" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F61" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2516,10 +2516,10 @@
         <v>132</v>
       </c>
       <c r="B62" t="s">
-        <v>214</v>
+        <v>133</v>
       </c>
       <c r="E62" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F62" t="s">
         <v>70</v>
@@ -2527,30 +2527,30 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B63" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
       <c r="E63" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F63" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E64" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F64" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2558,13 +2558,13 @@
         <v>137</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E65" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2572,13 +2572,13 @@
         <v>138</v>
       </c>
       <c r="B66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E66" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F66" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2586,24 +2586,24 @@
         <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>218</v>
+        <v>140</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E68" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="F68" t="s">
         <v>59</v>
@@ -2611,30 +2611,36 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E69" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F69" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="E70" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F70" t="s">
         <v>22</v>
+      </c>
+      <c r="G70" t="s">
+        <v>92</v>
+      </c>
+      <c r="H70" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2642,19 +2648,13 @@
         <v>146</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E71" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F71" t="s">
-        <v>22</v>
-      </c>
-      <c r="G71" t="s">
-        <v>92</v>
-      </c>
-      <c r="H71" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2662,13 +2662,13 @@
         <v>147</v>
       </c>
       <c r="B72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E72" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="F72" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2676,27 +2676,27 @@
         <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="E73" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="F73" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="E74" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F74" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2704,13 +2704,13 @@
         <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>222</v>
+        <v>47</v>
       </c>
       <c r="E75" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F75" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2718,13 +2718,13 @@
         <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>47</v>
+        <v>221</v>
       </c>
       <c r="E76" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F76" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2732,13 +2732,13 @@
         <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>223</v>
+        <v>77</v>
       </c>
       <c r="E77" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2746,13 +2746,13 @@
         <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="E78" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F78" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2760,13 +2760,13 @@
         <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="E79" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2774,13 +2774,13 @@
         <v>156</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E80" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="F80" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2788,38 +2788,38 @@
         <v>157</v>
       </c>
       <c r="B81" t="s">
-        <v>225</v>
+        <v>158</v>
       </c>
       <c r="E81" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="F81" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>238</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="E82" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F82" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>240</v>
+        <v>159</v>
       </c>
       <c r="B83" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="E83" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F83" t="s">
         <v>22</v>
@@ -2830,13 +2830,13 @@
         <v>160</v>
       </c>
       <c r="B84" t="s">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="E84" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F84" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2844,13 +2844,13 @@
         <v>161</v>
       </c>
       <c r="B85" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="E85" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F85" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2858,13 +2858,13 @@
         <v>162</v>
       </c>
       <c r="B86" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="E86" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F86" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2872,13 +2872,13 @@
         <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E87" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="F87" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2886,13 +2886,19 @@
         <v>164</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
+        <v>158</v>
       </c>
       <c r="E88" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="F88" t="s">
-        <v>80</v>
+        <v>22</v>
+      </c>
+      <c r="G88" t="s">
+        <v>92</v>
+      </c>
+      <c r="H88" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2900,19 +2906,13 @@
         <v>165</v>
       </c>
       <c r="B89" t="s">
-        <v>159</v>
+        <v>9</v>
       </c>
       <c r="E89" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F89" t="s">
         <v>22</v>
-      </c>
-      <c r="G89" t="s">
-        <v>92</v>
-      </c>
-      <c r="H89" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2920,13 +2920,13 @@
         <v>166</v>
       </c>
       <c r="B90" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="E90" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="F90" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2934,13 +2934,16 @@
         <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="E91" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="F91" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="H91" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2948,16 +2951,13 @@
         <v>168</v>
       </c>
       <c r="B92" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E92" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F92" t="s">
-        <v>22</v>
-      </c>
-      <c r="H92" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2965,24 +2965,24 @@
         <v>169</v>
       </c>
       <c r="B93" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E93" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F93" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B94" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E94" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="F94" t="s">
         <v>70</v>
@@ -2990,52 +2990,52 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="B95" t="s">
-        <v>229</v>
+        <v>44</v>
       </c>
       <c r="E95" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F95" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>237</v>
+        <v>170</v>
       </c>
       <c r="B96" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="E96" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="F96" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>171</v>
+        <v>241</v>
       </c>
       <c r="B97" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="E97" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="F97" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B98" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E98" t="s">
         <v>45</v>
@@ -3046,10 +3046,10 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>172</v>
+      </c>
+      <c r="B99" t="s">
         <v>173</v>
-      </c>
-      <c r="B99" t="s">
-        <v>174</v>
       </c>
       <c r="E99" t="s">
         <v>45</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B100" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E100" t="s">
         <v>61</v>
@@ -3074,10 +3074,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B101" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E101" t="s">
         <v>61</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>176</v>
+      </c>
+      <c r="B102" t="s">
         <v>177</v>
-      </c>
-      <c r="B102" t="s">
-        <v>178</v>
       </c>
       <c r="E102" t="s">
         <v>90</v>
@@ -3102,10 +3102,10 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B103" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E103" t="s">
         <v>17</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
@@ -3130,10 +3130,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B105" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E105" t="s">
         <v>45</v>
@@ -3142,15 +3142,15 @@
         <v>22</v>
       </c>
       <c r="G105" t="s">
+        <v>180</v>
+      </c>
+      <c r="H105" t="s">
         <v>181</v>
-      </c>
-      <c r="H105" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B106" t="s">
         <v>47</v>
@@ -3164,10 +3164,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B107" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E107" t="s">
         <v>61</v>
@@ -3178,10 +3178,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B108" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E108" t="s">
         <v>45</v>
@@ -3198,10 +3198,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B109" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E109" t="s">
         <v>39</v>
@@ -3212,10 +3212,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>185</v>
+      </c>
+      <c r="B110" t="s">
         <v>186</v>
-      </c>
-      <c r="B110" t="s">
-        <v>187</v>
       </c>
       <c r="E110" t="s">
         <v>14</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B111" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
argonne updates: hafidi and meziani out
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DCE871-3D81-D74F-8764-8215C98CAF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28925CBD-90AA-3840-AC19-C141AA447C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="240">
   <si>
     <t>LastName</t>
   </si>
@@ -358,9 +358,6 @@
     <t xml:space="preserve">Guenette                    </t>
   </si>
   <si>
-    <t xml:space="preserve">Hafidi                      </t>
-  </si>
-  <si>
     <t xml:space="preserve">Hauptman                    </t>
   </si>
   <si>
@@ -448,9 +445,6 @@
     <t xml:space="preserve">Mart\'inez-Vara             </t>
   </si>
   <si>
-    <t xml:space="preserve">Meziani                     </t>
-  </si>
-  <si>
     <t>Miller</t>
   </si>
   <si>
@@ -680,9 +674,6 @@
   </si>
   <si>
     <t xml:space="preserve">M.        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z.E.      </t>
   </si>
   <si>
     <t xml:space="preserve">F.        </t>
@@ -1601,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1668,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -1710,7 +1701,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -1724,7 +1715,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1766,7 +1757,7 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1780,7 +1771,7 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1794,7 +1785,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
@@ -1850,7 +1841,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
@@ -1884,7 +1875,7 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E19" t="s">
         <v>58</v>
@@ -1898,7 +1889,7 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -1909,10 +1900,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
@@ -1926,7 +1917,7 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -1940,7 +1931,7 @@
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E23" t="s">
         <v>30</v>
@@ -1968,7 +1959,7 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
@@ -1982,7 +1973,7 @@
         <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E26" t="s">
         <v>72</v>
@@ -2030,7 +2021,7 @@
         <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E29" t="s">
         <v>79</v>
@@ -2055,7 +2046,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
@@ -2086,7 +2077,7 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E33" t="s">
         <v>53</v>
@@ -2100,7 +2091,7 @@
         <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
@@ -2114,7 +2105,7 @@
         <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C35" t="s">
         <v>87</v>
@@ -2131,7 +2122,7 @@
         <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E36" t="s">
         <v>90</v>
@@ -2145,7 +2136,7 @@
         <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E37" t="s">
         <v>45</v>
@@ -2165,7 +2156,7 @@
         <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E38" t="s">
         <v>39</v>
@@ -2250,7 +2241,7 @@
         <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E43" t="s">
         <v>14</v>
@@ -2264,7 +2255,7 @@
         <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
@@ -2278,27 +2269,27 @@
         <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="F46" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2306,41 +2297,41 @@
         <v>112</v>
       </c>
       <c r="B47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E47" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F47" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="F48" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>205</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2348,13 +2339,13 @@
         <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="F50" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2362,13 +2353,13 @@
         <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>206</v>
       </c>
       <c r="E51" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2376,41 +2367,41 @@
         <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F52" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>236</v>
       </c>
       <c r="B53" t="s">
-        <v>209</v>
+        <v>33</v>
       </c>
       <c r="E53" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F53" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>239</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F54" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2418,10 +2409,10 @@
         <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E55" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F55" t="s">
         <v>22</v>
@@ -2432,27 +2423,27 @@
         <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="E56" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="F56" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="E57" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2460,13 +2451,13 @@
         <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>209</v>
       </c>
       <c r="E58" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2474,13 +2465,13 @@
         <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="F59" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,13 +2479,13 @@
         <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="E60" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F60" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2502,10 +2493,10 @@
         <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>212</v>
+        <v>132</v>
       </c>
       <c r="E61" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F61" t="s">
         <v>70</v>
@@ -2513,30 +2504,30 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="E62" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F62" t="s">
-        <v>70</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F63" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2544,13 +2535,13 @@
         <v>136</v>
       </c>
       <c r="B64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E64" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2558,69 +2549,75 @@
         <v>137</v>
       </c>
       <c r="B65" t="s">
-        <v>215</v>
+        <v>138</v>
       </c>
       <c r="E65" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="F65" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66" t="s">
-        <v>216</v>
+        <v>140</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="F66" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E67" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="F67" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="E68" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F68" t="s">
-        <v>59</v>
+        <v>22</v>
+      </c>
+      <c r="G68" t="s">
+        <v>92</v>
+      </c>
+      <c r="H68" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="E69" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="F69" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2628,19 +2625,13 @@
         <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E70" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F70" t="s">
-        <v>22</v>
-      </c>
-      <c r="G70" t="s">
-        <v>92</v>
-      </c>
-      <c r="H70" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2648,41 +2639,41 @@
         <v>146</v>
       </c>
       <c r="B71" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="E71" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="F71" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B72" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E72" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F72" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="E73" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F73" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2690,13 +2681,13 @@
         <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E74" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F74" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2704,13 +2695,13 @@
         <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="E75" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F75" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2718,13 +2709,13 @@
         <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>221</v>
+        <v>142</v>
       </c>
       <c r="E76" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F76" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2732,13 +2723,13 @@
         <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>219</v>
       </c>
       <c r="E77" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F77" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2746,13 +2737,13 @@
         <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>220</v>
       </c>
       <c r="E78" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="F78" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2760,27 +2751,27 @@
         <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>156</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="F79" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>156</v>
+        <v>235</v>
       </c>
       <c r="B80" t="s">
-        <v>223</v>
+        <v>47</v>
       </c>
       <c r="E80" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="F80" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2788,27 +2779,27 @@
         <v>157</v>
       </c>
       <c r="B81" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E81" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F81" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>238</v>
+        <v>158</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E82" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2816,13 +2807,13 @@
         <v>159</v>
       </c>
       <c r="B83" t="s">
-        <v>144</v>
+        <v>213</v>
       </c>
       <c r="E83" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F83" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2830,13 +2821,13 @@
         <v>160</v>
       </c>
       <c r="B84" t="s">
-        <v>44</v>
+        <v>221</v>
       </c>
       <c r="E84" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F84" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2844,13 +2835,13 @@
         <v>161</v>
       </c>
       <c r="B85" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E85" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F85" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2858,13 +2849,19 @@
         <v>162</v>
       </c>
       <c r="B86" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
       <c r="E86" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="F86" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="G86" t="s">
+        <v>92</v>
+      </c>
+      <c r="H86" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2872,13 +2869,13 @@
         <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>213</v>
+        <v>9</v>
       </c>
       <c r="E87" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="F87" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2886,19 +2883,13 @@
         <v>164</v>
       </c>
       <c r="B88" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="E88" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F88" t="s">
-        <v>22</v>
-      </c>
-      <c r="G88" t="s">
-        <v>92</v>
-      </c>
-      <c r="H88" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2906,13 +2897,16 @@
         <v>165</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="E89" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F89" t="s">
         <v>22</v>
+      </c>
+      <c r="H89" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2920,13 +2914,13 @@
         <v>166</v>
       </c>
       <c r="B90" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="E90" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="F90" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2934,128 +2928,125 @@
         <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E91" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F91" t="s">
-        <v>22</v>
-      </c>
-      <c r="H91" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E92" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="F92" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="B93" t="s">
-        <v>226</v>
+        <v>44</v>
       </c>
       <c r="E93" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F93" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B94" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
       <c r="E94" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="F94" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B95" t="s">
-        <v>44</v>
+        <v>239</v>
       </c>
       <c r="E95" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F95" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B96" t="s">
-        <v>158</v>
+        <v>225</v>
       </c>
       <c r="E96" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="F96" t="s">
-        <v>117</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>241</v>
+        <v>170</v>
       </c>
       <c r="B97" t="s">
-        <v>242</v>
+        <v>171</v>
       </c>
       <c r="E97" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F97" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B98" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="E98" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F98" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="E99" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F99" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3063,178 +3054,150 @@
         <v>174</v>
       </c>
       <c r="B100" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="E100" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="F100" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>144</v>
+        <v>226</v>
       </c>
       <c r="E101" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="F101" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>176</v>
+        <v>237</v>
       </c>
       <c r="B102" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="E102" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F102" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>177</v>
+      </c>
+      <c r="B103" t="s">
+        <v>211</v>
+      </c>
+      <c r="E103" t="s">
+        <v>45</v>
+      </c>
+      <c r="F103" t="s">
+        <v>22</v>
+      </c>
+      <c r="G103" t="s">
         <v>178</v>
       </c>
-      <c r="B103" t="s">
-        <v>229</v>
-      </c>
-      <c r="E103" t="s">
-        <v>17</v>
-      </c>
-      <c r="F103" t="s">
-        <v>18</v>
+      <c r="H103" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E104" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F104" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B105" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E105" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F105" t="s">
-        <v>22</v>
-      </c>
-      <c r="G105" t="s">
-        <v>180</v>
-      </c>
-      <c r="H105" t="s">
-        <v>181</v>
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
       <c r="B106" t="s">
-        <v>47</v>
+        <v>234</v>
       </c>
       <c r="E106" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F106" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="G106" t="s">
+        <v>25</v>
+      </c>
+      <c r="H106" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B107" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E107" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="F107" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="B108" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
       <c r="E108" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F108" t="s">
-        <v>22</v>
-      </c>
-      <c r="G108" t="s">
-        <v>25</v>
-      </c>
-      <c r="H108" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>184</v>
+        <v>230</v>
       </c>
       <c r="B109" t="s">
-        <v>230</v>
+        <v>47</v>
       </c>
       <c r="E109" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F109" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>185</v>
-      </c>
-      <c r="B110" t="s">
-        <v>186</v>
-      </c>
-      <c r="E110" t="s">
-        <v>14</v>
-      </c>
-      <c r="F110" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>233</v>
-      </c>
-      <c r="B111" t="s">
-        <v>47</v>
-      </c>
-      <c r="E111" t="s">
-        <v>45</v>
-      </c>
-      <c r="F111" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ific update: s. teruel-pardo in
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28925CBD-90AA-3840-AC19-C141AA447C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304D470-5677-8C4A-AA5B-F6278C4504D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="241">
   <si>
     <t>LastName</t>
   </si>
@@ -752,6 +752,9 @@
   </si>
   <si>
     <t>P.A.O.C.</t>
+  </si>
+  <si>
+    <t>Teruel-Pardo</t>
   </si>
 </sst>
 </file>
@@ -1592,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3065,38 +3068,38 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="B101" t="s">
-        <v>226</v>
+        <v>35</v>
       </c>
       <c r="E101" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F101" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>237</v>
+        <v>176</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="E102" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F102" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="B103" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="E103" t="s">
         <v>45</v>
@@ -3104,100 +3107,114 @@
       <c r="F103" t="s">
         <v>22</v>
       </c>
-      <c r="G103" t="s">
-        <v>178</v>
-      </c>
-      <c r="H103" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B104" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="E104" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F104" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="G104" t="s">
+        <v>178</v>
+      </c>
+      <c r="H104" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B105" t="s">
-        <v>220</v>
+        <v>47</v>
       </c>
       <c r="E105" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F105" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="B106" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="E106" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F106" t="s">
-        <v>22</v>
-      </c>
-      <c r="G106" t="s">
-        <v>25</v>
-      </c>
-      <c r="H106" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
       <c r="B107" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E107" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F107" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="G107" t="s">
+        <v>25</v>
+      </c>
+      <c r="H107" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B108" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="E108" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F108" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>183</v>
+      </c>
+      <c r="B109" t="s">
+        <v>184</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>230</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>47</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E110" t="s">
         <v>45</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F110" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UPV Valencia update: Garcia-Barrena in
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304D470-5677-8C4A-AA5B-F6278C4504D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E53FA2-CE40-B741-ADE2-EC041A4AB9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="242">
   <si>
     <t>LastName</t>
   </si>
@@ -755,6 +755,9 @@
   </si>
   <si>
     <t>Teruel-Pardo</t>
+  </si>
+  <si>
+    <t>Garc\'ia-Barrena</t>
   </si>
 </sst>
 </file>
@@ -1595,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2204,33 +2207,27 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>241</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="E41" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" t="s">
-        <v>92</v>
-      </c>
-      <c r="H41" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
+        <v>103</v>
       </c>
       <c r="E42" t="s">
         <v>45</v>
@@ -2238,27 +2235,33 @@
       <c r="F42" t="s">
         <v>22</v>
       </c>
+      <c r="G42" t="s">
+        <v>92</v>
+      </c>
+      <c r="H42" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>231</v>
+        <v>105</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
@@ -2269,153 +2272,153 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E45" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="F45" t="s">
-        <v>110</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E46" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="F47" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>204</v>
       </c>
       <c r="E48" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="F48" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>205</v>
+        <v>124</v>
       </c>
       <c r="E49" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="F49" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>205</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>113</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="F51" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E52" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>236</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>207</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>236</v>
       </c>
       <c r="B54" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="E55" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F55" t="s">
         <v>22</v>
@@ -2423,83 +2426,83 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
-        <v>209</v>
+        <v>33</v>
       </c>
       <c r="E58" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>209</v>
       </c>
       <c r="E59" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B60" t="s">
-        <v>210</v>
+        <v>105</v>
       </c>
       <c r="E60" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F60" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
+        <v>210</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="F61" t="s">
         <v>70</v>
@@ -2507,69 +2510,69 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>132</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F62" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E63" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="F63" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E64" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F64" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>213</v>
       </c>
       <c r="E65" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E66" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="F66" t="s">
         <v>59</v>
@@ -2577,215 +2580,215 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E67" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="F67" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>214</v>
+        <v>142</v>
       </c>
       <c r="E68" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F68" t="s">
         <v>22</v>
-      </c>
-      <c r="G68" t="s">
-        <v>92</v>
-      </c>
-      <c r="H68" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E69" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>70</v>
+        <v>22</v>
+      </c>
+      <c r="G69" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E70" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="F70" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="E71" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F71" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>217</v>
+        <v>147</v>
       </c>
       <c r="E72" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F72" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>217</v>
       </c>
       <c r="E73" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F73" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>218</v>
+        <v>47</v>
       </c>
       <c r="E74" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F74" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
       <c r="E75" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F75" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="E76" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F76" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>219</v>
+        <v>142</v>
       </c>
       <c r="E77" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F77" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B78" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E78" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>220</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="F79" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>235</v>
+        <v>155</v>
       </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="E80" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F80" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="B81" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="E81" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F81" t="s">
         <v>22</v>
@@ -2793,151 +2796,151 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B82" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E82" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="F82" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B83" t="s">
-        <v>213</v>
+        <v>44</v>
       </c>
       <c r="E83" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F83" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B84" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="E84" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="F84" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B85" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="E85" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F85" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B86" t="s">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="E86" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F86" t="s">
-        <v>22</v>
-      </c>
-      <c r="G86" t="s">
-        <v>92</v>
-      </c>
-      <c r="H86" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="E87" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F87" t="s">
         <v>22</v>
+      </c>
+      <c r="G87" t="s">
+        <v>92</v>
+      </c>
+      <c r="H87" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B88" t="s">
-        <v>208</v>
+        <v>9</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="F88" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B89" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="E89" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F89" t="s">
-        <v>22</v>
-      </c>
-      <c r="H89" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B90" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E90" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F90" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="H90" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E91" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F91" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2945,10 +2948,10 @@
         <v>167</v>
       </c>
       <c r="B92" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E92" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F92" t="s">
         <v>70</v>
@@ -2956,66 +2959,66 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>232</v>
+        <v>167</v>
       </c>
       <c r="B93" t="s">
-        <v>44</v>
+        <v>224</v>
       </c>
       <c r="E93" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F93" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>168</v>
+        <v>232</v>
       </c>
       <c r="B94" t="s">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="E94" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="F94" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
       <c r="B95" t="s">
-        <v>239</v>
+        <v>156</v>
       </c>
       <c r="E95" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="F95" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>169</v>
+        <v>238</v>
       </c>
       <c r="B96" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="E96" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F96" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B97" t="s">
-        <v>171</v>
+        <v>225</v>
       </c>
       <c r="E97" t="s">
         <v>45</v>
@@ -3026,24 +3029,24 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B98" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="E98" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F98" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
       <c r="E99" t="s">
         <v>61</v>
@@ -3054,66 +3057,66 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="E100" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="F100" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>240</v>
+        <v>174</v>
       </c>
       <c r="B101" t="s">
-        <v>35</v>
+        <v>175</v>
       </c>
       <c r="E101" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="F101" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="B102" t="s">
-        <v>226</v>
+        <v>35</v>
       </c>
       <c r="E102" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F102" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>237</v>
+        <v>176</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="E103" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F103" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="B104" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="E104" t="s">
         <v>45</v>
@@ -3121,100 +3124,114 @@
       <c r="F104" t="s">
         <v>22</v>
       </c>
-      <c r="G104" t="s">
-        <v>178</v>
-      </c>
-      <c r="H104" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="E105" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F105" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="G105" t="s">
+        <v>178</v>
+      </c>
+      <c r="H105" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B106" t="s">
-        <v>220</v>
+        <v>47</v>
       </c>
       <c r="E106" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F106" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="B107" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="E107" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F107" t="s">
-        <v>22</v>
-      </c>
-      <c r="G107" t="s">
-        <v>25</v>
-      </c>
-      <c r="H107" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
       <c r="B108" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E108" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F108" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="G108" t="s">
+        <v>25</v>
+      </c>
+      <c r="H108" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B109" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="E109" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F109" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>183</v>
+      </c>
+      <c r="B110" t="s">
+        <v>184</v>
+      </c>
+      <c r="E110" t="s">
+        <v>14</v>
+      </c>
+      <c r="F110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>230</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>47</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E111" t="s">
         <v>45</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F111" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DIPC update: from yubero to yubero-navarro
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E53FA2-CE40-B741-ADE2-EC041A4AB9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D086DD06-C525-8A44-9E22-06FB032677EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -724,9 +724,6 @@
     <t>Echevarria</t>
   </si>
   <si>
-    <t>Yubero</t>
-  </si>
-  <si>
     <t>J.W.R.</t>
   </si>
   <si>
@@ -758,6 +755,9 @@
   </si>
   <si>
     <t>Garc\'ia-Barrena</t>
+  </si>
+  <si>
+    <t>Yubero-Navarro</t>
   </si>
 </sst>
 </file>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B41" t="s">
         <v>142</v>
@@ -2261,7 +2261,7 @@
         <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B54" t="s">
         <v>33</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B81" t="s">
         <v>47</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B94" t="s">
         <v>44</v>
@@ -3001,10 +3001,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>237</v>
+      </c>
+      <c r="B96" t="s">
         <v>238</v>
-      </c>
-      <c r="B96" t="s">
-        <v>239</v>
       </c>
       <c r="E96" t="s">
         <v>90</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B102" t="s">
         <v>35</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
@@ -3175,10 +3175,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>232</v>
+      </c>
+      <c r="B108" t="s">
         <v>233</v>
-      </c>
-      <c r="B108" t="s">
-        <v>234</v>
       </c>
       <c r="E108" t="s">
         <v>45</v>
@@ -3223,7 +3223,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="B111" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Giessen/IFIC update: Ayet now signs as IFIC
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D086DD06-C525-8A44-9E22-06FB032677EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AC97624E-797F-654E-A788-DAB3177C0BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1752,10 +1752,10 @@
         <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update emails of ja hernando, p herrero, m sorel and j soto
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben.jones/Library/Mobile Documents/com~apple~CloudDocs/Work/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6380ACB-59BE-0F43-AD6B-C6B4A661230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0495E1-C4C8-004F-90C7-C6BCFC84C133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -901,12 +901,6 @@
     <t>henriques@gian.fis.uc.pt</t>
   </si>
   <si>
-    <t>jose.hernando@cern.ch</t>
-  </si>
-  <si>
-    <t>pablogfr94@gmail.com</t>
-  </si>
-  <si>
     <t>viherbos@eln.upv.es</t>
   </si>
   <si>
@@ -1054,12 +1048,6 @@
     <t>roberto.soleti@dipc.org</t>
   </si>
   <si>
-    <t>sorel@fnal.gov</t>
-  </si>
-  <si>
-    <t>j.soto@cern.ch</t>
-  </si>
-  <si>
     <t>jmrt@uc.pt</t>
   </si>
   <si>
@@ -1091,6 +1079,18 @@
   </si>
   <si>
     <t>alfonso.yubero@dipc.org</t>
+  </si>
+  <si>
+    <t>sorel@ific.uv.es</t>
+  </si>
+  <si>
+    <t>jose.hernando@usc.es</t>
+  </si>
+  <si>
+    <t>pablo.herrero-gomez@mail.huji.ac.il</t>
+  </si>
+  <si>
+    <t>josealfonso.soto@ific.uv.es</t>
   </si>
 </sst>
 </file>
@@ -1646,9 +1646,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1686,7 +1686,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1792,7 +1792,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1934,7 +1934,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1944,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2805,7 +2805,7 @@
         <v>204</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>289</v>
+        <v>350</v>
       </c>
       <c r="F48" t="s">
         <v>79</v>
@@ -2822,7 +2822,7 @@
         <v>124</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>290</v>
+        <v>351</v>
       </c>
       <c r="F49" t="s">
         <v>115</v>
@@ -2839,7 +2839,7 @@
         <v>205</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F50" t="s">
         <v>17</v>
@@ -2856,7 +2856,7 @@
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F51" t="s">
         <v>79</v>
@@ -2873,7 +2873,7 @@
         <v>206</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F52" t="s">
         <v>27</v>
@@ -2890,7 +2890,7 @@
         <v>207</v>
       </c>
       <c r="E53" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F53" t="s">
         <v>58</v>
@@ -2907,7 +2907,7 @@
         <v>33</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F54" t="s">
         <v>61</v>
@@ -2924,7 +2924,7 @@
         <v>68</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F55" t="s">
         <v>45</v>
@@ -2941,7 +2941,7 @@
         <v>47</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F56" t="s">
         <v>21</v>
@@ -2958,7 +2958,7 @@
         <v>124</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F57" t="s">
         <v>125</v>
@@ -2975,7 +2975,7 @@
         <v>33</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F58" t="s">
         <v>45</v>
@@ -2992,7 +2992,7 @@
         <v>209</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F59" t="s">
         <v>61</v>
@@ -3009,7 +3009,7 @@
         <v>105</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F60" t="s">
         <v>98</v>
@@ -3026,7 +3026,7 @@
         <v>210</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F61" t="s">
         <v>90</v>
@@ -3043,7 +3043,7 @@
         <v>132</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F62" t="s">
         <v>53</v>
@@ -3060,7 +3060,7 @@
         <v>211</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F63" t="s">
         <v>61</v>
@@ -3077,7 +3077,7 @@
         <v>212</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F64" t="s">
         <v>27</v>
@@ -3094,7 +3094,7 @@
         <v>213</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F65" t="s">
         <v>45</v>
@@ -3111,7 +3111,7 @@
         <v>138</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F66" t="s">
         <v>98</v>
@@ -3128,7 +3128,7 @@
         <v>140</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F67" t="s">
         <v>58</v>
@@ -3145,7 +3145,7 @@
         <v>142</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F68" t="s">
         <v>21</v>
@@ -3162,7 +3162,7 @@
         <v>214</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F69" t="s">
         <v>45</v>
@@ -3185,7 +3185,7 @@
         <v>215</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F70" t="s">
         <v>90</v>
@@ -3202,7 +3202,7 @@
         <v>216</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -3219,7 +3219,7 @@
         <v>147</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F72" t="s">
         <v>58</v>
@@ -3236,7 +3236,7 @@
         <v>217</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F73" t="s">
         <v>61</v>
@@ -3253,7 +3253,7 @@
         <v>47</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F74" t="s">
         <v>48</v>
@@ -3270,7 +3270,7 @@
         <v>218</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F75" t="s">
         <v>58</v>
@@ -3287,7 +3287,7 @@
         <v>77</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F76" t="s">
         <v>45</v>
@@ -3304,7 +3304,7 @@
         <v>142</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F77" t="s">
         <v>48</v>
@@ -3321,7 +3321,7 @@
         <v>219</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F78" t="s">
         <v>14</v>
@@ -3338,7 +3338,7 @@
         <v>220</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F79" t="s">
         <v>125</v>
@@ -3355,7 +3355,7 @@
         <v>156</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F80" t="s">
         <v>58</v>
@@ -3372,7 +3372,7 @@
         <v>47</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F81" t="s">
         <v>25</v>
@@ -3389,7 +3389,7 @@
         <v>142</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F82" t="s">
         <v>45</v>
@@ -3406,7 +3406,7 @@
         <v>44</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F83" t="s">
         <v>79</v>
@@ -3423,7 +3423,7 @@
         <v>213</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F84" t="s">
         <v>61</v>
@@ -3440,7 +3440,7 @@
         <v>221</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F85" t="s">
         <v>27</v>
@@ -3457,7 +3457,7 @@
         <v>211</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F86" t="s">
         <v>79</v>
@@ -3474,7 +3474,7 @@
         <v>156</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F87" t="s">
         <v>45</v>
@@ -3497,7 +3497,7 @@
         <v>9</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F88" t="s">
         <v>56</v>
@@ -3514,7 +3514,7 @@
         <v>208</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -3531,7 +3531,7 @@
         <v>219</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F90" t="s">
         <v>45</v>
@@ -3551,7 +3551,7 @@
         <v>222</v>
       </c>
       <c r="E91" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F91" t="s">
         <v>61</v>
@@ -3568,7 +3568,7 @@
         <v>223</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F92" t="s">
         <v>53</v>
@@ -3585,7 +3585,7 @@
         <v>224</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F93" t="s">
         <v>90</v>
@@ -3602,7 +3602,7 @@
         <v>44</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F94" t="s">
         <v>45</v>
@@ -3619,7 +3619,7 @@
         <v>156</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F95" t="s">
         <v>115</v>
@@ -3636,7 +3636,7 @@
         <v>238</v>
       </c>
       <c r="E96" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F96" t="s">
         <v>90</v>
@@ -3653,7 +3653,7 @@
         <v>225</v>
       </c>
       <c r="E97" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F97" t="s">
         <v>45</v>
@@ -3670,7 +3670,7 @@
         <v>171</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F98" t="s">
         <v>45</v>
@@ -3687,7 +3687,7 @@
         <v>213</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="F99" t="s">
         <v>61</v>
@@ -3704,7 +3704,7 @@
         <v>142</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="F100" t="s">
         <v>61</v>
@@ -3721,7 +3721,7 @@
         <v>175</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F101" t="s">
         <v>90</v>
@@ -3738,7 +3738,7 @@
         <v>35</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F102" t="s">
         <v>61</v>
@@ -3755,7 +3755,7 @@
         <v>226</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F103" t="s">
         <v>17</v>
@@ -3772,7 +3772,7 @@
         <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F104" t="s">
         <v>45</v>
@@ -3789,7 +3789,7 @@
         <v>211</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F105" t="s">
         <v>45</v>
@@ -3812,7 +3812,7 @@
         <v>47</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F106" t="s">
         <v>14</v>
@@ -3829,7 +3829,7 @@
         <v>220</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F107" t="s">
         <v>61</v>
@@ -3846,7 +3846,7 @@
         <v>233</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F108" t="s">
         <v>45</v>
@@ -3869,7 +3869,7 @@
         <v>227</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F109" t="s">
         <v>39</v>
@@ -3886,7 +3886,7 @@
         <v>184</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F110" t="s">
         <v>14</v>
@@ -3903,7 +3903,7 @@
         <v>47</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F111" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
add San Nacienciano, UPV/EHU
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0495E1-C4C8-004F-90C7-C6BCFC84C133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48921D0F-D29E-DA41-88AB-612CC69ABE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7800" yWindow="680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="356">
   <si>
     <t>LastName</t>
   </si>
@@ -1091,6 +1091,15 @@
   </si>
   <si>
     <t>josealfonso.soto@ific.uv.es</t>
+  </si>
+  <si>
+    <t>San Nacienciano</t>
+  </si>
+  <si>
+    <t>V.</t>
+  </si>
+  <si>
+    <t>virginia.sannacianceno@ehu.eus</t>
   </si>
 </sst>
 </file>
@@ -1942,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3562,19 +3571,19 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>167</v>
+        <v>353</v>
       </c>
       <c r="B92" t="s">
-        <v>223</v>
+        <v>354</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>331</v>
+        <v>355</v>
       </c>
       <c r="F92" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="G92" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -3582,13 +3591,13 @@
         <v>167</v>
       </c>
       <c r="B93" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F93" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="G93" t="s">
         <v>70</v>
@@ -3596,81 +3605,81 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>231</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>44</v>
+        <v>224</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F94" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="G94" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>168</v>
+        <v>231</v>
       </c>
       <c r="B95" t="s">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F95" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="G95" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>237</v>
+        <v>168</v>
       </c>
       <c r="B96" t="s">
-        <v>238</v>
-      </c>
-      <c r="E96" t="s">
-        <v>335</v>
+        <v>156</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="F96" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="G96" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="B97" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="E97" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F97" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="G97" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B98" t="s">
-        <v>171</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>337</v>
+        <v>225</v>
+      </c>
+      <c r="E98" t="s">
+        <v>336</v>
       </c>
       <c r="F98" t="s">
         <v>45</v>
@@ -3681,30 +3690,30 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B99" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="F99" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="G99" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B100" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F100" t="s">
         <v>61</v>
@@ -3715,81 +3724,81 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="F101" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="G101" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>239</v>
+        <v>174</v>
       </c>
       <c r="B102" t="s">
-        <v>35</v>
+        <v>175</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F102" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="G102" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>176</v>
+        <v>239</v>
       </c>
       <c r="B103" t="s">
-        <v>226</v>
+        <v>35</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F103" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="G103" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>236</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F104" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G104" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="B105" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F105" t="s">
         <v>45</v>
@@ -3797,118 +3806,135 @@
       <c r="G105" t="s">
         <v>22</v>
       </c>
-      <c r="H105" t="s">
-        <v>178</v>
-      </c>
-      <c r="I105" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B106" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F106" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G106" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="H106" t="s">
+        <v>178</v>
+      </c>
+      <c r="I106" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B107" t="s">
-        <v>220</v>
+        <v>47</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F107" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="G107" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>232</v>
+        <v>181</v>
       </c>
       <c r="B108" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F108" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="G108" t="s">
-        <v>22</v>
-      </c>
-      <c r="H108" t="s">
-        <v>25</v>
-      </c>
-      <c r="I108" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>182</v>
+        <v>232</v>
       </c>
       <c r="B109" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F109" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G109" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="H109" t="s">
+        <v>25</v>
+      </c>
+      <c r="I109" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B110" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F110" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="G110" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>183</v>
+      </c>
+      <c r="B111" t="s">
+        <v>184</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>241</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>47</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F112" t="s">
         <v>45</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G112" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3971,24 +3997,24 @@
     <hyperlink ref="E88" r:id="rId55" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
     <hyperlink ref="E89" r:id="rId56" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
     <hyperlink ref="E90" r:id="rId57" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E107" r:id="rId58" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
-    <hyperlink ref="E92" r:id="rId59" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E94" r:id="rId60" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E98" r:id="rId61" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E100" r:id="rId62" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E101" r:id="rId63" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E102" r:id="rId64" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E103" r:id="rId65" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E104" r:id="rId66" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E105" r:id="rId67" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E106" r:id="rId68" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E109" r:id="rId69" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E110" r:id="rId70" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E111" r:id="rId71" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E108" r:id="rId58" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
+    <hyperlink ref="E93" r:id="rId59" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E95" r:id="rId60" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E99" r:id="rId61" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E101" r:id="rId62" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E102" r:id="rId63" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E103" r:id="rId64" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E104" r:id="rId65" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E105" r:id="rId66" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E106" r:id="rId67" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E107" r:id="rId68" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E110" r:id="rId69" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E111" r:id="rId70" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E112" r:id="rId71" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
     <hyperlink ref="E60" r:id="rId72" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
     <hyperlink ref="E70" r:id="rId73" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E93" r:id="rId74" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E99" r:id="rId75" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E94" r:id="rId74" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E100" r:id="rId75" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
     <hyperlink ref="E6" r:id="rId76" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
     <hyperlink ref="E13" r:id="rId77" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
     <hyperlink ref="E62" r:id="rId78" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
@@ -4002,12 +4028,13 @@
     <hyperlink ref="E9" r:id="rId86" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
     <hyperlink ref="E56" r:id="rId87" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
     <hyperlink ref="E68" r:id="rId88" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E95" r:id="rId89" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E108" r:id="rId90" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E96" r:id="rId89" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E109" r:id="rId90" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
     <hyperlink ref="E26" r:id="rId91" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
     <hyperlink ref="E83" r:id="rId92" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId93" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
     <hyperlink ref="E38" r:id="rId94" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
+    <hyperlink ref="E92" r:id="rId95" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update hebrew univ affiliation string
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben.jones/Library/Mobile Documents/com~apple~CloudDocs/Work/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48921D0F-D29E-DA41-88AB-612CC69ABE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F474CE-203C-4541-89D3-5359A401CFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6520" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -379,12 +379,6 @@
     <t>Herrero-G\'omez</t>
   </si>
   <si>
-    <t>Hebrew University</t>
-  </si>
-  <si>
-    <t>Edmond J. Safra Campus, Jerusalem 9190401 Israel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Herrero                     </t>
   </si>
   <si>
@@ -1100,6 +1094,12 @@
   </si>
   <si>
     <t>virginia.sannacianceno@ehu.eus</t>
+  </si>
+  <si>
+    <t>Racah Institute of Physics, The Hebrew University of Jerusalem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerusalem 9190401, Israel </t>
   </si>
 </sst>
 </file>
@@ -1655,9 +1655,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1695,7 +1695,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1801,7 +1801,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1943,7 +1943,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1953,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1973,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1996,7 +1996,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2013,7 +2013,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2027,10 +2027,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2047,7 +2047,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -2064,7 +2064,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -2078,10 +2078,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -2095,10 +2095,10 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
@@ -2115,7 +2115,7 @@
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
@@ -2132,7 +2132,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F10" t="s">
         <v>61</v>
@@ -2146,10 +2146,10 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -2163,10 +2163,10 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2180,10 +2180,10 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -2200,7 +2200,7 @@
         <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F14" t="s">
         <v>45</v>
@@ -2217,7 +2217,7 @@
         <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F15" t="s">
         <v>48</v>
@@ -2234,7 +2234,7 @@
         <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F16" t="s">
         <v>45</v>
@@ -2248,10 +2248,10 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F17" t="s">
         <v>53</v>
@@ -2268,7 +2268,7 @@
         <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F18" t="s">
         <v>45</v>
@@ -2288,10 +2288,10 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F19" t="s">
         <v>58</v>
@@ -2305,10 +2305,10 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F20" t="s">
         <v>61</v>
@@ -2319,13 +2319,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E21" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F21" t="s">
         <v>45</v>
@@ -2339,10 +2339,10 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E22" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F22" t="s">
         <v>64</v>
@@ -2356,10 +2356,10 @@
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F23" t="s">
         <v>30</v>
@@ -2376,7 +2376,7 @@
         <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F24" t="s">
         <v>48</v>
@@ -2390,10 +2390,10 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F25" t="s">
         <v>53</v>
@@ -2407,10 +2407,10 @@
         <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F26" t="s">
         <v>72</v>
@@ -2427,7 +2427,7 @@
         <v>75</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F27" t="s">
         <v>45</v>
@@ -2450,7 +2450,7 @@
         <v>77</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F28" t="s">
         <v>58</v>
@@ -2464,10 +2464,10 @@
         <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F29" t="s">
         <v>79</v>
@@ -2484,7 +2484,7 @@
         <v>82</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F30" t="s">
         <v>36</v>
@@ -2495,13 +2495,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F31" t="s">
         <v>45</v>
@@ -2518,7 +2518,7 @@
         <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F32" t="s">
         <v>45</v>
@@ -2532,10 +2532,10 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F33" t="s">
         <v>53</v>
@@ -2549,10 +2549,10 @@
         <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F34" t="s">
         <v>17</v>
@@ -2566,13 +2566,13 @@
         <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
         <v>87</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F35" t="s">
         <v>27</v>
@@ -2586,10 +2586,10 @@
         <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E36" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F36" t="s">
         <v>90</v>
@@ -2603,10 +2603,10 @@
         <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F37" t="s">
         <v>45</v>
@@ -2626,10 +2626,10 @@
         <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F38" t="s">
         <v>39</v>
@@ -2646,7 +2646,7 @@
         <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F39" t="s">
         <v>98</v>
@@ -2663,7 +2663,7 @@
         <v>100</v>
       </c>
       <c r="E40" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F40" t="s">
         <v>25</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E41" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F41" t="s">
         <v>17</v>
@@ -2706,7 +2706,7 @@
         <v>103</v>
       </c>
       <c r="E42" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F42" t="s">
         <v>45</v>
@@ -2729,7 +2729,7 @@
         <v>105</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F43" t="s">
         <v>45</v>
@@ -2743,10 +2743,10 @@
         <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F44" t="s">
         <v>14</v>
@@ -2760,10 +2760,10 @@
         <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -2777,10 +2777,10 @@
         <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F46" t="s">
         <v>109</v>
@@ -2794,10 +2794,10 @@
         <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F47" t="s">
         <v>90</v>
@@ -2811,10 +2811,10 @@
         <v>112</v>
       </c>
       <c r="B48" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F48" t="s">
         <v>79</v>
@@ -2828,27 +2828,27 @@
         <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F49" t="s">
-        <v>115</v>
+        <v>354</v>
       </c>
       <c r="G49" t="s">
-        <v>116</v>
+        <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F50" t="s">
         <v>17</v>
@@ -2859,13 +2859,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F51" t="s">
         <v>79</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F52" t="s">
         <v>27</v>
@@ -2893,13 +2893,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E53" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F53" t="s">
         <v>58</v>
@@ -2910,13 +2910,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B54" t="s">
         <v>33</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F54" t="s">
         <v>61</v>
@@ -2927,13 +2927,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
         <v>68</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F55" t="s">
         <v>45</v>
@@ -2944,13 +2944,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
         <v>47</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F56" t="s">
         <v>21</v>
@@ -2961,30 +2961,30 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F57" t="s">
         <v>123</v>
       </c>
-      <c r="B57" t="s">
+      <c r="G57" t="s">
         <v>124</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F57" t="s">
-        <v>125</v>
-      </c>
-      <c r="G57" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B58" t="s">
         <v>33</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F58" t="s">
         <v>45</v>
@@ -2995,13 +2995,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B59" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F59" t="s">
         <v>61</v>
@@ -3012,13 +3012,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
         <v>105</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F60" t="s">
         <v>98</v>
@@ -3029,13 +3029,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B61" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F61" t="s">
         <v>90</v>
@@ -3046,13 +3046,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F62" t="s">
         <v>53</v>
@@ -3063,30 +3063,30 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F63" t="s">
         <v>61</v>
       </c>
       <c r="G63" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F64" t="s">
         <v>27</v>
@@ -3097,13 +3097,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F65" t="s">
         <v>45</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F66" t="s">
         <v>98</v>
@@ -3131,13 +3131,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F67" t="s">
         <v>58</v>
@@ -3148,13 +3148,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F68" t="s">
         <v>21</v>
@@ -3165,13 +3165,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F69" t="s">
         <v>45</v>
@@ -3188,13 +3188,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F70" t="s">
         <v>90</v>
@@ -3205,13 +3205,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -3222,13 +3222,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F72" t="s">
         <v>58</v>
@@ -3239,13 +3239,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B73" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F73" t="s">
         <v>61</v>
@@ -3256,13 +3256,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B74" t="s">
         <v>47</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F74" t="s">
         <v>48</v>
@@ -3273,13 +3273,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F75" t="s">
         <v>58</v>
@@ -3290,13 +3290,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B76" t="s">
         <v>77</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F76" t="s">
         <v>45</v>
@@ -3307,13 +3307,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F77" t="s">
         <v>48</v>
@@ -3324,13 +3324,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F78" t="s">
         <v>14</v>
@@ -3341,30 +3341,30 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F79" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G79" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F80" t="s">
         <v>58</v>
@@ -3375,13 +3375,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B81" t="s">
         <v>47</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F81" t="s">
         <v>25</v>
@@ -3392,13 +3392,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B82" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F82" t="s">
         <v>45</v>
@@ -3409,13 +3409,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B83" t="s">
         <v>44</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F83" t="s">
         <v>79</v>
@@ -3426,13 +3426,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B84" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F84" t="s">
         <v>61</v>
@@ -3443,13 +3443,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B85" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F85" t="s">
         <v>27</v>
@@ -3460,13 +3460,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B86" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F86" t="s">
         <v>79</v>
@@ -3477,13 +3477,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B87" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F87" t="s">
         <v>45</v>
@@ -3500,13 +3500,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F88" t="s">
         <v>56</v>
@@ -3517,13 +3517,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B89" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -3534,13 +3534,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B90" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F90" t="s">
         <v>45</v>
@@ -3554,13 +3554,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E91" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F91" t="s">
         <v>61</v>
@@ -3571,13 +3571,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>351</v>
+      </c>
+      <c r="B92" t="s">
+        <v>352</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="B92" t="s">
-        <v>354</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="F92" t="s">
         <v>21</v>
@@ -3588,13 +3588,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B93" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F93" t="s">
         <v>53</v>
@@ -3605,13 +3605,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B94" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F94" t="s">
         <v>90</v>
@@ -3622,13 +3622,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B95" t="s">
         <v>44</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F95" t="s">
         <v>45</v>
@@ -3639,30 +3639,30 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B96" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F96" t="s">
-        <v>115</v>
+        <v>354</v>
       </c>
       <c r="G96" t="s">
-        <v>116</v>
+        <v>355</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B97" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E97" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F97" t="s">
         <v>90</v>
@@ -3673,13 +3673,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B98" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E98" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F98" t="s">
         <v>45</v>
@@ -3690,13 +3690,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B99" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F99" t="s">
         <v>45</v>
@@ -3707,13 +3707,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B100" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F100" t="s">
         <v>61</v>
@@ -3724,13 +3724,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B101" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F101" t="s">
         <v>61</v>
@@ -3741,13 +3741,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B102" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F102" t="s">
         <v>90</v>
@@ -3758,13 +3758,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B103" t="s">
         <v>35</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F103" t="s">
         <v>61</v>
@@ -3775,13 +3775,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B104" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F104" t="s">
         <v>17</v>
@@ -3792,13 +3792,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F105" t="s">
         <v>45</v>
@@ -3809,13 +3809,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F106" t="s">
         <v>45</v>
@@ -3824,21 +3824,21 @@
         <v>22</v>
       </c>
       <c r="H106" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I106" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B107" t="s">
         <v>47</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F107" t="s">
         <v>14</v>
@@ -3849,13 +3849,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B108" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F108" t="s">
         <v>61</v>
@@ -3866,13 +3866,13 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B109" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F109" t="s">
         <v>45</v>
@@ -3889,13 +3889,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B110" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F110" t="s">
         <v>39</v>
@@ -3906,13 +3906,13 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B111" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F111" t="s">
         <v>14</v>
@@ -3923,13 +3923,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B112" t="s">
         <v>47</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F112" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
add 2nd affiliation of dept of physics for university of the basque country to several DIPC members
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben.jones/Library/Mobile Documents/com~apple~CloudDocs/Work/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F474CE-203C-4541-89D3-5359A401CFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EADB88-C8C3-2644-AB36-807371970D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="358">
   <si>
     <t>LastName</t>
   </si>
@@ -1100,6 +1100,12 @@
   </si>
   <si>
     <t xml:space="preserve">Jerusalem 9190401, Israel </t>
+  </si>
+  <si>
+    <t>Department of Physics, University of the Basque Country UPV/EHU, PO Box 644</t>
+  </si>
+  <si>
+    <t>Bilbao, E-48080, Spain</t>
   </si>
 </sst>
 </file>
@@ -1655,9 +1661,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1695,7 +1701,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1801,7 +1807,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1943,7 +1949,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1953,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49:G49"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2208,6 +2214,12 @@
       <c r="G14" t="s">
         <v>22</v>
       </c>
+      <c r="H14" t="s">
+        <v>356</v>
+      </c>
+      <c r="I14" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -2526,6 +2538,12 @@
       <c r="G32" t="s">
         <v>22</v>
       </c>
+      <c r="H32" t="s">
+        <v>356</v>
+      </c>
+      <c r="I32" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -2823,7 +2841,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>114</v>
       </c>
@@ -2840,7 +2858,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -2857,7 +2875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>116</v>
       </c>
@@ -2874,7 +2892,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>117</v>
       </c>
@@ -2891,7 +2909,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>118</v>
       </c>
@@ -2908,7 +2926,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>233</v>
       </c>
@@ -2925,7 +2943,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -2941,8 +2959,14 @@
       <c r="G55" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>356</v>
+      </c>
+      <c r="I55" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>120</v>
       </c>
@@ -2959,7 +2983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -2976,7 +3000,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -2993,7 +3017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -3010,7 +3034,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -3027,7 +3051,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -3044,7 +3068,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>129</v>
       </c>
@@ -3061,7 +3085,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>131</v>
       </c>
@@ -3078,7 +3102,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -3636,6 +3660,12 @@
       <c r="G95" t="s">
         <v>22</v>
       </c>
+      <c r="H95" t="s">
+        <v>356</v>
+      </c>
+      <c r="I95" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -3936,6 +3966,12 @@
       </c>
       <c r="G112" t="s">
         <v>22</v>
+      </c>
+      <c r="H112" t="s">
+        <v>356</v>
+      </c>
+      <c r="I112" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dipc changes: add s. tonelli, change 2nd institution for del barrio, seeman, larizgoitia
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EADB88-C8C3-2644-AB36-807371970D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FC6146-2CA8-7C4A-915E-95E8D02608A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18960" yWindow="4620" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="362">
   <si>
     <t>LastName</t>
   </si>
@@ -1106,13 +1106,25 @@
   </si>
   <si>
     <t>Bilbao, E-48080, Spain</t>
+  </si>
+  <si>
+    <t>Torelli</t>
+  </si>
+  <si>
+    <t>samuele.torelli@dipc.org</t>
+  </si>
+  <si>
+    <t>Leoia, E-48940, Spain</t>
+  </si>
+  <si>
+    <t>Faculty of Science and Technology, University of the Basque Country (UPV/EHU), Sarriena Auzoa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1254,6 +1266,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1598,9 +1616,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1957,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="I112" sqref="I112"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2215,10 +2234,10 @@
         <v>22</v>
       </c>
       <c r="H14" t="s">
-        <v>356</v>
-      </c>
-      <c r="I14" t="s">
-        <v>357</v>
+        <v>361</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2960,10 +2979,10 @@
         <v>22</v>
       </c>
       <c r="H55" t="s">
-        <v>356</v>
-      </c>
-      <c r="I55" t="s">
-        <v>357</v>
+        <v>361</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -3661,10 +3680,10 @@
         <v>22</v>
       </c>
       <c r="H95" t="s">
-        <v>356</v>
-      </c>
-      <c r="I95" t="s">
-        <v>357</v>
+        <v>361</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -3839,13 +3858,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>175</v>
+        <v>358</v>
       </c>
       <c r="B106" t="s">
-        <v>209</v>
+        <v>35</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>340</v>
+        <v>359</v>
       </c>
       <c r="F106" t="s">
         <v>45</v>
@@ -3853,124 +3872,141 @@
       <c r="G106" t="s">
         <v>22</v>
       </c>
-      <c r="H106" t="s">
-        <v>176</v>
-      </c>
-      <c r="I106" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
-        <v>47</v>
+        <v>209</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F107" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G107" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="H107" t="s">
+        <v>176</v>
+      </c>
+      <c r="I107" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B108" t="s">
-        <v>218</v>
+        <v>47</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F108" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="G108" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>230</v>
+        <v>179</v>
       </c>
       <c r="B109" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F109" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="G109" t="s">
-        <v>22</v>
-      </c>
-      <c r="H109" t="s">
-        <v>25</v>
-      </c>
-      <c r="I109" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="B110" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F110" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G110" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="H110" t="s">
+        <v>25</v>
+      </c>
+      <c r="I110" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B111" t="s">
-        <v>182</v>
+        <v>225</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F111" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="G111" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>181</v>
+      </c>
+      <c r="B112" t="s">
+        <v>182</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F112" t="s">
+        <v>14</v>
+      </c>
+      <c r="G112" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>239</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>47</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="E113" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F113" t="s">
         <v>45</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G113" t="s">
         <v>22</v>
       </c>
-      <c r="H112" t="s">
+      <c r="H113" t="s">
         <v>356</v>
       </c>
-      <c r="I112" t="s">
+      <c r="I113" t="s">
         <v>357</v>
       </c>
     </row>
@@ -4033,7 +4069,7 @@
     <hyperlink ref="E88" r:id="rId55" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
     <hyperlink ref="E89" r:id="rId56" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
     <hyperlink ref="E90" r:id="rId57" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E108" r:id="rId58" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
+    <hyperlink ref="E109" r:id="rId58" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
     <hyperlink ref="E93" r:id="rId59" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
     <hyperlink ref="E95" r:id="rId60" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
     <hyperlink ref="E99" r:id="rId61" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
@@ -4042,11 +4078,11 @@
     <hyperlink ref="E103" r:id="rId64" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
     <hyperlink ref="E104" r:id="rId65" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
     <hyperlink ref="E105" r:id="rId66" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E106" r:id="rId67" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E107" r:id="rId68" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E110" r:id="rId69" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E111" r:id="rId70" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E112" r:id="rId71" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E107" r:id="rId67" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E108" r:id="rId68" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E111" r:id="rId69" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E112" r:id="rId70" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E113" r:id="rId71" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
     <hyperlink ref="E60" r:id="rId72" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
     <hyperlink ref="E70" r:id="rId73" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
     <hyperlink ref="E94" r:id="rId74" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
@@ -4065,12 +4101,13 @@
     <hyperlink ref="E56" r:id="rId87" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
     <hyperlink ref="E68" r:id="rId88" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
     <hyperlink ref="E96" r:id="rId89" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E109" r:id="rId90" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E110" r:id="rId90" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
     <hyperlink ref="E26" r:id="rId91" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
     <hyperlink ref="E83" r:id="rId92" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId93" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
     <hyperlink ref="E38" r:id="rId94" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
     <hyperlink ref="E92" r:id="rId95" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
+    <hyperlink ref="E106" r:id="rId96" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UPV/EHU now spelled in spanish, undo 2nd affiliation change for del barrio, seeman, larizgoitia
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FC6146-2CA8-7C4A-915E-95E8D02608A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F1F6E01A-03A3-5545-B6E1-FD2F405E4768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18960" yWindow="4620" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5080" yWindow="3680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="360">
   <si>
     <t>LastName</t>
   </si>
@@ -97,9 +97,6 @@
     <t>B.</t>
   </si>
   <si>
-    <t>Department of Organic Chemistry I, University of the Basque Country (UPV/EHU), Centro de Innovaci\'on en Qu\'imica Avanzada (ORFEO-CINQA)</t>
-  </si>
-  <si>
     <t>San Sebasti\'an / Donostia, E-20018, Spain</t>
   </si>
   <si>
@@ -1102,9 +1099,6 @@
     <t xml:space="preserve">Jerusalem 9190401, Israel </t>
   </si>
   <si>
-    <t>Department of Physics, University of the Basque Country UPV/EHU, PO Box 644</t>
-  </si>
-  <si>
     <t>Bilbao, E-48080, Spain</t>
   </si>
   <si>
@@ -1114,17 +1108,17 @@
     <t>samuele.torelli@dipc.org</t>
   </si>
   <si>
-    <t>Leoia, E-48940, Spain</t>
-  </si>
-  <si>
-    <t>Faculty of Science and Technology, University of the Basque Country (UPV/EHU), Sarriena Auzoa</t>
+    <t>Department of Organic Chemistry I, Universidad del Pais Vasco (UPV/EHU), Centro de Innovaci\'on en Qu\'imica Avanzada (ORFEO-CINQA)</t>
+  </si>
+  <si>
+    <t>Department of Physics, Universidad del Pais Vasco (UPV/EHU), PO Box 644</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1266,12 +1260,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1616,10 +1604,9 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1978,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1998,7 +1985,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -2021,7 +2008,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2038,7 +2025,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2052,10 +2039,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2072,126 +2059,126 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F5" t="s">
+        <v>358</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>188</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F9" t="s">
+        <v>358</v>
+      </c>
+      <c r="G9" t="s">
         <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
         <v>61</v>
-      </c>
-      <c r="G10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>189</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2202,13 +2189,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -2219,377 +2206,377 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
+        <v>252</v>
+      </c>
+      <c r="F14" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
-      </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>361</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
+      </c>
+      <c r="I14" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>48</v>
-      </c>
-      <c r="G15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
-        <v>192</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>53</v>
-      </c>
-      <c r="G17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
         <v>55</v>
       </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" t="s">
-        <v>56</v>
-      </c>
       <c r="I18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F19" t="s">
         <v>57</v>
       </c>
-      <c r="B19" t="s">
-        <v>185</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>58</v>
-      </c>
-      <c r="G19" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>192</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F20" t="s">
         <v>60</v>
       </c>
-      <c r="B20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>61</v>
-      </c>
-      <c r="G20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" t="s">
+        <v>260</v>
+      </c>
+      <c r="F22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
-        <v>193</v>
-      </c>
-      <c r="E22" t="s">
-        <v>261</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>64</v>
-      </c>
-      <c r="G22" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
         <v>30</v>
-      </c>
-      <c r="G23" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
       <c r="E24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
         <v>48</v>
-      </c>
-      <c r="G24" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>183</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
         <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>184</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F25" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>194</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F26" t="s">
         <v>71</v>
       </c>
-      <c r="B26" t="s">
-        <v>195</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>72</v>
-      </c>
-      <c r="G26" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="B27" t="s">
-        <v>75</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
         <v>76</v>
       </c>
-      <c r="B28" t="s">
-        <v>77</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" t="s">
         <v>58</v>
-      </c>
-      <c r="G28" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F29" t="s">
         <v>78</v>
       </c>
-      <c r="B29" t="s">
-        <v>183</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>79</v>
-      </c>
-      <c r="G29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
-        <v>82</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" t="s">
         <v>36</v>
-      </c>
-      <c r="G30" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>270</v>
+      </c>
+      <c r="F32" t="s">
         <v>44</v>
       </c>
-      <c r="E32" t="s">
-        <v>271</v>
-      </c>
-      <c r="F32" t="s">
-        <v>45</v>
-      </c>
       <c r="G32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H32" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I32" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F34" t="s">
         <v>17</v>
@@ -2600,130 +2587,130 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" t="s">
         <v>86</v>
       </c>
-      <c r="B35" t="s">
-        <v>197</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="E35" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" t="s">
         <v>87</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F35" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" t="s">
+        <v>274</v>
+      </c>
+      <c r="F36" t="s">
         <v>89</v>
       </c>
-      <c r="B36" t="s">
-        <v>198</v>
-      </c>
-      <c r="E36" t="s">
-        <v>275</v>
-      </c>
-      <c r="F36" t="s">
-        <v>90</v>
-      </c>
       <c r="G36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>198</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" t="s">
         <v>91</v>
       </c>
-      <c r="B37" t="s">
-        <v>199</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F37" t="s">
-        <v>45</v>
-      </c>
-      <c r="G37" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>92</v>
-      </c>
-      <c r="I37" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
+        <v>199</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" t="s">
         <v>94</v>
-      </c>
-      <c r="B38" t="s">
-        <v>200</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F38" t="s">
-        <v>39</v>
-      </c>
-      <c r="G38" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" t="s">
         <v>96</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E39" t="s">
+        <v>277</v>
+      </c>
+      <c r="F39" t="s">
         <v>97</v>
       </c>
-      <c r="E39" t="s">
-        <v>278</v>
-      </c>
-      <c r="F39" t="s">
-        <v>98</v>
-      </c>
       <c r="G39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
         <v>99</v>
       </c>
-      <c r="B40" t="s">
-        <v>100</v>
-      </c>
       <c r="E40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H40" t="s">
+        <v>91</v>
+      </c>
+      <c r="I40" t="s">
         <v>92</v>
-      </c>
-      <c r="I40" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F41" t="s">
         <v>17</v>
@@ -2734,56 +2721,56 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>102</v>
       </c>
-      <c r="C42" t="s">
-        <v>103</v>
-      </c>
       <c r="E42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H42" t="s">
+        <v>91</v>
+      </c>
+      <c r="I42" t="s">
         <v>92</v>
-      </c>
-      <c r="I42" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
         <v>104</v>
       </c>
-      <c r="B43" t="s">
-        <v>105</v>
-      </c>
       <c r="E43" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F44" t="s">
         <v>14</v>
@@ -2794,13 +2781,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -2811,81 +2798,81 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F46" t="s">
         <v>108</v>
       </c>
-      <c r="B46" t="s">
-        <v>196</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>109</v>
-      </c>
-      <c r="G46" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" t="s">
+        <v>201</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F48" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" t="s">
         <v>112</v>
-      </c>
-      <c r="B48" t="s">
-        <v>202</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="F48" t="s">
-        <v>79</v>
-      </c>
-      <c r="G48" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F49" t="s">
+        <v>353</v>
+      </c>
+      <c r="G49" t="s">
         <v>354</v>
-      </c>
-      <c r="G49" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F50" t="s">
         <v>17</v>
@@ -2896,365 +2883,365 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E53" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F53" t="s">
+        <v>57</v>
+      </c>
+      <c r="G53" t="s">
         <v>58</v>
-      </c>
-      <c r="G53" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F54" t="s">
+        <v>60</v>
+      </c>
+      <c r="G54" t="s">
         <v>61</v>
-      </c>
-      <c r="G54" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H55" t="s">
-        <v>361</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
+      </c>
+      <c r="I55" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F56" t="s">
+        <v>358</v>
+      </c>
+      <c r="G56" t="s">
         <v>21</v>
-      </c>
-      <c r="G56" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" t="s">
         <v>121</v>
       </c>
-      <c r="B57" t="s">
+      <c r="E57" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F57" t="s">
         <v>122</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>123</v>
-      </c>
-      <c r="G57" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F59" t="s">
+        <v>60</v>
+      </c>
+      <c r="G59" t="s">
         <v>61</v>
-      </c>
-      <c r="G59" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" t="s">
         <v>129</v>
       </c>
-      <c r="B62" t="s">
-        <v>130</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" t="s">
+        <v>208</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F63" t="s">
+        <v>60</v>
+      </c>
+      <c r="G63" t="s">
         <v>131</v>
-      </c>
-      <c r="B63" t="s">
-        <v>209</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F63" t="s">
-        <v>61</v>
-      </c>
-      <c r="G63" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F64" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" t="s">
         <v>27</v>
-      </c>
-      <c r="G64" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
         <v>135</v>
       </c>
-      <c r="B66" t="s">
-        <v>136</v>
-      </c>
       <c r="E66" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
         <v>137</v>
       </c>
-      <c r="B67" t="s">
-        <v>138</v>
-      </c>
       <c r="E67" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G67" t="s">
         <v>58</v>
-      </c>
-      <c r="G67" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" t="s">
         <v>139</v>
       </c>
-      <c r="B68" t="s">
-        <v>140</v>
-      </c>
       <c r="E68" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F68" t="s">
+        <v>358</v>
+      </c>
+      <c r="G68" t="s">
         <v>21</v>
-      </c>
-      <c r="G68" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H69" t="s">
+        <v>91</v>
+      </c>
+      <c r="I69" t="s">
         <v>92</v>
-      </c>
-      <c r="I69" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F70" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B71" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -3265,115 +3252,115 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" t="s">
         <v>144</v>
       </c>
-      <c r="B72" t="s">
-        <v>145</v>
-      </c>
       <c r="E72" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F72" t="s">
+        <v>57</v>
+      </c>
+      <c r="G72" t="s">
         <v>58</v>
-      </c>
-      <c r="G72" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F73" t="s">
+        <v>60</v>
+      </c>
+      <c r="G73" t="s">
         <v>61</v>
-      </c>
-      <c r="G73" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B74" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F74" t="s">
         <v>47</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>48</v>
-      </c>
-      <c r="G74" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B75" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F75" t="s">
+        <v>57</v>
+      </c>
+      <c r="G75" t="s">
         <v>58</v>
-      </c>
-      <c r="G75" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F76" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B77" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F77" t="s">
+        <v>47</v>
+      </c>
+      <c r="G77" t="s">
         <v>48</v>
-      </c>
-      <c r="G77" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F78" t="s">
         <v>14</v>
@@ -3384,189 +3371,189 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B79" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F79" t="s">
+        <v>122</v>
+      </c>
+      <c r="G79" t="s">
         <v>123</v>
-      </c>
-      <c r="G79" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" t="s">
         <v>153</v>
       </c>
-      <c r="B80" t="s">
-        <v>154</v>
-      </c>
       <c r="E80" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F80" t="s">
+        <v>57</v>
+      </c>
+      <c r="G80" t="s">
         <v>58</v>
-      </c>
-      <c r="G80" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F81" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B82" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F84" t="s">
+        <v>60</v>
+      </c>
+      <c r="G84" t="s">
         <v>61</v>
-      </c>
-      <c r="G84" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B85" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F85" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85" t="s">
         <v>27</v>
-      </c>
-      <c r="G85" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F86" t="s">
+        <v>78</v>
+      </c>
+      <c r="G86" t="s">
         <v>79</v>
-      </c>
-      <c r="G86" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B87" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F87" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G87" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H87" t="s">
+        <v>91</v>
+      </c>
+      <c r="I87" t="s">
         <v>92</v>
-      </c>
-      <c r="I87" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F88" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G88" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -3577,260 +3564,260 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B90" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I90" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E91" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F91" t="s">
+        <v>60</v>
+      </c>
+      <c r="G91" t="s">
         <v>61</v>
-      </c>
-      <c r="G91" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>350</v>
+      </c>
+      <c r="B92" t="s">
         <v>351</v>
       </c>
-      <c r="B92" t="s">
+      <c r="E92" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="F92" t="s">
+        <v>358</v>
+      </c>
+      <c r="G92" t="s">
         <v>21</v>
-      </c>
-      <c r="G92" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B93" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F93" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B94" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B95" t="s">
+        <v>43</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F95" t="s">
         <v>44</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="F95" t="s">
-        <v>45</v>
-      </c>
       <c r="G95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H95" t="s">
-        <v>361</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
+      </c>
+      <c r="I95" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B96" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F96" t="s">
+        <v>353</v>
+      </c>
+      <c r="G96" t="s">
         <v>354</v>
-      </c>
-      <c r="G96" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>234</v>
+      </c>
+      <c r="B97" t="s">
         <v>235</v>
       </c>
-      <c r="B97" t="s">
-        <v>236</v>
-      </c>
       <c r="E97" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F97" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E98" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F98" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G98" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>167</v>
+      </c>
+      <c r="B99" t="s">
         <v>168</v>
       </c>
-      <c r="B99" t="s">
-        <v>169</v>
-      </c>
       <c r="E99" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F99" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G99" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F100" t="s">
+        <v>60</v>
+      </c>
+      <c r="G100" t="s">
         <v>61</v>
-      </c>
-      <c r="G100" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B101" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F101" t="s">
+        <v>60</v>
+      </c>
+      <c r="G101" t="s">
         <v>61</v>
-      </c>
-      <c r="G101" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>171</v>
+      </c>
+      <c r="B102" t="s">
         <v>172</v>
       </c>
-      <c r="B102" t="s">
-        <v>173</v>
-      </c>
       <c r="E102" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G102" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F103" t="s">
+        <v>60</v>
+      </c>
+      <c r="G103" t="s">
         <v>61</v>
-      </c>
-      <c r="G103" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B104" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F104" t="s">
         <v>17</v>
@@ -3841,70 +3828,70 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F105" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B106" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F106" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G106" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>174</v>
+      </c>
+      <c r="B107" t="s">
+        <v>208</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F107" t="s">
+        <v>44</v>
+      </c>
+      <c r="G107" t="s">
+        <v>21</v>
+      </c>
+      <c r="H107" t="s">
         <v>175</v>
       </c>
-      <c r="B107" t="s">
-        <v>209</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F107" t="s">
-        <v>45</v>
-      </c>
-      <c r="G107" t="s">
-        <v>22</v>
-      </c>
-      <c r="H107" t="s">
+      <c r="I107" t="s">
         <v>176</v>
-      </c>
-      <c r="I107" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B108" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F108" t="s">
         <v>14</v>
@@ -3915,70 +3902,70 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B109" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F109" t="s">
+        <v>60</v>
+      </c>
+      <c r="G109" t="s">
         <v>61</v>
-      </c>
-      <c r="G109" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>229</v>
+      </c>
+      <c r="B110" t="s">
         <v>230</v>
       </c>
-      <c r="B110" t="s">
-        <v>231</v>
-      </c>
       <c r="E110" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F110" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G110" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H110" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I110" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B111" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F111" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>180</v>
+      </c>
+      <c r="B112" t="s">
         <v>181</v>
       </c>
-      <c r="B112" t="s">
-        <v>182</v>
-      </c>
       <c r="E112" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F112" t="s">
         <v>14</v>
@@ -3989,25 +3976,25 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B113" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F113" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G113" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H113" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I113" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add ikerbasque as 2nd affiliation for soleti
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F1F6E01A-03A3-5545-B6E1-FD2F405E4768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E2F53A-F5F5-6E45-8064-FD6BA860379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="3680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="360">
   <si>
     <t>LastName</t>
   </si>
@@ -1965,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3739,6 +3739,12 @@
       </c>
       <c r="G99" t="s">
         <v>21</v>
+      </c>
+      <c r="H99" t="s">
+        <v>91</v>
+      </c>
+      <c r="I99" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
BGU: Redwine deleted; DIPC: Gonzalez deleted, Romeo changed; Giessen: Dickel deleted; IFIC: Romo-Luque changed; LIP: Conde changed; Manchester: Coupe added; Zaragoza: Cebrian deleted.
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E2F53A-F5F5-6E45-8064-FD6BA860379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D04E29-72B0-244F-B1D8-6AC68382AA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="3680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="351">
   <si>
     <t>LastName</t>
   </si>
@@ -139,12 +139,6 @@
     <t>S.</t>
   </si>
   <si>
-    <t>II. Physikalisches Institut, Justus-Liebig-Universitat Giessen</t>
-  </si>
-  <si>
-    <t>Giessen, Germany</t>
-  </si>
-  <si>
     <t xml:space="preserve">Azevedo                      </t>
   </si>
   <si>
@@ -220,15 +214,6 @@
     <t xml:space="preserve"> Paterna, E-46980, Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">Cebri\'an                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centro de Astropart\'iculas y F\'isica de Altas Energ\'ias (CAPA), Universidad de Zaragoza, Calle Pedro Cerbuna, 12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Zaragoza, E-50009, Spain</t>
-  </si>
-  <si>
     <t xml:space="preserve">Church                       </t>
   </si>
   <si>
@@ -274,12 +259,6 @@
     <t xml:space="preserve"> Santiago de Compostela, E-15782, Spain </t>
   </si>
   <si>
-    <t>Dickel</t>
-  </si>
-  <si>
-    <t>T.</t>
-  </si>
-  <si>
     <t>Elorza</t>
   </si>
   <si>
@@ -343,9 +322,6 @@
     <t xml:space="preserve">NEXT Spokesperson. </t>
   </si>
   <si>
-    <t xml:space="preserve">Gonz\'alez           </t>
-  </si>
-  <si>
     <t>R.</t>
   </si>
   <si>
@@ -505,9 +481,6 @@
     <t xml:space="preserve">Querol                      </t>
   </si>
   <si>
-    <t xml:space="preserve">Redwine                     </t>
-  </si>
-  <si>
     <t xml:space="preserve">Renner                      </t>
   </si>
   <si>
@@ -688,9 +661,6 @@
     <t xml:space="preserve">A.        </t>
   </si>
   <si>
-    <t xml:space="preserve">A.B.      </t>
-  </si>
-  <si>
     <t xml:space="preserve">C.        </t>
   </si>
   <si>
@@ -814,9 +784,6 @@
     <t>asier.castillo@dipc.org</t>
   </si>
   <si>
-    <t>scebrian@unizar.es</t>
-  </si>
-  <si>
     <t>eric.church@pnnl.gov</t>
   </si>
   <si>
@@ -838,9 +805,6 @@
     <t>gonzalodiazlopez10@gmail.com</t>
   </si>
   <si>
-    <t>t.dickel@gsi.de</t>
-  </si>
-  <si>
     <t>carlos.echeverria@dipc.org</t>
   </si>
   <si>
@@ -877,9 +841,6 @@
     <t>jjgomezcadenas@dipc.org</t>
   </si>
   <si>
-    <t>ruben.gonzalez.moreno@csic.es</t>
-  </si>
-  <si>
     <t>joshua.grocott@postgrad.manchester.ac.uk</t>
   </si>
   <si>
@@ -997,9 +958,6 @@
     <t>marcque@ific.uv.es</t>
   </si>
   <si>
-    <t>redwine@post.bgu.ac.il</t>
-  </si>
-  <si>
     <t>josh.e.renner@gmail.com</t>
   </si>
   <si>
@@ -1112,6 +1070,21 @@
   </si>
   <si>
     <t>Department of Physics, Universidad del Pais Vasco (UPV/EHU), PO Box 644</t>
+  </si>
+  <si>
+    <t>Now at Los Alamos National Laboratory, USA.</t>
+  </si>
+  <si>
+    <t>Deceased.</t>
+  </si>
+  <si>
+    <t>Now at University of North Carolina, USA.</t>
+  </si>
+  <si>
+    <t>Coupe</t>
+  </si>
+  <si>
+    <t>rhiannon.coupe@postgrad.manchester.ac.uk</t>
   </si>
 </sst>
 </file>
@@ -1963,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="K110" sqref="K110"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1985,7 +1958,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -2008,7 +1981,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2025,7 +1998,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2039,10 +2012,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2059,10 +2032,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F5" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2076,10 +2049,10 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
@@ -2090,10 +2063,10 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -2107,10 +2080,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="F8" t="s">
         <v>29</v>
@@ -2127,10 +2100,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="F9" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2144,41 +2117,41 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2189,13 +2162,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -2206,56 +2179,56 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F14" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>252</v>
-      </c>
-      <c r="F14" t="s">
-        <v>44</v>
       </c>
       <c r="G14" t="s">
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="I14" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="s">
+      <c r="G15" t="s">
         <v>46</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
@@ -2263,39 +2236,39 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>191</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
         <v>21</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I18" t="s">
         <v>21</v>
@@ -2303,50 +2276,50 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
         <v>56</v>
-      </c>
-      <c r="B19" t="s">
-        <v>184</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
         <v>59</v>
-      </c>
-      <c r="B20" t="s">
-        <v>192</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E21" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
         <v>21</v>
@@ -2354,636 +2327,639 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" t="s">
-        <v>260</v>
+        <v>184</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>261</v>
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>251</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="G23" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" t="s">
-        <v>262</v>
+        <v>174</v>
+      </c>
+      <c r="C24" t="s">
+        <v>347</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="G25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>69</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>21</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>349</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>265</v>
+        <v>350</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="F29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G29" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>216</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>226</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>269</v>
+        <v>41</v>
+      </c>
+      <c r="E31" t="s">
+        <v>258</v>
       </c>
       <c r="F31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
         <v>21</v>
       </c>
+      <c r="H31" t="s">
+        <v>345</v>
+      </c>
+      <c r="I31" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" t="s">
-        <v>270</v>
+        <v>186</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" t="s">
-        <v>359</v>
-      </c>
-      <c r="I32" t="s">
-        <v>355</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>271</v>
+        <v>187</v>
+      </c>
+      <c r="E33" t="s">
+        <v>260</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="G33" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E34" t="s">
-        <v>272</v>
+        <v>187</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="F34" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G34" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>273</v>
+        <v>188</v>
+      </c>
+      <c r="E35" t="s">
+        <v>262</v>
       </c>
       <c r="F35" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="G35" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E36" t="s">
-        <v>274</v>
+        <v>189</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="F36" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
+        <v>21</v>
+      </c>
+      <c r="H36" t="s">
+        <v>84</v>
+      </c>
+      <c r="I36" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" t="s">
-        <v>91</v>
-      </c>
-      <c r="I37" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>199</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>276</v>
+        <v>89</v>
+      </c>
+      <c r="E38" t="s">
+        <v>265</v>
       </c>
       <c r="F38" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="G38" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E39" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="F39" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="H39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>227</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="E40" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="F40" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" t="s">
-        <v>91</v>
-      </c>
-      <c r="I40" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>237</v>
+        <v>93</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>94</v>
+      </c>
+      <c r="C41" t="s">
+        <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="F41" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G41" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="H41" t="s">
+        <v>84</v>
+      </c>
+      <c r="I41" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" t="s">
-        <v>102</v>
-      </c>
-      <c r="E42" t="s">
-        <v>280</v>
+        <v>217</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="F42" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G42" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" t="s">
-        <v>91</v>
-      </c>
-      <c r="I42" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>187</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F43" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G43" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>227</v>
+        <v>186</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="F44" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>284</v>
+        <v>333</v>
       </c>
       <c r="F46" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="G46" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>113</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
       <c r="F47" t="s">
-        <v>89</v>
+        <v>339</v>
       </c>
       <c r="G47" t="s">
-        <v>69</v>
+        <v>340</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>347</v>
+        <v>273</v>
       </c>
       <c r="F48" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="G48" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>348</v>
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>274</v>
       </c>
       <c r="F49" t="s">
-        <v>353</v>
+        <v>73</v>
       </c>
       <c r="G49" t="s">
-        <v>354</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="F50" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G50" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>195</v>
       </c>
       <c r="E51" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="F51" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="B52" t="s">
-        <v>203</v>
+        <v>32</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="G52" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B53" t="s">
-        <v>204</v>
-      </c>
-      <c r="E53" t="s">
-        <v>289</v>
+        <v>62</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="F53" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G53" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="H53" t="s">
+        <v>345</v>
+      </c>
+      <c r="I53" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>232</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="F54" t="s">
-        <v>60</v>
+        <v>344</v>
       </c>
       <c r="G54" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="F55" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="G55" t="s">
-        <v>21</v>
-      </c>
-      <c r="H55" t="s">
-        <v>359</v>
-      </c>
-      <c r="I55" t="s">
-        <v>355</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="F56" t="s">
-        <v>358</v>
+        <v>42</v>
       </c>
       <c r="G56" t="s">
         <v>21</v>
@@ -2991,1016 +2967,971 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="F57" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="G57" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="F58" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="G58" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="F59" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="G59" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="F60" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="G60" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F61" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="G61" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>200</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F62" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="G62" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F63" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G63" t="s">
-        <v>131</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>209</v>
+        <v>127</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="F64" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="G64" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>210</v>
+        <v>129</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="F65" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G65" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="F66" t="s">
-        <v>97</v>
+        <v>344</v>
       </c>
       <c r="G66" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>202</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="F67" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G67" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="H67" t="s">
+        <v>84</v>
+      </c>
+      <c r="I67" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="F68" t="s">
-        <v>358</v>
+        <v>82</v>
       </c>
       <c r="G68" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="F69" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="G69" t="s">
-        <v>21</v>
-      </c>
-      <c r="H69" t="s">
-        <v>91</v>
-      </c>
-      <c r="I69" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B70" t="s">
-        <v>212</v>
+        <v>136</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F70" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="G70" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F71" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="G71" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F72" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="G72" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B73" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F73" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G73" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B74" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F74" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G74" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B75" t="s">
-        <v>215</v>
+        <v>131</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="F75" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="G75" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>207</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="F76" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G76" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B77" t="s">
-        <v>139</v>
+        <v>208</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="F77" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="G77" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="F78" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="G78" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>221</v>
       </c>
       <c r="B79" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="F79" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="G79" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="F80" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G80" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F81" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="G81" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B82" t="s">
-        <v>139</v>
+        <v>201</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="F82" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G82" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="F83" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G83" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B84" t="s">
-        <v>210</v>
+        <v>145</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="F84" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G84" t="s">
-        <v>61</v>
+        <v>21</v>
+      </c>
+      <c r="H84" t="s">
+        <v>84</v>
+      </c>
+      <c r="I84" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B85" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="F85" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="G85" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B86" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F86" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="G86" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B87" t="s">
-        <v>153</v>
+        <v>207</v>
+      </c>
+      <c r="C87" t="s">
+        <v>348</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F87" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G87" t="s">
         <v>21</v>
       </c>
-      <c r="H87" t="s">
-        <v>91</v>
-      </c>
       <c r="I87" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>324</v>
+        <v>209</v>
+      </c>
+      <c r="C88" t="s">
+        <v>346</v>
+      </c>
+      <c r="E88" t="s">
+        <v>313</v>
       </c>
       <c r="F88" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G88" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>161</v>
+        <v>336</v>
       </c>
       <c r="B89" t="s">
-        <v>205</v>
+        <v>337</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="F89" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="G89" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B90" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="F90" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G90" t="s">
-        <v>21</v>
-      </c>
-      <c r="I90" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B91" t="s">
-        <v>219</v>
-      </c>
-      <c r="E91" t="s">
-        <v>327</v>
+        <v>211</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="F91" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="G91" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>350</v>
+        <v>218</v>
       </c>
       <c r="B92" t="s">
-        <v>351</v>
+        <v>41</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>352</v>
+        <v>316</v>
       </c>
       <c r="F92" t="s">
-        <v>358</v>
+        <v>42</v>
       </c>
       <c r="G92" t="s">
         <v>21</v>
       </c>
+      <c r="H92" t="s">
+        <v>345</v>
+      </c>
+      <c r="I92" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B93" t="s">
-        <v>220</v>
+        <v>145</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F93" t="s">
-        <v>52</v>
+        <v>339</v>
       </c>
       <c r="G93" t="s">
-        <v>69</v>
+        <v>340</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>164</v>
+        <v>224</v>
       </c>
       <c r="B94" t="s">
-        <v>221</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="E94" t="s">
+        <v>318</v>
       </c>
       <c r="F94" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G94" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>228</v>
+        <v>157</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>330</v>
+        <v>212</v>
+      </c>
+      <c r="E95" t="s">
+        <v>319</v>
       </c>
       <c r="F95" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G95" t="s">
         <v>21</v>
       </c>
-      <c r="H95" t="s">
-        <v>359</v>
-      </c>
-      <c r="I95" t="s">
-        <v>355</v>
-      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B96" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="F96" t="s">
-        <v>353</v>
+        <v>42</v>
       </c>
       <c r="G96" t="s">
-        <v>354</v>
+        <v>21</v>
+      </c>
+      <c r="H96" t="s">
+        <v>84</v>
+      </c>
+      <c r="I96" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>234</v>
+        <v>160</v>
       </c>
       <c r="B97" t="s">
-        <v>235</v>
-      </c>
-      <c r="E97" t="s">
+        <v>201</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>332</v>
       </c>
       <c r="F97" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="G97" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B98" t="s">
-        <v>222</v>
-      </c>
-      <c r="E98" t="s">
-        <v>333</v>
+        <v>131</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="F98" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G98" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B99" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="F99" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="G99" t="s">
-        <v>21</v>
-      </c>
-      <c r="H99" t="s">
-        <v>91</v>
-      </c>
-      <c r="I99" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>169</v>
+        <v>226</v>
       </c>
       <c r="B100" t="s">
-        <v>210</v>
+        <v>34</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="F100" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G100" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B101" t="s">
-        <v>139</v>
+        <v>213</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="F101" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="G101" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="B102" t="s">
-        <v>172</v>
+        <v>9</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="F102" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="G102" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>236</v>
+        <v>342</v>
       </c>
       <c r="B103" t="s">
         <v>34</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="F103" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G103" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B104" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="F104" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G104" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="H104" t="s">
+        <v>166</v>
+      </c>
+      <c r="I104" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="F105" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G105" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>356</v>
+        <v>169</v>
       </c>
       <c r="B106" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>357</v>
+        <v>327</v>
       </c>
       <c r="F106" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G106" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="B107" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="F107" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G107" t="s">
         <v>21</v>
       </c>
       <c r="H107" t="s">
-        <v>175</v>
+        <v>24</v>
       </c>
       <c r="I107" t="s">
-        <v>176</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B108" t="s">
-        <v>46</v>
+        <v>214</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="F108" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G108" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B109" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="F109" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="G109" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B110" t="s">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="F110" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G110" t="s">
         <v>21</v>
       </c>
       <c r="H110" t="s">
-        <v>24</v>
+        <v>345</v>
       </c>
       <c r="I110" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>179</v>
-      </c>
-      <c r="B111" t="s">
-        <v>224</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F111" t="s">
-        <v>38</v>
-      </c>
-      <c r="G111" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>180</v>
-      </c>
-      <c r="B112" t="s">
-        <v>181</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="F112" t="s">
-        <v>14</v>
-      </c>
-      <c r="G112" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>238</v>
-      </c>
-      <c r="B113" t="s">
-        <v>46</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F113" t="s">
-        <v>44</v>
-      </c>
-      <c r="G113" t="s">
-        <v>21</v>
-      </c>
-      <c r="H113" t="s">
-        <v>359</v>
-      </c>
-      <c r="I113" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -4014,93 +3945,91 @@
     <hyperlink ref="E17" r:id="rId7" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
     <hyperlink ref="E18" r:id="rId8" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
     <hyperlink ref="E19" r:id="rId9" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
-    <hyperlink ref="E23" r:id="rId10" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
-    <hyperlink ref="E25" r:id="rId11" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
+    <hyperlink ref="E22" r:id="rId10" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
+    <hyperlink ref="E24" r:id="rId11" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
     <hyperlink ref="E28" r:id="rId12" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
     <hyperlink ref="E29" r:id="rId13" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
-    <hyperlink ref="E30" r:id="rId14" xr:uid="{D9FC349A-F140-484D-8EE4-45259D1328B0}"/>
-    <hyperlink ref="E31" r:id="rId15" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
-    <hyperlink ref="E33" r:id="rId16" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
-    <hyperlink ref="E35" r:id="rId17" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
-    <hyperlink ref="E37" r:id="rId18" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
-    <hyperlink ref="E44" r:id="rId19" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
-    <hyperlink ref="E45" r:id="rId20" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
-    <hyperlink ref="E46" r:id="rId21" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
-    <hyperlink ref="E47" r:id="rId22" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
-    <hyperlink ref="E48" r:id="rId23" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
-    <hyperlink ref="E49" r:id="rId24" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
-    <hyperlink ref="E50" r:id="rId25" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
-    <hyperlink ref="E52" r:id="rId26" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E54" r:id="rId27" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E55" r:id="rId28" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E57" r:id="rId29" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E61" r:id="rId30" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E66" r:id="rId31" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
-    <hyperlink ref="E63" r:id="rId32" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E67" r:id="rId33" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E69" r:id="rId34" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E71" r:id="rId35" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E72" r:id="rId36" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
-    <hyperlink ref="E3" r:id="rId37" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E64" r:id="rId38" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E73" r:id="rId39" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E74" r:id="rId40" xr:uid="{EA26648E-6DAB-DC40-9C69-6623C07441D4}"/>
-    <hyperlink ref="E75" r:id="rId41" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
-    <hyperlink ref="E27" r:id="rId42" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E76" r:id="rId43" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E77" r:id="rId44" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E78" r:id="rId45" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E79" r:id="rId46" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E80" r:id="rId47" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E81" r:id="rId48" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E82" r:id="rId49" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E84" r:id="rId50" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E85" r:id="rId51" xr:uid="{3E81E32D-856A-EB46-A9F2-4506E65AD8AB}"/>
-    <hyperlink ref="E20" r:id="rId52" xr:uid="{A2BAD517-F57E-E349-A5CF-829B0DD5671E}"/>
-    <hyperlink ref="E86" r:id="rId53" xr:uid="{52677827-962A-FC40-9163-7DD84D008F5D}"/>
-    <hyperlink ref="E87" r:id="rId54" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E88" r:id="rId55" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E89" r:id="rId56" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E90" r:id="rId57" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E109" r:id="rId58" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
-    <hyperlink ref="E93" r:id="rId59" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E95" r:id="rId60" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E99" r:id="rId61" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E101" r:id="rId62" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E102" r:id="rId63" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E103" r:id="rId64" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E104" r:id="rId65" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E105" r:id="rId66" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E107" r:id="rId67" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E108" r:id="rId68" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E111" r:id="rId69" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E112" r:id="rId70" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E113" r:id="rId71" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E60" r:id="rId72" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E70" r:id="rId73" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E94" r:id="rId74" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E100" r:id="rId75" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
-    <hyperlink ref="E6" r:id="rId76" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
-    <hyperlink ref="E13" r:id="rId77" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E62" r:id="rId78" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
-    <hyperlink ref="E8" r:id="rId79" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
-    <hyperlink ref="E12" r:id="rId80" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E43" r:id="rId81" xr:uid="{3856727F-6945-0447-AA02-540567CE0114}"/>
-    <hyperlink ref="E65" r:id="rId82" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E58" r:id="rId83" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E59" r:id="rId84" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
-    <hyperlink ref="E5" r:id="rId85" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
-    <hyperlink ref="E9" r:id="rId86" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E56" r:id="rId87" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E68" r:id="rId88" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E96" r:id="rId89" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E110" r:id="rId90" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E26" r:id="rId91" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E83" r:id="rId92" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
-    <hyperlink ref="E4" r:id="rId93" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E38" r:id="rId94" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
-    <hyperlink ref="E92" r:id="rId95" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
-    <hyperlink ref="E106" r:id="rId96" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E30" r:id="rId14" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
+    <hyperlink ref="E32" r:id="rId15" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
+    <hyperlink ref="E34" r:id="rId16" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
+    <hyperlink ref="E36" r:id="rId17" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
+    <hyperlink ref="E42" r:id="rId18" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
+    <hyperlink ref="E43" r:id="rId19" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
+    <hyperlink ref="E44" r:id="rId20" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
+    <hyperlink ref="E45" r:id="rId21" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
+    <hyperlink ref="E46" r:id="rId22" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
+    <hyperlink ref="E47" r:id="rId23" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
+    <hyperlink ref="E48" r:id="rId24" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
+    <hyperlink ref="E50" r:id="rId25" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
+    <hyperlink ref="E52" r:id="rId26" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E53" r:id="rId27" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E55" r:id="rId28" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E59" r:id="rId29" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E64" r:id="rId30" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E61" r:id="rId31" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
+    <hyperlink ref="E65" r:id="rId32" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E67" r:id="rId33" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E69" r:id="rId34" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E70" r:id="rId35" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E3" r:id="rId36" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
+    <hyperlink ref="E62" r:id="rId37" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E71" r:id="rId38" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E72" r:id="rId39" xr:uid="{EA26648E-6DAB-DC40-9C69-6623C07441D4}"/>
+    <hyperlink ref="E73" r:id="rId40" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E26" r:id="rId41" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
+    <hyperlink ref="E74" r:id="rId42" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E75" r:id="rId43" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E76" r:id="rId44" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E77" r:id="rId45" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E78" r:id="rId46" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E79" r:id="rId47" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E80" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E82" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E20" r:id="rId50" xr:uid="{A2BAD517-F57E-E349-A5CF-829B0DD5671E}"/>
+    <hyperlink ref="E83" r:id="rId51" xr:uid="{52677827-962A-FC40-9163-7DD84D008F5D}"/>
+    <hyperlink ref="E84" r:id="rId52" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E85" r:id="rId53" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E86" r:id="rId54" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E87" r:id="rId55" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E106" r:id="rId56" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
+    <hyperlink ref="E90" r:id="rId57" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E92" r:id="rId58" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E96" r:id="rId59" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E98" r:id="rId60" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E99" r:id="rId61" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E100" r:id="rId62" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E101" r:id="rId63" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E102" r:id="rId64" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E104" r:id="rId65" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E105" r:id="rId66" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E108" r:id="rId67" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E109" r:id="rId68" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E110" r:id="rId69" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E58" r:id="rId70" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E68" r:id="rId71" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E91" r:id="rId72" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E97" r:id="rId73" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E6" r:id="rId74" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
+    <hyperlink ref="E13" r:id="rId75" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
+    <hyperlink ref="E60" r:id="rId76" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E8" r:id="rId77" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
+    <hyperlink ref="E12" r:id="rId78" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
+    <hyperlink ref="E63" r:id="rId79" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E56" r:id="rId80" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E57" r:id="rId81" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E5" r:id="rId82" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
+    <hyperlink ref="E9" r:id="rId83" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
+    <hyperlink ref="E54" r:id="rId84" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E66" r:id="rId85" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E93" r:id="rId86" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E107" r:id="rId87" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E25" r:id="rId88" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
+    <hyperlink ref="E81" r:id="rId89" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E4" r:id="rId90" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
+    <hyperlink ref="E37" r:id="rId91" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
+    <hyperlink ref="E89" r:id="rId92" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
+    <hyperlink ref="E103" r:id="rId93" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E27" r:id="rId94" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
affiliation changed for Renner
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D04E29-72B0-244F-B1D8-6AC68382AA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EE37BB-F201-5A43-A4D2-00F049905189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -958,9 +958,6 @@
     <t>marcque@ific.uv.es</t>
   </si>
   <si>
-    <t>josh.e.renner@gmail.com</t>
-  </si>
-  <si>
     <t>ivan.rivilla@ehu.es</t>
   </si>
   <si>
@@ -1085,6 +1082,9 @@
   </si>
   <si>
     <t>rhiannon.coupe@postgrad.manchester.ac.uk</t>
+  </si>
+  <si>
+    <t>jrenner@ific.uv.es</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2035,7 +2035,7 @@
         <v>233</v>
       </c>
       <c r="F5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2103,7 +2103,7 @@
         <v>237</v>
       </c>
       <c r="F9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2194,10 +2194,10 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2367,7 +2367,7 @@
         <v>174</v>
       </c>
       <c r="C24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>252</v>
@@ -2421,13 +2421,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B27" t="s">
         <v>96</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2504,10 +2504,10 @@
         <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I31" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2780,7 +2780,7 @@
         <v>192</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F46" t="s">
         <v>73</v>
@@ -2797,13 +2797,13 @@
         <v>113</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F47" t="s">
+        <v>338</v>
+      </c>
+      <c r="G47" t="s">
         <v>339</v>
-      </c>
-      <c r="G47" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2908,10 +2908,10 @@
         <v>21</v>
       </c>
       <c r="H53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I53" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -2925,7 +2925,7 @@
         <v>279</v>
       </c>
       <c r="F54" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G54" t="s">
         <v>21</v>
@@ -3129,7 +3129,7 @@
         <v>291</v>
       </c>
       <c r="F66" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G66" t="s">
         <v>21</v>
@@ -3421,13 +3421,13 @@
         <v>199</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>308</v>
+        <v>350</v>
       </c>
       <c r="F83" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="G83" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -3438,7 +3438,7 @@
         <v>145</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F84" t="s">
         <v>42</v>
@@ -3461,7 +3461,7 @@
         <v>9</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F85" t="s">
         <v>53</v>
@@ -3478,7 +3478,7 @@
         <v>196</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F86" t="s">
         <v>10</v>
@@ -3495,10 +3495,10 @@
         <v>207</v>
       </c>
       <c r="C87" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F87" t="s">
         <v>42</v>
@@ -3518,10 +3518,10 @@
         <v>209</v>
       </c>
       <c r="C88" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E88" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F88" t="s">
         <v>58</v>
@@ -3532,16 +3532,16 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>335</v>
+      </c>
+      <c r="B89" t="s">
         <v>336</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="F89" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G89" t="s">
         <v>21</v>
@@ -3555,7 +3555,7 @@
         <v>210</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F90" t="s">
         <v>50</v>
@@ -3572,7 +3572,7 @@
         <v>211</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F91" t="s">
         <v>82</v>
@@ -3589,7 +3589,7 @@
         <v>41</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F92" t="s">
         <v>42</v>
@@ -3598,10 +3598,10 @@
         <v>21</v>
       </c>
       <c r="H92" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I92" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -3612,13 +3612,13 @@
         <v>145</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F93" t="s">
+        <v>338</v>
+      </c>
+      <c r="G93" t="s">
         <v>339</v>
-      </c>
-      <c r="G93" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -3629,7 +3629,7 @@
         <v>225</v>
       </c>
       <c r="E94" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F94" t="s">
         <v>82</v>
@@ -3646,7 +3646,7 @@
         <v>212</v>
       </c>
       <c r="E95" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F95" t="s">
         <v>42</v>
@@ -3663,7 +3663,7 @@
         <v>159</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F96" t="s">
         <v>42</v>
@@ -3686,7 +3686,7 @@
         <v>201</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F97" t="s">
         <v>58</v>
@@ -3703,7 +3703,7 @@
         <v>131</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F98" t="s">
         <v>58</v>
@@ -3720,7 +3720,7 @@
         <v>163</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F99" t="s">
         <v>82</v>
@@ -3737,7 +3737,7 @@
         <v>34</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F100" t="s">
         <v>58</v>
@@ -3754,7 +3754,7 @@
         <v>213</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F101" t="s">
         <v>17</v>
@@ -3771,7 +3771,7 @@
         <v>9</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F102" t="s">
         <v>42</v>
@@ -3782,13 +3782,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B103" t="s">
         <v>34</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F103" t="s">
         <v>42</v>
@@ -3805,7 +3805,7 @@
         <v>199</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3828,7 +3828,7 @@
         <v>44</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F105" t="s">
         <v>14</v>
@@ -3845,7 +3845,7 @@
         <v>208</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F106" t="s">
         <v>58</v>
@@ -3862,7 +3862,7 @@
         <v>220</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F107" t="s">
         <v>42</v>
@@ -3885,7 +3885,7 @@
         <v>214</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F108" t="s">
         <v>36</v>
@@ -3902,7 +3902,7 @@
         <v>172</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F109" t="s">
         <v>14</v>
@@ -3919,7 +3919,7 @@
         <v>44</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F110" t="s">
         <v>42</v>
@@ -3928,10 +3928,10 @@
         <v>21</v>
       </c>
       <c r="H110" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I110" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3986,50 +3986,50 @@
     <hyperlink ref="E80" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
     <hyperlink ref="E82" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
     <hyperlink ref="E20" r:id="rId50" xr:uid="{A2BAD517-F57E-E349-A5CF-829B0DD5671E}"/>
-    <hyperlink ref="E83" r:id="rId51" xr:uid="{52677827-962A-FC40-9163-7DD84D008F5D}"/>
-    <hyperlink ref="E84" r:id="rId52" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E85" r:id="rId53" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E86" r:id="rId54" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E87" r:id="rId55" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E106" r:id="rId56" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
-    <hyperlink ref="E90" r:id="rId57" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E92" r:id="rId58" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E96" r:id="rId59" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E98" r:id="rId60" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E99" r:id="rId61" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E100" r:id="rId62" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E101" r:id="rId63" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E102" r:id="rId64" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E104" r:id="rId65" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E105" r:id="rId66" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E108" r:id="rId67" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E109" r:id="rId68" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E110" r:id="rId69" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E58" r:id="rId70" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E68" r:id="rId71" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E91" r:id="rId72" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E97" r:id="rId73" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
-    <hyperlink ref="E6" r:id="rId74" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
-    <hyperlink ref="E13" r:id="rId75" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E60" r:id="rId76" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
-    <hyperlink ref="E8" r:id="rId77" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
-    <hyperlink ref="E12" r:id="rId78" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E63" r:id="rId79" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E56" r:id="rId80" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E57" r:id="rId81" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
-    <hyperlink ref="E5" r:id="rId82" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
-    <hyperlink ref="E9" r:id="rId83" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E54" r:id="rId84" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E66" r:id="rId85" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E93" r:id="rId86" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E107" r:id="rId87" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E25" r:id="rId88" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E81" r:id="rId89" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
-    <hyperlink ref="E4" r:id="rId90" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E37" r:id="rId91" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
-    <hyperlink ref="E89" r:id="rId92" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
-    <hyperlink ref="E103" r:id="rId93" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E27" r:id="rId94" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E84" r:id="rId51" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E85" r:id="rId52" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E86" r:id="rId53" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E87" r:id="rId54" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E106" r:id="rId55" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
+    <hyperlink ref="E90" r:id="rId56" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E92" r:id="rId57" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E96" r:id="rId58" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E98" r:id="rId59" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E99" r:id="rId60" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E100" r:id="rId61" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E101" r:id="rId62" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E102" r:id="rId63" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E104" r:id="rId64" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E105" r:id="rId65" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E108" r:id="rId66" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E109" r:id="rId67" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E110" r:id="rId68" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E58" r:id="rId69" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E68" r:id="rId70" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E91" r:id="rId71" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E97" r:id="rId72" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E6" r:id="rId73" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
+    <hyperlink ref="E13" r:id="rId74" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
+    <hyperlink ref="E60" r:id="rId75" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E8" r:id="rId76" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
+    <hyperlink ref="E12" r:id="rId77" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
+    <hyperlink ref="E63" r:id="rId78" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E56" r:id="rId79" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E57" r:id="rId80" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E5" r:id="rId81" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
+    <hyperlink ref="E9" r:id="rId82" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
+    <hyperlink ref="E54" r:id="rId83" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E66" r:id="rId84" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E93" r:id="rId85" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E107" r:id="rId86" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E25" r:id="rId87" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
+    <hyperlink ref="E81" r:id="rId88" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E4" r:id="rId89" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
+    <hyperlink ref="E37" r:id="rId90" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
+    <hyperlink ref="E89" r:id="rId91" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
+    <hyperlink ref="E103" r:id="rId92" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E27" r:id="rId93" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E83" r:id="rId94" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IFIC updates: Carcel and Uson out; Cortes-Parra, Saharia, Villamil in; Simon change of institution
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EE37BB-F201-5A43-A4D2-00F049905189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8B3EAE-446D-F047-91FC-5B68397D4EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="354">
   <si>
     <t>LastName</t>
   </si>
@@ -205,9 +205,6 @@
     <t xml:space="preserve"> Arlington, TX 76019, USA</t>
   </si>
   <si>
-    <t xml:space="preserve">C\'arcel                     </t>
-  </si>
-  <si>
     <t xml:space="preserve">Instituto de F\'isica Corpuscular (IFIC), CSIC \&amp; Universitat de Val\`encia, Calle Catedr\'atico Jos\'e Beltr\'an, 2 </t>
   </si>
   <si>
@@ -541,9 +538,6 @@
     <t>Trettin</t>
   </si>
   <si>
-    <t xml:space="preserve">Us\'on                      </t>
-  </si>
-  <si>
     <t xml:space="preserve">Veloso                      </t>
   </si>
   <si>
@@ -583,9 +577,6 @@
     <t xml:space="preserve">F.I.G.M.   </t>
   </si>
   <si>
-    <t xml:space="preserve">S.         </t>
-  </si>
-  <si>
     <t xml:space="preserve">E.         </t>
   </si>
   <si>
@@ -778,9 +769,6 @@
     <t>byrnes.nicholas@mavs.uta.edu</t>
   </si>
   <si>
-    <t>sara.carcel@ific.uv.es</t>
-  </si>
-  <si>
     <t>asier.castillo@dipc.org</t>
   </si>
   <si>
@@ -1012,9 +1000,6 @@
     <t>alexander.trettin@manchester.ac.uk</t>
   </si>
   <si>
-    <t>ausonandres@gmail.com</t>
-  </si>
-  <si>
     <t>pablo.garcia@dipc.org</t>
   </si>
   <si>
@@ -1085,6 +1070,30 @@
   </si>
   <si>
     <t>jrenner@ific.uv.es</t>
+  </si>
+  <si>
+    <t>Saharia</t>
+  </si>
+  <si>
+    <t>P.</t>
+  </si>
+  <si>
+    <t>Villamil</t>
+  </si>
+  <si>
+    <t>J.D.</t>
+  </si>
+  <si>
+    <t>Cortes-Parra</t>
+  </si>
+  <si>
+    <t>Pokhee.Saharia@ific.uv.es</t>
+  </si>
+  <si>
+    <t>Juan.Villamil@ific.uv.es</t>
+  </si>
+  <si>
+    <t>Camilo.Cortes@ific.uv.es</t>
   </si>
 </sst>
 </file>
@@ -1936,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1958,7 +1967,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1981,7 +1990,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1998,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2012,10 +2021,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2032,10 +2041,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2049,7 +2058,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -2063,10 +2072,10 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -2080,10 +2089,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F8" t="s">
         <v>29</v>
@@ -2100,10 +2109,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F9" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2117,13 +2126,13 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
         <v>58</v>
-      </c>
-      <c r="G10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2131,10 +2140,10 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -2148,10 +2157,10 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2165,10 +2174,10 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -2185,7 +2194,7 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F14" t="s">
         <v>42</v>
@@ -2194,10 +2203,10 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I14" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2208,7 +2217,7 @@
         <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F15" t="s">
         <v>45</v>
@@ -2225,7 +2234,7 @@
         <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F16" t="s">
         <v>42</v>
@@ -2239,10 +2248,10 @@
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F17" t="s">
         <v>50</v>
@@ -2259,7 +2268,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F18" t="s">
         <v>42</v>
@@ -2279,10 +2288,10 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
@@ -2293,36 +2302,36 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>248</v>
+        <v>209</v>
+      </c>
+      <c r="E20" t="s">
+        <v>245</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" t="s">
-        <v>249</v>
+        <v>181</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2330,81 +2339,81 @@
         <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>250</v>
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>247</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="G22" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" t="s">
-        <v>251</v>
+        <v>172</v>
+      </c>
+      <c r="C23" t="s">
+        <v>341</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" t="s">
-        <v>346</v>
+        <v>182</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>350</v>
       </c>
       <c r="B25" t="s">
-        <v>185</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>253</v>
+        <v>353</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="B26" t="s">
-        <v>69</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F26" t="s">
         <v>42</v>
@@ -2421,13 +2430,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2438,13 +2447,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F28" t="s">
         <v>55</v>
@@ -2455,30 +2464,30 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" t="s">
-        <v>173</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>73</v>
-      </c>
-      <c r="G29" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F30" t="s">
         <v>42</v>
@@ -2489,13 +2498,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
         <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F31" t="s">
         <v>42</v>
@@ -2504,38 +2513,38 @@
         <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I31" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E33" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F33" t="s">
         <v>17</v>
@@ -2546,50 +2555,50 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C34" t="s">
         <v>78</v>
       </c>
-      <c r="B34" t="s">
-        <v>187</v>
-      </c>
-      <c r="C34" t="s">
-        <v>79</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F34" t="s">
         <v>26</v>
       </c>
       <c r="G34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>185</v>
+      </c>
+      <c r="E35" t="s">
+        <v>258</v>
+      </c>
+      <c r="F35" t="s">
         <v>81</v>
       </c>
-      <c r="B35" t="s">
-        <v>188</v>
-      </c>
-      <c r="E35" t="s">
-        <v>262</v>
-      </c>
-      <c r="F35" t="s">
-        <v>82</v>
-      </c>
       <c r="G35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F36" t="s">
         <v>42</v>
@@ -2598,41 +2607,41 @@
         <v>21</v>
       </c>
       <c r="H36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" t="s">
         <v>84</v>
-      </c>
-      <c r="I36" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F37" t="s">
         <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
         <v>88</v>
       </c>
-      <c r="B38" t="s">
+      <c r="E38" t="s">
+        <v>261</v>
+      </c>
+      <c r="F38" t="s">
         <v>89</v>
-      </c>
-      <c r="E38" t="s">
-        <v>265</v>
-      </c>
-      <c r="F38" t="s">
-        <v>90</v>
       </c>
       <c r="G38" t="s">
         <v>56</v>
@@ -2640,13 +2649,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
         <v>91</v>
       </c>
-      <c r="B39" t="s">
-        <v>92</v>
-      </c>
       <c r="E39" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F39" t="s">
         <v>24</v>
@@ -2655,21 +2664,21 @@
         <v>21</v>
       </c>
       <c r="H39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" t="s">
         <v>84</v>
-      </c>
-      <c r="I39" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F40" t="s">
         <v>17</v>
@@ -2680,16 +2689,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
         <v>93</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>94</v>
       </c>
-      <c r="C41" t="s">
-        <v>95</v>
-      </c>
       <c r="E41" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F41" t="s">
         <v>42</v>
@@ -2698,21 +2707,21 @@
         <v>21</v>
       </c>
       <c r="H41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" t="s">
         <v>84</v>
-      </c>
-      <c r="I41" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -2723,13 +2732,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F43" t="s">
         <v>14</v>
@@ -2740,81 +2749,81 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
+        <v>183</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F44" t="s">
         <v>99</v>
       </c>
-      <c r="B44" t="s">
-        <v>186</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>100</v>
-      </c>
-      <c r="G44" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>189</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F46" t="s">
+        <v>72</v>
+      </c>
+      <c r="G46" t="s">
         <v>103</v>
-      </c>
-      <c r="B46" t="s">
-        <v>192</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F46" t="s">
-        <v>73</v>
-      </c>
-      <c r="G46" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F47" t="s">
         <v>333</v>
       </c>
-      <c r="F47" t="s">
-        <v>338</v>
-      </c>
       <c r="G47" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F48" t="s">
         <v>17</v>
@@ -2825,47 +2834,47 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F50" t="s">
         <v>26</v>
       </c>
       <c r="G50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E51" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
@@ -2876,30 +2885,30 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B52" t="s">
         <v>32</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F52" t="s">
+        <v>57</v>
+      </c>
+      <c r="G52" t="s">
         <v>58</v>
-      </c>
-      <c r="G52" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F53" t="s">
         <v>42</v>
@@ -2908,24 +2917,24 @@
         <v>21</v>
       </c>
       <c r="H53" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I53" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
         <v>44</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F54" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G54" t="s">
         <v>21</v>
@@ -2933,30 +2942,30 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" t="s">
         <v>112</v>
       </c>
-      <c r="B55" t="s">
+      <c r="E55" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F55" t="s">
         <v>113</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>114</v>
-      </c>
-      <c r="G55" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
         <v>32</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F56" t="s">
         <v>42</v>
@@ -2967,33 +2976,33 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F57" t="s">
+        <v>57</v>
+      </c>
+      <c r="G57" t="s">
         <v>58</v>
-      </c>
-      <c r="G57" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G58" t="s">
         <v>56</v>
@@ -3001,64 +3010,64 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" t="s">
         <v>120</v>
       </c>
-      <c r="B60" t="s">
-        <v>121</v>
-      </c>
       <c r="E60" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F60" t="s">
         <v>50</v>
       </c>
       <c r="G60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
+        <v>196</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F61" t="s">
+        <v>57</v>
+      </c>
+      <c r="G61" t="s">
         <v>122</v>
-      </c>
-      <c r="B61" t="s">
-        <v>199</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F61" t="s">
-        <v>58</v>
-      </c>
-      <c r="G61" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F62" t="s">
         <v>26</v>
@@ -3069,13 +3078,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F63" t="s">
         <v>42</v>
@@ -3086,16 +3095,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" t="s">
         <v>126</v>
       </c>
-      <c r="B64" t="s">
-        <v>127</v>
-      </c>
       <c r="E64" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G64" t="s">
         <v>56</v>
@@ -3103,13 +3112,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" t="s">
         <v>128</v>
       </c>
-      <c r="B65" t="s">
-        <v>129</v>
-      </c>
       <c r="E65" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -3120,16 +3129,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" t="s">
         <v>130</v>
       </c>
-      <c r="B66" t="s">
-        <v>131</v>
-      </c>
       <c r="E66" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F66" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G66" t="s">
         <v>21</v>
@@ -3137,13 +3146,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F67" t="s">
         <v>42</v>
@@ -3152,38 +3161,38 @@
         <v>21</v>
       </c>
       <c r="H67" t="s">
+        <v>83</v>
+      </c>
+      <c r="I67" t="s">
         <v>84</v>
-      </c>
-      <c r="I67" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F69" t="s">
         <v>17</v>
@@ -3194,13 +3203,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" t="s">
         <v>135</v>
       </c>
-      <c r="B70" t="s">
-        <v>136</v>
-      </c>
       <c r="E70" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F70" t="s">
         <v>55</v>
@@ -3211,30 +3220,30 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F71" t="s">
+        <v>57</v>
+      </c>
+      <c r="G71" t="s">
         <v>58</v>
-      </c>
-      <c r="G71" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
         <v>44</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F72" t="s">
         <v>45</v>
@@ -3245,13 +3254,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F73" t="s">
         <v>55</v>
@@ -3262,13 +3271,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F74" t="s">
         <v>42</v>
@@ -3279,13 +3288,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F75" t="s">
         <v>45</v>
@@ -3296,13 +3305,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B76" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F76" t="s">
         <v>14</v>
@@ -3313,30 +3322,30 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B77" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F77" t="s">
+        <v>113</v>
+      </c>
+      <c r="G77" t="s">
         <v>114</v>
-      </c>
-      <c r="G77" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" t="s">
         <v>144</v>
       </c>
-      <c r="B78" t="s">
-        <v>145</v>
-      </c>
       <c r="E78" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F78" t="s">
         <v>55</v>
@@ -3347,13 +3356,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B79" t="s">
         <v>44</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F79" t="s">
         <v>24</v>
@@ -3364,13 +3373,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F80" t="s">
         <v>42</v>
@@ -3381,64 +3390,64 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B81" t="s">
         <v>41</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F82" t="s">
+        <v>57</v>
+      </c>
+      <c r="G82" t="s">
         <v>58</v>
-      </c>
-      <c r="G82" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F83" t="s">
+        <v>57</v>
+      </c>
+      <c r="G83" t="s">
         <v>58</v>
-      </c>
-      <c r="G83" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F84" t="s">
         <v>42</v>
@@ -3447,21 +3456,21 @@
         <v>21</v>
       </c>
       <c r="H84" t="s">
+        <v>83</v>
+      </c>
+      <c r="I84" t="s">
         <v>84</v>
-      </c>
-      <c r="I84" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F85" t="s">
         <v>53</v>
@@ -3472,13 +3481,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B86" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F86" t="s">
         <v>10</v>
@@ -3489,16 +3498,16 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B87" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C87" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F87" t="s">
         <v>42</v>
@@ -3512,283 +3521,283 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B88" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C88" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E88" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F88" t="s">
+        <v>57</v>
+      </c>
+      <c r="G88" t="s">
         <v>58</v>
-      </c>
-      <c r="G88" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="B89" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="F89" t="s">
-        <v>343</v>
+        <v>57</v>
       </c>
       <c r="G89" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>155</v>
+        <v>330</v>
       </c>
       <c r="B90" t="s">
-        <v>210</v>
+        <v>331</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="F90" t="s">
-        <v>50</v>
+        <v>338</v>
       </c>
       <c r="G90" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B91" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F91" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="G91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>218</v>
+        <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F92" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="G92" t="s">
-        <v>21</v>
-      </c>
-      <c r="H92" t="s">
-        <v>344</v>
-      </c>
-      <c r="I92" t="s">
-        <v>340</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>156</v>
+        <v>215</v>
       </c>
       <c r="B93" t="s">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F93" t="s">
-        <v>338</v>
+        <v>42</v>
       </c>
       <c r="G93" t="s">
+        <v>21</v>
+      </c>
+      <c r="H93" t="s">
         <v>339</v>
+      </c>
+      <c r="I93" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>224</v>
+        <v>155</v>
       </c>
       <c r="B94" t="s">
-        <v>225</v>
-      </c>
-      <c r="E94" t="s">
-        <v>317</v>
+        <v>144</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="F94" t="s">
-        <v>82</v>
+        <v>333</v>
       </c>
       <c r="G94" t="s">
-        <v>64</v>
+        <v>334</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>221</v>
       </c>
       <c r="B95" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="E95" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F95" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="G95" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B96" t="s">
-        <v>159</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>319</v>
+        <v>209</v>
+      </c>
+      <c r="E96" t="s">
+        <v>314</v>
       </c>
       <c r="F96" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G96" t="s">
-        <v>21</v>
-      </c>
-      <c r="H96" t="s">
-        <v>84</v>
-      </c>
-      <c r="I96" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B97" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="F97" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G97" t="s">
-        <v>59</v>
+        <v>21</v>
+      </c>
+      <c r="H97" t="s">
+        <v>83</v>
+      </c>
+      <c r="I97" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>198</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="F98" t="s">
+        <v>57</v>
+      </c>
+      <c r="G98" t="s">
         <v>58</v>
-      </c>
-      <c r="G98" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B99" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="F99" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="G99" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>226</v>
+        <v>161</v>
       </c>
       <c r="B100" t="s">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F100" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="G100" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>164</v>
+        <v>223</v>
       </c>
       <c r="B101" t="s">
-        <v>213</v>
+        <v>34</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F101" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="G101" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F102" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G102" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>341</v>
+        <v>220</v>
       </c>
       <c r="B103" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="F103" t="s">
         <v>42</v>
@@ -3799,13 +3808,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>165</v>
+        <v>336</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>34</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3813,56 +3822,56 @@
       <c r="G104" t="s">
         <v>21</v>
       </c>
-      <c r="H104" t="s">
-        <v>166</v>
-      </c>
-      <c r="I104" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B105" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F105" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G105" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="H105" t="s">
+        <v>165</v>
+      </c>
+      <c r="I105" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B106" t="s">
-        <v>208</v>
+        <v>44</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="F106" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G106" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B107" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F107" t="s">
         <v>42</v>
@@ -3879,59 +3888,76 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F108" t="s">
         <v>36</v>
       </c>
       <c r="G108" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>171</v>
+        <v>348</v>
       </c>
       <c r="B109" t="s">
-        <v>172</v>
+        <v>349</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="F109" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="G109" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>228</v>
+        <v>169</v>
       </c>
       <c r="B110" t="s">
+        <v>170</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F110" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>225</v>
+      </c>
+      <c r="B111" t="s">
         <v>44</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F110" t="s">
+      <c r="E111" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F111" t="s">
         <v>42</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G111" t="s">
         <v>21</v>
       </c>
-      <c r="H110" t="s">
-        <v>344</v>
-      </c>
-      <c r="I110" t="s">
-        <v>340</v>
+      <c r="H111" t="s">
+        <v>339</v>
+      </c>
+      <c r="I111" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -3945,8 +3971,8 @@
     <hyperlink ref="E17" r:id="rId7" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
     <hyperlink ref="E18" r:id="rId8" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
     <hyperlink ref="E19" r:id="rId9" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
-    <hyperlink ref="E22" r:id="rId10" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
-    <hyperlink ref="E24" r:id="rId11" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
+    <hyperlink ref="E23" r:id="rId11" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
     <hyperlink ref="E28" r:id="rId12" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
     <hyperlink ref="E29" r:id="rId13" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
     <hyperlink ref="E30" r:id="rId14" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
@@ -3985,51 +4011,52 @@
     <hyperlink ref="E79" r:id="rId47" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
     <hyperlink ref="E80" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
     <hyperlink ref="E82" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E20" r:id="rId50" xr:uid="{A2BAD517-F57E-E349-A5CF-829B0DD5671E}"/>
-    <hyperlink ref="E84" r:id="rId51" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E85" r:id="rId52" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E86" r:id="rId53" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E87" r:id="rId54" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E106" r:id="rId55" xr:uid="{891BCBBD-1732-AC4C-ACE3-996487A72144}"/>
-    <hyperlink ref="E90" r:id="rId56" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E92" r:id="rId57" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E96" r:id="rId58" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E98" r:id="rId59" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E99" r:id="rId60" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E100" r:id="rId61" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E101" r:id="rId62" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E102" r:id="rId63" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E104" r:id="rId64" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E105" r:id="rId65" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E108" r:id="rId66" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E109" r:id="rId67" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E110" r:id="rId68" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E58" r:id="rId69" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E68" r:id="rId70" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E91" r:id="rId71" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E97" r:id="rId72" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
-    <hyperlink ref="E6" r:id="rId73" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
-    <hyperlink ref="E13" r:id="rId74" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E60" r:id="rId75" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
-    <hyperlink ref="E8" r:id="rId76" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
-    <hyperlink ref="E12" r:id="rId77" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E63" r:id="rId78" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E56" r:id="rId79" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E57" r:id="rId80" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
-    <hyperlink ref="E5" r:id="rId81" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
-    <hyperlink ref="E9" r:id="rId82" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E54" r:id="rId83" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E66" r:id="rId84" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E93" r:id="rId85" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E107" r:id="rId86" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E25" r:id="rId87" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E81" r:id="rId88" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
-    <hyperlink ref="E4" r:id="rId89" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E37" r:id="rId90" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
-    <hyperlink ref="E89" r:id="rId91" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
-    <hyperlink ref="E103" r:id="rId92" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E27" r:id="rId93" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E83" r:id="rId94" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E84" r:id="rId50" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E85" r:id="rId51" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E86" r:id="rId52" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E87" r:id="rId53" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E91" r:id="rId54" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E93" r:id="rId55" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E97" r:id="rId56" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E99" r:id="rId57" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E100" r:id="rId58" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E101" r:id="rId59" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E102" r:id="rId60" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E103" r:id="rId61" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E105" r:id="rId62" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E106" r:id="rId63" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E108" r:id="rId64" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E110" r:id="rId65" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E111" r:id="rId66" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E58" r:id="rId67" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E68" r:id="rId68" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E92" r:id="rId69" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E98" r:id="rId70" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E6" r:id="rId71" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
+    <hyperlink ref="E13" r:id="rId72" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
+    <hyperlink ref="E60" r:id="rId73" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E8" r:id="rId74" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
+    <hyperlink ref="E12" r:id="rId75" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
+    <hyperlink ref="E63" r:id="rId76" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E56" r:id="rId77" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E57" r:id="rId78" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E5" r:id="rId79" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
+    <hyperlink ref="E9" r:id="rId80" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
+    <hyperlink ref="E54" r:id="rId81" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E66" r:id="rId82" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E94" r:id="rId83" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E107" r:id="rId84" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E24" r:id="rId85" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
+    <hyperlink ref="E81" r:id="rId86" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E4" r:id="rId87" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
+    <hyperlink ref="E37" r:id="rId88" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
+    <hyperlink ref="E90" r:id="rId89" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
+    <hyperlink ref="E104" r:id="rId90" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E27" r:id="rId91" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E83" r:id="rId92" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E89" r:id="rId93" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E109" r:id="rId94" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E25" r:id="rId95" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UPV-Valencia updates: Martinez in
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8B3EAE-446D-F047-91FC-5B68397D4EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{568CA25D-331A-AC43-B159-960FA4F9EC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2860" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="356">
   <si>
     <t>LastName</t>
   </si>
@@ -1094,6 +1094,12 @@
   </si>
   <si>
     <t>Camilo.Cortes@ific.uv.es</t>
+  </si>
+  <si>
+    <t>Mart\'inez</t>
+  </si>
+  <si>
+    <t>alberto.martinez.perez@ific.uv.es</t>
   </si>
 </sst>
 </file>
@@ -1945,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3061,67 +3067,67 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>354</v>
       </c>
       <c r="B62" t="s">
-        <v>197</v>
+        <v>44</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>283</v>
+        <v>355</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G62" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F63" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G63" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>198</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F64" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="G64" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F65" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="G65" t="s">
         <v>56</v>
@@ -3129,260 +3135,260 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F66" t="s">
-        <v>338</v>
+        <v>55</v>
       </c>
       <c r="G66" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>130</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F67" t="s">
-        <v>42</v>
+        <v>338</v>
       </c>
       <c r="G67" t="s">
         <v>21</v>
       </c>
-      <c r="H67" t="s">
-        <v>83</v>
-      </c>
-      <c r="I67" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F68" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="G68" t="s">
-        <v>63</v>
+        <v>21</v>
+      </c>
+      <c r="H68" t="s">
+        <v>83</v>
+      </c>
+      <c r="I68" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F69" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="G69" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F70" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G70" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B71" t="s">
-        <v>202</v>
+        <v>135</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F71" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G71" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B72" t="s">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F72" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G72" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B73" t="s">
-        <v>203</v>
+        <v>44</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F73" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G73" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F74" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G74" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B75" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F75" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G75" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>204</v>
+        <v>130</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F76" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G76" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F77" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>114</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>205</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F78" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="G78" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>218</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F79" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="G79" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>218</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F80" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G80" t="s">
         <v>21</v>
@@ -3390,47 +3396,47 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F81" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="G81" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>198</v>
+        <v>41</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F82" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="G82" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>345</v>
+        <v>303</v>
       </c>
       <c r="F83" t="s">
         <v>57</v>
@@ -3441,113 +3447,113 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B84" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>304</v>
+        <v>345</v>
       </c>
       <c r="F84" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G84" t="s">
-        <v>21</v>
-      </c>
-      <c r="H84" t="s">
-        <v>83</v>
-      </c>
-      <c r="I84" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F85" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G85" t="s">
         <v>21</v>
       </c>
+      <c r="H85" t="s">
+        <v>83</v>
+      </c>
+      <c r="I85" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="G86" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B87" t="s">
-        <v>204</v>
-      </c>
-      <c r="C87" t="s">
-        <v>342</v>
+        <v>193</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F87" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G87" t="s">
-        <v>21</v>
-      </c>
-      <c r="I87" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B88" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C88" t="s">
-        <v>340</v>
-      </c>
-      <c r="E88" t="s">
-        <v>308</v>
+        <v>342</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="F88" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G88" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="I88" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>346</v>
+        <v>153</v>
       </c>
       <c r="B89" t="s">
-        <v>347</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>351</v>
+        <v>206</v>
+      </c>
+      <c r="C89" t="s">
+        <v>340</v>
+      </c>
+      <c r="E89" t="s">
+        <v>308</v>
       </c>
       <c r="F89" t="s">
         <v>57</v>
@@ -3558,36 +3564,36 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>330</v>
+        <v>346</v>
       </c>
       <c r="B90" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="F90" t="s">
-        <v>338</v>
+        <v>57</v>
       </c>
       <c r="G90" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>154</v>
+        <v>330</v>
       </c>
       <c r="B91" t="s">
-        <v>207</v>
+        <v>331</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="F91" t="s">
-        <v>50</v>
+        <v>338</v>
       </c>
       <c r="G91" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3595,13 +3601,13 @@
         <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F92" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="G92" t="s">
         <v>63</v>
@@ -3609,127 +3615,127 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>215</v>
+        <v>154</v>
       </c>
       <c r="B93" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F93" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="G93" t="s">
-        <v>21</v>
-      </c>
-      <c r="H93" t="s">
-        <v>339</v>
-      </c>
-      <c r="I93" t="s">
-        <v>335</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>215</v>
       </c>
       <c r="B94" t="s">
-        <v>144</v>
+        <v>41</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F94" t="s">
-        <v>333</v>
+        <v>42</v>
       </c>
       <c r="G94" t="s">
-        <v>334</v>
+        <v>21</v>
+      </c>
+      <c r="H94" t="s">
+        <v>339</v>
+      </c>
+      <c r="I94" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>221</v>
+        <v>155</v>
       </c>
       <c r="B95" t="s">
-        <v>222</v>
-      </c>
-      <c r="E95" t="s">
-        <v>313</v>
+        <v>144</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="F95" t="s">
-        <v>81</v>
+        <v>333</v>
       </c>
       <c r="G95" t="s">
-        <v>63</v>
+        <v>334</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>221</v>
       </c>
       <c r="B96" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="E96" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F96" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G96" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B97" t="s">
-        <v>158</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>315</v>
+        <v>209</v>
+      </c>
+      <c r="E97" t="s">
+        <v>314</v>
       </c>
       <c r="F97" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G97" t="s">
-        <v>21</v>
-      </c>
-      <c r="H97" t="s">
-        <v>83</v>
-      </c>
-      <c r="I97" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B98" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="F98" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G98" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="H98" t="s">
+        <v>83</v>
+      </c>
+      <c r="I98" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B99" t="s">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F99" t="s">
         <v>57</v>
@@ -3740,81 +3746,81 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B100" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="F100" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="G100" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>223</v>
+        <v>161</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F101" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G101" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>163</v>
+        <v>223</v>
       </c>
       <c r="B102" t="s">
-        <v>210</v>
+        <v>34</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F102" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="G102" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>220</v>
+        <v>163</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F103" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G103" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>336</v>
+        <v>220</v>
       </c>
       <c r="B104" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3825,13 +3831,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>164</v>
+        <v>336</v>
       </c>
       <c r="B105" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="F105" t="s">
         <v>42</v>
@@ -3839,124 +3845,141 @@
       <c r="G105" t="s">
         <v>21</v>
       </c>
-      <c r="H105" t="s">
-        <v>165</v>
-      </c>
-      <c r="I105" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B106" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F106" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G106" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="H106" t="s">
+        <v>165</v>
+      </c>
+      <c r="I106" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>216</v>
+        <v>167</v>
       </c>
       <c r="B107" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F107" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G107" t="s">
-        <v>21</v>
-      </c>
-      <c r="H107" t="s">
-        <v>24</v>
-      </c>
-      <c r="I107" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>216</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F108" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G108" t="s">
-        <v>86</v>
+        <v>21</v>
+      </c>
+      <c r="H108" t="s">
+        <v>24</v>
+      </c>
+      <c r="I108" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>348</v>
+        <v>168</v>
       </c>
       <c r="B109" t="s">
-        <v>349</v>
+        <v>211</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>352</v>
+        <v>323</v>
       </c>
       <c r="F109" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="G109" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>169</v>
+        <v>348</v>
       </c>
       <c r="B110" t="s">
-        <v>170</v>
+        <v>349</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="F110" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="G110" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>169</v>
+      </c>
+      <c r="B111" t="s">
+        <v>170</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>225</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>44</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F112" t="s">
         <v>42</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G112" t="s">
         <v>21</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H112" t="s">
         <v>339</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I112" t="s">
         <v>335</v>
       </c>
     </row>
@@ -3991,72 +4014,73 @@
     <hyperlink ref="E53" r:id="rId27" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
     <hyperlink ref="E55" r:id="rId28" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
     <hyperlink ref="E59" r:id="rId29" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E64" r:id="rId30" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E65" r:id="rId30" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
     <hyperlink ref="E61" r:id="rId31" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E65" r:id="rId32" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E67" r:id="rId33" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E69" r:id="rId34" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E70" r:id="rId35" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E66" r:id="rId32" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E68" r:id="rId33" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E70" r:id="rId34" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E71" r:id="rId35" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
     <hyperlink ref="E3" r:id="rId36" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E62" r:id="rId37" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E71" r:id="rId38" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E72" r:id="rId39" xr:uid="{EA26648E-6DAB-DC40-9C69-6623C07441D4}"/>
-    <hyperlink ref="E73" r:id="rId40" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E63" r:id="rId37" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E72" r:id="rId38" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E73" r:id="rId39" xr:uid="{EA26648E-6DAB-DC40-9C69-6623C07441D4}"/>
+    <hyperlink ref="E74" r:id="rId40" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
     <hyperlink ref="E26" r:id="rId41" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E74" r:id="rId42" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E75" r:id="rId43" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E76" r:id="rId44" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E77" r:id="rId45" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E78" r:id="rId46" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E79" r:id="rId47" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E80" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E82" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E84" r:id="rId50" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E85" r:id="rId51" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E86" r:id="rId52" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E87" r:id="rId53" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E91" r:id="rId54" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E93" r:id="rId55" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E97" r:id="rId56" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E99" r:id="rId57" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E100" r:id="rId58" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E101" r:id="rId59" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E102" r:id="rId60" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E103" r:id="rId61" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E105" r:id="rId62" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E106" r:id="rId63" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E108" r:id="rId64" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E110" r:id="rId65" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E111" r:id="rId66" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E75" r:id="rId42" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E76" r:id="rId43" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E77" r:id="rId44" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E78" r:id="rId45" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E79" r:id="rId46" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E80" r:id="rId47" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E81" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E83" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E85" r:id="rId50" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E86" r:id="rId51" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E87" r:id="rId52" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E88" r:id="rId53" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E92" r:id="rId54" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E94" r:id="rId55" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E98" r:id="rId56" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E100" r:id="rId57" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E101" r:id="rId58" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E102" r:id="rId59" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E103" r:id="rId60" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E104" r:id="rId61" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E106" r:id="rId62" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E107" r:id="rId63" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E109" r:id="rId64" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E111" r:id="rId65" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E112" r:id="rId66" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
     <hyperlink ref="E58" r:id="rId67" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E68" r:id="rId68" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E92" r:id="rId69" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E98" r:id="rId70" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E69" r:id="rId68" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E93" r:id="rId69" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E99" r:id="rId70" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
     <hyperlink ref="E6" r:id="rId71" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
     <hyperlink ref="E13" r:id="rId72" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
     <hyperlink ref="E60" r:id="rId73" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
     <hyperlink ref="E8" r:id="rId74" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
     <hyperlink ref="E12" r:id="rId75" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E63" r:id="rId76" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E64" r:id="rId76" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
     <hyperlink ref="E56" r:id="rId77" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
     <hyperlink ref="E57" r:id="rId78" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
     <hyperlink ref="E5" r:id="rId79" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
     <hyperlink ref="E9" r:id="rId80" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
     <hyperlink ref="E54" r:id="rId81" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E66" r:id="rId82" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E94" r:id="rId83" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E107" r:id="rId84" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E67" r:id="rId82" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E95" r:id="rId83" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E108" r:id="rId84" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
     <hyperlink ref="E24" r:id="rId85" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E81" r:id="rId86" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E82" r:id="rId86" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId87" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
     <hyperlink ref="E37" r:id="rId88" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
-    <hyperlink ref="E90" r:id="rId89" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
-    <hyperlink ref="E104" r:id="rId90" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E91" r:id="rId89" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
+    <hyperlink ref="E105" r:id="rId90" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
     <hyperlink ref="E27" r:id="rId91" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E83" r:id="rId92" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E89" r:id="rId93" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E109" r:id="rId94" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E84" r:id="rId92" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E90" r:id="rId93" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E110" r:id="rId94" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
     <hyperlink ref="E25" r:id="rId95" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
+    <hyperlink ref="E62" r:id="rId96" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
DIPC updstes: Almazan change of institution
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{568CA25D-331A-AC43-B159-960FA4F9EC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CFCBF265-3921-0F45-B23F-51A791FF167E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2860" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -718,9 +718,6 @@
     <t>corey.adams@anl.gov</t>
   </si>
   <si>
-    <t>helena.almazanmolina@manchester.ac.uk</t>
-  </si>
-  <si>
     <t>vicente.alvarez@ific.uv.es</t>
   </si>
   <si>
@@ -1100,6 +1097,9 @@
   </si>
   <si>
     <t>alberto.martinez.perez@ific.uv.es</t>
+  </si>
+  <si>
+    <t>helena.almazan@dipc.org</t>
   </si>
 </sst>
 </file>
@@ -1953,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2013,13 +2013,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>228</v>
+        <v>355</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2030,7 +2030,7 @@
         <v>174</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2047,10 +2047,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2064,7 +2064,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -2081,7 +2081,7 @@
         <v>175</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -2098,7 +2098,7 @@
         <v>176</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F8" t="s">
         <v>29</v>
@@ -2115,10 +2115,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2132,7 +2132,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F10" t="s">
         <v>57</v>
@@ -2149,7 +2149,7 @@
         <v>177</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -2166,7 +2166,7 @@
         <v>178</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2183,7 +2183,7 @@
         <v>179</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -2200,7 +2200,7 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F14" t="s">
         <v>42</v>
@@ -2209,10 +2209,10 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2223,7 +2223,7 @@
         <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F15" t="s">
         <v>45</v>
@@ -2240,7 +2240,7 @@
         <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F16" t="s">
         <v>42</v>
@@ -2257,7 +2257,7 @@
         <v>180</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F17" t="s">
         <v>50</v>
@@ -2274,7 +2274,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F18" t="s">
         <v>42</v>
@@ -2297,7 +2297,7 @@
         <v>173</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
@@ -2314,7 +2314,7 @@
         <v>209</v>
       </c>
       <c r="E20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F20" t="s">
         <v>42</v>
@@ -2331,7 +2331,7 @@
         <v>181</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F21" t="s">
         <v>29</v>
@@ -2348,7 +2348,7 @@
         <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F22" t="s">
         <v>45</v>
@@ -2365,10 +2365,10 @@
         <v>172</v>
       </c>
       <c r="C23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F23" t="s">
         <v>50</v>
@@ -2385,7 +2385,7 @@
         <v>182</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F24" t="s">
         <v>65</v>
@@ -2396,13 +2396,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F25" t="s">
         <v>57</v>
@@ -2419,7 +2419,7 @@
         <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F26" t="s">
         <v>42</v>
@@ -2436,13 +2436,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B27" t="s">
         <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2459,7 +2459,7 @@
         <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F28" t="s">
         <v>55</v>
@@ -2476,7 +2476,7 @@
         <v>171</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F29" t="s">
         <v>72</v>
@@ -2493,7 +2493,7 @@
         <v>9</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F30" t="s">
         <v>42</v>
@@ -2510,7 +2510,7 @@
         <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F31" t="s">
         <v>42</v>
@@ -2519,10 +2519,10 @@
         <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2533,7 +2533,7 @@
         <v>183</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
@@ -2550,7 +2550,7 @@
         <v>184</v>
       </c>
       <c r="E33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F33" t="s">
         <v>17</v>
@@ -2570,7 +2570,7 @@
         <v>78</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F34" t="s">
         <v>26</v>
@@ -2587,7 +2587,7 @@
         <v>185</v>
       </c>
       <c r="E35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F35" t="s">
         <v>81</v>
@@ -2604,7 +2604,7 @@
         <v>186</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F36" t="s">
         <v>42</v>
@@ -2627,7 +2627,7 @@
         <v>187</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F37" t="s">
         <v>36</v>
@@ -2644,7 +2644,7 @@
         <v>88</v>
       </c>
       <c r="E38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F38" t="s">
         <v>89</v>
@@ -2661,7 +2661,7 @@
         <v>91</v>
       </c>
       <c r="E39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F39" t="s">
         <v>24</v>
@@ -2684,7 +2684,7 @@
         <v>130</v>
       </c>
       <c r="E40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F40" t="s">
         <v>17</v>
@@ -2704,7 +2704,7 @@
         <v>94</v>
       </c>
       <c r="E41" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F41" t="s">
         <v>42</v>
@@ -2727,7 +2727,7 @@
         <v>214</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -2744,7 +2744,7 @@
         <v>184</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F43" t="s">
         <v>14</v>
@@ -2761,7 +2761,7 @@
         <v>183</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F44" t="s">
         <v>99</v>
@@ -2778,7 +2778,7 @@
         <v>188</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F45" t="s">
         <v>81</v>
@@ -2795,7 +2795,7 @@
         <v>189</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F46" t="s">
         <v>72</v>
@@ -2812,13 +2812,13 @@
         <v>112</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F47" t="s">
+        <v>332</v>
+      </c>
+      <c r="G47" t="s">
         <v>333</v>
-      </c>
-      <c r="G47" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2829,7 +2829,7 @@
         <v>190</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F48" t="s">
         <v>17</v>
@@ -2846,7 +2846,7 @@
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F49" t="s">
         <v>72</v>
@@ -2863,7 +2863,7 @@
         <v>191</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F50" t="s">
         <v>26</v>
@@ -2880,7 +2880,7 @@
         <v>192</v>
       </c>
       <c r="E51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
@@ -2897,7 +2897,7 @@
         <v>32</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F52" t="s">
         <v>57</v>
@@ -2914,7 +2914,7 @@
         <v>61</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F53" t="s">
         <v>42</v>
@@ -2923,10 +2923,10 @@
         <v>21</v>
       </c>
       <c r="H53" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -2937,10 +2937,10 @@
         <v>44</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F54" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G54" t="s">
         <v>21</v>
@@ -2954,7 +2954,7 @@
         <v>112</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F55" t="s">
         <v>113</v>
@@ -2971,7 +2971,7 @@
         <v>32</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F56" t="s">
         <v>42</v>
@@ -2988,7 +2988,7 @@
         <v>194</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F57" t="s">
         <v>57</v>
@@ -3005,7 +3005,7 @@
         <v>95</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F58" t="s">
         <v>89</v>
@@ -3022,7 +3022,7 @@
         <v>195</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F59" t="s">
         <v>81</v>
@@ -3039,7 +3039,7 @@
         <v>120</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F60" t="s">
         <v>50</v>
@@ -3056,7 +3056,7 @@
         <v>196</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F61" t="s">
         <v>57</v>
@@ -3067,13 +3067,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B62" t="s">
         <v>44</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F62" t="s">
         <v>17</v>
@@ -3090,7 +3090,7 @@
         <v>197</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F63" t="s">
         <v>26</v>
@@ -3107,7 +3107,7 @@
         <v>198</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F64" t="s">
         <v>42</v>
@@ -3124,7 +3124,7 @@
         <v>126</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F65" t="s">
         <v>89</v>
@@ -3141,7 +3141,7 @@
         <v>128</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F66" t="s">
         <v>55</v>
@@ -3158,10 +3158,10 @@
         <v>130</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F67" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G67" t="s">
         <v>21</v>
@@ -3175,7 +3175,7 @@
         <v>199</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F68" t="s">
         <v>42</v>
@@ -3198,7 +3198,7 @@
         <v>200</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F69" t="s">
         <v>81</v>
@@ -3215,7 +3215,7 @@
         <v>201</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F70" t="s">
         <v>17</v>
@@ -3232,7 +3232,7 @@
         <v>135</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F71" t="s">
         <v>55</v>
@@ -3249,7 +3249,7 @@
         <v>202</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F72" t="s">
         <v>57</v>
@@ -3266,7 +3266,7 @@
         <v>44</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F73" t="s">
         <v>45</v>
@@ -3283,7 +3283,7 @@
         <v>203</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F74" t="s">
         <v>55</v>
@@ -3300,7 +3300,7 @@
         <v>70</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F75" t="s">
         <v>42</v>
@@ -3317,7 +3317,7 @@
         <v>130</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F76" t="s">
         <v>45</v>
@@ -3334,7 +3334,7 @@
         <v>204</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F77" t="s">
         <v>14</v>
@@ -3351,7 +3351,7 @@
         <v>205</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F78" t="s">
         <v>113</v>
@@ -3368,7 +3368,7 @@
         <v>144</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F79" t="s">
         <v>55</v>
@@ -3385,7 +3385,7 @@
         <v>44</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F80" t="s">
         <v>24</v>
@@ -3402,7 +3402,7 @@
         <v>130</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F81" t="s">
         <v>42</v>
@@ -3419,7 +3419,7 @@
         <v>41</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F82" t="s">
         <v>72</v>
@@ -3436,7 +3436,7 @@
         <v>198</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F83" t="s">
         <v>57</v>
@@ -3453,7 +3453,7 @@
         <v>196</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F84" t="s">
         <v>57</v>
@@ -3470,7 +3470,7 @@
         <v>144</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F85" t="s">
         <v>42</v>
@@ -3493,7 +3493,7 @@
         <v>9</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F86" t="s">
         <v>53</v>
@@ -3510,7 +3510,7 @@
         <v>193</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F87" t="s">
         <v>10</v>
@@ -3527,10 +3527,10 @@
         <v>204</v>
       </c>
       <c r="C88" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F88" t="s">
         <v>42</v>
@@ -3550,10 +3550,10 @@
         <v>206</v>
       </c>
       <c r="C89" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E89" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F89" t="s">
         <v>57</v>
@@ -3564,13 +3564,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>345</v>
+      </c>
+      <c r="B90" t="s">
         <v>346</v>
       </c>
-      <c r="B90" t="s">
-        <v>347</v>
-      </c>
       <c r="E90" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F90" t="s">
         <v>57</v>
@@ -3581,16 +3581,16 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>329</v>
+      </c>
+      <c r="B91" t="s">
         <v>330</v>
       </c>
-      <c r="B91" t="s">
+      <c r="E91" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E91" s="1" t="s">
-        <v>332</v>
-      </c>
       <c r="F91" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G91" t="s">
         <v>21</v>
@@ -3604,7 +3604,7 @@
         <v>207</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F92" t="s">
         <v>50</v>
@@ -3621,7 +3621,7 @@
         <v>208</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F93" t="s">
         <v>81</v>
@@ -3638,7 +3638,7 @@
         <v>41</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F94" t="s">
         <v>42</v>
@@ -3647,10 +3647,10 @@
         <v>21</v>
       </c>
       <c r="H94" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I94" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
@@ -3661,13 +3661,13 @@
         <v>144</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F95" t="s">
+        <v>332</v>
+      </c>
+      <c r="G95" t="s">
         <v>333</v>
-      </c>
-      <c r="G95" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -3678,7 +3678,7 @@
         <v>222</v>
       </c>
       <c r="E96" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F96" t="s">
         <v>81</v>
@@ -3695,7 +3695,7 @@
         <v>209</v>
       </c>
       <c r="E97" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F97" t="s">
         <v>57</v>
@@ -3712,7 +3712,7 @@
         <v>158</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F98" t="s">
         <v>42</v>
@@ -3735,7 +3735,7 @@
         <v>198</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F99" t="s">
         <v>57</v>
@@ -3752,7 +3752,7 @@
         <v>130</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F100" t="s">
         <v>57</v>
@@ -3769,7 +3769,7 @@
         <v>162</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F101" t="s">
         <v>81</v>
@@ -3786,7 +3786,7 @@
         <v>34</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F102" t="s">
         <v>57</v>
@@ -3803,7 +3803,7 @@
         <v>210</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F103" t="s">
         <v>17</v>
@@ -3820,7 +3820,7 @@
         <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3831,13 +3831,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B105" t="s">
         <v>34</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F105" t="s">
         <v>42</v>
@@ -3854,7 +3854,7 @@
         <v>196</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F106" t="s">
         <v>42</v>
@@ -3877,7 +3877,7 @@
         <v>44</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F107" t="s">
         <v>14</v>
@@ -3894,7 +3894,7 @@
         <v>217</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F108" t="s">
         <v>42</v>
@@ -3917,7 +3917,7 @@
         <v>211</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F109" t="s">
         <v>36</v>
@@ -3928,13 +3928,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>347</v>
+      </c>
+      <c r="B110" t="s">
         <v>348</v>
       </c>
-      <c r="B110" t="s">
-        <v>349</v>
-      </c>
       <c r="E110" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F110" t="s">
         <v>57</v>
@@ -3951,7 +3951,7 @@
         <v>170</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F111" t="s">
         <v>14</v>
@@ -3968,7 +3968,7 @@
         <v>44</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F112" t="s">
         <v>42</v>
@@ -3977,10 +3977,10 @@
         <v>21</v>
       </c>
       <c r="H112" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I112" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aveiro updates: Ferreira out; Silva in
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CFCBF265-3921-0F45-B23F-51A791FF167E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{915EA619-6458-9846-870A-2FD2C08DBF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2860" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="355">
   <si>
     <t>LastName</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Bilbao, E-48009, Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">Ferreira                     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Aveiro, 3810-193, Portugal</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
     <t xml:space="preserve">P.         </t>
   </si>
   <si>
-    <t xml:space="preserve">A.L.       </t>
-  </si>
-  <si>
     <t xml:space="preserve">C.A.O.     </t>
   </si>
   <si>
@@ -811,9 +805,6 @@
     <t>paola.ferrario@dipc.org</t>
   </si>
   <si>
-    <t>alf@ua.pt</t>
-  </si>
-  <si>
     <t>ffoss@uta.edu</t>
   </si>
   <si>
@@ -1100,6 +1091,12 @@
   </si>
   <si>
     <t>helena.almazan@dipc.org</t>
+  </si>
+  <si>
+    <t>A.L.M.</t>
+  </si>
+  <si>
+    <t>analuisa.silva@ua.pt</t>
   </si>
 </sst>
 </file>
@@ -1953,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1973,7 +1970,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1996,7 +1993,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2013,7 +2010,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -2027,10 +2024,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2047,10 +2044,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2064,7 +2061,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -2078,10 +2075,10 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -2095,10 +2092,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F8" t="s">
         <v>29</v>
@@ -2115,10 +2112,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F9" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2132,7 +2129,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F10" t="s">
         <v>57</v>
@@ -2146,10 +2143,10 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -2163,10 +2160,10 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2180,10 +2177,10 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -2200,7 +2197,7 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F14" t="s">
         <v>42</v>
@@ -2209,10 +2206,10 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I14" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2223,7 +2220,7 @@
         <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F15" t="s">
         <v>45</v>
@@ -2240,7 +2237,7 @@
         <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F16" t="s">
         <v>42</v>
@@ -2254,10 +2251,10 @@
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F17" t="s">
         <v>50</v>
@@ -2274,7 +2271,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F18" t="s">
         <v>42</v>
@@ -2294,10 +2291,10 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
@@ -2308,13 +2305,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F20" t="s">
         <v>42</v>
@@ -2328,10 +2325,10 @@
         <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F21" t="s">
         <v>29</v>
@@ -2348,7 +2345,7 @@
         <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F22" t="s">
         <v>45</v>
@@ -2362,13 +2359,13 @@
         <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F23" t="s">
         <v>50</v>
@@ -2382,10 +2379,10 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F24" t="s">
         <v>65</v>
@@ -2396,13 +2393,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F25" t="s">
         <v>57</v>
@@ -2419,7 +2416,7 @@
         <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F26" t="s">
         <v>42</v>
@@ -2436,13 +2433,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2459,7 +2456,7 @@
         <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F28" t="s">
         <v>55</v>
@@ -2473,10 +2470,10 @@
         <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F29" t="s">
         <v>72</v>
@@ -2487,13 +2484,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F30" t="s">
         <v>42</v>
@@ -2510,7 +2507,7 @@
         <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F31" t="s">
         <v>42</v>
@@ -2519,10 +2516,10 @@
         <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I31" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2530,10 +2527,10 @@
         <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
@@ -2547,10 +2544,10 @@
         <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F33" t="s">
         <v>17</v>
@@ -2564,13 +2561,13 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
         <v>78</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F34" t="s">
         <v>26</v>
@@ -2584,10 +2581,10 @@
         <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E35" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F35" t="s">
         <v>81</v>
@@ -2601,10 +2598,10 @@
         <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F36" t="s">
         <v>42</v>
@@ -2621,102 +2618,102 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>187</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>259</v>
+        <v>87</v>
+      </c>
+      <c r="E37" t="s">
+        <v>257</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E38" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F38" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="G38" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="H38" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="E39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F39" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G39" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I39" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>224</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>92</v>
+      </c>
+      <c r="C40" t="s">
+        <v>93</v>
       </c>
       <c r="E40" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G40" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="H40" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" t="s">
-        <v>263</v>
+        <v>212</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="F41" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I41" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -2724,10 +2721,10 @@
         <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -2741,33 +2738,33 @@
         <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F44" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="G44" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2775,33 +2772,33 @@
         <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>267</v>
+        <v>323</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G45" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>189</v>
+        <v>111</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F46" t="s">
-        <v>72</v>
+        <v>329</v>
       </c>
       <c r="G46" t="s">
-        <v>103</v>
+        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2809,16 +2806,16 @@
         <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>188</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>327</v>
+        <v>265</v>
       </c>
       <c r="F47" t="s">
-        <v>332</v>
+        <v>17</v>
       </c>
       <c r="G47" t="s">
-        <v>333</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2826,16 +2823,16 @@
         <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>268</v>
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>266</v>
       </c>
       <c r="F48" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="G48" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -2843,16 +2840,16 @@
         <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" t="s">
-        <v>269</v>
+        <v>189</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="F49" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="G49" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -2860,50 +2857,56 @@
         <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>191</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>270</v>
+        <v>190</v>
+      </c>
+      <c r="E50" t="s">
+        <v>268</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="G50" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>217</v>
       </c>
       <c r="B51" t="s">
-        <v>192</v>
-      </c>
-      <c r="E51" t="s">
-        <v>271</v>
+        <v>32</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="F51" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>219</v>
+        <v>108</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F52" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G52" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="H52" t="s">
+        <v>335</v>
+      </c>
+      <c r="I52" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2911,22 +2914,16 @@
         <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F53" t="s">
-        <v>42</v>
+        <v>334</v>
       </c>
       <c r="G53" t="s">
         <v>21</v>
-      </c>
-      <c r="H53" t="s">
-        <v>338</v>
-      </c>
-      <c r="I53" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -2934,33 +2931,33 @@
         <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F54" t="s">
-        <v>337</v>
+        <v>112</v>
       </c>
       <c r="G54" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F55" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="G55" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -2968,16 +2965,16 @@
         <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F56" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G56" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -2985,16 +2982,16 @@
         <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>194</v>
+        <v>94</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F57" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="G57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -3002,16 +2999,16 @@
         <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>193</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F58" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G58" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -3019,13 +3016,13 @@
         <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F59" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="G59" t="s">
         <v>63</v>
@@ -3033,53 +3030,53 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>194</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F60" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G60" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>350</v>
       </c>
       <c r="B61" t="s">
-        <v>196</v>
+        <v>44</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>281</v>
+        <v>351</v>
       </c>
       <c r="F61" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="G61" t="s">
-        <v>122</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>353</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>195</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>354</v>
+        <v>279</v>
       </c>
       <c r="F62" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G62" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -3087,16 +3084,16 @@
         <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F63" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="G63" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -3104,30 +3101,30 @@
         <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>198</v>
+        <v>125</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F64" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="G64" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F65" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="G65" t="s">
         <v>56</v>
@@ -3135,36 +3132,42 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F66" t="s">
-        <v>55</v>
+        <v>334</v>
       </c>
       <c r="G66" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>197</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F67" t="s">
-        <v>337</v>
+        <v>42</v>
       </c>
       <c r="G67" t="s">
         <v>21</v>
+      </c>
+      <c r="H67" t="s">
+        <v>83</v>
+      </c>
+      <c r="I67" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -3172,22 +3175,16 @@
         <v>131</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F68" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="G68" t="s">
-        <v>21</v>
-      </c>
-      <c r="H68" t="s">
-        <v>83</v>
-      </c>
-      <c r="I68" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -3195,16 +3192,16 @@
         <v>132</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F69" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="G69" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -3212,33 +3209,33 @@
         <v>133</v>
       </c>
       <c r="B70" t="s">
-        <v>201</v>
+        <v>134</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F70" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="G70" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F71" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G71" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -3246,16 +3243,16 @@
         <v>136</v>
       </c>
       <c r="B72" t="s">
-        <v>202</v>
+        <v>44</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F72" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="G72" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -3263,16 +3260,16 @@
         <v>137</v>
       </c>
       <c r="B73" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F73" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G73" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -3280,16 +3277,16 @@
         <v>138</v>
       </c>
       <c r="B74" t="s">
-        <v>203</v>
+        <v>70</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F74" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G74" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3297,16 +3294,16 @@
         <v>139</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F75" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G75" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3314,16 +3311,16 @@
         <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F76" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G76" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3331,16 +3328,16 @@
         <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F77" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="G77" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -3348,47 +3345,47 @@
         <v>142</v>
       </c>
       <c r="B78" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F78" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="G78" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>216</v>
       </c>
       <c r="B79" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F79" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="G79" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>218</v>
+        <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F80" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="G80" t="s">
         <v>21</v>
@@ -3399,16 +3396,16 @@
         <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F81" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="G81" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -3416,16 +3413,16 @@
         <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>41</v>
+        <v>196</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F82" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G82" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -3433,10 +3430,10 @@
         <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
       <c r="F83" t="s">
         <v>57</v>
@@ -3450,16 +3447,22 @@
         <v>148</v>
       </c>
       <c r="B84" t="s">
-        <v>196</v>
+        <v>143</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>344</v>
+        <v>300</v>
       </c>
       <c r="F84" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G84" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="H84" t="s">
+        <v>83</v>
+      </c>
+      <c r="I84" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -3467,22 +3470,16 @@
         <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F85" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="G85" t="s">
         <v>21</v>
-      </c>
-      <c r="H85" t="s">
-        <v>83</v>
-      </c>
-      <c r="I85" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -3490,16 +3487,16 @@
         <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
+        <v>191</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F86" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="G86" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -3507,16 +3504,22 @@
         <v>151</v>
       </c>
       <c r="B87" t="s">
-        <v>193</v>
+        <v>202</v>
+      </c>
+      <c r="C87" t="s">
+        <v>338</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G87" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="I87" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -3527,33 +3530,27 @@
         <v>204</v>
       </c>
       <c r="C88" t="s">
-        <v>341</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>306</v>
+        <v>336</v>
+      </c>
+      <c r="E88" t="s">
+        <v>304</v>
       </c>
       <c r="F88" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G88" t="s">
-        <v>21</v>
-      </c>
-      <c r="I88" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>153</v>
+        <v>342</v>
       </c>
       <c r="B89" t="s">
-        <v>206</v>
-      </c>
-      <c r="C89" t="s">
-        <v>339</v>
-      </c>
-      <c r="E89" t="s">
-        <v>307</v>
+        <v>343</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="F89" t="s">
         <v>57</v>
@@ -3564,50 +3561,50 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="B90" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="F90" t="s">
-        <v>57</v>
+        <v>334</v>
       </c>
       <c r="G90" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>329</v>
+        <v>153</v>
       </c>
       <c r="B91" t="s">
-        <v>330</v>
+        <v>205</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="F91" t="s">
-        <v>337</v>
+        <v>50</v>
       </c>
       <c r="G91" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B92" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F92" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="G92" t="s">
         <v>63</v>
@@ -3615,70 +3612,70 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="B93" t="s">
-        <v>208</v>
+        <v>41</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F93" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="G93" t="s">
-        <v>63</v>
+        <v>21</v>
+      </c>
+      <c r="H93" t="s">
+        <v>335</v>
+      </c>
+      <c r="I93" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>215</v>
+        <v>154</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F94" t="s">
-        <v>42</v>
+        <v>329</v>
       </c>
       <c r="G94" t="s">
-        <v>21</v>
-      </c>
-      <c r="H94" t="s">
-        <v>338</v>
-      </c>
-      <c r="I94" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>219</v>
       </c>
       <c r="B95" t="s">
-        <v>144</v>
+        <v>353</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>311</v>
+        <v>354</v>
       </c>
       <c r="F95" t="s">
-        <v>332</v>
+        <v>36</v>
       </c>
       <c r="G95" t="s">
-        <v>333</v>
+        <v>37</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B96" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E96" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F96" t="s">
         <v>81</v>
@@ -3689,13 +3686,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B97" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E97" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F97" t="s">
         <v>57</v>
@@ -3706,13 +3703,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>156</v>
+      </c>
+      <c r="B98" t="s">
         <v>157</v>
       </c>
-      <c r="B98" t="s">
-        <v>158</v>
-      </c>
       <c r="E98" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F98" t="s">
         <v>42</v>
@@ -3729,13 +3726,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B99" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F99" t="s">
         <v>57</v>
@@ -3746,13 +3743,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B100" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F100" t="s">
         <v>57</v>
@@ -3763,13 +3760,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>160</v>
+      </c>
+      <c r="B101" t="s">
         <v>161</v>
       </c>
-      <c r="B101" t="s">
-        <v>162</v>
-      </c>
       <c r="E101" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F101" t="s">
         <v>81</v>
@@ -3780,13 +3777,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B102" t="s">
         <v>34</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F102" t="s">
         <v>57</v>
@@ -3797,13 +3794,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F103" t="s">
         <v>17</v>
@@ -3814,13 +3811,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3831,13 +3828,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B105" t="s">
         <v>34</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F105" t="s">
         <v>42</v>
@@ -3848,13 +3845,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B106" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F106" t="s">
         <v>42</v>
@@ -3863,21 +3860,21 @@
         <v>21</v>
       </c>
       <c r="H106" t="s">
+        <v>164</v>
+      </c>
+      <c r="I106" t="s">
         <v>165</v>
-      </c>
-      <c r="I106" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B107" t="s">
         <v>44</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F107" t="s">
         <v>14</v>
@@ -3888,13 +3885,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B108" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F108" t="s">
         <v>42</v>
@@ -3911,30 +3908,30 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B109" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F109" t="s">
         <v>36</v>
       </c>
       <c r="G109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B110" t="s">
+        <v>345</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>351</v>
       </c>
       <c r="F110" t="s">
         <v>57</v>
@@ -3945,13 +3942,13 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>168</v>
+      </c>
+      <c r="B111" t="s">
         <v>169</v>
       </c>
-      <c r="B111" t="s">
-        <v>170</v>
-      </c>
       <c r="E111" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F111" t="s">
         <v>14</v>
@@ -3962,13 +3959,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B112" t="s">
         <v>44</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F112" t="s">
         <v>42</v>
@@ -3977,10 +3974,10 @@
         <v>21</v>
       </c>
       <c r="H112" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I112" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -4002,44 +3999,44 @@
     <hyperlink ref="E32" r:id="rId15" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
     <hyperlink ref="E34" r:id="rId16" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
     <hyperlink ref="E36" r:id="rId17" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
-    <hyperlink ref="E42" r:id="rId18" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
-    <hyperlink ref="E43" r:id="rId19" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
-    <hyperlink ref="E44" r:id="rId20" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
-    <hyperlink ref="E45" r:id="rId21" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
-    <hyperlink ref="E46" r:id="rId22" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
-    <hyperlink ref="E47" r:id="rId23" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
-    <hyperlink ref="E48" r:id="rId24" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
-    <hyperlink ref="E50" r:id="rId25" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E52" r:id="rId26" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E53" r:id="rId27" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E55" r:id="rId28" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E59" r:id="rId29" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E65" r:id="rId30" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
-    <hyperlink ref="E61" r:id="rId31" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E66" r:id="rId32" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E68" r:id="rId33" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E70" r:id="rId34" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E71" r:id="rId35" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E41" r:id="rId18" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
+    <hyperlink ref="E42" r:id="rId19" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
+    <hyperlink ref="E43" r:id="rId20" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
+    <hyperlink ref="E44" r:id="rId21" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
+    <hyperlink ref="E45" r:id="rId22" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
+    <hyperlink ref="E46" r:id="rId23" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
+    <hyperlink ref="E47" r:id="rId24" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
+    <hyperlink ref="E49" r:id="rId25" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
+    <hyperlink ref="E51" r:id="rId26" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E52" r:id="rId27" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E54" r:id="rId28" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E58" r:id="rId29" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E64" r:id="rId30" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E60" r:id="rId31" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
+    <hyperlink ref="E65" r:id="rId32" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E67" r:id="rId33" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E69" r:id="rId34" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E70" r:id="rId35" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
     <hyperlink ref="E3" r:id="rId36" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E63" r:id="rId37" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E72" r:id="rId38" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E73" r:id="rId39" xr:uid="{EA26648E-6DAB-DC40-9C69-6623C07441D4}"/>
-    <hyperlink ref="E74" r:id="rId40" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E62" r:id="rId37" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E71" r:id="rId38" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E72" r:id="rId39" xr:uid="{EA26648E-6DAB-DC40-9C69-6623C07441D4}"/>
+    <hyperlink ref="E73" r:id="rId40" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
     <hyperlink ref="E26" r:id="rId41" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E75" r:id="rId42" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E76" r:id="rId43" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E77" r:id="rId44" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E78" r:id="rId45" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E79" r:id="rId46" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E80" r:id="rId47" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E81" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E83" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E85" r:id="rId50" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E86" r:id="rId51" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E87" r:id="rId52" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E88" r:id="rId53" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E92" r:id="rId54" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E94" r:id="rId55" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E74" r:id="rId42" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E75" r:id="rId43" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E76" r:id="rId44" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E77" r:id="rId45" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E78" r:id="rId46" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E79" r:id="rId47" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E80" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E82" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E84" r:id="rId50" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E85" r:id="rId51" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E86" r:id="rId52" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E87" r:id="rId53" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E91" r:id="rId54" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E93" r:id="rId55" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
     <hyperlink ref="E98" r:id="rId56" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
     <hyperlink ref="E100" r:id="rId57" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
     <hyperlink ref="E101" r:id="rId58" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
@@ -4051,36 +4048,36 @@
     <hyperlink ref="E109" r:id="rId64" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
     <hyperlink ref="E111" r:id="rId65" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
     <hyperlink ref="E112" r:id="rId66" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E58" r:id="rId67" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E69" r:id="rId68" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E93" r:id="rId69" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E57" r:id="rId67" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E68" r:id="rId68" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E92" r:id="rId69" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
     <hyperlink ref="E99" r:id="rId70" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
     <hyperlink ref="E6" r:id="rId71" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
     <hyperlink ref="E13" r:id="rId72" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E60" r:id="rId73" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E59" r:id="rId73" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
     <hyperlink ref="E8" r:id="rId74" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
     <hyperlink ref="E12" r:id="rId75" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E64" r:id="rId76" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E56" r:id="rId77" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E57" r:id="rId78" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E63" r:id="rId76" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E55" r:id="rId77" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E56" r:id="rId78" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
     <hyperlink ref="E5" r:id="rId79" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
     <hyperlink ref="E9" r:id="rId80" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E54" r:id="rId81" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E67" r:id="rId82" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E95" r:id="rId83" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E53" r:id="rId81" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E66" r:id="rId82" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E94" r:id="rId83" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
     <hyperlink ref="E108" r:id="rId84" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
     <hyperlink ref="E24" r:id="rId85" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E82" r:id="rId86" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E81" r:id="rId86" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId87" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E37" r:id="rId88" xr:uid="{CA67A91B-A592-6C4D-A384-814AB8E0413B}"/>
-    <hyperlink ref="E91" r:id="rId89" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
-    <hyperlink ref="E105" r:id="rId90" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E27" r:id="rId91" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E84" r:id="rId92" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E90" r:id="rId93" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E110" r:id="rId94" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
-    <hyperlink ref="E25" r:id="rId95" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
-    <hyperlink ref="E62" r:id="rId96" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E90" r:id="rId88" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
+    <hyperlink ref="E105" r:id="rId89" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E27" r:id="rId90" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E83" r:id="rId91" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E89" r:id="rId92" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E110" r:id="rId93" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E25" r:id="rId94" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
+    <hyperlink ref="E61" r:id="rId95" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E95" r:id="rId96" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IFIC updates 2: change of email for Romo-Luque
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{915EA619-6458-9846-870A-2FD2C08DBF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0E404AA8-5620-E44F-8F8F-537D3E310F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -946,9 +946,6 @@
     <t>bromeo@dipc.org</t>
   </si>
   <si>
-    <t>carmenromoluque@gmail.com</t>
-  </si>
-  <si>
     <t>filomena@gian.fis.uc.pt</t>
   </si>
   <si>
@@ -1097,6 +1094,9 @@
   </si>
   <si>
     <t>analuisa.silva@ua.pt</t>
+  </si>
+  <si>
+    <t>romoluque_c@lanl.gov</t>
   </si>
 </sst>
 </file>
@@ -1950,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2010,7 +2010,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -2047,7 +2047,7 @@
         <v>227</v>
       </c>
       <c r="F5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2115,7 +2115,7 @@
         <v>231</v>
       </c>
       <c r="F9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2206,10 +2206,10 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2362,7 +2362,7 @@
         <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>245</v>
@@ -2393,13 +2393,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F25" t="s">
         <v>57</v>
@@ -2433,13 +2433,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B27" t="s">
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2516,10 +2516,10 @@
         <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I31" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2775,7 +2775,7 @@
         <v>187</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F45" t="s">
         <v>72</v>
@@ -2792,13 +2792,13 @@
         <v>111</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F46" t="s">
+        <v>328</v>
+      </c>
+      <c r="G46" t="s">
         <v>329</v>
-      </c>
-      <c r="G46" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2903,10 +2903,10 @@
         <v>21</v>
       </c>
       <c r="H52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I52" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2920,7 +2920,7 @@
         <v>271</v>
       </c>
       <c r="F53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G53" t="s">
         <v>21</v>
@@ -3047,13 +3047,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B61" t="s">
         <v>44</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F61" t="s">
         <v>17</v>
@@ -3141,7 +3141,7 @@
         <v>283</v>
       </c>
       <c r="F66" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G66" t="s">
         <v>21</v>
@@ -3433,7 +3433,7 @@
         <v>194</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F83" t="s">
         <v>57</v>
@@ -3507,7 +3507,7 @@
         <v>202</v>
       </c>
       <c r="C87" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>303</v>
@@ -3530,10 +3530,10 @@
         <v>204</v>
       </c>
       <c r="C88" t="s">
-        <v>336</v>
-      </c>
-      <c r="E88" t="s">
-        <v>304</v>
+        <v>335</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="F88" t="s">
         <v>57</v>
@@ -3544,13 +3544,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>341</v>
+      </c>
+      <c r="B89" t="s">
         <v>342</v>
       </c>
-      <c r="B89" t="s">
-        <v>343</v>
-      </c>
       <c r="E89" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F89" t="s">
         <v>57</v>
@@ -3561,16 +3561,16 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>325</v>
+      </c>
+      <c r="B90" t="s">
         <v>326</v>
       </c>
-      <c r="B90" t="s">
+      <c r="E90" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="F90" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G90" t="s">
         <v>21</v>
@@ -3584,7 +3584,7 @@
         <v>205</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F91" t="s">
         <v>50</v>
@@ -3601,7 +3601,7 @@
         <v>206</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F92" t="s">
         <v>81</v>
@@ -3618,7 +3618,7 @@
         <v>41</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F93" t="s">
         <v>42</v>
@@ -3627,10 +3627,10 @@
         <v>21</v>
       </c>
       <c r="H93" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I93" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -3641,13 +3641,13 @@
         <v>143</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F94" t="s">
+        <v>328</v>
+      </c>
+      <c r="G94" t="s">
         <v>329</v>
-      </c>
-      <c r="G94" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
@@ -3655,10 +3655,10 @@
         <v>219</v>
       </c>
       <c r="B95" t="s">
+        <v>352</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>354</v>
       </c>
       <c r="F95" t="s">
         <v>36</v>
@@ -3675,7 +3675,7 @@
         <v>220</v>
       </c>
       <c r="E96" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F96" t="s">
         <v>81</v>
@@ -3692,7 +3692,7 @@
         <v>207</v>
       </c>
       <c r="E97" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F97" t="s">
         <v>57</v>
@@ -3709,7 +3709,7 @@
         <v>157</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F98" t="s">
         <v>42</v>
@@ -3732,7 +3732,7 @@
         <v>196</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F99" t="s">
         <v>57</v>
@@ -3749,7 +3749,7 @@
         <v>129</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F100" t="s">
         <v>57</v>
@@ -3766,7 +3766,7 @@
         <v>161</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F101" t="s">
         <v>81</v>
@@ -3783,7 +3783,7 @@
         <v>34</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F102" t="s">
         <v>57</v>
@@ -3800,7 +3800,7 @@
         <v>208</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F103" t="s">
         <v>17</v>
@@ -3817,7 +3817,7 @@
         <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3828,13 +3828,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B105" t="s">
         <v>34</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F105" t="s">
         <v>42</v>
@@ -3851,7 +3851,7 @@
         <v>194</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F106" t="s">
         <v>42</v>
@@ -3874,7 +3874,7 @@
         <v>44</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F107" t="s">
         <v>14</v>
@@ -3891,7 +3891,7 @@
         <v>215</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F108" t="s">
         <v>42</v>
@@ -3914,7 +3914,7 @@
         <v>209</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F109" t="s">
         <v>36</v>
@@ -3925,13 +3925,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>343</v>
+      </c>
+      <c r="B110" t="s">
         <v>344</v>
       </c>
-      <c r="B110" t="s">
-        <v>345</v>
-      </c>
       <c r="E110" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F110" t="s">
         <v>57</v>
@@ -3948,7 +3948,7 @@
         <v>169</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F111" t="s">
         <v>14</v>
@@ -3965,7 +3965,7 @@
         <v>44</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F112" t="s">
         <v>42</v>
@@ -3974,10 +3974,10 @@
         <v>21</v>
       </c>
       <c r="H112" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I112" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4078,6 +4078,7 @@
     <hyperlink ref="E25" r:id="rId94" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
     <hyperlink ref="E61" r:id="rId95" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
     <hyperlink ref="E95" r:id="rId96" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E88" r:id="rId97" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ANL updates: change of email for Rogers
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0E404AA8-5620-E44F-8F8F-537D3E310F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61F1E33F-C964-A748-9361-57E73E601087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2840" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,9 +940,6 @@
     <t>celia.rogero@csic.es</t>
   </si>
   <si>
-    <t>rogersl@anl.gov</t>
-  </si>
-  <si>
     <t>bromeo@dipc.org</t>
   </si>
   <si>
@@ -1097,6 +1094,9 @@
   </si>
   <si>
     <t>romoluque_c@lanl.gov</t>
+  </si>
+  <si>
+    <t>Leslie.rogers776@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1950,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2010,7 +2010,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -2047,7 +2047,7 @@
         <v>227</v>
       </c>
       <c r="F5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2115,7 +2115,7 @@
         <v>231</v>
       </c>
       <c r="F9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2206,10 +2206,10 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2362,7 +2362,7 @@
         <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>245</v>
@@ -2393,13 +2393,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F25" t="s">
         <v>57</v>
@@ -2433,13 +2433,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B27" t="s">
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2516,10 +2516,10 @@
         <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2775,7 +2775,7 @@
         <v>187</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F45" t="s">
         <v>72</v>
@@ -2792,13 +2792,13 @@
         <v>111</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F46" t="s">
+        <v>327</v>
+      </c>
+      <c r="G46" t="s">
         <v>328</v>
-      </c>
-      <c r="G46" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2903,10 +2903,10 @@
         <v>21</v>
       </c>
       <c r="H52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I52" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2920,7 +2920,7 @@
         <v>271</v>
       </c>
       <c r="F53" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G53" t="s">
         <v>21</v>
@@ -3047,13 +3047,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B61" t="s">
         <v>44</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F61" t="s">
         <v>17</v>
@@ -3141,7 +3141,7 @@
         <v>283</v>
       </c>
       <c r="F66" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G66" t="s">
         <v>21</v>
@@ -3433,7 +3433,7 @@
         <v>194</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F83" t="s">
         <v>57</v>
@@ -3490,7 +3490,7 @@
         <v>191</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>302</v>
+        <v>354</v>
       </c>
       <c r="F86" t="s">
         <v>10</v>
@@ -3507,10 +3507,10 @@
         <v>202</v>
       </c>
       <c r="C87" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F87" t="s">
         <v>42</v>
@@ -3530,10 +3530,10 @@
         <v>204</v>
       </c>
       <c r="C88" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F88" t="s">
         <v>57</v>
@@ -3544,13 +3544,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>340</v>
+      </c>
+      <c r="B89" t="s">
         <v>341</v>
       </c>
-      <c r="B89" t="s">
-        <v>342</v>
-      </c>
       <c r="E89" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F89" t="s">
         <v>57</v>
@@ -3561,16 +3561,16 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>324</v>
+      </c>
+      <c r="B90" t="s">
         <v>325</v>
       </c>
-      <c r="B90" t="s">
+      <c r="E90" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>327</v>
-      </c>
       <c r="F90" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G90" t="s">
         <v>21</v>
@@ -3584,7 +3584,7 @@
         <v>205</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F91" t="s">
         <v>50</v>
@@ -3601,7 +3601,7 @@
         <v>206</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F92" t="s">
         <v>81</v>
@@ -3618,7 +3618,7 @@
         <v>41</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F93" t="s">
         <v>42</v>
@@ -3627,10 +3627,10 @@
         <v>21</v>
       </c>
       <c r="H93" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I93" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -3641,13 +3641,13 @@
         <v>143</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F94" t="s">
+        <v>327</v>
+      </c>
+      <c r="G94" t="s">
         <v>328</v>
-      </c>
-      <c r="G94" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
@@ -3655,10 +3655,10 @@
         <v>219</v>
       </c>
       <c r="B95" t="s">
+        <v>351</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="F95" t="s">
         <v>36</v>
@@ -3675,7 +3675,7 @@
         <v>220</v>
       </c>
       <c r="E96" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F96" t="s">
         <v>81</v>
@@ -3692,7 +3692,7 @@
         <v>207</v>
       </c>
       <c r="E97" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F97" t="s">
         <v>57</v>
@@ -3709,7 +3709,7 @@
         <v>157</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F98" t="s">
         <v>42</v>
@@ -3732,7 +3732,7 @@
         <v>196</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F99" t="s">
         <v>57</v>
@@ -3749,7 +3749,7 @@
         <v>129</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F100" t="s">
         <v>57</v>
@@ -3766,7 +3766,7 @@
         <v>161</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F101" t="s">
         <v>81</v>
@@ -3783,7 +3783,7 @@
         <v>34</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F102" t="s">
         <v>57</v>
@@ -3800,7 +3800,7 @@
         <v>208</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F103" t="s">
         <v>17</v>
@@ -3817,7 +3817,7 @@
         <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3828,13 +3828,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B105" t="s">
         <v>34</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F105" t="s">
         <v>42</v>
@@ -3851,7 +3851,7 @@
         <v>194</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F106" t="s">
         <v>42</v>
@@ -3874,7 +3874,7 @@
         <v>44</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F107" t="s">
         <v>14</v>
@@ -3891,7 +3891,7 @@
         <v>215</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F108" t="s">
         <v>42</v>
@@ -3914,7 +3914,7 @@
         <v>209</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F109" t="s">
         <v>36</v>
@@ -3925,13 +3925,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>342</v>
+      </c>
+      <c r="B110" t="s">
         <v>343</v>
       </c>
-      <c r="B110" t="s">
-        <v>344</v>
-      </c>
       <c r="E110" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F110" t="s">
         <v>57</v>
@@ -3948,7 +3948,7 @@
         <v>169</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F111" t="s">
         <v>14</v>
@@ -3965,7 +3965,7 @@
         <v>44</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F112" t="s">
         <v>42</v>
@@ -3974,10 +3974,10 @@
         <v>21</v>
       </c>
       <c r="H112" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I112" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LSC updates: Bayo, Cid, Nunez out; Ruiz in
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61F1E33F-C964-A748-9361-57E73E601087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{64DB39DB-8769-F24C-8442-882249319044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10180" yWindow="2860" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="350">
   <si>
     <t>LastName</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Donostia International Physics Center, BERC Basque Excellence Research Centre, Manuel de Lardizabal 4</t>
   </si>
   <si>
-    <t>Bayo</t>
-  </si>
-  <si>
     <t>A.</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t xml:space="preserve">Church                       </t>
   </si>
   <si>
-    <t>Cid</t>
-  </si>
-  <si>
     <t>L.</t>
   </si>
   <si>
@@ -442,9 +436,6 @@
     <t xml:space="preserve">Novella                     </t>
   </si>
   <si>
-    <t>Nu\~{n}ez</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nygren                      </t>
   </si>
   <si>
@@ -745,9 +736,6 @@
     <t>mariandelbarrio@gmail.com</t>
   </si>
   <si>
-    <t>abayo@lsc-canfranc.es</t>
-  </si>
-  <si>
     <t>info@jmbenlloch.net</t>
   </si>
   <si>
@@ -766,9 +754,6 @@
     <t>eric.church@pnnl.gov</t>
   </si>
   <si>
-    <t>lcid@lsc-canfranc.es</t>
-  </si>
-  <si>
     <t>canconde@gian.fis.uc.pt</t>
   </si>
   <si>
@@ -901,9 +886,6 @@
     <t>pau.novella@ific.uv.es</t>
   </si>
   <si>
-    <t>anunez@lsc-canfranc.es</t>
-  </si>
-  <si>
     <t>nygren@uta.edu</t>
   </si>
   <si>
@@ -1097,6 +1079,9 @@
   </si>
   <si>
     <t>Leslie.rogers776@gmail.com</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
   </si>
 </sst>
 </file>
@@ -1948,10 +1933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1970,7 +1955,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1993,7 +1978,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2010,7 +1995,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -2024,10 +2009,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2044,10 +2029,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F5" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -2061,7 +2046,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -2075,10 +2060,10 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -2092,10 +2077,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F8" t="s">
         <v>29</v>
@@ -2112,10 +2097,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F9" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -2129,13 +2114,13 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
         <v>57</v>
-      </c>
-      <c r="G10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2143,10 +2128,10 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -2160,10 +2145,10 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2177,10 +2162,10 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -2197,7 +2182,7 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F14" t="s">
         <v>42</v>
@@ -2206,206 +2191,212 @@
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="I14" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>179</v>
+        <v>43</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>241</v>
+        <v>204</v>
+      </c>
+      <c r="E19" t="s">
+        <v>238</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
-      </c>
-      <c r="E20" t="s">
-        <v>242</v>
+        <v>177</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>168</v>
+      </c>
+      <c r="C21" t="s">
+        <v>329</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" t="s">
-        <v>244</v>
+        <v>178</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>338</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
-      </c>
-      <c r="C23" t="s">
-        <v>335</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>245</v>
+        <v>341</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>181</v>
+        <v>66</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F24" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -2416,87 +2407,87 @@
         <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>337</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>338</v>
+        <v>244</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>208</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>249</v>
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>246</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>21</v>
+      </c>
+      <c r="H29" t="s">
+        <v>327</v>
+      </c>
+      <c r="I29" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>211</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>179</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -2504,22 +2495,16 @@
         <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="E31" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F31" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" t="s">
-        <v>333</v>
-      </c>
-      <c r="I31" t="s">
-        <v>329</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2527,110 +2512,116 @@
         <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>180</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F32" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="G32" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E33" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F33" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
-      </c>
-      <c r="C34" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F34" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>21</v>
+      </c>
+      <c r="H34" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>184</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F35" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>185</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>256</v>
+        <v>88</v>
+      </c>
+      <c r="E36" t="s">
+        <v>253</v>
       </c>
       <c r="F36" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G36" t="s">
         <v>21</v>
       </c>
       <c r="H36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>219</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="E37" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="G37" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -2640,63 +2631,57 @@
       <c r="B38" t="s">
         <v>90</v>
       </c>
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
       <c r="E38" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F38" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="G38" t="s">
         <v>21</v>
       </c>
       <c r="H38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>222</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" t="s">
-        <v>259</v>
+        <v>209</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" t="s">
-        <v>260</v>
+        <v>180</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" t="s">
-        <v>83</v>
-      </c>
-      <c r="I40" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -2704,84 +2689,84 @@
         <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B42" t="s">
         <v>183</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>263</v>
+        <v>315</v>
       </c>
       <c r="F43" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="G43" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>109</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>264</v>
+        <v>316</v>
       </c>
       <c r="F44" t="s">
-        <v>81</v>
+        <v>321</v>
       </c>
       <c r="G44" t="s">
-        <v>63</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>321</v>
+        <v>260</v>
       </c>
       <c r="F45" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="G45" t="s">
-        <v>102</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2789,16 +2774,16 @@
         <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>322</v>
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>261</v>
       </c>
       <c r="F46" t="s">
-        <v>327</v>
+        <v>70</v>
       </c>
       <c r="G46" t="s">
-        <v>328</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2806,16 +2791,16 @@
         <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F47" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G47" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2823,67 +2808,73 @@
         <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="E48" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F48" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G48" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>214</v>
       </c>
       <c r="B49" t="s">
-        <v>189</v>
+        <v>32</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="G49" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>190</v>
-      </c>
-      <c r="E50" t="s">
-        <v>268</v>
+        <v>59</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="F50" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G50" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="H50" t="s">
+        <v>327</v>
+      </c>
+      <c r="I50" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>217</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F51" t="s">
-        <v>57</v>
+        <v>326</v>
       </c>
       <c r="G51" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -2891,36 +2882,30 @@
         <v>108</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F52" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="G52" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" t="s">
-        <v>333</v>
-      </c>
-      <c r="I52" t="s">
-        <v>329</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F53" t="s">
-        <v>332</v>
+        <v>42</v>
       </c>
       <c r="G53" t="s">
         <v>21</v>
@@ -2928,19 +2913,19 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>189</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F54" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="G54" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -2948,16 +2933,16 @@
         <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F55" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="G55" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -2965,16 +2950,16 @@
         <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F56" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="G56" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -2982,50 +2967,50 @@
         <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F57" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="G57" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F58" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="G58" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>342</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>277</v>
+        <v>343</v>
       </c>
       <c r="F59" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="G59" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -3033,33 +3018,33 @@
         <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F60" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="G60" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>348</v>
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>193</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>349</v>
+        <v>275</v>
       </c>
       <c r="F61" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G61" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -3067,84 +3052,90 @@
         <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>195</v>
+        <v>123</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="G62" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F63" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G63" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F64" t="s">
-        <v>88</v>
+        <v>326</v>
       </c>
       <c r="G64" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>194</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F65" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G65" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="H65" t="s">
+        <v>81</v>
+      </c>
+      <c r="I65" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F66" t="s">
-        <v>332</v>
+        <v>79</v>
       </c>
       <c r="G66" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -3152,22 +3143,16 @@
         <v>130</v>
       </c>
       <c r="B67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F67" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G67" t="s">
-        <v>21</v>
-      </c>
-      <c r="H67" t="s">
-        <v>83</v>
-      </c>
-      <c r="I67" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -3175,50 +3160,50 @@
         <v>131</v>
       </c>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>132</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F68" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="G68" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F69" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G69" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>198</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F70" t="s">
+        <v>54</v>
+      </c>
+      <c r="G70" t="s">
         <v>55</v>
-      </c>
-      <c r="G70" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -3226,16 +3211,16 @@
         <v>135</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>68</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F71" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G71" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -3243,16 +3228,16 @@
         <v>136</v>
       </c>
       <c r="B72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F72" t="s">
         <v>44</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>45</v>
-      </c>
-      <c r="G72" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -3260,16 +3245,16 @@
         <v>137</v>
       </c>
       <c r="B73" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F73" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="G73" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -3277,16 +3262,16 @@
         <v>138</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F74" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="G74" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3294,33 +3279,33 @@
         <v>139</v>
       </c>
       <c r="B75" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F75" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G75" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>213</v>
       </c>
       <c r="B76" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F76" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G76" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3328,16 +3313,16 @@
         <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>203</v>
+        <v>127</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F77" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="G77" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -3345,33 +3330,33 @@
         <v>142</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F78" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G78" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>216</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>193</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F79" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="G79" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -3379,16 +3364,16 @@
         <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>129</v>
+        <v>191</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>297</v>
+        <v>333</v>
       </c>
       <c r="F80" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G80" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3396,16 +3381,22 @@
         <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F81" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="G81" t="s">
-        <v>102</v>
+        <v>21</v>
+      </c>
+      <c r="H81" t="s">
+        <v>81</v>
+      </c>
+      <c r="I81" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -3413,16 +3404,16 @@
         <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>196</v>
+        <v>9</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F82" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G82" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -3430,16 +3421,16 @@
         <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="F83" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="G83" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -3447,10 +3438,13 @@
         <v>148</v>
       </c>
       <c r="B84" t="s">
-        <v>143</v>
+        <v>199</v>
+      </c>
+      <c r="C84" t="s">
+        <v>330</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F84" t="s">
         <v>42</v>
@@ -3458,11 +3452,8 @@
       <c r="G84" t="s">
         <v>21</v>
       </c>
-      <c r="H84" t="s">
-        <v>83</v>
-      </c>
       <c r="I84" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -3470,218 +3461,216 @@
         <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>201</v>
+      </c>
+      <c r="C85" t="s">
+        <v>328</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>301</v>
+        <v>347</v>
       </c>
       <c r="F85" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G85" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>349</v>
       </c>
       <c r="B86" t="s">
-        <v>191</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>354</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E86" s="1"/>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="G86" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>151</v>
+        <v>334</v>
       </c>
       <c r="B87" t="s">
-        <v>202</v>
-      </c>
-      <c r="C87" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>302</v>
+        <v>339</v>
       </c>
       <c r="F87" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G87" t="s">
-        <v>21</v>
-      </c>
-      <c r="I87" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>318</v>
       </c>
       <c r="B88" t="s">
-        <v>204</v>
-      </c>
-      <c r="C88" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>353</v>
+        <v>320</v>
       </c>
       <c r="F88" t="s">
-        <v>57</v>
+        <v>326</v>
       </c>
       <c r="G88" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>340</v>
+        <v>150</v>
       </c>
       <c r="B89" t="s">
-        <v>341</v>
+        <v>202</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="F89" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G89" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>324</v>
+        <v>150</v>
       </c>
       <c r="B90" t="s">
-        <v>325</v>
+        <v>203</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>326</v>
+        <v>298</v>
       </c>
       <c r="F90" t="s">
-        <v>332</v>
+        <v>79</v>
       </c>
       <c r="G90" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="B91" t="s">
-        <v>205</v>
+        <v>41</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F91" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G91" t="s">
-        <v>63</v>
+        <v>21</v>
+      </c>
+      <c r="H91" t="s">
+        <v>327</v>
+      </c>
+      <c r="I91" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B92" t="s">
-        <v>206</v>
+        <v>140</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F92" t="s">
-        <v>81</v>
+        <v>321</v>
       </c>
       <c r="G92" t="s">
-        <v>63</v>
+        <v>322</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B93" t="s">
-        <v>41</v>
+        <v>345</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>305</v>
+        <v>346</v>
       </c>
       <c r="F93" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G93" t="s">
-        <v>21</v>
-      </c>
-      <c r="H93" t="s">
-        <v>333</v>
-      </c>
-      <c r="I93" t="s">
-        <v>329</v>
+        <v>37</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="B94" t="s">
-        <v>143</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>306</v>
+        <v>217</v>
+      </c>
+      <c r="E94" t="s">
+        <v>301</v>
       </c>
       <c r="F94" t="s">
-        <v>327</v>
+        <v>79</v>
       </c>
       <c r="G94" t="s">
-        <v>328</v>
+        <v>61</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>219</v>
+        <v>152</v>
       </c>
       <c r="B95" t="s">
-        <v>351</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>352</v>
+        <v>204</v>
+      </c>
+      <c r="E95" t="s">
+        <v>302</v>
       </c>
       <c r="F95" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G95" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>219</v>
+        <v>153</v>
       </c>
       <c r="B96" t="s">
-        <v>220</v>
-      </c>
-      <c r="E96" t="s">
-        <v>307</v>
+        <v>154</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="F96" t="s">
+        <v>42</v>
+      </c>
+      <c r="G96" t="s">
+        <v>21</v>
+      </c>
+      <c r="H96" t="s">
         <v>81</v>
       </c>
-      <c r="G96" t="s">
-        <v>63</v>
+      <c r="I96" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -3689,16 +3678,16 @@
         <v>155</v>
       </c>
       <c r="B97" t="s">
-        <v>207</v>
-      </c>
-      <c r="E97" t="s">
-        <v>308</v>
+        <v>193</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="F97" t="s">
+        <v>56</v>
+      </c>
+      <c r="G97" t="s">
         <v>57</v>
-      </c>
-      <c r="G97" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -3706,118 +3695,112 @@
         <v>156</v>
       </c>
       <c r="B98" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="F98" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G98" t="s">
-        <v>21</v>
-      </c>
-      <c r="H98" t="s">
-        <v>83</v>
-      </c>
-      <c r="I98" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>157</v>
+      </c>
+      <c r="B99" t="s">
         <v>158</v>
       </c>
-      <c r="B99" t="s">
-        <v>196</v>
-      </c>
       <c r="E99" s="1" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="F99" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="G99" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="B100" t="s">
-        <v>129</v>
+        <v>34</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="F100" t="s">
+        <v>56</v>
+      </c>
+      <c r="G100" t="s">
         <v>57</v>
-      </c>
-      <c r="G100" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B101" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F101" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="G101" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B102" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F102" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G102" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>162</v>
+        <v>324</v>
       </c>
       <c r="B103" t="s">
-        <v>208</v>
+        <v>34</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="F103" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G103" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>218</v>
+        <v>160</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>191</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F104" t="s">
         <v>42</v>
@@ -3825,33 +3808,39 @@
       <c r="G104" t="s">
         <v>21</v>
       </c>
+      <c r="H104" t="s">
+        <v>161</v>
+      </c>
+      <c r="I104" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>330</v>
+        <v>163</v>
       </c>
       <c r="B105" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="F105" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G105" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>163</v>
+        <v>211</v>
       </c>
       <c r="B106" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F106" t="s">
         <v>42</v>
@@ -3860,124 +3849,84 @@
         <v>21</v>
       </c>
       <c r="H106" t="s">
-        <v>164</v>
+        <v>24</v>
       </c>
       <c r="I106" t="s">
-        <v>165</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B107" t="s">
-        <v>44</v>
+        <v>206</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F107" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G107" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>214</v>
+        <v>336</v>
       </c>
       <c r="B108" t="s">
-        <v>215</v>
+        <v>337</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>316</v>
+        <v>340</v>
       </c>
       <c r="F108" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G108" t="s">
-        <v>21</v>
-      </c>
-      <c r="H108" t="s">
-        <v>24</v>
-      </c>
-      <c r="I108" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B109" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F109" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="G109" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>342</v>
+        <v>220</v>
       </c>
       <c r="B110" t="s">
-        <v>343</v>
+        <v>43</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>346</v>
+        <v>313</v>
       </c>
       <c r="F110" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G110" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>168</v>
-      </c>
-      <c r="B111" t="s">
-        <v>169</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="F111" t="s">
-        <v>14</v>
-      </c>
-      <c r="G111" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>223</v>
-      </c>
-      <c r="B112" t="s">
-        <v>44</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F112" t="s">
-        <v>42</v>
-      </c>
-      <c r="G112" t="s">
         <v>21</v>
       </c>
-      <c r="H112" t="s">
-        <v>333</v>
-      </c>
-      <c r="I112" t="s">
-        <v>329</v>
+      <c r="H110" t="s">
+        <v>327</v>
+      </c>
+      <c r="I110" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3986,99 +3935,97 @@
     <hyperlink ref="E7" r:id="rId2" xr:uid="{D72FCA14-EA08-4749-BB11-D24B8A62C2FD}"/>
     <hyperlink ref="E10" r:id="rId3" xr:uid="{E6DBC748-9C42-444A-9719-EDB7AD21ED31}"/>
     <hyperlink ref="E11" r:id="rId4" xr:uid="{D72F2EFB-3573-5D41-9B63-CA5C8A903FE7}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{05A2D3D0-A226-F349-848E-360308510428}"/>
-    <hyperlink ref="E16" r:id="rId6" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
-    <hyperlink ref="E17" r:id="rId7" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
-    <hyperlink ref="E18" r:id="rId8" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
-    <hyperlink ref="E19" r:id="rId9" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
-    <hyperlink ref="E21" r:id="rId10" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
-    <hyperlink ref="E23" r:id="rId11" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
-    <hyperlink ref="E28" r:id="rId12" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
-    <hyperlink ref="E29" r:id="rId13" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
-    <hyperlink ref="E30" r:id="rId14" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
-    <hyperlink ref="E32" r:id="rId15" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
-    <hyperlink ref="E34" r:id="rId16" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
-    <hyperlink ref="E36" r:id="rId17" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
-    <hyperlink ref="E41" r:id="rId18" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
-    <hyperlink ref="E42" r:id="rId19" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
-    <hyperlink ref="E43" r:id="rId20" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
-    <hyperlink ref="E44" r:id="rId21" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
-    <hyperlink ref="E45" r:id="rId22" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
-    <hyperlink ref="E46" r:id="rId23" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
-    <hyperlink ref="E47" r:id="rId24" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
-    <hyperlink ref="E49" r:id="rId25" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E51" r:id="rId26" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E52" r:id="rId27" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E54" r:id="rId28" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E58" r:id="rId29" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E64" r:id="rId30" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
-    <hyperlink ref="E60" r:id="rId31" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E65" r:id="rId32" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E67" r:id="rId33" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E69" r:id="rId34" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E70" r:id="rId35" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
-    <hyperlink ref="E3" r:id="rId36" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E62" r:id="rId37" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E71" r:id="rId38" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E72" r:id="rId39" xr:uid="{EA26648E-6DAB-DC40-9C69-6623C07441D4}"/>
-    <hyperlink ref="E73" r:id="rId40" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
-    <hyperlink ref="E26" r:id="rId41" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E74" r:id="rId42" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E75" r:id="rId43" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E76" r:id="rId44" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E77" r:id="rId45" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E78" r:id="rId46" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E79" r:id="rId47" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E80" r:id="rId48" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E82" r:id="rId49" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E84" r:id="rId50" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E85" r:id="rId51" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E86" r:id="rId52" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E87" r:id="rId53" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E91" r:id="rId54" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E93" r:id="rId55" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E98" r:id="rId56" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E100" r:id="rId57" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E101" r:id="rId58" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E102" r:id="rId59" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E103" r:id="rId60" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E104" r:id="rId61" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E106" r:id="rId62" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E107" r:id="rId63" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E109" r:id="rId64" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E111" r:id="rId65" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E112" r:id="rId66" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E57" r:id="rId67" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E68" r:id="rId68" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E92" r:id="rId69" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E99" r:id="rId70" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
-    <hyperlink ref="E6" r:id="rId71" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
-    <hyperlink ref="E13" r:id="rId72" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E59" r:id="rId73" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
-    <hyperlink ref="E8" r:id="rId74" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
-    <hyperlink ref="E12" r:id="rId75" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E63" r:id="rId76" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E55" r:id="rId77" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E56" r:id="rId78" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
-    <hyperlink ref="E5" r:id="rId79" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
-    <hyperlink ref="E9" r:id="rId80" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E53" r:id="rId81" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E66" r:id="rId82" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E94" r:id="rId83" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E108" r:id="rId84" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E24" r:id="rId85" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E81" r:id="rId86" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
-    <hyperlink ref="E4" r:id="rId87" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E90" r:id="rId88" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
-    <hyperlink ref="E105" r:id="rId89" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E27" r:id="rId90" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E83" r:id="rId91" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E89" r:id="rId92" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E110" r:id="rId93" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
-    <hyperlink ref="E25" r:id="rId94" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
-    <hyperlink ref="E61" r:id="rId95" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
-    <hyperlink ref="E95" r:id="rId96" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
-    <hyperlink ref="E88" r:id="rId97" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
+    <hyperlink ref="E18" r:id="rId8" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
+    <hyperlink ref="E26" r:id="rId11" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
+    <hyperlink ref="E27" r:id="rId12" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
+    <hyperlink ref="E28" r:id="rId13" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
+    <hyperlink ref="E30" r:id="rId14" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
+    <hyperlink ref="E32" r:id="rId15" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
+    <hyperlink ref="E34" r:id="rId16" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
+    <hyperlink ref="E39" r:id="rId17" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
+    <hyperlink ref="E40" r:id="rId18" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
+    <hyperlink ref="E41" r:id="rId19" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
+    <hyperlink ref="E42" r:id="rId20" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
+    <hyperlink ref="E43" r:id="rId21" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
+    <hyperlink ref="E44" r:id="rId22" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
+    <hyperlink ref="E45" r:id="rId23" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
+    <hyperlink ref="E47" r:id="rId24" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
+    <hyperlink ref="E49" r:id="rId25" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E50" r:id="rId26" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E52" r:id="rId27" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E56" r:id="rId28" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E62" r:id="rId29" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E58" r:id="rId30" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
+    <hyperlink ref="E63" r:id="rId31" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E65" r:id="rId32" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E67" r:id="rId33" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E68" r:id="rId34" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E3" r:id="rId35" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
+    <hyperlink ref="E60" r:id="rId36" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E69" r:id="rId37" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E70" r:id="rId38" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E24" r:id="rId39" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
+    <hyperlink ref="E71" r:id="rId40" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E72" r:id="rId41" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E73" r:id="rId42" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E74" r:id="rId43" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E75" r:id="rId44" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E76" r:id="rId45" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E77" r:id="rId46" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E79" r:id="rId47" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E81" r:id="rId48" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E82" r:id="rId49" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E83" r:id="rId50" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E84" r:id="rId51" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E89" r:id="rId52" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E91" r:id="rId53" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E96" r:id="rId54" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E98" r:id="rId55" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E99" r:id="rId56" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E100" r:id="rId57" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E101" r:id="rId58" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E102" r:id="rId59" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E104" r:id="rId60" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E105" r:id="rId61" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E107" r:id="rId62" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E109" r:id="rId63" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E110" r:id="rId64" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E55" r:id="rId65" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E66" r:id="rId66" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E90" r:id="rId67" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E97" r:id="rId68" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E6" r:id="rId69" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
+    <hyperlink ref="E13" r:id="rId70" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
+    <hyperlink ref="E57" r:id="rId71" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E8" r:id="rId72" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
+    <hyperlink ref="E12" r:id="rId73" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
+    <hyperlink ref="E61" r:id="rId74" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E53" r:id="rId75" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E54" r:id="rId76" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E5" r:id="rId77" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
+    <hyperlink ref="E9" r:id="rId78" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
+    <hyperlink ref="E51" r:id="rId79" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E64" r:id="rId80" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E92" r:id="rId81" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E106" r:id="rId82" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E22" r:id="rId83" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
+    <hyperlink ref="E78" r:id="rId84" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E4" r:id="rId85" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
+    <hyperlink ref="E88" r:id="rId86" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
+    <hyperlink ref="E103" r:id="rId87" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E25" r:id="rId88" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E80" r:id="rId89" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E87" r:id="rId90" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E108" r:id="rId91" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E23" r:id="rId92" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
+    <hyperlink ref="E59" r:id="rId93" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E93" r:id="rId94" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E85" r:id="rId95" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UPV-EHU Organic Chemistry updates: Aparicio, San Nancianceno out; Marauri in; change of affiliation for Cossio and Rivilla
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{64DB39DB-8769-F24C-8442-882249319044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C73B5C79-8E29-E844-8D06-2A85A79861E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="2860" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2320" yWindow="3720" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="345">
   <si>
     <t>LastName</t>
   </si>
@@ -91,12 +91,6 @@
     <t xml:space="preserve"> Valencia, E-46022, Spain</t>
   </si>
   <si>
-    <t>Aparicio</t>
-  </si>
-  <si>
-    <t>B.</t>
-  </si>
-  <si>
     <t>San Sebasti\'an / Donostia, E-20018, Spain</t>
   </si>
   <si>
@@ -706,9 +700,6 @@
     <t>vicente.alvarez@ific.uv.es</t>
   </si>
   <si>
-    <t>borja.aparicio@usc.es</t>
-  </si>
-  <si>
     <t>aneiaranburu.94@gmail.com</t>
   </si>
   <si>
@@ -988,15 +979,6 @@
     <t>josealfonso.soto@ific.uv.es</t>
   </si>
   <si>
-    <t>San Nacienciano</t>
-  </si>
-  <si>
-    <t>V.</t>
-  </si>
-  <si>
-    <t>virginia.sannacianceno@ehu.eus</t>
-  </si>
-  <si>
     <t>Racah Institute of Physics, The Hebrew University of Jerusalem</t>
   </si>
   <si>
@@ -1082,6 +1064,9 @@
   </si>
   <si>
     <t>Ruiz</t>
+  </si>
+  <si>
+    <t>Marauri</t>
   </si>
 </sst>
 </file>
@@ -1933,10 +1918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:XFD88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1955,7 +1940,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1978,7 +1963,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1995,13 +1980,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2009,10 +1994,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2023,70 +2008,70 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F5" t="s">
-        <v>326</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>320</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2097,13 +2082,13 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F9" t="s">
-        <v>326</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2111,90 +2096,90 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F10" t="s">
-        <v>56</v>
-      </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>232</v>
+      <c r="E13" t="s">
+        <v>230</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>321</v>
+      </c>
+      <c r="I13" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>233</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
       <c r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" t="s">
-        <v>327</v>
-      </c>
-      <c r="I14" t="s">
-        <v>323</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2202,33 +2187,39 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F15" t="s">
-        <v>42</v>
-      </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
         <v>50</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -2236,56 +2227,50 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>167</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>205</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>237</v>
+        <v>202</v>
+      </c>
+      <c r="E18" t="s">
+        <v>235</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>207</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>204</v>
-      </c>
-      <c r="E19" t="s">
-        <v>238</v>
+        <v>175</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -2293,16 +2278,19 @@
         <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>177</v>
+        <v>166</v>
+      </c>
+      <c r="C20" t="s">
+        <v>323</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G20" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -2310,93 +2298,84 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
-      </c>
-      <c r="C21" t="s">
-        <v>329</v>
+        <v>176</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>332</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>241</v>
+        <v>335</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>338</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>341</v>
+        <v>239</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>320</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>325</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>242</v>
+        <v>326</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>331</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>332</v>
+        <v>240</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -2404,127 +2383,127 @@
         <v>67</v>
       </c>
       <c r="B26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F26" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="F26" t="s">
-        <v>54</v>
-      </c>
       <c r="G26" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>206</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>245</v>
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>243</v>
       </c>
       <c r="F28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H28" t="s">
+        <v>321</v>
+      </c>
+      <c r="I28" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" t="s">
-        <v>246</v>
+        <v>177</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" t="s">
-        <v>327</v>
-      </c>
-      <c r="I29" t="s">
-        <v>323</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>247</v>
+        <v>178</v>
+      </c>
+      <c r="E30" t="s">
+        <v>245</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="G30" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" t="s">
         <v>74</v>
       </c>
-      <c r="B31" t="s">
-        <v>180</v>
-      </c>
-      <c r="E31" t="s">
-        <v>248</v>
+      <c r="E31" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="F31" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G31" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>249</v>
+        <v>179</v>
+      </c>
+      <c r="E32" t="s">
+        <v>247</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G32" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -2532,133 +2511,133 @@
         <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" t="s">
-        <v>250</v>
+        <v>180</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="F33" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" t="s">
         <v>79</v>
       </c>
-      <c r="G33" t="s">
-        <v>61</v>
+      <c r="I33" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>251</v>
+        <v>83</v>
+      </c>
+      <c r="E34" t="s">
+        <v>249</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="G34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" t="s">
-        <v>81</v>
-      </c>
-      <c r="I34" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F35" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="H35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I35" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>217</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="E36" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F36" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>88</v>
+      </c>
+      <c r="C37" t="s">
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F37" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H37" t="s">
+        <v>79</v>
+      </c>
+      <c r="I37" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" t="s">
-        <v>255</v>
+        <v>207</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="F38" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>21</v>
-      </c>
-      <c r="H38" t="s">
-        <v>81</v>
-      </c>
-      <c r="I38" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>209</v>
+        <v>178</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -2669,53 +2648,53 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F40" t="s">
         <v>94</v>
       </c>
-      <c r="B40" t="s">
-        <v>180</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F40" t="s">
-        <v>14</v>
-      </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F41" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="G41" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
+        <v>182</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F42" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" t="s">
         <v>98</v>
-      </c>
-      <c r="B42" t="s">
-        <v>183</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F42" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -2723,95 +2702,95 @@
         <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F43" t="s">
         <v>315</v>
       </c>
-      <c r="F43" t="s">
-        <v>70</v>
-      </c>
       <c r="G43" t="s">
-        <v>100</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>316</v>
+        <v>257</v>
       </c>
       <c r="F44" t="s">
-        <v>321</v>
+        <v>17</v>
       </c>
       <c r="G44" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>260</v>
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>258</v>
       </c>
       <c r="F45" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="G45" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" t="s">
-        <v>261</v>
+        <v>184</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="F46" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="G46" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>186</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>262</v>
+        <v>185</v>
+      </c>
+      <c r="E47" t="s">
+        <v>260</v>
       </c>
       <c r="F47" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>212</v>
       </c>
       <c r="B48" t="s">
-        <v>187</v>
-      </c>
-      <c r="E48" t="s">
-        <v>263</v>
+        <v>30</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="F48" t="s">
         <v>54</v>
@@ -2822,189 +2801,186 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>214</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F49" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G49" t="s">
-        <v>57</v>
+        <v>19</v>
+      </c>
+      <c r="H49" t="s">
+        <v>321</v>
+      </c>
+      <c r="I49" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F50" t="s">
-        <v>42</v>
+        <v>320</v>
       </c>
       <c r="G50" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" t="s">
-        <v>327</v>
-      </c>
-      <c r="I50" t="s">
-        <v>323</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" t="s">
         <v>107</v>
       </c>
-      <c r="B51" t="s">
-        <v>43</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F51" t="s">
-        <v>326</v>
+        <v>108</v>
       </c>
       <c r="G51" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F52" t="s">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="G52" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F53" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G53" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F54" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="G54" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>188</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F55" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G55" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>344</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>271</v>
+        <v>41</v>
       </c>
       <c r="F56" t="s">
-        <v>79</v>
+        <v>320</v>
       </c>
       <c r="G56" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G57" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F58" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G58" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="F59" t="s">
         <v>17</v>
@@ -3015,138 +2991,138 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G60" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F61" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G61" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F63" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F64" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="G64" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F65" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G65" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H65" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I65" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F66" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F67" t="s">
         <v>17</v>
@@ -3157,98 +3133,98 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F68" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G68" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B69" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B70" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F70" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F71" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F72" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G72" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F73" t="s">
         <v>14</v>
@@ -3259,172 +3235,172 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F74" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G74" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F75" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G75" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F76" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F77" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G77" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G78" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F79" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G79" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B80" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="F80" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F81" t="s">
-        <v>42</v>
+        <v>320</v>
       </c>
       <c r="G81" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H81" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="I81" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F82" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G82" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B83" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -3435,219 +3411,225 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C84" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F84" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G84" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I84" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B85" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C85" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="F85" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G85" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B86" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G86" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B87" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F87" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G87" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>318</v>
+        <v>148</v>
       </c>
       <c r="B88" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="F88" t="s">
-        <v>326</v>
+        <v>47</v>
       </c>
       <c r="G88" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B89" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F89" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="G89" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="B90" t="s">
-        <v>203</v>
+        <v>39</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F90" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="G90" t="s">
-        <v>61</v>
+        <v>19</v>
+      </c>
+      <c r="H90" t="s">
+        <v>321</v>
+      </c>
+      <c r="I90" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
       <c r="B91" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F91" t="s">
-        <v>42</v>
+        <v>315</v>
       </c>
       <c r="G91" t="s">
-        <v>21</v>
-      </c>
-      <c r="H91" t="s">
-        <v>327</v>
-      </c>
-      <c r="I91" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="B92" t="s">
-        <v>140</v>
+        <v>339</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="F92" t="s">
-        <v>321</v>
+        <v>34</v>
       </c>
       <c r="G92" t="s">
-        <v>322</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B93" t="s">
-        <v>345</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>346</v>
+        <v>215</v>
+      </c>
+      <c r="E93" t="s">
+        <v>298</v>
       </c>
       <c r="F93" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="G93" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>216</v>
+        <v>150</v>
       </c>
       <c r="B94" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="E94" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F94" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="G94" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>151</v>
+      </c>
+      <c r="B95" t="s">
         <v>152</v>
       </c>
-      <c r="B95" t="s">
-        <v>204</v>
-      </c>
-      <c r="E95" t="s">
-        <v>302</v>
+      <c r="E95" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="F95" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G95" t="s">
-        <v>57</v>
+        <v>19</v>
+      </c>
+      <c r="H95" t="s">
+        <v>79</v>
+      </c>
+      <c r="I95" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -3655,310 +3637,287 @@
         <v>153</v>
       </c>
       <c r="B96" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="F96" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G96" t="s">
-        <v>21</v>
-      </c>
-      <c r="H96" t="s">
-        <v>81</v>
-      </c>
-      <c r="I96" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B97" t="s">
-        <v>193</v>
+        <v>125</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>314</v>
       </c>
       <c r="F97" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G97" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>155</v>
+      </c>
+      <c r="B98" t="s">
         <v>156</v>
       </c>
-      <c r="B98" t="s">
-        <v>127</v>
-      </c>
       <c r="E98" s="1" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="F98" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="G98" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>157</v>
+        <v>216</v>
       </c>
       <c r="B99" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F99" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="G99" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>218</v>
+        <v>157</v>
       </c>
       <c r="B100" t="s">
-        <v>34</v>
+        <v>203</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F100" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="G100" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="B101" t="s">
-        <v>205</v>
+        <v>9</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F101" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G101" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>215</v>
+        <v>318</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="F102" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G102" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>324</v>
+        <v>158</v>
       </c>
       <c r="B103" t="s">
-        <v>34</v>
+        <v>189</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="F103" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G103" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H103" t="s">
+        <v>159</v>
+      </c>
+      <c r="I103" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B104" t="s">
-        <v>191</v>
+        <v>41</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F104" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G104" t="s">
-        <v>21</v>
-      </c>
-      <c r="H104" t="s">
-        <v>161</v>
-      </c>
-      <c r="I104" t="s">
-        <v>162</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="B105" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F105" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G105" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="H105" t="s">
+        <v>22</v>
+      </c>
+      <c r="I105" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="B106" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F106" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G106" t="s">
-        <v>21</v>
-      </c>
-      <c r="H106" t="s">
-        <v>24</v>
-      </c>
-      <c r="I106" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>164</v>
+        <v>330</v>
       </c>
       <c r="B107" t="s">
-        <v>206</v>
+        <v>331</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="F107" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="G107" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>336</v>
+        <v>163</v>
       </c>
       <c r="B108" t="s">
-        <v>337</v>
+        <v>164</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>340</v>
+        <v>309</v>
       </c>
       <c r="F108" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G108" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>165</v>
+        <v>218</v>
       </c>
       <c r="B109" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F109" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G109" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>220</v>
-      </c>
-      <c r="B110" t="s">
-        <v>43</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F110" t="s">
-        <v>42</v>
-      </c>
-      <c r="G110" t="s">
-        <v>21</v>
-      </c>
-      <c r="H110" t="s">
-        <v>327</v>
-      </c>
-      <c r="I110" t="s">
-        <v>323</v>
+        <v>19</v>
+      </c>
+      <c r="H109" t="s">
+        <v>321</v>
+      </c>
+      <c r="I109" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{0FF3DA65-AAFE-A544-B83F-3B8DBBA655D2}"/>
-    <hyperlink ref="E7" r:id="rId2" xr:uid="{D72FCA14-EA08-4749-BB11-D24B8A62C2FD}"/>
-    <hyperlink ref="E10" r:id="rId3" xr:uid="{E6DBC748-9C42-444A-9719-EDB7AD21ED31}"/>
-    <hyperlink ref="E11" r:id="rId4" xr:uid="{D72F2EFB-3573-5D41-9B63-CA5C8A903FE7}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
-    <hyperlink ref="E16" r:id="rId6" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
-    <hyperlink ref="E17" r:id="rId7" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
-    <hyperlink ref="E18" r:id="rId8" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
-    <hyperlink ref="E20" r:id="rId9" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
-    <hyperlink ref="E21" r:id="rId10" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
-    <hyperlink ref="E26" r:id="rId11" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
-    <hyperlink ref="E27" r:id="rId12" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
-    <hyperlink ref="E28" r:id="rId13" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
-    <hyperlink ref="E30" r:id="rId14" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
-    <hyperlink ref="E32" r:id="rId15" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
-    <hyperlink ref="E34" r:id="rId16" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
-    <hyperlink ref="E39" r:id="rId17" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
-    <hyperlink ref="E40" r:id="rId18" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
-    <hyperlink ref="E41" r:id="rId19" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
-    <hyperlink ref="E42" r:id="rId20" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
-    <hyperlink ref="E43" r:id="rId21" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
-    <hyperlink ref="E44" r:id="rId22" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
-    <hyperlink ref="E45" r:id="rId23" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
-    <hyperlink ref="E47" r:id="rId24" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E49" r:id="rId25" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E50" r:id="rId26" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E52" r:id="rId27" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E56" r:id="rId28" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{D72FCA14-EA08-4749-BB11-D24B8A62C2FD}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{E6DBC748-9C42-444A-9719-EDB7AD21ED31}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{D72F2EFB-3573-5D41-9B63-CA5C8A903FE7}"/>
+    <hyperlink ref="E14" r:id="rId5" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
+    <hyperlink ref="E15" r:id="rId6" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
+    <hyperlink ref="E16" r:id="rId7" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
+    <hyperlink ref="E17" r:id="rId8" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
+    <hyperlink ref="E19" r:id="rId9" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
+    <hyperlink ref="E20" r:id="rId10" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
+    <hyperlink ref="E25" r:id="rId11" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
+    <hyperlink ref="E26" r:id="rId12" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
+    <hyperlink ref="E27" r:id="rId13" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
+    <hyperlink ref="E29" r:id="rId14" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
+    <hyperlink ref="E31" r:id="rId15" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
+    <hyperlink ref="E33" r:id="rId16" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
+    <hyperlink ref="E38" r:id="rId17" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
+    <hyperlink ref="E39" r:id="rId18" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
+    <hyperlink ref="E40" r:id="rId19" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
+    <hyperlink ref="E41" r:id="rId20" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
+    <hyperlink ref="E42" r:id="rId21" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
+    <hyperlink ref="E43" r:id="rId22" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
+    <hyperlink ref="E44" r:id="rId23" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
+    <hyperlink ref="E46" r:id="rId24" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
+    <hyperlink ref="E48" r:id="rId25" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E49" r:id="rId26" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E51" r:id="rId27" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E55" r:id="rId28" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
     <hyperlink ref="E62" r:id="rId29" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
     <hyperlink ref="E58" r:id="rId30" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
     <hyperlink ref="E63" r:id="rId31" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
@@ -3969,7 +3928,7 @@
     <hyperlink ref="E60" r:id="rId36" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
     <hyperlink ref="E69" r:id="rId37" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
     <hyperlink ref="E70" r:id="rId38" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
-    <hyperlink ref="E24" r:id="rId39" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
+    <hyperlink ref="E23" r:id="rId39" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
     <hyperlink ref="E71" r:id="rId40" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
     <hyperlink ref="E72" r:id="rId41" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
     <hyperlink ref="E73" r:id="rId42" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
@@ -3982,50 +3941,48 @@
     <hyperlink ref="E82" r:id="rId49" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
     <hyperlink ref="E83" r:id="rId50" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
     <hyperlink ref="E84" r:id="rId51" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E89" r:id="rId52" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E91" r:id="rId53" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E96" r:id="rId54" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E98" r:id="rId55" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E99" r:id="rId56" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E100" r:id="rId57" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E101" r:id="rId58" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E102" r:id="rId59" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E104" r:id="rId60" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E105" r:id="rId61" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E107" r:id="rId62" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E109" r:id="rId63" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E110" r:id="rId64" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E55" r:id="rId65" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E88" r:id="rId52" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E90" r:id="rId53" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E95" r:id="rId54" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E97" r:id="rId55" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E98" r:id="rId56" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E99" r:id="rId57" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E100" r:id="rId58" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E101" r:id="rId59" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E103" r:id="rId60" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E104" r:id="rId61" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E106" r:id="rId62" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E108" r:id="rId63" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E109" r:id="rId64" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E54" r:id="rId65" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
     <hyperlink ref="E66" r:id="rId66" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E90" r:id="rId67" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E97" r:id="rId68" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
-    <hyperlink ref="E6" r:id="rId69" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
-    <hyperlink ref="E13" r:id="rId70" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
+    <hyperlink ref="E89" r:id="rId67" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E96" r:id="rId68" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E5" r:id="rId69" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
+    <hyperlink ref="E12" r:id="rId70" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
     <hyperlink ref="E57" r:id="rId71" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
-    <hyperlink ref="E8" r:id="rId72" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
-    <hyperlink ref="E12" r:id="rId73" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
+    <hyperlink ref="E7" r:id="rId72" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
+    <hyperlink ref="E11" r:id="rId73" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
     <hyperlink ref="E61" r:id="rId74" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E53" r:id="rId75" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E54" r:id="rId76" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
-    <hyperlink ref="E5" r:id="rId77" xr:uid="{42CB9E98-0AE9-7E45-B0F1-C1F2FBA53A31}"/>
-    <hyperlink ref="E9" r:id="rId78" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E51" r:id="rId79" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E64" r:id="rId80" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E92" r:id="rId81" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E106" r:id="rId82" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E22" r:id="rId83" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E78" r:id="rId84" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
-    <hyperlink ref="E4" r:id="rId85" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E88" r:id="rId86" xr:uid="{B18DAE31-D98B-3D46-B664-E3C64B43832B}"/>
-    <hyperlink ref="E103" r:id="rId87" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E25" r:id="rId88" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E80" r:id="rId89" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E87" r:id="rId90" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E108" r:id="rId91" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
-    <hyperlink ref="E23" r:id="rId92" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
-    <hyperlink ref="E59" r:id="rId93" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
-    <hyperlink ref="E93" r:id="rId94" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
-    <hyperlink ref="E85" r:id="rId95" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E52" r:id="rId75" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E53" r:id="rId76" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E8" r:id="rId77" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
+    <hyperlink ref="E50" r:id="rId78" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E64" r:id="rId79" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E91" r:id="rId80" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E105" r:id="rId81" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E21" r:id="rId82" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
+    <hyperlink ref="E78" r:id="rId83" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E4" r:id="rId84" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
+    <hyperlink ref="E102" r:id="rId85" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E24" r:id="rId86" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E80" r:id="rId87" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E87" r:id="rId88" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E107" r:id="rId89" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E22" r:id="rId90" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
+    <hyperlink ref="E59" r:id="rId91" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E92" r:id="rId92" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E85" r:id="rId93" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Coimbra-LIBPhys updates: change of emails for Fernandes, Henriques, Santos, Silva
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C73B5C79-8E29-E844-8D06-2A85A79861E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2134550C-5A68-BB45-838A-527E26E02DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="3720" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="5900" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -775,9 +775,6 @@
     <t>ryan.felkai@gmail.com</t>
   </si>
   <si>
-    <t>pancho@gian.fis.uc.pt</t>
-  </si>
-  <si>
     <t>paola.ferrario@dipc.org</t>
   </si>
   <si>
@@ -802,9 +799,6 @@
     <t>hauptman@iastate.edu</t>
   </si>
   <si>
-    <t>henriques@gian.fis.uc.pt</t>
-  </si>
-  <si>
     <t>viherbos@eln.upv.es</t>
   </si>
   <si>
@@ -919,18 +913,12 @@
     <t>filomena@gian.fis.uc.pt</t>
   </si>
   <si>
-    <t>jmf@gian.fis.uc.pt</t>
-  </si>
-  <si>
     <t>marc.seemann@dipc.org</t>
   </si>
   <si>
     <t>itay.shomroni@mail.huji.ac.il</t>
   </si>
   <si>
-    <t>psidonio@uc.pt</t>
-  </si>
-  <si>
     <t>ander.simon@dipc.org</t>
   </si>
   <si>
@@ -1067,6 +1055,18 @@
   </si>
   <si>
     <t>Marauri</t>
+  </si>
+  <si>
+    <t>pancho@uc.pt</t>
+  </si>
+  <si>
+    <t>henriques@uc.pt</t>
+  </si>
+  <si>
+    <t>jmf@uc.pt</t>
+  </si>
+  <si>
+    <t>pesilva@uc.pt</t>
   </si>
 </sst>
 </file>
@@ -1920,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD88"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1980,7 +1980,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
@@ -2068,7 +2068,7 @@
         <v>225</v>
       </c>
       <c r="F8" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -2159,10 +2159,10 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I13" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2281,7 +2281,7 @@
         <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>237</v>
@@ -2312,13 +2312,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
@@ -2338,7 +2338,7 @@
         <v>239</v>
       </c>
       <c r="F23" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G23" t="s">
         <v>19</v>
@@ -2346,13 +2346,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B24" t="s">
         <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -2429,10 +2429,10 @@
         <v>19</v>
       </c>
       <c r="H28" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I28" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2496,8 +2496,8 @@
       <c r="B32" t="s">
         <v>179</v>
       </c>
-      <c r="E32" t="s">
-        <v>247</v>
+      <c r="E32" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="F32" t="s">
         <v>77</v>
@@ -2514,7 +2514,7 @@
         <v>180</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F33" t="s">
         <v>40</v>
@@ -2537,7 +2537,7 @@
         <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F34" t="s">
         <v>84</v>
@@ -2554,7 +2554,7 @@
         <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
@@ -2577,7 +2577,7 @@
         <v>125</v>
       </c>
       <c r="E36" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F36" t="s">
         <v>17</v>
@@ -2597,7 +2597,7 @@
         <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F37" t="s">
         <v>40</v>
@@ -2620,7 +2620,7 @@
         <v>207</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -2637,7 +2637,7 @@
         <v>178</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -2654,7 +2654,7 @@
         <v>177</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F40" t="s">
         <v>94</v>
@@ -2671,7 +2671,7 @@
         <v>181</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>256</v>
+        <v>342</v>
       </c>
       <c r="F41" t="s">
         <v>77</v>
@@ -2688,7 +2688,7 @@
         <v>182</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F42" t="s">
         <v>68</v>
@@ -2705,13 +2705,13 @@
         <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F43" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G43" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -2722,7 +2722,7 @@
         <v>183</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F44" t="s">
         <v>17</v>
@@ -2739,7 +2739,7 @@
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F45" t="s">
         <v>68</v>
@@ -2756,7 +2756,7 @@
         <v>184</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F46" t="s">
         <v>24</v>
@@ -2773,7 +2773,7 @@
         <v>185</v>
       </c>
       <c r="E47" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F47" t="s">
         <v>52</v>
@@ -2790,7 +2790,7 @@
         <v>30</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F48" t="s">
         <v>54</v>
@@ -2807,7 +2807,7 @@
         <v>57</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F49" t="s">
         <v>40</v>
@@ -2816,10 +2816,10 @@
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I49" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -2830,10 +2830,10 @@
         <v>41</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F50" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -2847,7 +2847,7 @@
         <v>107</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F51" t="s">
         <v>108</v>
@@ -2864,7 +2864,7 @@
         <v>30</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F52" t="s">
         <v>40</v>
@@ -2881,7 +2881,7 @@
         <v>187</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F53" t="s">
         <v>54</v>
@@ -2898,7 +2898,7 @@
         <v>90</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F54" t="s">
         <v>84</v>
@@ -2915,7 +2915,7 @@
         <v>188</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F55" t="s">
         <v>77</v>
@@ -2926,13 +2926,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B56" t="s">
         <v>41</v>
       </c>
       <c r="F56" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G56" t="s">
         <v>19</v>
@@ -2946,7 +2946,7 @@
         <v>115</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F57" t="s">
         <v>47</v>
@@ -2963,7 +2963,7 @@
         <v>189</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F58" t="s">
         <v>54</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B59" t="s">
         <v>41</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F59" t="s">
         <v>17</v>
@@ -2997,7 +2997,7 @@
         <v>190</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F60" t="s">
         <v>24</v>
@@ -3014,7 +3014,7 @@
         <v>191</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F61" t="s">
         <v>40</v>
@@ -3031,7 +3031,7 @@
         <v>121</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F62" t="s">
         <v>84</v>
@@ -3048,7 +3048,7 @@
         <v>123</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F63" t="s">
         <v>52</v>
@@ -3065,10 +3065,10 @@
         <v>125</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F64" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G64" t="s">
         <v>19</v>
@@ -3082,7 +3082,7 @@
         <v>192</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F65" t="s">
         <v>40</v>
@@ -3105,7 +3105,7 @@
         <v>193</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F66" t="s">
         <v>77</v>
@@ -3122,7 +3122,7 @@
         <v>194</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F67" t="s">
         <v>17</v>
@@ -3139,7 +3139,7 @@
         <v>130</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F68" t="s">
         <v>52</v>
@@ -3156,7 +3156,7 @@
         <v>195</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F69" t="s">
         <v>54</v>
@@ -3173,7 +3173,7 @@
         <v>196</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F70" t="s">
         <v>52</v>
@@ -3190,7 +3190,7 @@
         <v>66</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F71" t="s">
         <v>40</v>
@@ -3207,7 +3207,7 @@
         <v>125</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F72" t="s">
         <v>42</v>
@@ -3224,7 +3224,7 @@
         <v>197</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F73" t="s">
         <v>14</v>
@@ -3241,7 +3241,7 @@
         <v>198</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F74" t="s">
         <v>108</v>
@@ -3258,7 +3258,7 @@
         <v>138</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F75" t="s">
         <v>52</v>
@@ -3275,7 +3275,7 @@
         <v>41</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F76" t="s">
         <v>22</v>
@@ -3292,7 +3292,7 @@
         <v>125</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F77" t="s">
         <v>40</v>
@@ -3309,7 +3309,7 @@
         <v>39</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F78" t="s">
         <v>68</v>
@@ -3326,7 +3326,7 @@
         <v>191</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F79" t="s">
         <v>54</v>
@@ -3343,7 +3343,7 @@
         <v>189</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F80" t="s">
         <v>54</v>
@@ -3360,10 +3360,10 @@
         <v>138</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F81" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G81" t="s">
         <v>19</v>
@@ -3383,7 +3383,7 @@
         <v>9</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F82" t="s">
         <v>50</v>
@@ -3400,7 +3400,7 @@
         <v>186</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -3417,10 +3417,10 @@
         <v>197</v>
       </c>
       <c r="C84" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F84" t="s">
         <v>40</v>
@@ -3440,10 +3440,10 @@
         <v>199</v>
       </c>
       <c r="C85" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F85" t="s">
         <v>54</v>
@@ -3454,7 +3454,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B86" t="s">
         <v>66</v>
@@ -3469,13 +3469,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B87" t="s">
+        <v>325</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="F87" t="s">
         <v>54</v>
@@ -3492,7 +3492,7 @@
         <v>200</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F88" t="s">
         <v>47</v>
@@ -3509,7 +3509,7 @@
         <v>201</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>295</v>
+        <v>343</v>
       </c>
       <c r="F89" t="s">
         <v>77</v>
@@ -3526,7 +3526,7 @@
         <v>39</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F90" t="s">
         <v>40</v>
@@ -3535,10 +3535,10 @@
         <v>19</v>
       </c>
       <c r="H90" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I90" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3549,13 +3549,13 @@
         <v>138</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F91" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G91" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3563,10 +3563,10 @@
         <v>214</v>
       </c>
       <c r="B92" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F92" t="s">
         <v>34</v>
@@ -3582,8 +3582,8 @@
       <c r="B93" t="s">
         <v>215</v>
       </c>
-      <c r="E93" t="s">
-        <v>298</v>
+      <c r="E93" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="F93" t="s">
         <v>77</v>
@@ -3600,7 +3600,7 @@
         <v>202</v>
       </c>
       <c r="E94" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F94" t="s">
         <v>54</v>
@@ -3617,7 +3617,7 @@
         <v>152</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F95" t="s">
         <v>40</v>
@@ -3640,7 +3640,7 @@
         <v>191</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F96" t="s">
         <v>54</v>
@@ -3657,7 +3657,7 @@
         <v>125</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F97" t="s">
         <v>54</v>
@@ -3674,7 +3674,7 @@
         <v>156</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F98" t="s">
         <v>77</v>
@@ -3691,7 +3691,7 @@
         <v>32</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F99" t="s">
         <v>54</v>
@@ -3708,7 +3708,7 @@
         <v>203</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F100" t="s">
         <v>17</v>
@@ -3725,7 +3725,7 @@
         <v>9</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F101" t="s">
         <v>40</v>
@@ -3736,13 +3736,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B102" t="s">
         <v>32</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F102" t="s">
         <v>40</v>
@@ -3759,7 +3759,7 @@
         <v>189</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F103" t="s">
         <v>40</v>
@@ -3782,7 +3782,7 @@
         <v>41</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F104" t="s">
         <v>14</v>
@@ -3799,7 +3799,7 @@
         <v>210</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F105" t="s">
         <v>40</v>
@@ -3822,7 +3822,7 @@
         <v>204</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F106" t="s">
         <v>34</v>
@@ -3833,13 +3833,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>326</v>
+      </c>
+      <c r="B107" t="s">
+        <v>327</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="B107" t="s">
-        <v>331</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>334</v>
       </c>
       <c r="F107" t="s">
         <v>54</v>
@@ -3856,7 +3856,7 @@
         <v>164</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F108" t="s">
         <v>14</v>
@@ -3873,7 +3873,7 @@
         <v>41</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F109" t="s">
         <v>40</v>
@@ -3882,10 +3882,10 @@
         <v>19</v>
       </c>
       <c r="H109" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I109" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3983,6 +3983,8 @@
     <hyperlink ref="E59" r:id="rId91" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
     <hyperlink ref="E92" r:id="rId92" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
     <hyperlink ref="E85" r:id="rId93" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E32" r:id="rId94" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
+    <hyperlink ref="E93" r:id="rId95" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
DIPC updates 2: footnote added to Ferrario
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2134550C-5A68-BB45-838A-527E26E02DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D433FDF-98AE-824B-A02E-171B7226D3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="5900" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="346">
   <si>
     <t>LastName</t>
   </si>
@@ -256,9 +256,6 @@
     <t xml:space="preserve">Felkai                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> Now at Weizmann Institute of Science, Israel.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Beer-Sheva, 8410501, Israel </t>
   </si>
   <si>
@@ -1067,6 +1064,12 @@
   </si>
   <si>
     <t>pesilva@uc.pt</t>
+  </si>
+  <si>
+    <t>Now at Weizmann Institute of Science, Israel.</t>
+  </si>
+  <si>
+    <t>On leave.</t>
   </si>
 </sst>
 </file>
@@ -1920,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1940,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1963,7 +1966,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1980,7 +1983,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
@@ -1994,10 +1997,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2014,7 +2017,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F5" t="s">
         <v>40</v>
@@ -2028,10 +2031,10 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -2045,10 +2048,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -2065,10 +2068,10 @@
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -2082,7 +2085,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F9" t="s">
         <v>54</v>
@@ -2096,10 +2099,10 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
@@ -2113,10 +2116,10 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2130,10 +2133,10 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -2150,7 +2153,7 @@
         <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F13" t="s">
         <v>40</v>
@@ -2159,10 +2162,10 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2173,7 +2176,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F14" t="s">
         <v>40</v>
@@ -2187,10 +2190,10 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F15" t="s">
         <v>47</v>
@@ -2207,7 +2210,7 @@
         <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F16" t="s">
         <v>40</v>
@@ -2227,10 +2230,10 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F17" t="s">
         <v>52</v>
@@ -2241,13 +2244,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F18" t="s">
         <v>40</v>
@@ -2261,10 +2264,10 @@
         <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F19" t="s">
         <v>27</v>
@@ -2278,13 +2281,13 @@
         <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F20" t="s">
         <v>47</v>
@@ -2298,10 +2301,10 @@
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F21" t="s">
         <v>61</v>
@@ -2312,13 +2315,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
@@ -2335,10 +2338,10 @@
         <v>64</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G23" t="s">
         <v>19</v>
@@ -2346,13 +2349,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>320</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -2369,7 +2372,7 @@
         <v>66</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F25" t="s">
         <v>52</v>
@@ -2383,10 +2386,10 @@
         <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F26" t="s">
         <v>68</v>
@@ -2397,13 +2400,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F27" t="s">
         <v>40</v>
@@ -2420,7 +2423,7 @@
         <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F28" t="s">
         <v>40</v>
@@ -2429,10 +2432,10 @@
         <v>19</v>
       </c>
       <c r="H28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2440,10 +2443,10 @@
         <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F29" t="s">
         <v>47</v>
@@ -2457,10 +2460,10 @@
         <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F30" t="s">
         <v>17</v>
@@ -2474,33 +2477,33 @@
         <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>344</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F31" t="s">
         <v>24</v>
       </c>
       <c r="G31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F32" t="s">
         <v>76</v>
-      </c>
-      <c r="B32" t="s">
-        <v>179</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F32" t="s">
-        <v>77</v>
       </c>
       <c r="G32" t="s">
         <v>59</v>
@@ -2508,13 +2511,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>180</v>
+        <v>179</v>
+      </c>
+      <c r="C33" t="s">
+        <v>345</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F33" t="s">
         <v>40</v>
@@ -2523,24 +2529,24 @@
         <v>19</v>
       </c>
       <c r="H33" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" t="s">
         <v>79</v>
-      </c>
-      <c r="I33" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
         <v>82</v>
       </c>
-      <c r="B34" t="s">
+      <c r="E34" t="s">
+        <v>247</v>
+      </c>
+      <c r="F34" t="s">
         <v>83</v>
-      </c>
-      <c r="E34" t="s">
-        <v>248</v>
-      </c>
-      <c r="F34" t="s">
-        <v>84</v>
       </c>
       <c r="G34" t="s">
         <v>53</v>
@@ -2548,13 +2554,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
         <v>85</v>
       </c>
-      <c r="B35" t="s">
-        <v>86</v>
-      </c>
       <c r="E35" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
@@ -2563,21 +2569,21 @@
         <v>19</v>
       </c>
       <c r="H35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I35" t="s">
         <v>79</v>
-      </c>
-      <c r="I35" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F36" t="s">
         <v>17</v>
@@ -2588,16 +2594,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
         <v>87</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>88</v>
       </c>
-      <c r="C37" t="s">
-        <v>89</v>
-      </c>
       <c r="E37" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F37" t="s">
         <v>40</v>
@@ -2606,21 +2612,21 @@
         <v>19</v>
       </c>
       <c r="H37" t="s">
+        <v>78</v>
+      </c>
+      <c r="I37" t="s">
         <v>79</v>
-      </c>
-      <c r="I37" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -2631,13 +2637,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -2648,33 +2654,33 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F40" t="s">
         <v>93</v>
       </c>
-      <c r="B40" t="s">
-        <v>177</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>94</v>
-      </c>
-      <c r="G40" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G41" t="s">
         <v>59</v>
@@ -2682,47 +2688,47 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F42" t="s">
         <v>68</v>
       </c>
       <c r="G42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F43" t="s">
+        <v>310</v>
+      </c>
+      <c r="G43" t="s">
         <v>311</v>
-      </c>
-      <c r="G43" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F44" t="s">
         <v>17</v>
@@ -2733,47 +2739,47 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F45" t="s">
         <v>68</v>
       </c>
       <c r="G45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F46" t="s">
         <v>24</v>
       </c>
       <c r="G46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E47" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F47" t="s">
         <v>52</v>
@@ -2784,13 +2790,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
         <v>30</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F48" t="s">
         <v>54</v>
@@ -2801,13 +2807,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F49" t="s">
         <v>40</v>
@@ -2816,24 +2822,24 @@
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -2841,30 +2847,30 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
         <v>106</v>
       </c>
-      <c r="B51" t="s">
+      <c r="E51" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F51" t="s">
         <v>107</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>108</v>
-      </c>
-      <c r="G51" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
         <v>30</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F52" t="s">
         <v>40</v>
@@ -2875,13 +2881,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F53" t="s">
         <v>54</v>
@@ -2892,16 +2898,16 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G54" t="s">
         <v>53</v>
@@ -2909,16 +2915,16 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G55" t="s">
         <v>59</v>
@@ -2926,13 +2932,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B56" t="s">
         <v>41</v>
       </c>
       <c r="F56" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G56" t="s">
         <v>19</v>
@@ -2940,13 +2946,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
         <v>114</v>
       </c>
-      <c r="B57" t="s">
-        <v>115</v>
-      </c>
       <c r="E57" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F57" t="s">
         <v>47</v>
@@ -2957,30 +2963,30 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F58" t="s">
         <v>54</v>
       </c>
       <c r="G58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B59" t="s">
         <v>41</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F59" t="s">
         <v>17</v>
@@ -2991,13 +2997,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F60" t="s">
         <v>24</v>
@@ -3008,13 +3014,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F61" t="s">
         <v>40</v>
@@ -3025,16 +3031,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" t="s">
         <v>120</v>
       </c>
-      <c r="B62" t="s">
-        <v>121</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G62" t="s">
         <v>53</v>
@@ -3042,13 +3048,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" t="s">
         <v>122</v>
       </c>
-      <c r="B63" t="s">
-        <v>123</v>
-      </c>
       <c r="E63" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F63" t="s">
         <v>52</v>
@@ -3059,16 +3065,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" t="s">
         <v>124</v>
       </c>
-      <c r="B64" t="s">
-        <v>125</v>
-      </c>
       <c r="E64" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F64" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G64" t="s">
         <v>19</v>
@@ -3076,13 +3082,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F65" t="s">
         <v>40</v>
@@ -3091,24 +3097,24 @@
         <v>19</v>
       </c>
       <c r="H65" t="s">
+        <v>78</v>
+      </c>
+      <c r="I65" t="s">
         <v>79</v>
-      </c>
-      <c r="I65" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G66" t="s">
         <v>59</v>
@@ -3116,13 +3122,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B67" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F67" t="s">
         <v>17</v>
@@ -3133,13 +3139,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" t="s">
         <v>129</v>
       </c>
-      <c r="B68" t="s">
-        <v>130</v>
-      </c>
       <c r="E68" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F68" t="s">
         <v>52</v>
@@ -3150,13 +3156,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F69" t="s">
         <v>54</v>
@@ -3167,13 +3173,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F70" t="s">
         <v>52</v>
@@ -3184,13 +3190,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" t="s">
         <v>66</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F71" t="s">
         <v>40</v>
@@ -3201,13 +3207,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B72" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F72" t="s">
         <v>42</v>
@@ -3218,13 +3224,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F73" t="s">
         <v>14</v>
@@ -3235,30 +3241,30 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F74" t="s">
+        <v>107</v>
+      </c>
+      <c r="G74" t="s">
         <v>108</v>
-      </c>
-      <c r="G74" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75" t="s">
         <v>137</v>
       </c>
-      <c r="B75" t="s">
-        <v>138</v>
-      </c>
       <c r="E75" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F75" t="s">
         <v>52</v>
@@ -3269,13 +3275,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B76" t="s">
         <v>41</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F76" t="s">
         <v>22</v>
@@ -3286,13 +3292,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F77" t="s">
         <v>40</v>
@@ -3303,30 +3309,30 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B78" t="s">
         <v>39</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F78" t="s">
         <v>68</v>
       </c>
       <c r="G78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B79" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F79" t="s">
         <v>54</v>
@@ -3337,13 +3343,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B80" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F80" t="s">
         <v>54</v>
@@ -3354,16 +3360,16 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B81" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F81" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G81" t="s">
         <v>19</v>
@@ -3377,13 +3383,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F82" t="s">
         <v>50</v>
@@ -3394,13 +3400,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -3411,16 +3417,16 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B84" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C84" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F84" t="s">
         <v>40</v>
@@ -3434,16 +3440,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C85" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F85" t="s">
         <v>54</v>
@@ -3454,7 +3460,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B86" t="s">
         <v>66</v>
@@ -3469,13 +3475,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>323</v>
+      </c>
+      <c r="B87" t="s">
         <v>324</v>
       </c>
-      <c r="B87" t="s">
-        <v>325</v>
-      </c>
       <c r="E87" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F87" t="s">
         <v>54</v>
@@ -3486,13 +3492,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F88" t="s">
         <v>47</v>
@@ -3503,16 +3509,16 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F89" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G89" t="s">
         <v>59</v>
@@ -3520,13 +3526,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B90" t="s">
         <v>39</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F90" t="s">
         <v>40</v>
@@ -3535,38 +3541,38 @@
         <v>19</v>
       </c>
       <c r="H90" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I90" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B91" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F91" t="s">
+        <v>310</v>
+      </c>
+      <c r="G91" t="s">
         <v>311</v>
-      </c>
-      <c r="G91" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B92" t="s">
+        <v>334</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="F92" t="s">
         <v>34</v>
@@ -3577,16 +3583,16 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>213</v>
+      </c>
+      <c r="B93" t="s">
         <v>214</v>
       </c>
-      <c r="B93" t="s">
-        <v>215</v>
-      </c>
       <c r="E93" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G93" t="s">
         <v>59</v>
@@ -3594,13 +3600,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B94" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E94" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F94" t="s">
         <v>54</v>
@@ -3611,13 +3617,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>150</v>
+      </c>
+      <c r="B95" t="s">
         <v>151</v>
       </c>
-      <c r="B95" t="s">
-        <v>152</v>
-      </c>
       <c r="E95" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F95" t="s">
         <v>40</v>
@@ -3626,21 +3632,21 @@
         <v>19</v>
       </c>
       <c r="H95" t="s">
+        <v>78</v>
+      </c>
+      <c r="I95" t="s">
         <v>79</v>
-      </c>
-      <c r="I95" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F96" t="s">
         <v>54</v>
@@ -3651,13 +3657,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F97" t="s">
         <v>54</v>
@@ -3668,16 +3674,16 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" t="s">
         <v>155</v>
       </c>
-      <c r="B98" t="s">
-        <v>156</v>
-      </c>
       <c r="E98" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G98" t="s">
         <v>59</v>
@@ -3685,13 +3691,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B99" t="s">
         <v>32</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F99" t="s">
         <v>54</v>
@@ -3702,13 +3708,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B100" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F100" t="s">
         <v>17</v>
@@ -3719,13 +3725,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F101" t="s">
         <v>40</v>
@@ -3736,13 +3742,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B102" t="s">
         <v>32</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F102" t="s">
         <v>40</v>
@@ -3753,13 +3759,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B103" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F103" t="s">
         <v>40</v>
@@ -3768,21 +3774,21 @@
         <v>19</v>
       </c>
       <c r="H103" t="s">
+        <v>158</v>
+      </c>
+      <c r="I103" t="s">
         <v>159</v>
-      </c>
-      <c r="I103" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B104" t="s">
         <v>41</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F104" t="s">
         <v>14</v>
@@ -3793,13 +3799,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
         <v>209</v>
       </c>
-      <c r="B105" t="s">
-        <v>210</v>
-      </c>
       <c r="E105" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F105" t="s">
         <v>40</v>
@@ -3816,30 +3822,30 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B106" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F106" t="s">
         <v>34</v>
       </c>
       <c r="G106" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>325</v>
+      </c>
+      <c r="B107" t="s">
         <v>326</v>
       </c>
-      <c r="B107" t="s">
-        <v>327</v>
-      </c>
       <c r="E107" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F107" t="s">
         <v>54</v>
@@ -3850,13 +3856,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>162</v>
+      </c>
+      <c r="B108" t="s">
         <v>163</v>
       </c>
-      <c r="B108" t="s">
-        <v>164</v>
-      </c>
       <c r="E108" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F108" t="s">
         <v>14</v>
@@ -3867,13 +3873,13 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B109" t="s">
         <v>41</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F109" t="s">
         <v>40</v>
@@ -3882,10 +3888,10 @@
         <v>19</v>
       </c>
       <c r="H109" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I109" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LSC updates 2: add email for ruiz
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D433FDF-98AE-824B-A02E-171B7226D3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BF37228-2C3B-2948-BC0C-51DA306C8314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="5900" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4000" yWindow="3020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="347">
   <si>
     <t>LastName</t>
   </si>
@@ -1070,6 +1070,9 @@
   </si>
   <si>
     <t>On leave.</t>
+  </si>
+  <si>
+    <t>eruiz@lsc-canfranc.es</t>
   </si>
 </sst>
 </file>
@@ -1923,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3465,7 +3468,9 @@
       <c r="B86" t="s">
         <v>66</v>
       </c>
-      <c r="E86" s="1"/>
+      <c r="E86" s="1" t="s">
+        <v>346</v>
+      </c>
       <c r="F86" t="s">
         <v>42</v>
       </c>
@@ -3991,6 +3996,7 @@
     <hyperlink ref="E85" r:id="rId93" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
     <hyperlink ref="E32" r:id="rId94" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
     <hyperlink ref="E93" r:id="rId95" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
+    <hyperlink ref="E86" r:id="rId96" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IFIC update: change of email for Simon
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BF37228-2C3B-2948-BC0C-51DA306C8314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C5B98FD-E2A6-274E-B978-93DB70790410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="3020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -916,9 +916,6 @@
     <t>itay.shomroni@mail.huji.ac.il</t>
   </si>
   <si>
-    <t>ander.simon@dipc.org</t>
-  </si>
-  <si>
     <t>roberto.soleti@dipc.org</t>
   </si>
   <si>
@@ -1073,6 +1070,9 @@
   </si>
   <si>
     <t>eruiz@lsc-canfranc.es</t>
+  </si>
+  <si>
+    <t>ander.simon@ific.uv.es</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1927,7 @@
   <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1986,7 +1986,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
@@ -2074,7 +2074,7 @@
         <v>224</v>
       </c>
       <c r="F8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -2165,10 +2165,10 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2287,7 +2287,7 @@
         <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>236</v>
@@ -2318,13 +2318,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
@@ -2344,7 +2344,7 @@
         <v>238</v>
       </c>
       <c r="F23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G23" t="s">
         <v>19</v>
@@ -2352,13 +2352,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -2435,10 +2435,10 @@
         <v>19</v>
       </c>
       <c r="H28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2483,7 +2483,7 @@
         <v>177</v>
       </c>
       <c r="C31" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>245</v>
@@ -2503,7 +2503,7 @@
         <v>178</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F32" t="s">
         <v>76</v>
@@ -2520,7 +2520,7 @@
         <v>179</v>
       </c>
       <c r="C33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>246</v>
@@ -2680,7 +2680,7 @@
         <v>180</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F41" t="s">
         <v>76</v>
@@ -2697,7 +2697,7 @@
         <v>181</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F42" t="s">
         <v>68</v>
@@ -2714,13 +2714,13 @@
         <v>106</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F43" t="s">
+        <v>309</v>
+      </c>
+      <c r="G43" t="s">
         <v>310</v>
-      </c>
-      <c r="G43" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -2825,10 +2825,10 @@
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -2842,7 +2842,7 @@
         <v>260</v>
       </c>
       <c r="F50" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -2935,13 +2935,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B56" t="s">
         <v>41</v>
       </c>
       <c r="F56" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G56" t="s">
         <v>19</v>
@@ -2983,13 +2983,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B59" t="s">
         <v>41</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F59" t="s">
         <v>17</v>
@@ -3077,7 +3077,7 @@
         <v>272</v>
       </c>
       <c r="F64" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G64" t="s">
         <v>19</v>
@@ -3352,7 +3352,7 @@
         <v>188</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F80" t="s">
         <v>54</v>
@@ -3372,7 +3372,7 @@
         <v>288</v>
       </c>
       <c r="F81" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G81" t="s">
         <v>19</v>
@@ -3409,7 +3409,7 @@
         <v>185</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -3426,7 +3426,7 @@
         <v>196</v>
       </c>
       <c r="C84" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>290</v>
@@ -3449,10 +3449,10 @@
         <v>198</v>
       </c>
       <c r="C85" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F85" t="s">
         <v>54</v>
@@ -3463,13 +3463,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B86" t="s">
         <v>66</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F86" t="s">
         <v>42</v>
@@ -3480,13 +3480,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>322</v>
+      </c>
+      <c r="B87" t="s">
         <v>323</v>
       </c>
-      <c r="B87" t="s">
-        <v>324</v>
-      </c>
       <c r="E87" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F87" t="s">
         <v>54</v>
@@ -3520,7 +3520,7 @@
         <v>200</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F89" t="s">
         <v>76</v>
@@ -3546,10 +3546,10 @@
         <v>19</v>
       </c>
       <c r="H90" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I90" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3563,10 +3563,10 @@
         <v>293</v>
       </c>
       <c r="F91" t="s">
+        <v>309</v>
+      </c>
+      <c r="G91" t="s">
         <v>310</v>
-      </c>
-      <c r="G91" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3574,10 +3574,10 @@
         <v>213</v>
       </c>
       <c r="B92" t="s">
+        <v>333</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>335</v>
       </c>
       <c r="F92" t="s">
         <v>34</v>
@@ -3594,7 +3594,7 @@
         <v>214</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F93" t="s">
         <v>76</v>
@@ -3610,8 +3610,8 @@
       <c r="B94" t="s">
         <v>201</v>
       </c>
-      <c r="E94" t="s">
-        <v>294</v>
+      <c r="E94" s="1" t="s">
+        <v>346</v>
       </c>
       <c r="F94" t="s">
         <v>54</v>
@@ -3628,7 +3628,7 @@
         <v>151</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F95" t="s">
         <v>40</v>
@@ -3651,7 +3651,7 @@
         <v>190</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F96" t="s">
         <v>54</v>
@@ -3668,7 +3668,7 @@
         <v>124</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F97" t="s">
         <v>54</v>
@@ -3685,7 +3685,7 @@
         <v>155</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F98" t="s">
         <v>76</v>
@@ -3702,7 +3702,7 @@
         <v>32</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F99" t="s">
         <v>54</v>
@@ -3719,7 +3719,7 @@
         <v>202</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F100" t="s">
         <v>17</v>
@@ -3736,7 +3736,7 @@
         <v>9</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F101" t="s">
         <v>40</v>
@@ -3747,13 +3747,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B102" t="s">
         <v>32</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F102" t="s">
         <v>40</v>
@@ -3770,7 +3770,7 @@
         <v>188</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F103" t="s">
         <v>40</v>
@@ -3793,7 +3793,7 @@
         <v>41</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F104" t="s">
         <v>14</v>
@@ -3810,7 +3810,7 @@
         <v>209</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F105" t="s">
         <v>40</v>
@@ -3833,7 +3833,7 @@
         <v>203</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F106" t="s">
         <v>34</v>
@@ -3844,13 +3844,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>324</v>
+      </c>
+      <c r="B107" t="s">
         <v>325</v>
       </c>
-      <c r="B107" t="s">
-        <v>326</v>
-      </c>
       <c r="E107" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F107" t="s">
         <v>54</v>
@@ -3867,7 +3867,7 @@
         <v>163</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F108" t="s">
         <v>14</v>
@@ -3884,7 +3884,7 @@
         <v>41</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F109" t="s">
         <v>40</v>
@@ -3893,10 +3893,10 @@
         <v>19</v>
       </c>
       <c r="H109" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I109" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -3997,6 +3997,7 @@
     <hyperlink ref="E32" r:id="rId94" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
     <hyperlink ref="E93" r:id="rId95" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
     <hyperlink ref="E86" r:id="rId96" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
+    <hyperlink ref="E94" r:id="rId97" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UPV/EHU Organic Chemistry update: add email for Marauri
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C5B98FD-E2A6-274E-B978-93DB70790410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1552DF8D-F8EE-A24A-ACAF-71FBFCE9F603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="3020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="348">
   <si>
     <t>LastName</t>
   </si>
@@ -1073,6 +1073,9 @@
   </si>
   <si>
     <t>ander.simon@ific.uv.es</t>
+  </si>
+  <si>
+    <t>aimar.marauri@ehu.eus</t>
   </si>
 </sst>
 </file>
@@ -1926,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2939,6 +2942,9 @@
       </c>
       <c r="B56" t="s">
         <v>41</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="F56" t="s">
         <v>314</v>
@@ -3998,6 +4004,7 @@
     <hyperlink ref="E93" r:id="rId95" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
     <hyperlink ref="E86" r:id="rId96" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
     <hyperlink ref="E94" r:id="rId97" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
+    <hyperlink ref="E56" r:id="rId98" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
DIPC and IFIC updates: Barcelon and Dietz in; change of affiliation for Martinez-Vara
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1552DF8D-F8EE-A24A-ACAF-71FBFCE9F603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4591044-C71C-E142-8C2E-6B67B17F878F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="3020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14260" yWindow="2900" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="353">
   <si>
     <t>LastName</t>
   </si>
@@ -1076,6 +1076,21 @@
   </si>
   <si>
     <t>aimar.marauri@ehu.eus</t>
+  </si>
+  <si>
+    <t>Dietz</t>
+  </si>
+  <si>
+    <t>pablo.dietz@dipc.org</t>
+  </si>
+  <si>
+    <t>Barcelon</t>
+  </si>
+  <si>
+    <t>J.E.</t>
+  </si>
+  <si>
+    <t>joseeduardo.barcelon@dipc.org</t>
   </si>
 </sst>
 </file>
@@ -1927,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2153,13 +2168,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>350</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>229</v>
+        <v>351</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="F13" t="s">
         <v>40</v>
@@ -2167,22 +2182,16 @@
       <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="H13" t="s">
-        <v>315</v>
-      </c>
-      <c r="I13" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>230</v>
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>229</v>
       </c>
       <c r="F14" t="s">
         <v>40</v>
@@ -2190,246 +2199,252 @@
       <c r="G14" t="s">
         <v>19</v>
       </c>
+      <c r="H14" t="s">
+        <v>315</v>
+      </c>
+      <c r="I14" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E18" t="s">
-        <v>234</v>
+        <v>166</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>235</v>
+        <v>201</v>
+      </c>
+      <c r="E19" t="s">
+        <v>234</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" t="s">
-        <v>317</v>
+        <v>174</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
+        <v>165</v>
+      </c>
+      <c r="C21" t="s">
+        <v>317</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>326</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>329</v>
+        <v>237</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>326</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>238</v>
+        <v>329</v>
       </c>
       <c r="F23" t="s">
-        <v>314</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>319</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>320</v>
+        <v>238</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>314</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>319</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>239</v>
+        <v>320</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>66</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>205</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F27" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="G27" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>348</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" t="s">
-        <v>242</v>
+        <v>323</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="F28" t="s">
         <v>40</v>
@@ -2437,139 +2452,133 @@
       <c r="G28" t="s">
         <v>19</v>
       </c>
-      <c r="H28" t="s">
-        <v>315</v>
-      </c>
-      <c r="I28" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>205</v>
       </c>
       <c r="B29" t="s">
-        <v>176</v>
+        <v>9</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H30" t="s">
+        <v>315</v>
+      </c>
+      <c r="I30" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" t="s">
-        <v>343</v>
+        <v>176</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F31" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G31" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>339</v>
+        <v>177</v>
+      </c>
+      <c r="E32" t="s">
+        <v>244</v>
       </c>
       <c r="F32" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="G32" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F33" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" t="s">
-        <v>78</v>
-      </c>
-      <c r="I33" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" t="s">
-        <v>247</v>
+        <v>178</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="F34" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G34" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" t="s">
-        <v>248</v>
+        <v>179</v>
+      </c>
+      <c r="C35" t="s">
+        <v>344</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G35" t="s">
         <v>19</v>
@@ -2583,36 +2592,33 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="E36" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="G36" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E37" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F37" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G37" t="s">
         <v>19</v>
@@ -2626,260 +2632,269 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>216</v>
       </c>
       <c r="B38" t="s">
-        <v>206</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>251</v>
+        <v>124</v>
+      </c>
+      <c r="E38" t="s">
+        <v>249</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>177</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>252</v>
+        <v>87</v>
+      </c>
+      <c r="C39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" t="s">
+        <v>250</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="H39" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F40" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="G40" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>340</v>
+        <v>252</v>
       </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>306</v>
+        <v>253</v>
       </c>
       <c r="F42" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="G42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>180</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>307</v>
+        <v>340</v>
       </c>
       <c r="F43" t="s">
-        <v>309</v>
+        <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>310</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>254</v>
+        <v>306</v>
       </c>
       <c r="F44" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="G44" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" t="s">
-        <v>255</v>
+        <v>106</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="F45" t="s">
-        <v>68</v>
+        <v>309</v>
       </c>
       <c r="G45" t="s">
-        <v>97</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F46" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G46" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F47" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="G47" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>211</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>183</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F48" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="G48" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>259</v>
+        <v>184</v>
+      </c>
+      <c r="E49" t="s">
+        <v>257</v>
       </c>
       <c r="F49" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G49" t="s">
-        <v>19</v>
-      </c>
-      <c r="H49" t="s">
-        <v>315</v>
-      </c>
-      <c r="I49" t="s">
-        <v>311</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F50" t="s">
-        <v>314</v>
+        <v>54</v>
       </c>
       <c r="G50" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F51" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="G51" t="s">
-        <v>108</v>
+        <v>19</v>
+      </c>
+      <c r="H51" t="s">
+        <v>315</v>
+      </c>
+      <c r="I51" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F52" t="s">
-        <v>40</v>
+        <v>314</v>
       </c>
       <c r="G52" t="s">
         <v>19</v>
@@ -2887,84 +2902,84 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>186</v>
+        <v>106</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F53" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="G53" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F54" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="G54" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F55" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="G55" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>338</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>347</v>
+        <v>264</v>
       </c>
       <c r="F56" t="s">
-        <v>314</v>
+        <v>83</v>
       </c>
       <c r="G56" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>187</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F57" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="G57" t="s">
         <v>59</v>
@@ -2972,223 +2987,223 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>338</v>
       </c>
       <c r="B58" t="s">
-        <v>188</v>
+        <v>41</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>267</v>
+        <v>347</v>
       </c>
       <c r="F58" t="s">
-        <v>54</v>
+        <v>314</v>
       </c>
       <c r="G58" t="s">
-        <v>116</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>330</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>331</v>
+        <v>266</v>
       </c>
       <c r="F59" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="G59" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F60" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G60" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>330</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>269</v>
+        <v>331</v>
       </c>
       <c r="F61" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="G61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F62" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="G62" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F63" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G63" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F64" t="s">
-        <v>314</v>
+        <v>83</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B65" t="s">
-        <v>191</v>
+        <v>122</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F65" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G65" t="s">
-        <v>19</v>
-      </c>
-      <c r="H65" t="s">
-        <v>78</v>
-      </c>
-      <c r="I65" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>192</v>
+        <v>124</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F66" t="s">
-        <v>76</v>
+        <v>314</v>
       </c>
       <c r="G66" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B67" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F67" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G67" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H67" t="s">
+        <v>78</v>
+      </c>
+      <c r="I67" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F68" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="G68" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B69" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F69" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="G69" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B70" t="s">
-        <v>195</v>
+        <v>129</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F70" t="s">
         <v>52</v>
@@ -3199,300 +3214,300 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>194</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F71" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G71" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B72" t="s">
-        <v>124</v>
+        <v>195</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F72" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G72" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
-        <v>196</v>
+        <v>66</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F73" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G73" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F74" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="G74" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B75" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F75" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="G75" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>197</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F76" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="G76" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B77" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F77" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G77" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>210</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F78" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="G78" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B79" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F79" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G79" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="F80" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G80" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B81" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F81" t="s">
-        <v>314</v>
+        <v>54</v>
       </c>
       <c r="G81" t="s">
-        <v>19</v>
-      </c>
-      <c r="H81" t="s">
-        <v>40</v>
-      </c>
-      <c r="I81" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>188</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>289</v>
+        <v>321</v>
       </c>
       <c r="F82" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G82" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B83" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="F83" t="s">
-        <v>10</v>
+        <v>314</v>
       </c>
       <c r="G83" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="H83" t="s">
+        <v>40</v>
+      </c>
+      <c r="I83" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B84" t="s">
-        <v>196</v>
-      </c>
-      <c r="C84" t="s">
-        <v>318</v>
+        <v>9</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F84" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G84" t="s">
         <v>19</v>
       </c>
-      <c r="I84" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B85" t="s">
-        <v>198</v>
-      </c>
-      <c r="C85" t="s">
-        <v>316</v>
+        <v>185</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F85" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="G85" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>337</v>
+        <v>145</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
+        <v>196</v>
+      </c>
+      <c r="C86" t="s">
+        <v>318</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>345</v>
+        <v>290</v>
       </c>
       <c r="F86" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G86" t="s">
+        <v>19</v>
+      </c>
+      <c r="I86" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>322</v>
+        <v>146</v>
       </c>
       <c r="B87" t="s">
-        <v>323</v>
+        <v>198</v>
+      </c>
+      <c r="C87" t="s">
+        <v>316</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="F87" t="s">
         <v>54</v>
@@ -3503,161 +3518,155 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>147</v>
+        <v>337</v>
       </c>
       <c r="B88" t="s">
-        <v>199</v>
+        <v>66</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>291</v>
+        <v>345</v>
       </c>
       <c r="F88" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G88" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>147</v>
+        <v>322</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>323</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="F89" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="G89" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>207</v>
+        <v>147</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>199</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F90" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G90" t="s">
-        <v>19</v>
-      </c>
-      <c r="H90" t="s">
-        <v>315</v>
-      </c>
-      <c r="I90" t="s">
-        <v>311</v>
+        <v>59</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B91" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>293</v>
+        <v>341</v>
       </c>
       <c r="F91" t="s">
-        <v>309</v>
+        <v>76</v>
       </c>
       <c r="G91" t="s">
-        <v>310</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B92" t="s">
-        <v>333</v>
+        <v>39</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="F92" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G92" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="H92" t="s">
+        <v>315</v>
+      </c>
+      <c r="I92" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>213</v>
+        <v>148</v>
       </c>
       <c r="B93" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="F93" t="s">
-        <v>76</v>
+        <v>309</v>
       </c>
       <c r="G93" t="s">
-        <v>59</v>
+        <v>310</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>149</v>
+        <v>213</v>
       </c>
       <c r="B94" t="s">
-        <v>201</v>
+        <v>333</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="F94" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="G94" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>150</v>
+        <v>213</v>
       </c>
       <c r="B95" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>294</v>
+        <v>342</v>
       </c>
       <c r="F95" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="G95" t="s">
-        <v>19</v>
-      </c>
-      <c r="H95" t="s">
-        <v>78</v>
-      </c>
-      <c r="I95" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>305</v>
+        <v>346</v>
       </c>
       <c r="F96" t="s">
         <v>54</v>
@@ -3668,47 +3677,53 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B97" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="F97" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G97" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="H97" t="s">
+        <v>78</v>
+      </c>
+      <c r="I97" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B98" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="F98" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="G98" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>215</v>
+        <v>153</v>
       </c>
       <c r="B99" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="F99" t="s">
         <v>54</v>
@@ -3719,64 +3734,64 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B100" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F100" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="G100" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B101" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F101" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G101" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>312</v>
+        <v>156</v>
       </c>
       <c r="B102" t="s">
-        <v>32</v>
+        <v>202</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="F102" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="G102" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="B103" t="s">
-        <v>188</v>
+        <v>9</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F103" t="s">
         <v>40</v>
@@ -3784,39 +3799,33 @@
       <c r="G103" t="s">
         <v>19</v>
       </c>
-      <c r="H103" t="s">
-        <v>158</v>
-      </c>
-      <c r="I103" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="F104" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G104" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="B105" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F105" t="s">
         <v>40</v>
@@ -3825,83 +3834,123 @@
         <v>19</v>
       </c>
       <c r="H105" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="I105" t="s">
-        <v>19</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>41</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F106" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G106" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>324</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
-        <v>325</v>
+        <v>209</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="F107" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G107" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="H107" t="s">
+        <v>22</v>
+      </c>
+      <c r="I107" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B108" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F108" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G108" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>324</v>
+      </c>
+      <c r="B109" t="s">
+        <v>325</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F109" t="s">
+        <v>54</v>
+      </c>
+      <c r="G109" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>162</v>
+      </c>
+      <c r="B110" t="s">
+        <v>163</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F110" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>217</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
         <v>41</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F111" t="s">
         <v>40</v>
       </c>
-      <c r="G109" t="s">
+      <c r="G111" t="s">
         <v>19</v>
       </c>
-      <c r="H109" t="s">
+      <c r="H111" t="s">
         <v>315</v>
       </c>
-      <c r="I109" t="s">
+      <c r="I111" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3911,100 +3960,102 @@
     <hyperlink ref="E6" r:id="rId2" xr:uid="{D72FCA14-EA08-4749-BB11-D24B8A62C2FD}"/>
     <hyperlink ref="E9" r:id="rId3" xr:uid="{E6DBC748-9C42-444A-9719-EDB7AD21ED31}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{D72F2EFB-3573-5D41-9B63-CA5C8A903FE7}"/>
-    <hyperlink ref="E14" r:id="rId5" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
-    <hyperlink ref="E15" r:id="rId6" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
-    <hyperlink ref="E16" r:id="rId7" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
-    <hyperlink ref="E17" r:id="rId8" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
-    <hyperlink ref="E19" r:id="rId9" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
-    <hyperlink ref="E20" r:id="rId10" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
-    <hyperlink ref="E25" r:id="rId11" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
-    <hyperlink ref="E26" r:id="rId12" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
-    <hyperlink ref="E27" r:id="rId13" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
-    <hyperlink ref="E29" r:id="rId14" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
-    <hyperlink ref="E31" r:id="rId15" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
-    <hyperlink ref="E33" r:id="rId16" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
-    <hyperlink ref="E38" r:id="rId17" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
-    <hyperlink ref="E39" r:id="rId18" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
-    <hyperlink ref="E40" r:id="rId19" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
-    <hyperlink ref="E41" r:id="rId20" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
-    <hyperlink ref="E42" r:id="rId21" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
-    <hyperlink ref="E43" r:id="rId22" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
-    <hyperlink ref="E44" r:id="rId23" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
-    <hyperlink ref="E46" r:id="rId24" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E48" r:id="rId25" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E49" r:id="rId26" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E51" r:id="rId27" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E55" r:id="rId28" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E62" r:id="rId29" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
-    <hyperlink ref="E58" r:id="rId30" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E63" r:id="rId31" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E65" r:id="rId32" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E67" r:id="rId33" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E68" r:id="rId34" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
+    <hyperlink ref="E18" r:id="rId8" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{504D87C1-AAD3-EE49-B4E8-E4EBEADF17A4}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
+    <hyperlink ref="E26" r:id="rId11" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
+    <hyperlink ref="E27" r:id="rId12" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
+    <hyperlink ref="E29" r:id="rId13" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
+    <hyperlink ref="E31" r:id="rId14" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
+    <hyperlink ref="E33" r:id="rId15" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
+    <hyperlink ref="E35" r:id="rId16" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
+    <hyperlink ref="E40" r:id="rId17" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
+    <hyperlink ref="E41" r:id="rId18" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
+    <hyperlink ref="E42" r:id="rId19" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
+    <hyperlink ref="E43" r:id="rId20" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
+    <hyperlink ref="E44" r:id="rId21" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
+    <hyperlink ref="E45" r:id="rId22" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
+    <hyperlink ref="E46" r:id="rId23" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
+    <hyperlink ref="E48" r:id="rId24" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
+    <hyperlink ref="E50" r:id="rId25" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E51" r:id="rId26" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E53" r:id="rId27" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E57" r:id="rId28" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E64" r:id="rId29" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E60" r:id="rId30" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
+    <hyperlink ref="E65" r:id="rId31" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E67" r:id="rId32" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E69" r:id="rId33" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E70" r:id="rId34" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
     <hyperlink ref="E3" r:id="rId35" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E60" r:id="rId36" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E69" r:id="rId37" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E70" r:id="rId38" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
-    <hyperlink ref="E23" r:id="rId39" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E71" r:id="rId40" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E72" r:id="rId41" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E73" r:id="rId42" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E74" r:id="rId43" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E75" r:id="rId44" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E76" r:id="rId45" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E77" r:id="rId46" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E79" r:id="rId47" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E81" r:id="rId48" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E82" r:id="rId49" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E83" r:id="rId50" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E84" r:id="rId51" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E88" r:id="rId52" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E90" r:id="rId53" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E95" r:id="rId54" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E97" r:id="rId55" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E98" r:id="rId56" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E99" r:id="rId57" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E100" r:id="rId58" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E101" r:id="rId59" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E103" r:id="rId60" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E104" r:id="rId61" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E106" r:id="rId62" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E108" r:id="rId63" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E109" r:id="rId64" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E54" r:id="rId65" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E66" r:id="rId66" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E89" r:id="rId67" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E96" r:id="rId68" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E62" r:id="rId36" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E71" r:id="rId37" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E72" r:id="rId38" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E24" r:id="rId39" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
+    <hyperlink ref="E73" r:id="rId40" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E74" r:id="rId41" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E75" r:id="rId42" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E76" r:id="rId43" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E77" r:id="rId44" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E78" r:id="rId45" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E79" r:id="rId46" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E81" r:id="rId47" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E83" r:id="rId48" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E84" r:id="rId49" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E85" r:id="rId50" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E86" r:id="rId51" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E90" r:id="rId52" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E92" r:id="rId53" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E97" r:id="rId54" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E99" r:id="rId55" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E100" r:id="rId56" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E101" r:id="rId57" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E102" r:id="rId58" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E103" r:id="rId59" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E105" r:id="rId60" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E106" r:id="rId61" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E108" r:id="rId62" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E110" r:id="rId63" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E111" r:id="rId64" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E56" r:id="rId65" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E68" r:id="rId66" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E91" r:id="rId67" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E98" r:id="rId68" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
     <hyperlink ref="E5" r:id="rId69" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
     <hyperlink ref="E12" r:id="rId70" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E57" r:id="rId71" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E59" r:id="rId71" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
     <hyperlink ref="E7" r:id="rId72" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
     <hyperlink ref="E11" r:id="rId73" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E61" r:id="rId74" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E52" r:id="rId75" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E53" r:id="rId76" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E63" r:id="rId74" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E54" r:id="rId75" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E55" r:id="rId76" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
     <hyperlink ref="E8" r:id="rId77" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E50" r:id="rId78" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E64" r:id="rId79" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E91" r:id="rId80" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E105" r:id="rId81" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E21" r:id="rId82" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E78" r:id="rId83" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E52" r:id="rId78" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E66" r:id="rId79" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E93" r:id="rId80" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E107" r:id="rId81" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E22" r:id="rId82" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
+    <hyperlink ref="E80" r:id="rId83" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId84" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E102" r:id="rId85" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E24" r:id="rId86" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E80" r:id="rId87" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E87" r:id="rId88" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E107" r:id="rId89" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
-    <hyperlink ref="E22" r:id="rId90" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
-    <hyperlink ref="E59" r:id="rId91" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
-    <hyperlink ref="E92" r:id="rId92" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
-    <hyperlink ref="E85" r:id="rId93" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
-    <hyperlink ref="E32" r:id="rId94" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
-    <hyperlink ref="E93" r:id="rId95" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
-    <hyperlink ref="E86" r:id="rId96" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
-    <hyperlink ref="E94" r:id="rId97" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
-    <hyperlink ref="E56" r:id="rId98" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
+    <hyperlink ref="E104" r:id="rId85" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E25" r:id="rId86" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E82" r:id="rId87" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E89" r:id="rId88" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E109" r:id="rId89" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E23" r:id="rId90" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
+    <hyperlink ref="E61" r:id="rId91" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E94" r:id="rId92" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E87" r:id="rId93" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E34" r:id="rId94" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
+    <hyperlink ref="E95" r:id="rId95" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
+    <hyperlink ref="E88" r:id="rId96" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
+    <hyperlink ref="E96" r:id="rId97" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
+    <hyperlink ref="E58" r:id="rId98" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
+    <hyperlink ref="E28" r:id="rId99" xr:uid="{E24B841F-2272-CA43-9614-50B7F36AD8C5}"/>
+    <hyperlink ref="E13" r:id="rId100" xr:uid="{29460556-99EB-6943-BF02-EAF45B9A2438}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Coimbra-LIP udates: Escada out; change of email for Santos
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4591044-C71C-E142-8C2E-6B67B17F878F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94737B18-3D38-1E43-95C6-5760840FB249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14260" yWindow="2900" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="351">
   <si>
     <t>LastName</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Elorza</t>
   </si>
   <si>
-    <t xml:space="preserve">Escada                       </t>
-  </si>
-  <si>
     <t xml:space="preserve">Esteve                       </t>
   </si>
   <si>
@@ -763,9 +760,6 @@
     <t>mikel.elorza@dipc.org</t>
   </si>
   <si>
-    <t>jose.escada@coimbra.lip.pt</t>
-  </si>
-  <si>
     <t>rauesbos@upvnet.upv.es</t>
   </si>
   <si>
@@ -907,9 +901,6 @@
     <t>bromeo@dipc.org</t>
   </si>
   <si>
-    <t>filomena@gian.fis.uc.pt</t>
-  </si>
-  <si>
     <t>marc.seemann@dipc.org</t>
   </si>
   <si>
@@ -1091,6 +1082,9 @@
   </si>
   <si>
     <t>joseeduardo.barcelon@dipc.org</t>
+  </si>
+  <si>
+    <t>filomena.santos@coimbra.lip.pt</t>
   </si>
 </sst>
 </file>
@@ -1942,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1964,7 +1958,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1987,7 +1981,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2004,7 +1998,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
@@ -2018,10 +2012,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2038,7 +2032,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F5" t="s">
         <v>40</v>
@@ -2052,10 +2046,10 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -2069,10 +2063,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -2089,10 +2083,10 @@
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -2106,7 +2100,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F9" t="s">
         <v>54</v>
@@ -2120,10 +2114,10 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
@@ -2137,10 +2131,10 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2154,10 +2148,10 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -2168,13 +2162,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B13" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F13" t="s">
         <v>40</v>
@@ -2191,7 +2185,7 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F14" t="s">
         <v>40</v>
@@ -2200,10 +2194,10 @@
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I14" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2214,7 +2208,7 @@
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F15" t="s">
         <v>40</v>
@@ -2228,10 +2222,10 @@
         <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F16" t="s">
         <v>47</v>
@@ -2248,7 +2242,7 @@
         <v>41</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F17" t="s">
         <v>40</v>
@@ -2268,10 +2262,10 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F18" t="s">
         <v>52</v>
@@ -2282,13 +2276,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F19" t="s">
         <v>40</v>
@@ -2302,10 +2296,10 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F20" t="s">
         <v>27</v>
@@ -2319,13 +2313,13 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F21" t="s">
         <v>47</v>
@@ -2339,10 +2333,10 @@
         <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F22" t="s">
         <v>61</v>
@@ -2353,13 +2347,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F23" t="s">
         <v>54</v>
@@ -2376,10 +2370,10 @@
         <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G24" t="s">
         <v>19</v>
@@ -2387,13 +2381,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F25" t="s">
         <v>14</v>
@@ -2410,7 +2404,7 @@
         <v>66</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F26" t="s">
         <v>52</v>
@@ -2424,10 +2418,10 @@
         <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F27" t="s">
         <v>68</v>
@@ -2438,13 +2432,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B28" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F28" t="s">
         <v>40</v>
@@ -2455,13 +2449,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F29" t="s">
         <v>40</v>
@@ -2478,7 +2472,7 @@
         <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F30" t="s">
         <v>40</v>
@@ -2487,10 +2481,10 @@
         <v>19</v>
       </c>
       <c r="H30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I30" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -2500,14 +2494,14 @@
       <c r="B31" t="s">
         <v>176</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>243</v>
+      <c r="E31" t="s">
+        <v>242</v>
       </c>
       <c r="F31" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2515,162 +2509,162 @@
         <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>177</v>
-      </c>
-      <c r="E32" t="s">
-        <v>244</v>
+        <v>176</v>
+      </c>
+      <c r="C32" t="s">
+        <v>340</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G32" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>177</v>
       </c>
-      <c r="C33" t="s">
-        <v>343</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>245</v>
+        <v>336</v>
       </c>
       <c r="F33" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
         <v>178</v>
       </c>
+      <c r="C34" t="s">
+        <v>341</v>
+      </c>
       <c r="E34" s="1" t="s">
-        <v>339</v>
+        <v>244</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>77</v>
+      </c>
+      <c r="I34" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>179</v>
-      </c>
-      <c r="C35" t="s">
-        <v>344</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>246</v>
+        <v>81</v>
+      </c>
+      <c r="E35" t="s">
+        <v>245</v>
       </c>
       <c r="F35" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="G35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F36" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>215</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="E37" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G37" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" t="s">
-        <v>78</v>
-      </c>
-      <c r="I37" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>216</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>86</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G38" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E39" t="s">
-        <v>250</v>
+        <v>205</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="F39" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" t="s">
-        <v>78</v>
-      </c>
-      <c r="I39" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -2678,10 +2672,10 @@
         <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F40" t="s">
         <v>14</v>
@@ -2695,33 +2689,33 @@
         <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>253</v>
+        <v>337</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G42" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -2732,30 +2726,30 @@
         <v>180</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G43" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>105</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F44" t="s">
         <v>306</v>
       </c>
-      <c r="F44" t="s">
-        <v>68</v>
-      </c>
       <c r="G44" t="s">
-        <v>97</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2763,16 +2757,16 @@
         <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
       <c r="F45" t="s">
-        <v>309</v>
+        <v>17</v>
       </c>
       <c r="G45" t="s">
-        <v>310</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2780,16 +2774,16 @@
         <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>254</v>
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>253</v>
       </c>
       <c r="F46" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="G46" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2797,16 +2791,16 @@
         <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" t="s">
-        <v>255</v>
+        <v>182</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="F47" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="G47" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2816,48 +2810,54 @@
       <c r="B48" t="s">
         <v>183</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>256</v>
+      <c r="E48" t="s">
+        <v>255</v>
       </c>
       <c r="F48" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="G48" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>210</v>
       </c>
       <c r="B49" t="s">
-        <v>184</v>
-      </c>
-      <c r="E49" t="s">
-        <v>257</v>
+        <v>30</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="F49" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G49" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F50" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G50" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I50" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -2865,22 +2865,16 @@
         <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F51" t="s">
-        <v>40</v>
+        <v>311</v>
       </c>
       <c r="G51" t="s">
         <v>19</v>
-      </c>
-      <c r="H51" t="s">
-        <v>315</v>
-      </c>
-      <c r="I51" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -2888,33 +2882,33 @@
         <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F52" t="s">
-        <v>314</v>
+        <v>106</v>
       </c>
       <c r="G52" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F53" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="G53" t="s">
-        <v>108</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -2922,16 +2916,16 @@
         <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F54" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G54" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -2939,16 +2933,16 @@
         <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>186</v>
+        <v>88</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F55" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="G55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -2956,101 +2950,101 @@
         <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F56" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G56" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>335</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>41</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>265</v>
+        <v>344</v>
       </c>
       <c r="F57" t="s">
-        <v>76</v>
+        <v>311</v>
       </c>
       <c r="G57" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>338</v>
+        <v>112</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>347</v>
+        <v>264</v>
       </c>
       <c r="F58" t="s">
-        <v>314</v>
+        <v>47</v>
       </c>
       <c r="G58" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>187</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F59" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G59" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>327</v>
       </c>
       <c r="B60" t="s">
-        <v>188</v>
+        <v>41</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>267</v>
+        <v>328</v>
       </c>
       <c r="F60" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="G60" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>330</v>
+        <v>116</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>331</v>
+        <v>266</v>
       </c>
       <c r="F61" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G61" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -3061,13 +3055,13 @@
         <v>189</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F62" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G62" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -3075,30 +3069,30 @@
         <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F63" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="G63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F64" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="G64" t="s">
         <v>53</v>
@@ -3106,36 +3100,42 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F65" t="s">
-        <v>52</v>
+        <v>311</v>
       </c>
       <c r="G65" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F66" t="s">
-        <v>314</v>
+        <v>40</v>
       </c>
       <c r="G66" t="s">
         <v>19</v>
+      </c>
+      <c r="H66" t="s">
+        <v>77</v>
+      </c>
+      <c r="I66" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -3146,19 +3146,13 @@
         <v>191</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F67" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="G67" t="s">
-        <v>19</v>
-      </c>
-      <c r="H67" t="s">
-        <v>78</v>
-      </c>
-      <c r="I67" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -3169,13 +3163,13 @@
         <v>192</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F68" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="G68" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -3183,33 +3177,33 @@
         <v>127</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>128</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F69" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="G69" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B70" t="s">
-        <v>129</v>
+        <v>193</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F70" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G70" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -3220,13 +3214,13 @@
         <v>194</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F71" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G71" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -3234,16 +3228,16 @@
         <v>131</v>
       </c>
       <c r="B72" t="s">
-        <v>195</v>
+        <v>66</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F72" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G72" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -3251,16 +3245,16 @@
         <v>132</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F73" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G73" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -3268,16 +3262,16 @@
         <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>124</v>
+        <v>195</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F74" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G74" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3288,13 +3282,13 @@
         <v>196</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F75" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="G75" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3302,47 +3296,47 @@
         <v>135</v>
       </c>
       <c r="B76" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F76" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="G76" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>209</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F77" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="G77" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>210</v>
+        <v>137</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F78" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G78" t="s">
         <v>19</v>
@@ -3353,16 +3347,16 @@
         <v>138</v>
       </c>
       <c r="B79" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F79" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="G79" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -3370,16 +3364,16 @@
         <v>139</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>189</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F80" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G80" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3387,10 +3381,10 @@
         <v>140</v>
       </c>
       <c r="B81" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="F81" t="s">
         <v>54</v>
@@ -3404,16 +3398,22 @@
         <v>141</v>
       </c>
       <c r="B82" t="s">
-        <v>188</v>
+        <v>136</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="F82" t="s">
-        <v>54</v>
+        <v>311</v>
       </c>
       <c r="G82" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="H82" t="s">
+        <v>40</v>
+      </c>
+      <c r="I82" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -3421,21 +3421,15 @@
         <v>142</v>
       </c>
       <c r="B83" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F83" t="s">
-        <v>314</v>
+        <v>50</v>
       </c>
       <c r="G83" t="s">
-        <v>19</v>
-      </c>
-      <c r="H83" t="s">
-        <v>40</v>
-      </c>
-      <c r="I83" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3444,16 +3438,16 @@
         <v>143</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>184</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>289</v>
+        <v>333</v>
       </c>
       <c r="F84" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G84" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -3461,16 +3455,22 @@
         <v>144</v>
       </c>
       <c r="B85" t="s">
-        <v>185</v>
+        <v>195</v>
+      </c>
+      <c r="C85" t="s">
+        <v>315</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="F85" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G85" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="I85" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -3478,90 +3478,84 @@
         <v>145</v>
       </c>
       <c r="B86" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C86" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>290</v>
+        <v>332</v>
       </c>
       <c r="F86" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G86" t="s">
-        <v>19</v>
-      </c>
-      <c r="I86" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>146</v>
+        <v>334</v>
       </c>
       <c r="B87" t="s">
-        <v>198</v>
-      </c>
-      <c r="C87" t="s">
-        <v>316</v>
+        <v>66</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="F87" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G87" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="B88" t="s">
-        <v>66</v>
+        <v>320</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="F88" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G88" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>322</v>
+        <v>146</v>
       </c>
       <c r="B89" t="s">
-        <v>323</v>
+        <v>198</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
       <c r="F89" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G89" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B90" t="s">
         <v>199</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>291</v>
+        <v>338</v>
       </c>
       <c r="F90" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="G90" t="s">
         <v>59</v>
@@ -3569,93 +3563,93 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="B91" t="s">
-        <v>200</v>
+        <v>39</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="F91" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="G91" t="s">
-        <v>59</v>
+        <v>19</v>
+      </c>
+      <c r="H91" t="s">
+        <v>312</v>
+      </c>
+      <c r="I91" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>207</v>
+        <v>147</v>
       </c>
       <c r="B92" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F92" t="s">
-        <v>40</v>
+        <v>306</v>
       </c>
       <c r="G92" t="s">
-        <v>19</v>
-      </c>
-      <c r="H92" t="s">
-        <v>315</v>
-      </c>
-      <c r="I92" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>148</v>
+        <v>212</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
+        <v>330</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>293</v>
+        <v>331</v>
       </c>
       <c r="F93" t="s">
-        <v>309</v>
+        <v>34</v>
       </c>
       <c r="G93" t="s">
-        <v>310</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>212</v>
+      </c>
+      <c r="B94" t="s">
         <v>213</v>
       </c>
-      <c r="B94" t="s">
-        <v>333</v>
-      </c>
       <c r="E94" s="1" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="F94" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="G94" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>213</v>
+        <v>148</v>
       </c>
       <c r="B95" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F95" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="G95" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -3663,39 +3657,39 @@
         <v>149</v>
       </c>
       <c r="B96" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>346</v>
+        <v>291</v>
       </c>
       <c r="F96" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G96" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="H96" t="s">
+        <v>77</v>
+      </c>
+      <c r="I96" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B97" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="F97" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G97" t="s">
-        <v>19</v>
-      </c>
-      <c r="H97" t="s">
-        <v>78</v>
-      </c>
-      <c r="I97" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -3703,7 +3697,7 @@
         <v>152</v>
       </c>
       <c r="B98" t="s">
-        <v>190</v>
+        <v>123</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>305</v>
@@ -3720,78 +3714,78 @@
         <v>153</v>
       </c>
       <c r="B99" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="F99" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="G99" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>154</v>
+        <v>214</v>
       </c>
       <c r="B100" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F100" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="G100" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>215</v>
+        <v>155</v>
       </c>
       <c r="B101" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F101" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="G101" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
+        <v>9</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F102" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G102" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>212</v>
+        <v>309</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="F103" t="s">
         <v>40</v>
@@ -3802,13 +3796,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>312</v>
+        <v>156</v>
       </c>
       <c r="B104" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="F104" t="s">
         <v>40</v>
@@ -3816,142 +3810,125 @@
       <c r="G104" t="s">
         <v>19</v>
       </c>
+      <c r="H104" t="s">
+        <v>157</v>
+      </c>
+      <c r="I104" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B105" t="s">
-        <v>188</v>
+        <v>41</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F105" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="G105" t="s">
-        <v>19</v>
-      </c>
-      <c r="H105" t="s">
-        <v>158</v>
-      </c>
-      <c r="I105" t="s">
-        <v>159</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F106" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G106" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="H106" t="s">
+        <v>22</v>
+      </c>
+      <c r="I106" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F107" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G107" t="s">
-        <v>19</v>
-      </c>
-      <c r="H107" t="s">
-        <v>22</v>
-      </c>
-      <c r="I107" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>161</v>
+        <v>321</v>
       </c>
       <c r="B108" t="s">
-        <v>203</v>
+        <v>322</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="F108" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="G108" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>324</v>
+        <v>161</v>
       </c>
       <c r="B109" t="s">
-        <v>325</v>
+        <v>162</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>328</v>
+        <v>300</v>
       </c>
       <c r="F109" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G109" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>162</v>
+        <v>216</v>
       </c>
       <c r="B110" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F110" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G110" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>217</v>
-      </c>
-      <c r="B111" t="s">
-        <v>41</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F111" t="s">
-        <v>40</v>
-      </c>
-      <c r="G111" t="s">
         <v>19</v>
       </c>
-      <c r="H111" t="s">
-        <v>315</v>
-      </c>
-      <c r="I111" t="s">
-        <v>311</v>
+      <c r="H110" t="s">
+        <v>312</v>
+      </c>
+      <c r="I110" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3969,93 +3946,92 @@
     <hyperlink ref="E26" r:id="rId11" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
     <hyperlink ref="E27" r:id="rId12" xr:uid="{6275F301-257D-0D43-9E43-94D415C6C01C}"/>
     <hyperlink ref="E29" r:id="rId13" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
-    <hyperlink ref="E31" r:id="rId14" xr:uid="{DADE79A2-9B79-1946-9873-EEEE374D93E6}"/>
-    <hyperlink ref="E33" r:id="rId15" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
-    <hyperlink ref="E35" r:id="rId16" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
-    <hyperlink ref="E40" r:id="rId17" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
-    <hyperlink ref="E41" r:id="rId18" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
-    <hyperlink ref="E42" r:id="rId19" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
-    <hyperlink ref="E43" r:id="rId20" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
-    <hyperlink ref="E44" r:id="rId21" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
-    <hyperlink ref="E45" r:id="rId22" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
-    <hyperlink ref="E46" r:id="rId23" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
-    <hyperlink ref="E48" r:id="rId24" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E50" r:id="rId25" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E51" r:id="rId26" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E53" r:id="rId27" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E57" r:id="rId28" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E64" r:id="rId29" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
-    <hyperlink ref="E60" r:id="rId30" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E65" r:id="rId31" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E67" r:id="rId32" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E69" r:id="rId33" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E70" r:id="rId34" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
-    <hyperlink ref="E3" r:id="rId35" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E62" r:id="rId36" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E71" r:id="rId37" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E72" r:id="rId38" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
-    <hyperlink ref="E24" r:id="rId39" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E73" r:id="rId40" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E74" r:id="rId41" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E75" r:id="rId42" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E76" r:id="rId43" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E77" r:id="rId44" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E78" r:id="rId45" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E79" r:id="rId46" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E81" r:id="rId47" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E83" r:id="rId48" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E84" r:id="rId49" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E85" r:id="rId50" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E86" r:id="rId51" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E90" r:id="rId52" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E92" r:id="rId53" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E97" r:id="rId54" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E99" r:id="rId55" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E100" r:id="rId56" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E101" r:id="rId57" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E102" r:id="rId58" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E103" r:id="rId59" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E105" r:id="rId60" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E106" r:id="rId61" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E108" r:id="rId62" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E110" r:id="rId63" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E111" r:id="rId64" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E56" r:id="rId65" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E68" r:id="rId66" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E91" r:id="rId67" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E98" r:id="rId68" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
-    <hyperlink ref="E5" r:id="rId69" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
-    <hyperlink ref="E12" r:id="rId70" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E59" r:id="rId71" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
-    <hyperlink ref="E7" r:id="rId72" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
-    <hyperlink ref="E11" r:id="rId73" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E63" r:id="rId74" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E54" r:id="rId75" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E55" r:id="rId76" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
-    <hyperlink ref="E8" r:id="rId77" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E52" r:id="rId78" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E66" r:id="rId79" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E93" r:id="rId80" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E107" r:id="rId81" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E22" r:id="rId82" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
-    <hyperlink ref="E80" r:id="rId83" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
-    <hyperlink ref="E4" r:id="rId84" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E104" r:id="rId85" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E25" r:id="rId86" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E82" r:id="rId87" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E89" r:id="rId88" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E109" r:id="rId89" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
-    <hyperlink ref="E23" r:id="rId90" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
-    <hyperlink ref="E61" r:id="rId91" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
-    <hyperlink ref="E94" r:id="rId92" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
-    <hyperlink ref="E87" r:id="rId93" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
-    <hyperlink ref="E34" r:id="rId94" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
-    <hyperlink ref="E95" r:id="rId95" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
-    <hyperlink ref="E88" r:id="rId96" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
-    <hyperlink ref="E96" r:id="rId97" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
-    <hyperlink ref="E58" r:id="rId98" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
-    <hyperlink ref="E28" r:id="rId99" xr:uid="{E24B841F-2272-CA43-9614-50B7F36AD8C5}"/>
-    <hyperlink ref="E13" r:id="rId100" xr:uid="{29460556-99EB-6943-BF02-EAF45B9A2438}"/>
+    <hyperlink ref="E32" r:id="rId14" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
+    <hyperlink ref="E34" r:id="rId15" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
+    <hyperlink ref="E39" r:id="rId16" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
+    <hyperlink ref="E40" r:id="rId17" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
+    <hyperlink ref="E41" r:id="rId18" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
+    <hyperlink ref="E42" r:id="rId19" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
+    <hyperlink ref="E43" r:id="rId20" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
+    <hyperlink ref="E44" r:id="rId21" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
+    <hyperlink ref="E45" r:id="rId22" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
+    <hyperlink ref="E47" r:id="rId23" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
+    <hyperlink ref="E49" r:id="rId24" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E50" r:id="rId25" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E52" r:id="rId26" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E56" r:id="rId27" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E63" r:id="rId28" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E59" r:id="rId29" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
+    <hyperlink ref="E64" r:id="rId30" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E66" r:id="rId31" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E68" r:id="rId32" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E69" r:id="rId33" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E3" r:id="rId34" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
+    <hyperlink ref="E61" r:id="rId35" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E70" r:id="rId36" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E71" r:id="rId37" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E24" r:id="rId38" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
+    <hyperlink ref="E72" r:id="rId39" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E73" r:id="rId40" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E74" r:id="rId41" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E75" r:id="rId42" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E76" r:id="rId43" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E77" r:id="rId44" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E78" r:id="rId45" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E80" r:id="rId46" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E82" r:id="rId47" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E83" r:id="rId48" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E84" r:id="rId49" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E85" r:id="rId50" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E89" r:id="rId51" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E91" r:id="rId52" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E96" r:id="rId53" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E98" r:id="rId54" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E99" r:id="rId55" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E100" r:id="rId56" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E101" r:id="rId57" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E102" r:id="rId58" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E104" r:id="rId59" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E105" r:id="rId60" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E107" r:id="rId61" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E109" r:id="rId62" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E110" r:id="rId63" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E55" r:id="rId64" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E67" r:id="rId65" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E90" r:id="rId66" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E97" r:id="rId67" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E5" r:id="rId68" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
+    <hyperlink ref="E12" r:id="rId69" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
+    <hyperlink ref="E58" r:id="rId70" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E7" r:id="rId71" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
+    <hyperlink ref="E11" r:id="rId72" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
+    <hyperlink ref="E62" r:id="rId73" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E53" r:id="rId74" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E54" r:id="rId75" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E8" r:id="rId76" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
+    <hyperlink ref="E51" r:id="rId77" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E65" r:id="rId78" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E92" r:id="rId79" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E106" r:id="rId80" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E22" r:id="rId81" xr:uid="{DBF2E712-E251-3248-9D66-6C5E8582E940}"/>
+    <hyperlink ref="E79" r:id="rId82" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E4" r:id="rId83" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
+    <hyperlink ref="E103" r:id="rId84" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E25" r:id="rId85" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E81" r:id="rId86" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E88" r:id="rId87" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E108" r:id="rId88" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E23" r:id="rId89" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
+    <hyperlink ref="E60" r:id="rId90" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E93" r:id="rId91" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E86" r:id="rId92" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E33" r:id="rId93" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
+    <hyperlink ref="E94" r:id="rId94" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
+    <hyperlink ref="E87" r:id="rId95" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
+    <hyperlink ref="E95" r:id="rId96" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
+    <hyperlink ref="E57" r:id="rId97" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
+    <hyperlink ref="E28" r:id="rId98" xr:uid="{E24B841F-2272-CA43-9614-50B7F36AD8C5}"/>
+    <hyperlink ref="E13" r:id="rId99" xr:uid="{29460556-99EB-6943-BF02-EAF45B9A2438}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
LSC update: Ruiz to Ruiz-Choliz
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94737B18-3D38-1E43-95C6-5760840FB249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDA62C20-B291-0F49-B175-26C85A7CD69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14260" yWindow="2900" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,9 +1036,6 @@
     <t>Leslie.rogers776@gmail.com</t>
   </si>
   <si>
-    <t>Ruiz</t>
-  </si>
-  <si>
     <t>Marauri</t>
   </si>
   <si>
@@ -1085,6 +1082,9 @@
   </si>
   <si>
     <t>filomena.santos@coimbra.lip.pt</t>
+  </si>
+  <si>
+    <t>Ruiz-Ch\'oliz</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B13" t="s">
         <v>347</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="F13" t="s">
         <v>40</v>
@@ -2432,13 +2432,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B28" t="s">
         <v>320</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F28" t="s">
         <v>40</v>
@@ -2512,7 +2512,7 @@
         <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>243</v>
@@ -2532,7 +2532,7 @@
         <v>177</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F33" t="s">
         <v>75</v>
@@ -2549,7 +2549,7 @@
         <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>244</v>
@@ -2709,7 +2709,7 @@
         <v>179</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F42" t="s">
         <v>75</v>
@@ -2964,13 +2964,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B57" t="s">
         <v>41</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F57" t="s">
         <v>311</v>
@@ -3495,13 +3495,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="B87" t="s">
         <v>66</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F87" t="s">
         <v>42</v>
@@ -3535,7 +3535,7 @@
         <v>198</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F89" t="s">
         <v>47</v>
@@ -3552,7 +3552,7 @@
         <v>199</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F90" t="s">
         <v>75</v>
@@ -3626,7 +3626,7 @@
         <v>213</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F94" t="s">
         <v>75</v>
@@ -3643,7 +3643,7 @@
         <v>200</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F95" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
ANL update: footnote added and email changed for Adams
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDA62C20-B291-0F49-B175-26C85A7CD69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F0EF23B-C974-6245-8901-069E0A66816E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14260" yWindow="2900" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="352">
   <si>
     <t>LastName</t>
   </si>
@@ -688,9 +688,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>corey.adams@anl.gov</t>
-  </si>
-  <si>
     <t>vicente.alvarez@ific.uv.es</t>
   </si>
   <si>
@@ -1085,6 +1082,12 @@
   </si>
   <si>
     <t>Ruiz-Ch\'oliz</t>
+  </si>
+  <si>
+    <t>Now at NVIDIA.</t>
+  </si>
+  <si>
+    <t>coreya@nvidia.com</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1980,8 +1983,11 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
+      <c r="C2" t="s">
+        <v>350</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>218</v>
+        <v>351</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1998,7 +2004,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
@@ -2015,7 +2021,7 @@
         <v>166</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2032,7 +2038,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
         <v>40</v>
@@ -2049,7 +2055,7 @@
         <v>167</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -2066,7 +2072,7 @@
         <v>168</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -2083,10 +2089,10 @@
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -2100,7 +2106,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F9" t="s">
         <v>54</v>
@@ -2117,7 +2123,7 @@
         <v>169</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
@@ -2134,7 +2140,7 @@
         <v>170</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2151,7 +2157,7 @@
         <v>171</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -2162,13 +2168,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13" t="s">
         <v>346</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="F13" t="s">
         <v>40</v>
@@ -2185,7 +2191,7 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F14" t="s">
         <v>40</v>
@@ -2194,10 +2200,10 @@
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2208,7 +2214,7 @@
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F15" t="s">
         <v>40</v>
@@ -2225,7 +2231,7 @@
         <v>172</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F16" t="s">
         <v>47</v>
@@ -2242,7 +2248,7 @@
         <v>41</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F17" t="s">
         <v>40</v>
@@ -2265,7 +2271,7 @@
         <v>165</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F18" t="s">
         <v>52</v>
@@ -2282,7 +2288,7 @@
         <v>200</v>
       </c>
       <c r="E19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F19" t="s">
         <v>40</v>
@@ -2299,7 +2305,7 @@
         <v>173</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F20" t="s">
         <v>27</v>
@@ -2316,10 +2322,10 @@
         <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F21" t="s">
         <v>47</v>
@@ -2336,7 +2342,7 @@
         <v>174</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F22" t="s">
         <v>61</v>
@@ -2347,13 +2353,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F23" t="s">
         <v>54</v>
@@ -2370,10 +2376,10 @@
         <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G24" t="s">
         <v>19</v>
@@ -2381,13 +2387,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B25" t="s">
         <v>88</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F25" t="s">
         <v>14</v>
@@ -2404,7 +2410,7 @@
         <v>66</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F26" t="s">
         <v>52</v>
@@ -2421,7 +2427,7 @@
         <v>163</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F27" t="s">
         <v>68</v>
@@ -2432,13 +2438,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>343</v>
+      </c>
+      <c r="B28" t="s">
+        <v>319</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="B28" t="s">
-        <v>320</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="F28" t="s">
         <v>40</v>
@@ -2455,7 +2461,7 @@
         <v>9</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F29" t="s">
         <v>40</v>
@@ -2472,7 +2478,7 @@
         <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F30" t="s">
         <v>40</v>
@@ -2481,10 +2487,10 @@
         <v>19</v>
       </c>
       <c r="H30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -2495,7 +2501,7 @@
         <v>176</v>
       </c>
       <c r="E31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F31" t="s">
         <v>17</v>
@@ -2512,10 +2518,10 @@
         <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F32" t="s">
         <v>24</v>
@@ -2532,7 +2538,7 @@
         <v>177</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F33" t="s">
         <v>75</v>
@@ -2549,10 +2555,10 @@
         <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F34" t="s">
         <v>40</v>
@@ -2575,7 +2581,7 @@
         <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F35" t="s">
         <v>82</v>
@@ -2592,7 +2598,7 @@
         <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F36" t="s">
         <v>22</v>
@@ -2615,7 +2621,7 @@
         <v>123</v>
       </c>
       <c r="E37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F37" t="s">
         <v>17</v>
@@ -2635,7 +2641,7 @@
         <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F38" t="s">
         <v>40</v>
@@ -2658,7 +2664,7 @@
         <v>205</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -2675,7 +2681,7 @@
         <v>176</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F40" t="s">
         <v>14</v>
@@ -2692,7 +2698,7 @@
         <v>175</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F41" t="s">
         <v>92</v>
@@ -2709,7 +2715,7 @@
         <v>179</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F42" t="s">
         <v>75</v>
@@ -2726,7 +2732,7 @@
         <v>180</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F43" t="s">
         <v>68</v>
@@ -2743,13 +2749,13 @@
         <v>105</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F44" t="s">
+        <v>305</v>
+      </c>
+      <c r="G44" t="s">
         <v>306</v>
-      </c>
-      <c r="G44" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2760,7 +2766,7 @@
         <v>181</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F45" t="s">
         <v>17</v>
@@ -2777,7 +2783,7 @@
         <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F46" t="s">
         <v>68</v>
@@ -2794,7 +2800,7 @@
         <v>182</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F47" t="s">
         <v>24</v>
@@ -2811,7 +2817,7 @@
         <v>183</v>
       </c>
       <c r="E48" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F48" t="s">
         <v>52</v>
@@ -2828,7 +2834,7 @@
         <v>30</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F49" t="s">
         <v>54</v>
@@ -2845,7 +2851,7 @@
         <v>57</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F50" t="s">
         <v>40</v>
@@ -2854,10 +2860,10 @@
         <v>19</v>
       </c>
       <c r="H50" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -2868,10 +2874,10 @@
         <v>41</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G51" t="s">
         <v>19</v>
@@ -2885,7 +2891,7 @@
         <v>105</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F52" t="s">
         <v>106</v>
@@ -2902,7 +2908,7 @@
         <v>30</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F53" t="s">
         <v>40</v>
@@ -2919,7 +2925,7 @@
         <v>185</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F54" t="s">
         <v>54</v>
@@ -2936,7 +2942,7 @@
         <v>88</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F55" t="s">
         <v>82</v>
@@ -2953,7 +2959,7 @@
         <v>186</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F56" t="s">
         <v>75</v>
@@ -2964,16 +2970,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B57" t="s">
         <v>41</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F57" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G57" t="s">
         <v>19</v>
@@ -2987,7 +2993,7 @@
         <v>113</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F58" t="s">
         <v>47</v>
@@ -3004,7 +3010,7 @@
         <v>187</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F59" t="s">
         <v>54</v>
@@ -3015,13 +3021,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F60" t="s">
         <v>17</v>
@@ -3038,7 +3044,7 @@
         <v>188</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F61" t="s">
         <v>24</v>
@@ -3055,7 +3061,7 @@
         <v>189</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F62" t="s">
         <v>54</v>
@@ -3072,7 +3078,7 @@
         <v>119</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F63" t="s">
         <v>82</v>
@@ -3089,7 +3095,7 @@
         <v>121</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F64" t="s">
         <v>52</v>
@@ -3106,10 +3112,10 @@
         <v>123</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G65" t="s">
         <v>19</v>
@@ -3123,7 +3129,7 @@
         <v>190</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F66" t="s">
         <v>40</v>
@@ -3146,7 +3152,7 @@
         <v>191</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F67" t="s">
         <v>75</v>
@@ -3163,7 +3169,7 @@
         <v>192</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F68" t="s">
         <v>17</v>
@@ -3180,7 +3186,7 @@
         <v>128</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F69" t="s">
         <v>52</v>
@@ -3197,7 +3203,7 @@
         <v>193</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F70" t="s">
         <v>54</v>
@@ -3214,7 +3220,7 @@
         <v>194</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F71" t="s">
         <v>52</v>
@@ -3231,7 +3237,7 @@
         <v>66</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F72" t="s">
         <v>40</v>
@@ -3248,7 +3254,7 @@
         <v>123</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F73" t="s">
         <v>42</v>
@@ -3265,7 +3271,7 @@
         <v>195</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F74" t="s">
         <v>14</v>
@@ -3282,7 +3288,7 @@
         <v>196</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F75" t="s">
         <v>106</v>
@@ -3299,7 +3305,7 @@
         <v>136</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F76" t="s">
         <v>52</v>
@@ -3316,7 +3322,7 @@
         <v>41</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F77" t="s">
         <v>22</v>
@@ -3333,7 +3339,7 @@
         <v>123</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F78" t="s">
         <v>40</v>
@@ -3350,7 +3356,7 @@
         <v>39</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F79" t="s">
         <v>68</v>
@@ -3367,7 +3373,7 @@
         <v>189</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F80" t="s">
         <v>54</v>
@@ -3384,7 +3390,7 @@
         <v>187</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F81" t="s">
         <v>54</v>
@@ -3401,10 +3407,10 @@
         <v>136</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F82" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G82" t="s">
         <v>19</v>
@@ -3424,7 +3430,7 @@
         <v>9</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F83" t="s">
         <v>50</v>
@@ -3441,7 +3447,7 @@
         <v>184</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F84" t="s">
         <v>10</v>
@@ -3458,10 +3464,10 @@
         <v>195</v>
       </c>
       <c r="C85" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F85" t="s">
         <v>40</v>
@@ -3481,10 +3487,10 @@
         <v>197</v>
       </c>
       <c r="C86" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F86" t="s">
         <v>54</v>
@@ -3495,13 +3501,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B87" t="s">
         <v>66</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F87" t="s">
         <v>42</v>
@@ -3512,13 +3518,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>318</v>
+      </c>
+      <c r="B88" t="s">
         <v>319</v>
       </c>
-      <c r="B88" t="s">
-        <v>320</v>
-      </c>
       <c r="E88" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F88" t="s">
         <v>54</v>
@@ -3535,7 +3541,7 @@
         <v>198</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F89" t="s">
         <v>47</v>
@@ -3552,7 +3558,7 @@
         <v>199</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F90" t="s">
         <v>75</v>
@@ -3569,7 +3575,7 @@
         <v>39</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F91" t="s">
         <v>40</v>
@@ -3578,10 +3584,10 @@
         <v>19</v>
       </c>
       <c r="H91" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I91" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3592,13 +3598,13 @@
         <v>136</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F92" t="s">
+        <v>305</v>
+      </c>
+      <c r="G92" t="s">
         <v>306</v>
-      </c>
-      <c r="G92" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -3606,10 +3612,10 @@
         <v>212</v>
       </c>
       <c r="B93" t="s">
+        <v>329</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="F93" t="s">
         <v>34</v>
@@ -3626,7 +3632,7 @@
         <v>213</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F94" t="s">
         <v>75</v>
@@ -3643,7 +3649,7 @@
         <v>200</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F95" t="s">
         <v>54</v>
@@ -3660,7 +3666,7 @@
         <v>150</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F96" t="s">
         <v>40</v>
@@ -3683,7 +3689,7 @@
         <v>189</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F97" t="s">
         <v>54</v>
@@ -3700,7 +3706,7 @@
         <v>123</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F98" t="s">
         <v>54</v>
@@ -3717,7 +3723,7 @@
         <v>154</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F99" t="s">
         <v>75</v>
@@ -3734,7 +3740,7 @@
         <v>32</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F100" t="s">
         <v>54</v>
@@ -3751,7 +3757,7 @@
         <v>201</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F101" t="s">
         <v>17</v>
@@ -3768,7 +3774,7 @@
         <v>9</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F102" t="s">
         <v>40</v>
@@ -3779,13 +3785,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B103" t="s">
         <v>32</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F103" t="s">
         <v>40</v>
@@ -3802,7 +3808,7 @@
         <v>187</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F104" t="s">
         <v>40</v>
@@ -3825,7 +3831,7 @@
         <v>41</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F105" t="s">
         <v>14</v>
@@ -3842,7 +3848,7 @@
         <v>208</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F106" t="s">
         <v>40</v>
@@ -3865,7 +3871,7 @@
         <v>202</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F107" t="s">
         <v>34</v>
@@ -3876,13 +3882,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>320</v>
+      </c>
+      <c r="B108" t="s">
         <v>321</v>
       </c>
-      <c r="B108" t="s">
-        <v>322</v>
-      </c>
       <c r="E108" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F108" t="s">
         <v>54</v>
@@ -3899,7 +3905,7 @@
         <v>162</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F109" t="s">
         <v>14</v>
@@ -3916,7 +3922,7 @@
         <v>41</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F110" t="s">
         <v>40</v>
@@ -3925,10 +3931,10 @@
         <v>19</v>
       </c>
       <c r="H110" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I110" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spome missing orcids added
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B072AF8A-6735-D94A-966D-772F5192AD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E075033-B75E-F447-8BEF-A2675B738D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8240" yWindow="4420" windowWidth="22920" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7240" yWindow="5560" windowWidth="22920" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="455">
   <si>
     <t>LastName</t>
   </si>
@@ -889,9 +889,6 @@
     <t>jordi.torrent@udg.edu</t>
   </si>
   <si>
-    <t>alexander.trettin@manchester.ac.uk</t>
-  </si>
-  <si>
     <t>pablo.garcia@dipc.org</t>
   </si>
   <si>
@@ -1385,6 +1382,21 @@
   </si>
   <si>
     <t>ORCID</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0009-0006-7366-4950</t>
+  </si>
+  <si>
+    <t>alexandra.trettin@manchester.ac.uk</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0009-0009-0971-5559</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0009-0000-4219-6193</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-8363-0109</t>
   </si>
 </sst>
 </file>
@@ -2239,8 +2251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2265,10 +2277,10 @@
         <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -2291,13 +2303,13 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G2" s="2">
         <v>45478</v>
@@ -2317,10 +2329,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
@@ -2341,7 +2353,7 @@
         <v>209</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
@@ -2362,7 +2374,7 @@
         <v>210</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G5" s="2">
         <v>45597</v>
@@ -2385,7 +2397,7 @@
         <v>211</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
@@ -2406,7 +2418,7 @@
         <v>212</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
@@ -2427,11 +2439,11 @@
         <v>213</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I8" t="s">
         <v>19</v>
@@ -2448,7 +2460,7 @@
         <v>214</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
@@ -2469,7 +2481,7 @@
         <v>215</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
@@ -2490,7 +2502,7 @@
         <v>216</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G11" s="2">
         <v>45718</v>
@@ -2513,7 +2525,7 @@
         <v>217</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
@@ -2525,16 +2537,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>333</v>
+      </c>
+      <c r="B13" t="s">
         <v>334</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
@@ -2555,7 +2567,7 @@
         <v>218</v>
       </c>
       <c r="F14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H14" t="s">
         <v>40</v>
@@ -2564,24 +2576,24 @@
         <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G15" s="2">
         <v>45714</v>
@@ -2604,7 +2616,7 @@
         <v>219</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
@@ -2625,7 +2637,7 @@
         <v>220</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
@@ -2637,7 +2649,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
@@ -2646,7 +2658,7 @@
         <v>221</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
@@ -2692,7 +2704,7 @@
         <v>223</v>
       </c>
       <c r="F20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H20" t="s">
         <v>40</v>
@@ -2712,7 +2724,7 @@
         <v>224</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
@@ -2724,16 +2736,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B22" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G22" s="2">
         <v>45714</v>
@@ -2753,13 +2765,13 @@
         <v>157</v>
       </c>
       <c r="C23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>225</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
@@ -2771,16 +2783,16 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
@@ -2801,11 +2813,11 @@
         <v>226</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I25" t="s">
         <v>19</v>
@@ -2813,16 +2825,16 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
         <v>82</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
@@ -2843,7 +2855,7 @@
         <v>227</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
@@ -2855,16 +2867,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>331</v>
+      </c>
+      <c r="B28" t="s">
+        <v>307</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B28" t="s">
-        <v>308</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>333</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
@@ -2876,7 +2888,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
@@ -2903,6 +2915,9 @@
       <c r="E30" t="s">
         <v>229</v>
       </c>
+      <c r="F30" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="H30" t="s">
         <v>40</v>
       </c>
@@ -2910,10 +2925,10 @@
         <v>19</v>
       </c>
       <c r="J30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2927,7 +2942,7 @@
         <v>230</v>
       </c>
       <c r="F31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H31" t="s">
         <v>17</v>
@@ -2944,13 +2959,13 @@
         <v>168</v>
       </c>
       <c r="C32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>231</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G32" s="2">
         <v>45779</v>
@@ -2970,10 +2985,10 @@
         <v>169</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" t="s">
@@ -2991,13 +3006,13 @@
         <v>170</v>
       </c>
       <c r="C34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>232</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G34" s="2">
         <v>45496</v>
@@ -3026,7 +3041,7 @@
         <v>233</v>
       </c>
       <c r="F35" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H35" t="s">
         <v>76</v>
@@ -3046,7 +3061,7 @@
         <v>234</v>
       </c>
       <c r="F36" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H36" t="s">
         <v>22</v>
@@ -3072,7 +3087,7 @@
         <v>235</v>
       </c>
       <c r="F37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H37" t="s">
         <v>17</v>
@@ -3095,7 +3110,7 @@
         <v>236</v>
       </c>
       <c r="F38" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H38" t="s">
         <v>40</v>
@@ -3121,7 +3136,7 @@
         <v>237</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
@@ -3142,7 +3157,7 @@
         <v>238</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" t="s">
@@ -3163,7 +3178,7 @@
         <v>239</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" t="s">
@@ -3181,10 +3196,10 @@
         <v>171</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" t="s">
@@ -3202,10 +3217,10 @@
         <v>172</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" t="s">
@@ -3223,17 +3238,17 @@
         <v>99</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" t="s">
+        <v>293</v>
+      </c>
+      <c r="I44" t="s">
         <v>294</v>
-      </c>
-      <c r="I44" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -3247,7 +3262,7 @@
         <v>240</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" t="s">
@@ -3268,7 +3283,7 @@
         <v>241</v>
       </c>
       <c r="F46" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H46" t="s">
         <v>63</v>
@@ -3288,7 +3303,7 @@
         <v>242</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" t="s">
@@ -3309,7 +3324,7 @@
         <v>243</v>
       </c>
       <c r="F48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H48" t="s">
         <v>51</v>
@@ -3329,7 +3344,7 @@
         <v>244</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" t="s">
@@ -3350,7 +3365,7 @@
         <v>245</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
@@ -3360,10 +3375,10 @@
         <v>19</v>
       </c>
       <c r="J50" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -3377,11 +3392,11 @@
         <v>246</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I51" t="s">
         <v>19</v>
@@ -3398,7 +3413,7 @@
         <v>247</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="s">
@@ -3419,7 +3434,7 @@
         <v>248</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
@@ -3440,7 +3455,7 @@
         <v>249</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
@@ -3461,7 +3476,7 @@
         <v>250</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
@@ -3482,7 +3497,7 @@
         <v>251</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
@@ -3494,20 +3509,20 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B57" t="s">
         <v>41</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I57" t="s">
         <v>19</v>
@@ -3524,7 +3539,7 @@
         <v>252</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
@@ -3545,7 +3560,7 @@
         <v>253</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
@@ -3557,16 +3572,16 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
@@ -3587,7 +3602,7 @@
         <v>254</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
@@ -3608,7 +3623,7 @@
         <v>255</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
@@ -3629,7 +3644,7 @@
         <v>256</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
@@ -3650,7 +3665,7 @@
         <v>257</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
@@ -3671,11 +3686,11 @@
         <v>258</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I65" t="s">
         <v>19</v>
@@ -3692,7 +3707,7 @@
         <v>259</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" t="s">
@@ -3719,7 +3734,7 @@
         <v>260</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" t="s">
@@ -3740,7 +3755,7 @@
         <v>261</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" t="s">
@@ -3760,7 +3775,9 @@
       <c r="E69" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F69" s="1"/>
+      <c r="F69" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="G69" s="1"/>
       <c r="H69" t="s">
         <v>51</v>
@@ -3780,7 +3797,7 @@
         <v>263</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" t="s">
@@ -3801,7 +3818,7 @@
         <v>264</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" t="s">
@@ -3822,7 +3839,7 @@
         <v>265</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" t="s">
@@ -3843,7 +3860,7 @@
         <v>266</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" t="s">
@@ -3864,7 +3881,7 @@
         <v>267</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" t="s">
@@ -3904,7 +3921,7 @@
         <v>269</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G76" s="1"/>
       <c r="H76" t="s">
@@ -3925,7 +3942,7 @@
         <v>270</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" t="s">
@@ -3946,7 +3963,7 @@
         <v>271</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" t="s">
@@ -3967,7 +3984,7 @@
         <v>272</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G79" s="1"/>
       <c r="H79" t="s">
@@ -3988,7 +4005,7 @@
         <v>273</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" t="s">
@@ -4006,10 +4023,10 @@
         <v>179</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" t="s">
@@ -4030,11 +4047,11 @@
         <v>274</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I82" t="s">
         <v>19</v>
@@ -4057,7 +4074,7 @@
         <v>275</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" t="s">
@@ -4075,10 +4092,10 @@
         <v>176</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G84" s="2">
         <v>45718</v>
@@ -4098,13 +4115,13 @@
         <v>187</v>
       </c>
       <c r="C85" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G85" s="2">
         <v>45779</v>
@@ -4127,13 +4144,13 @@
         <v>189</v>
       </c>
       <c r="C86" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G86" s="2">
         <v>45779</v>
@@ -4147,16 +4164,16 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B87" t="s">
         <v>62</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" t="s">
@@ -4168,15 +4185,17 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>306</v>
+      </c>
+      <c r="B88" t="s">
         <v>307</v>
       </c>
-      <c r="B88" t="s">
-        <v>308</v>
-      </c>
       <c r="E88" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F88" s="1"/>
+        <v>311</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="G88" s="1"/>
       <c r="H88" t="s">
         <v>53</v>
@@ -4193,10 +4212,10 @@
         <v>190</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" t="s">
@@ -4214,10 +4233,10 @@
         <v>191</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" t="s">
@@ -4238,7 +4257,7 @@
         <v>277</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" t="s">
@@ -4248,10 +4267,10 @@
         <v>19</v>
       </c>
       <c r="J91" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K91" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -4265,14 +4284,14 @@
         <v>278</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" t="s">
+        <v>293</v>
+      </c>
+      <c r="I92" t="s">
         <v>294</v>
-      </c>
-      <c r="I92" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -4280,12 +4299,14 @@
         <v>203</v>
       </c>
       <c r="B93" t="s">
+        <v>317</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F93" s="1"/>
+      <c r="F93" s="1" t="s">
+        <v>454</v>
+      </c>
       <c r="G93" s="1"/>
       <c r="H93" t="s">
         <v>34</v>
@@ -4302,7 +4323,7 @@
         <v>204</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
@@ -4321,10 +4342,10 @@
         <v>192</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" t="s">
@@ -4345,7 +4366,7 @@
         <v>279</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" t="s">
@@ -4369,10 +4390,10 @@
         <v>181</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" t="s">
@@ -4390,10 +4411,10 @@
         <v>117</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" t="s">
@@ -4433,7 +4454,7 @@
         <v>281</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" t="s">
@@ -4454,7 +4475,7 @@
         <v>282</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" t="s">
@@ -4475,7 +4496,7 @@
         <v>283</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" t="s">
@@ -4487,16 +4508,16 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B103" t="s">
         <v>32</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" t="s">
@@ -4517,7 +4538,7 @@
         <v>284</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" t="s">
@@ -4541,10 +4562,10 @@
         <v>41</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>285</v>
+        <v>451</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" t="s">
@@ -4562,7 +4583,7 @@
         <v>199</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
@@ -4581,16 +4602,16 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B107" t="s">
         <v>39</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G107" s="1"/>
       <c r="H107" t="s">
@@ -4608,10 +4629,10 @@
         <v>194</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" t="s">
@@ -4623,16 +4644,16 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>308</v>
+      </c>
+      <c r="B109" t="s">
         <v>309</v>
       </c>
-      <c r="B109" t="s">
-        <v>310</v>
-      </c>
       <c r="E109" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" t="s">
@@ -4650,10 +4671,10 @@
         <v>156</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G110" s="1"/>
       <c r="H110" t="s">
@@ -4671,10 +4692,10 @@
         <v>41</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" t="s">
@@ -4684,10 +4705,10 @@
         <v>19</v>
       </c>
       <c r="J111" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K111" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -4792,6 +4813,10 @@
     <hyperlink ref="E21" r:id="rId98" xr:uid="{BFCD233B-85C4-684A-9E1F-CFD7E946453F}"/>
     <hyperlink ref="E15" r:id="rId99" tooltip="abayo@lsc-canfranc.es" display="mailto:abayo@lsc-canfranc.es" xr:uid="{9D231E2D-796B-5044-A575-DB475A1F4009}"/>
     <hyperlink ref="E22" r:id="rId100" tooltip="lcid@lsc-canfranc.es" display="mailto:lcid@lsc-canfranc.es" xr:uid="{2505E3E3-5341-1F45-B64F-DF1C414EDC59}"/>
+    <hyperlink ref="F88" r:id="rId101" xr:uid="{8A532988-D04F-D445-B8FD-AA64E787BB24}"/>
+    <hyperlink ref="F69" r:id="rId102" xr:uid="{D54F73F6-B34C-4044-9163-D80E3A8D31D1}"/>
+    <hyperlink ref="F30" r:id="rId103" xr:uid="{232B5F00-F258-A24E-BDEA-CF2F2635A32D}"/>
+    <hyperlink ref="F93" r:id="rId104" xr:uid="{219994FD-4BE4-D040-8000-FA1EAB97BA79}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Coimbra update: adding A.F.B. Isabel
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E075033-B75E-F447-8BEF-A2675B738D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D52CED-92BA-D746-AE35-BD352D542E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="5560" windowWidth="22920" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="7380" windowWidth="22920" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="459">
   <si>
     <t>LastName</t>
   </si>
@@ -1397,6 +1397,18 @@
   </si>
   <si>
     <t>https://orcid.org/0000-0002-8363-0109</t>
+  </si>
+  <si>
+    <t>Isabel</t>
+  </si>
+  <si>
+    <t>A.F.B.</t>
+  </si>
+  <si>
+    <t>afbisabel@fis.uc.pt</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-8025-8375</t>
   </si>
 </sst>
 </file>
@@ -2249,10 +2261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3315,361 +3327,361 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
-      </c>
-      <c r="E48" t="s">
-        <v>243</v>
-      </c>
-      <c r="F48" t="s">
-        <v>392</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="I48" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>201</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="G49" s="1"/>
+        <v>175</v>
+      </c>
+      <c r="E49" t="s">
+        <v>243</v>
+      </c>
+      <c r="F49" t="s">
+        <v>392</v>
+      </c>
       <c r="H49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I50" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" t="s">
-        <v>299</v>
-      </c>
-      <c r="K50" t="s">
-        <v>295</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>298</v>
+        <v>40</v>
       </c>
       <c r="I51" t="s">
         <v>19</v>
       </c>
+      <c r="J51" t="s">
+        <v>299</v>
+      </c>
+      <c r="K51" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" t="s">
-        <v>100</v>
+        <v>298</v>
       </c>
       <c r="I52" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="I53" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>30</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I54" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>177</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="I55" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I56" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>321</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>178</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>330</v>
+        <v>251</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>298</v>
+        <v>69</v>
       </c>
       <c r="I57" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>321</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>252</v>
+        <v>330</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>47</v>
+        <v>298</v>
       </c>
       <c r="I58" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>107</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I59" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>314</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>315</v>
+        <v>253</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="I60" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>110</v>
+        <v>314</v>
       </c>
       <c r="B61" t="s">
-        <v>180</v>
+        <v>41</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>254</v>
+        <v>315</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I61" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="I62" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B63" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="I63" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B64" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="I64" t="s">
         <v>52</v>
@@ -3677,297 +3689,297 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>298</v>
+        <v>51</v>
       </c>
       <c r="I65" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B66" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" t="s">
-        <v>40</v>
+        <v>298</v>
       </c>
       <c r="I66" t="s">
         <v>19</v>
       </c>
-      <c r="J66" t="s">
-        <v>71</v>
-      </c>
-      <c r="K66" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="I67" t="s">
-        <v>58</v>
+        <v>19</v>
+      </c>
+      <c r="J67" t="s">
+        <v>71</v>
+      </c>
+      <c r="K67" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B68" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="I68" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B69" t="s">
-        <v>122</v>
+        <v>184</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="I69" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B70" t="s">
-        <v>185</v>
+        <v>122</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>413</v>
+        <v>452</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I70" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B71" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I71" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B72" t="s">
-        <v>62</v>
+        <v>186</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I72" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B73" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I73" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B74" t="s">
-        <v>187</v>
+        <v>117</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I74" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F75" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>417</v>
+      </c>
       <c r="G75" s="1"/>
       <c r="H75" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="I75" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>418</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="I76" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="I77" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="I78" t="s">
         <v>19</v>
@@ -3975,58 +3987,58 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G79" s="1"/>
       <c r="H79" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="I79" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B80" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="I80" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B81" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" t="s">
@@ -4038,191 +4050,191 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B82" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" t="s">
-        <v>298</v>
+        <v>53</v>
       </c>
       <c r="I82" t="s">
-        <v>19</v>
-      </c>
-      <c r="J82" t="s">
-        <v>40</v>
-      </c>
-      <c r="K82" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" t="s">
-        <v>49</v>
+        <v>298</v>
       </c>
       <c r="I83" t="s">
         <v>19</v>
       </c>
+      <c r="J83" t="s">
+        <v>40</v>
+      </c>
+      <c r="K83" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
+        <v>9</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="G84" s="2">
-        <v>45718</v>
-      </c>
+        <v>425</v>
+      </c>
+      <c r="G84" s="1"/>
       <c r="H84" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="I84" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B85" t="s">
-        <v>187</v>
-      </c>
-      <c r="C85" t="s">
-        <v>302</v>
+        <v>176</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>276</v>
+        <v>320</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G85" s="2">
-        <v>45779</v>
+        <v>45718</v>
       </c>
       <c r="H85" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I85" t="s">
-        <v>19</v>
-      </c>
-      <c r="K85" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B86" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C86" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>319</v>
+        <v>276</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G86" s="2">
         <v>45779</v>
       </c>
       <c r="H86" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I86" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="K86" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>337</v>
+        <v>139</v>
       </c>
       <c r="B87" t="s">
-        <v>62</v>
+        <v>189</v>
+      </c>
+      <c r="C87" t="s">
+        <v>300</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="G87" s="1"/>
+        <v>428</v>
+      </c>
+      <c r="G87" s="2">
+        <v>45779</v>
+      </c>
       <c r="H87" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="I87" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="B88" t="s">
-        <v>307</v>
+        <v>62</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="G88" s="1"/>
       <c r="H88" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I88" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>140</v>
+        <v>306</v>
       </c>
       <c r="B89" t="s">
-        <v>190</v>
+        <v>307</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>336</v>
+        <v>311</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>430</v>
+        <v>450</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I89" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -4230,17 +4242,17 @@
         <v>140</v>
       </c>
       <c r="B90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="I90" t="s">
         <v>58</v>
@@ -4248,71 +4260,71 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>277</v>
+        <v>324</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="I91" t="s">
-        <v>19</v>
-      </c>
-      <c r="J91" t="s">
-        <v>299</v>
-      </c>
-      <c r="K91" t="s">
-        <v>295</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="B92" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" t="s">
-        <v>293</v>
+        <v>40</v>
       </c>
       <c r="I92" t="s">
-        <v>294</v>
+        <v>19</v>
+      </c>
+      <c r="J92" t="s">
+        <v>299</v>
+      </c>
+      <c r="K92" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>203</v>
+        <v>141</v>
       </c>
       <c r="B93" t="s">
-        <v>317</v>
+        <v>130</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>318</v>
+        <v>278</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>454</v>
+        <v>433</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" t="s">
-        <v>34</v>
+        <v>293</v>
       </c>
       <c r="I93" t="s">
-        <v>35</v>
+        <v>294</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -4320,101 +4332,101 @@
         <v>203</v>
       </c>
       <c r="B94" t="s">
-        <v>204</v>
+        <v>317</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F94" s="1"/>
+        <v>318</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>454</v>
+      </c>
       <c r="G94" s="1"/>
       <c r="H94" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="I94" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="B95" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>434</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I95" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B96" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>279</v>
+        <v>329</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I96" t="s">
-        <v>19</v>
-      </c>
-      <c r="J96" t="s">
-        <v>71</v>
-      </c>
-      <c r="K96" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B97" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I97" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="J97" t="s">
+        <v>71</v>
+      </c>
+      <c r="K97" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B98" t="s">
-        <v>117</v>
+        <v>181</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" t="s">
@@ -4426,98 +4438,98 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B99" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F99" s="1"/>
+        <v>292</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>437</v>
+      </c>
       <c r="G99" s="1"/>
       <c r="H99" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I99" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="B100" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>438</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I100" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>32</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="I101" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>149</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>193</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="I102" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>296</v>
+        <v>202</v>
       </c>
       <c r="B103" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" t="s">
@@ -4529,16 +4541,16 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>150</v>
+        <v>296</v>
       </c>
       <c r="B104" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" t="s">
@@ -4547,167 +4559,188 @@
       <c r="I104" t="s">
         <v>19</v>
       </c>
-      <c r="J104" t="s">
-        <v>151</v>
-      </c>
-      <c r="K104" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>451</v>
+        <v>284</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I105" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J105" t="s">
+        <v>151</v>
+      </c>
+      <c r="K105" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="B106" t="s">
-        <v>199</v>
+        <v>41</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>451</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>443</v>
+      </c>
       <c r="G106" s="1"/>
       <c r="H106" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="I106" t="s">
-        <v>19</v>
-      </c>
-      <c r="J106" t="s">
-        <v>22</v>
-      </c>
-      <c r="K106" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>340</v>
+        <v>198</v>
       </c>
       <c r="B107" t="s">
-        <v>39</v>
+        <v>199</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>444</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="I107" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="J107" t="s">
+        <v>22</v>
+      </c>
+      <c r="K107" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>154</v>
+        <v>340</v>
       </c>
       <c r="B108" t="s">
-        <v>194</v>
+        <v>39</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>286</v>
+        <v>341</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="I108" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>308</v>
+        <v>154</v>
       </c>
       <c r="B109" t="s">
-        <v>309</v>
+        <v>194</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>312</v>
+        <v>286</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="I109" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>155</v>
+        <v>308</v>
       </c>
       <c r="B110" t="s">
-        <v>156</v>
+        <v>309</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G110" s="1"/>
       <c r="H110" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="I110" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="B111" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" t="s">
+        <v>14</v>
+      </c>
+      <c r="I111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>207</v>
+      </c>
+      <c r="B112" t="s">
+        <v>41</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G112" s="1"/>
+      <c r="H112" t="s">
         <v>40</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I112" t="s">
         <v>19</v>
       </c>
-      <c r="J111" t="s">
+      <c r="J112" t="s">
         <v>299</v>
       </c>
-      <c r="K111" t="s">
+      <c r="K112" t="s">
         <v>295</v>
       </c>
     </row>
@@ -4734,89 +4767,91 @@
     <hyperlink ref="E44" r:id="rId19" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
     <hyperlink ref="E45" r:id="rId20" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
     <hyperlink ref="E47" r:id="rId21" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E49" r:id="rId22" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E50" r:id="rId23" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E52" r:id="rId24" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E56" r:id="rId25" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E63" r:id="rId26" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
-    <hyperlink ref="E59" r:id="rId27" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E64" r:id="rId28" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E66" r:id="rId29" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E68" r:id="rId30" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E69" r:id="rId31" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E50" r:id="rId22" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E51" r:id="rId23" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E53" r:id="rId24" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E57" r:id="rId25" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E64" r:id="rId26" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E60" r:id="rId27" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
+    <hyperlink ref="E65" r:id="rId28" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E67" r:id="rId29" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E69" r:id="rId30" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E70" r:id="rId31" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
     <hyperlink ref="E3" r:id="rId32" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E61" r:id="rId33" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E70" r:id="rId34" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E71" r:id="rId35" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E62" r:id="rId33" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E71" r:id="rId34" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E72" r:id="rId35" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
     <hyperlink ref="E25" r:id="rId36" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E72" r:id="rId37" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E73" r:id="rId38" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E74" r:id="rId39" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E75" r:id="rId40" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E76" r:id="rId41" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E77" r:id="rId42" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E78" r:id="rId43" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E80" r:id="rId44" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E82" r:id="rId45" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E83" r:id="rId46" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E84" r:id="rId47" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E85" r:id="rId48" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E89" r:id="rId49" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E91" r:id="rId50" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E96" r:id="rId51" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E98" r:id="rId52" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E99" r:id="rId53" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E100" r:id="rId54" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E101" r:id="rId55" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E102" r:id="rId56" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E104" r:id="rId57" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E105" r:id="rId58" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E108" r:id="rId59" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E110" r:id="rId60" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E111" r:id="rId61" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E55" r:id="rId62" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E67" r:id="rId63" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E90" r:id="rId64" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E97" r:id="rId65" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E73" r:id="rId37" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E74" r:id="rId38" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E75" r:id="rId39" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E76" r:id="rId40" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E77" r:id="rId41" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E78" r:id="rId42" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E79" r:id="rId43" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E81" r:id="rId44" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E83" r:id="rId45" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E84" r:id="rId46" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E85" r:id="rId47" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E86" r:id="rId48" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E90" r:id="rId49" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E92" r:id="rId50" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E97" r:id="rId51" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E99" r:id="rId52" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E100" r:id="rId53" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E101" r:id="rId54" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E102" r:id="rId55" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E103" r:id="rId56" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E105" r:id="rId57" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E106" r:id="rId58" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E109" r:id="rId59" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E111" r:id="rId60" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E112" r:id="rId61" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E56" r:id="rId62" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E68" r:id="rId63" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E91" r:id="rId64" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E98" r:id="rId65" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
     <hyperlink ref="E5" r:id="rId66" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
     <hyperlink ref="E12" r:id="rId67" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E58" r:id="rId68" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E59" r:id="rId68" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
     <hyperlink ref="E7" r:id="rId69" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
     <hyperlink ref="E11" r:id="rId70" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E62" r:id="rId71" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E53" r:id="rId72" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E54" r:id="rId73" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E63" r:id="rId71" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E54" r:id="rId72" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E55" r:id="rId73" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
     <hyperlink ref="E8" r:id="rId74" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E51" r:id="rId75" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E65" r:id="rId76" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E92" r:id="rId77" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E106" r:id="rId78" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E79" r:id="rId79" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E52" r:id="rId75" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E66" r:id="rId76" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E93" r:id="rId77" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E107" r:id="rId78" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E80" r:id="rId79" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId80" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E103" r:id="rId81" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E104" r:id="rId81" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
     <hyperlink ref="E26" r:id="rId82" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E81" r:id="rId83" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E88" r:id="rId84" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E109" r:id="rId85" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E82" r:id="rId83" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E89" r:id="rId84" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E110" r:id="rId85" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
     <hyperlink ref="E24" r:id="rId86" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
-    <hyperlink ref="E60" r:id="rId87" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
-    <hyperlink ref="E93" r:id="rId88" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
-    <hyperlink ref="E86" r:id="rId89" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E61" r:id="rId87" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E94" r:id="rId88" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E87" r:id="rId89" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
     <hyperlink ref="E33" r:id="rId90" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
-    <hyperlink ref="E94" r:id="rId91" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
-    <hyperlink ref="E87" r:id="rId92" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
-    <hyperlink ref="E95" r:id="rId93" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
-    <hyperlink ref="E57" r:id="rId94" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
+    <hyperlink ref="E95" r:id="rId91" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
+    <hyperlink ref="E88" r:id="rId92" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
+    <hyperlink ref="E96" r:id="rId93" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
+    <hyperlink ref="E58" r:id="rId94" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
     <hyperlink ref="E28" r:id="rId95" xr:uid="{E24B841F-2272-CA43-9614-50B7F36AD8C5}"/>
     <hyperlink ref="E13" r:id="rId96" xr:uid="{29460556-99EB-6943-BF02-EAF45B9A2438}"/>
-    <hyperlink ref="E107" r:id="rId97" xr:uid="{31EA1686-1B20-3342-8310-E26369FFF7C2}"/>
+    <hyperlink ref="E108" r:id="rId97" xr:uid="{31EA1686-1B20-3342-8310-E26369FFF7C2}"/>
     <hyperlink ref="E21" r:id="rId98" xr:uid="{BFCD233B-85C4-684A-9E1F-CFD7E946453F}"/>
     <hyperlink ref="E15" r:id="rId99" tooltip="abayo@lsc-canfranc.es" display="mailto:abayo@lsc-canfranc.es" xr:uid="{9D231E2D-796B-5044-A575-DB475A1F4009}"/>
     <hyperlink ref="E22" r:id="rId100" tooltip="lcid@lsc-canfranc.es" display="mailto:lcid@lsc-canfranc.es" xr:uid="{2505E3E3-5341-1F45-B64F-DF1C414EDC59}"/>
-    <hyperlink ref="F88" r:id="rId101" xr:uid="{8A532988-D04F-D445-B8FD-AA64E787BB24}"/>
-    <hyperlink ref="F69" r:id="rId102" xr:uid="{D54F73F6-B34C-4044-9163-D80E3A8D31D1}"/>
+    <hyperlink ref="F89" r:id="rId101" xr:uid="{8A532988-D04F-D445-B8FD-AA64E787BB24}"/>
+    <hyperlink ref="F70" r:id="rId102" xr:uid="{D54F73F6-B34C-4044-9163-D80E3A8D31D1}"/>
     <hyperlink ref="F30" r:id="rId103" xr:uid="{232B5F00-F258-A24E-BDEA-CF2F2635A32D}"/>
-    <hyperlink ref="F93" r:id="rId104" xr:uid="{219994FD-4BE4-D040-8000-FA1EAB97BA79}"/>
+    <hyperlink ref="F94" r:id="rId104" xr:uid="{219994FD-4BE4-D040-8000-FA1EAB97BA79}"/>
+    <hyperlink ref="E48" r:id="rId105" xr:uid="{5120D118-05B0-D540-BE4F-B9DCCD52040C}"/>
+    <hyperlink ref="F48" r:id="rId106" xr:uid="{BCA8D2A5-D5BD-AF4B-8D5E-2A79F1997BDF}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
four additions to igfae, dipc and ific: y. ayyad, m. cid, x.cid, p. vazquez
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjpjones/Documents/Work/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD88E3AC-9AA3-0845-BC9E-66C789EABD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111C7AF2-62EA-9447-9602-853B89650C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="760" windowWidth="22920" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="2400" windowWidth="22920" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="470">
   <si>
     <t>LastName</t>
   </si>
@@ -1409,6 +1409,39 @@
   </si>
   <si>
     <t>benjamin.jones-7@manchester.ac.uk</t>
+  </si>
+  <si>
+    <t>Ayyad</t>
+  </si>
+  <si>
+    <t>yassid.ayyad@usc.es</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-8604-4976</t>
+  </si>
+  <si>
+    <t>X.</t>
+  </si>
+  <si>
+    <t>xabier.cid@usc.es</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-0468-541X</t>
+  </si>
+  <si>
+    <t>maria.cid.laso@ific.uv.es</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0009-0003-4979-5668</t>
+  </si>
+  <si>
+    <t>V\'azquez Cabaleiro</t>
+  </si>
+  <si>
+    <t>pablo.vazquez@dipc.org</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0009-0007-0098-8927</t>
   </si>
 </sst>
 </file>
@@ -1965,9 +1998,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2005,7 +2038,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2111,7 +2144,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2253,7 +2286,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2261,10 +2294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="K112" sqref="K112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2484,415 +2517,421 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>459</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>215</v>
+        <v>460</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>354</v>
+        <v>461</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="G11" s="2">
-        <v>45718</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>355</v>
+      </c>
+      <c r="G12" s="2">
+        <v>45718</v>
+      </c>
       <c r="H12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>332</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>333</v>
+        <v>164</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>334</v>
+        <v>217</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>332</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>218</v>
-      </c>
-      <c r="F14" t="s">
-        <v>358</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G14" s="1"/>
       <c r="H14" t="s">
         <v>40</v>
       </c>
       <c r="I14" t="s">
         <v>19</v>
       </c>
-      <c r="J14" t="s">
-        <v>298</v>
-      </c>
-      <c r="K14" t="s">
-        <v>294</v>
-      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>342</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="G15" s="2">
-        <v>45714</v>
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>218</v>
+      </c>
+      <c r="F15" t="s">
+        <v>358</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I15" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>298</v>
+      </c>
+      <c r="K15" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>342</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>219</v>
+        <v>343</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>359</v>
+      </c>
+      <c r="G16" s="2">
+        <v>45714</v>
+      </c>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I16" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I17" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>363</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>165</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" t="s">
-        <v>49</v>
-      </c>
-      <c r="K18" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>363</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>221</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I19" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>192</v>
-      </c>
-      <c r="E20" t="s">
-        <v>223</v>
-      </c>
-      <c r="F20" t="s">
-        <v>364</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I20" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="E21" t="s">
+        <v>223</v>
+      </c>
+      <c r="F21" t="s">
+        <v>364</v>
+      </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>341</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>344</v>
+        <v>224</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="G22" s="2">
-        <v>45714</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="G22" s="1"/>
       <c r="H22" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="I22" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>341</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
-      </c>
-      <c r="C23" t="s">
-        <v>300</v>
+        <v>56</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>225</v>
+        <v>344</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>366</v>
+      </c>
+      <c r="G23" s="2">
+        <v>45714</v>
+      </c>
       <c r="H23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I23" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>309</v>
+        <v>341</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>312</v>
+        <v>465</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>466</v>
+      </c>
+      <c r="G24" s="2"/>
       <c r="H24" t="s">
         <v>53</v>
       </c>
       <c r="I24" t="s">
         <v>54</v>
       </c>
+      <c r="J24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>341</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>462</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>226</v>
+        <v>463</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>464</v>
+      </c>
+      <c r="G25" s="2"/>
       <c r="H25" t="s">
-        <v>297</v>
+        <v>63</v>
       </c>
       <c r="I25" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>302</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>157</v>
+      </c>
+      <c r="C26" t="s">
+        <v>300</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>309</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>227</v>
+        <v>312</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>330</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>60</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>331</v>
+        <v>226</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>40</v>
+        <v>297</v>
       </c>
       <c r="I28" t="s">
         <v>19</v>
@@ -2900,403 +2939,404 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>373</v>
+        <v>302</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="I29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" t="s">
-        <v>229</v>
+        <v>62</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>452</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I30" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" t="s">
-        <v>298</v>
-      </c>
-      <c r="K30" t="s">
-        <v>294</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>330</v>
       </c>
       <c r="B31" t="s">
-        <v>168</v>
-      </c>
-      <c r="E31" t="s">
-        <v>230</v>
-      </c>
-      <c r="F31" t="s">
-        <v>374</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="I31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>373</v>
       </c>
       <c r="B32" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" t="s">
-        <v>325</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="G32" s="2">
-        <v>45779</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="I32" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>321</v>
+        <v>39</v>
+      </c>
+      <c r="E33" t="s">
+        <v>229</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="G33" s="1"/>
+        <v>452</v>
+      </c>
       <c r="H33" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="I33" t="s">
-        <v>58</v>
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>298</v>
+      </c>
+      <c r="K33" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" t="s">
-        <v>326</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="G34" s="2">
-        <v>45496</v>
+        <v>168</v>
+      </c>
+      <c r="E34" t="s">
+        <v>230</v>
+      </c>
+      <c r="F34" t="s">
+        <v>374</v>
       </c>
       <c r="H34" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="I34" t="s">
-        <v>19</v>
-      </c>
-      <c r="J34" t="s">
-        <v>71</v>
-      </c>
-      <c r="K34" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" t="s">
-        <v>233</v>
-      </c>
-      <c r="F35" t="s">
-        <v>378</v>
+        <v>168</v>
+      </c>
+      <c r="C35" t="s">
+        <v>325</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G35" s="2">
+        <v>45779</v>
       </c>
       <c r="H35" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="I35" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" t="s">
-        <v>234</v>
-      </c>
-      <c r="F36" t="s">
-        <v>379</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="I36" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" t="s">
-        <v>71</v>
-      </c>
-      <c r="K36" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>206</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" t="s">
-        <v>235</v>
-      </c>
-      <c r="F37" t="s">
-        <v>380</v>
+        <v>170</v>
+      </c>
+      <c r="C37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G37" s="2">
+        <v>45496</v>
       </c>
       <c r="H37" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="I37" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="J37" t="s">
+        <v>71</v>
+      </c>
+      <c r="K37" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F38" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H38" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="I38" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" t="s">
-        <v>71</v>
-      </c>
-      <c r="K38" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>196</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="G39" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E39" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" t="s">
+        <v>379</v>
+      </c>
       <c r="H39" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I39" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K39" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>206</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="G40" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="E40" t="s">
+        <v>235</v>
+      </c>
+      <c r="F40" t="s">
+        <v>380</v>
+      </c>
       <c r="H40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I40" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>167</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="G41" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" t="s">
+        <v>236</v>
+      </c>
+      <c r="F41" t="s">
+        <v>381</v>
+      </c>
       <c r="H41" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="I41" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="J41" t="s">
+        <v>71</v>
+      </c>
+      <c r="K41" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>322</v>
+        <v>237</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="I42" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="I43" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>290</v>
+        <v>239</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" t="s">
-        <v>292</v>
+        <v>86</v>
       </c>
       <c r="I44" t="s">
-        <v>293</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>240</v>
+        <v>322</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="I45" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" t="s">
-        <v>241</v>
-      </c>
-      <c r="F46" t="s">
-        <v>389</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G46" s="1"/>
       <c r="H46" t="s">
         <v>63</v>
       </c>
@@ -3306,174 +3346,167 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>242</v>
+        <v>290</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" t="s">
-        <v>24</v>
+        <v>292</v>
       </c>
       <c r="I47" t="s">
-        <v>67</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>454</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>455</v>
+        <v>173</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>456</v>
+        <v>240</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>457</v>
+        <v>388</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="I48" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>175</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>458</v>
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>241</v>
       </c>
       <c r="F49" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H49" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="I49" t="s">
-        <v>52</v>
-      </c>
-      <c r="J49" t="s">
-        <v>14</v>
-      </c>
-      <c r="K49" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="I50" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>454</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>455</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>244</v>
+        <v>456</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>393</v>
+        <v>457</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="I51" t="s">
-        <v>19</v>
-      </c>
-      <c r="J51" t="s">
-        <v>298</v>
-      </c>
-      <c r="K51" t="s">
-        <v>294</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="G52" s="1"/>
+        <v>458</v>
+      </c>
+      <c r="F52" t="s">
+        <v>391</v>
+      </c>
       <c r="H52" t="s">
-        <v>297</v>
+        <v>51</v>
       </c>
       <c r="I52" t="s">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="J52" t="s">
+        <v>14</v>
+      </c>
+      <c r="K52" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>201</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="I53" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
@@ -3482,978 +3515,978 @@
       <c r="I54" t="s">
         <v>19</v>
       </c>
+      <c r="J54" t="s">
+        <v>298</v>
+      </c>
+      <c r="K54" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>41</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>53</v>
+        <v>297</v>
       </c>
       <c r="I55" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="I56" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>178</v>
+        <v>30</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="I57" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>320</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>177</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>329</v>
+        <v>248</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>297</v>
+        <v>53</v>
       </c>
       <c r="I58" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="I59" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I60" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="B61" t="s">
         <v>41</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>17</v>
+        <v>297</v>
       </c>
       <c r="I61" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>180</v>
+        <v>107</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="I62" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" t="s">
         <v>53</v>
       </c>
       <c r="I63" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>313</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="I64" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B65" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="I65" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B66" t="s">
-        <v>117</v>
+        <v>181</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" t="s">
-        <v>297</v>
+        <v>53</v>
       </c>
       <c r="I66" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>182</v>
+        <v>113</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="I67" t="s">
-        <v>19</v>
-      </c>
-      <c r="J67" t="s">
-        <v>71</v>
-      </c>
-      <c r="K67" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B68" t="s">
-        <v>183</v>
+        <v>115</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="I68" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B69" t="s">
-        <v>184</v>
+        <v>117</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" t="s">
-        <v>17</v>
+        <v>297</v>
       </c>
       <c r="I69" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B70" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>451</v>
+        <v>409</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I70" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="J70" t="s">
+        <v>71</v>
+      </c>
+      <c r="K70" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B71" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I71" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B72" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="I72" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B73" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>414</v>
+        <v>451</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I73" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B74" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="I74" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="I75" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>62</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F76" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>414</v>
+      </c>
       <c r="G76" s="1"/>
       <c r="H76" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="I76" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I77" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>200</v>
+        <v>127</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I78" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>419</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="I79" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I80" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>200</v>
       </c>
       <c r="B81" t="s">
-        <v>181</v>
+        <v>41</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="I81" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B82" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I82" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B83" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" t="s">
-        <v>297</v>
+        <v>63</v>
       </c>
       <c r="I83" t="s">
-        <v>19</v>
-      </c>
-      <c r="J83" t="s">
-        <v>40</v>
-      </c>
-      <c r="K83" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G84" s="1"/>
       <c r="H84" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I84" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B85" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="G85" s="2">
-        <v>45718</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="G85" s="1"/>
       <c r="H85" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="I85" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B86" t="s">
-        <v>187</v>
-      </c>
-      <c r="C86" t="s">
-        <v>301</v>
+        <v>130</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="G86" s="2">
-        <v>45779</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="G86" s="1"/>
       <c r="H86" t="s">
-        <v>40</v>
+        <v>297</v>
       </c>
       <c r="I86" t="s">
         <v>19</v>
       </c>
+      <c r="J86" t="s">
+        <v>40</v>
+      </c>
       <c r="K86" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
-      </c>
-      <c r="C87" t="s">
-        <v>299</v>
+        <v>9</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>318</v>
+        <v>274</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="G87" s="2">
-        <v>45779</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="G87" s="1"/>
       <c r="H87" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I87" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>336</v>
+        <v>137</v>
       </c>
       <c r="B88" t="s">
-        <v>62</v>
+        <v>176</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="G88" s="1"/>
+        <v>425</v>
+      </c>
+      <c r="G88" s="2">
+        <v>45718</v>
+      </c>
       <c r="H88" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="I88" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>305</v>
+        <v>138</v>
       </c>
       <c r="B89" t="s">
-        <v>306</v>
+        <v>187</v>
+      </c>
+      <c r="C89" t="s">
+        <v>301</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="G89" s="1"/>
+        <v>426</v>
+      </c>
+      <c r="G89" s="2">
+        <v>45779</v>
+      </c>
       <c r="H89" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I89" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="K89" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B90" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="C90" t="s">
+        <v>299</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="G90" s="1"/>
+        <v>427</v>
+      </c>
+      <c r="G90" s="2">
+        <v>45779</v>
+      </c>
       <c r="H90" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I90" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>140</v>
+        <v>336</v>
       </c>
       <c r="B91" t="s">
-        <v>191</v>
+        <v>62</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="I91" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>305</v>
       </c>
       <c r="B92" t="s">
-        <v>39</v>
+        <v>306</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>276</v>
+        <v>310</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>431</v>
+        <v>449</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I92" t="s">
-        <v>19</v>
-      </c>
-      <c r="J92" t="s">
-        <v>298</v>
-      </c>
-      <c r="K92" t="s">
-        <v>294</v>
+        <v>54</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B93" t="s">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>277</v>
+        <v>335</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" t="s">
-        <v>292</v>
+        <v>47</v>
       </c>
       <c r="I93" t="s">
-        <v>293</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>203</v>
+        <v>140</v>
       </c>
       <c r="B94" t="s">
-        <v>316</v>
+        <v>191</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="G94" s="1"/>
       <c r="H94" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="I94" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B95" t="s">
-        <v>204</v>
+        <v>39</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F95" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>431</v>
+      </c>
       <c r="G95" s="1"/>
       <c r="H95" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="I95" t="s">
-        <v>58</v>
+        <v>19</v>
+      </c>
+      <c r="J95" t="s">
+        <v>298</v>
+      </c>
+      <c r="K95" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B96" t="s">
-        <v>192</v>
+        <v>130</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>328</v>
+        <v>277</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" t="s">
-        <v>53</v>
+        <v>292</v>
       </c>
       <c r="I96" t="s">
-        <v>54</v>
+        <v>293</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>143</v>
+        <v>203</v>
       </c>
       <c r="B97" t="s">
-        <v>144</v>
+        <v>316</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>278</v>
+        <v>317</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>434</v>
+        <v>453</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I97" t="s">
-        <v>19</v>
-      </c>
-      <c r="J97" t="s">
-        <v>71</v>
-      </c>
-      <c r="K97" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="B98" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>435</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I98" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B99" t="s">
-        <v>117</v>
+        <v>192</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>291</v>
+        <v>328</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" t="s">
@@ -4465,35 +4498,43 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B100" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F100" s="1"/>
+        <v>278</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="G100" s="1"/>
       <c r="H100" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="I100" t="s">
-        <v>58</v>
+        <v>19</v>
+      </c>
+      <c r="J100" t="s">
+        <v>71</v>
+      </c>
+      <c r="K100" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="B101" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" t="s">
@@ -4505,126 +4546,120 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B102" t="s">
-        <v>193</v>
+        <v>117</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="I102" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>202</v>
+        <v>147</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>439</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="I103" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>295</v>
+        <v>205</v>
       </c>
       <c r="B104" t="s">
         <v>32</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I104" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B105" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="I105" t="s">
-        <v>19</v>
-      </c>
-      <c r="J105" t="s">
-        <v>151</v>
-      </c>
-      <c r="K105" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>450</v>
+        <v>282</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="G106" s="1"/>
       <c r="H106" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I106" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>295</v>
       </c>
       <c r="B107" t="s">
-        <v>199</v>
+        <v>32</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F107" s="1"/>
+        <v>296</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="G107" s="1"/>
       <c r="H107" t="s">
         <v>40</v>
@@ -4632,109 +4667,113 @@
       <c r="I107" t="s">
         <v>19</v>
       </c>
-      <c r="J107" t="s">
-        <v>22</v>
-      </c>
-      <c r="K107" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>339</v>
+        <v>150</v>
       </c>
       <c r="B108" t="s">
-        <v>39</v>
+        <v>179</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>340</v>
+        <v>283</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="I108" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="J108" t="s">
+        <v>151</v>
+      </c>
+      <c r="K108" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B109" t="s">
-        <v>194</v>
+        <v>41</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>285</v>
+        <v>450</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="I109" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>307</v>
+        <v>198</v>
       </c>
       <c r="B110" t="s">
-        <v>308</v>
+        <v>199</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>445</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I110" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="J110" t="s">
+        <v>22</v>
+      </c>
+      <c r="K110" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>155</v>
+        <v>339</v>
       </c>
       <c r="B111" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>286</v>
+        <v>340</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="I111" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>207</v>
+        <v>467</v>
       </c>
       <c r="B112" t="s">
-        <v>41</v>
+        <v>306</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>287</v>
+        <v>468</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>447</v>
+        <v>469</v>
       </c>
       <c r="G112" s="1"/>
       <c r="H112" t="s">
@@ -4744,9 +4783,99 @@
         <v>19</v>
       </c>
       <c r="J112" t="s">
+        <v>63</v>
+      </c>
+      <c r="K112" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>154</v>
+      </c>
+      <c r="B113" t="s">
+        <v>194</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G113" s="1"/>
+      <c r="H113" t="s">
+        <v>34</v>
+      </c>
+      <c r="I113" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>307</v>
+      </c>
+      <c r="B114" t="s">
+        <v>308</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G114" s="1"/>
+      <c r="H114" t="s">
+        <v>53</v>
+      </c>
+      <c r="I114" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>155</v>
+      </c>
+      <c r="B115" t="s">
+        <v>156</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G115" s="1"/>
+      <c r="H115" t="s">
+        <v>14</v>
+      </c>
+      <c r="I115" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" t="s">
+        <v>41</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G116" s="1"/>
+      <c r="H116" t="s">
+        <v>40</v>
+      </c>
+      <c r="I116" t="s">
+        <v>19</v>
+      </c>
+      <c r="J116" t="s">
         <v>298</v>
       </c>
-      <c r="K112" t="s">
+      <c r="K116" t="s">
         <v>294</v>
       </c>
     </row>
@@ -4755,110 +4884,119 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{0FF3DA65-AAFE-A544-B83F-3B8DBBA655D2}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{D72FCA14-EA08-4749-BB11-D24B8A62C2FD}"/>
     <hyperlink ref="E9" r:id="rId3" xr:uid="{E6DBC748-9C42-444A-9719-EDB7AD21ED31}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{D72F2EFB-3573-5D41-9B63-CA5C8A903FE7}"/>
-    <hyperlink ref="E16" r:id="rId5" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
-    <hyperlink ref="E17" r:id="rId6" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
-    <hyperlink ref="E18" r:id="rId7" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
-    <hyperlink ref="E19" r:id="rId8" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
-    <hyperlink ref="E23" r:id="rId9" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
-    <hyperlink ref="E27" r:id="rId10" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
-    <hyperlink ref="E29" r:id="rId11" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
-    <hyperlink ref="E32" r:id="rId12" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
-    <hyperlink ref="E34" r:id="rId13" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
-    <hyperlink ref="E39" r:id="rId14" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
-    <hyperlink ref="E40" r:id="rId15" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
-    <hyperlink ref="E41" r:id="rId16" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
-    <hyperlink ref="E42" r:id="rId17" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
-    <hyperlink ref="E43" r:id="rId18" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
-    <hyperlink ref="E44" r:id="rId19" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
-    <hyperlink ref="E45" r:id="rId20" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
-    <hyperlink ref="E47" r:id="rId21" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
-    <hyperlink ref="E50" r:id="rId22" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
-    <hyperlink ref="E51" r:id="rId23" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
-    <hyperlink ref="E53" r:id="rId24" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
-    <hyperlink ref="E57" r:id="rId25" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
-    <hyperlink ref="E64" r:id="rId26" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
-    <hyperlink ref="E60" r:id="rId27" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
-    <hyperlink ref="E65" r:id="rId28" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
-    <hyperlink ref="E67" r:id="rId29" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
-    <hyperlink ref="E69" r:id="rId30" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
-    <hyperlink ref="E70" r:id="rId31" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{D72F2EFB-3573-5D41-9B63-CA5C8A903FE7}"/>
+    <hyperlink ref="E17" r:id="rId5" xr:uid="{7BA53910-2895-8546-8C78-4ADAECEB1354}"/>
+    <hyperlink ref="E18" r:id="rId6" xr:uid="{5B370D66-5FA2-8A4A-A92C-48946FC643B8}"/>
+    <hyperlink ref="E19" r:id="rId7" xr:uid="{E1E20BC8-2BB4-C34E-8CA8-2ED92BB0838B}"/>
+    <hyperlink ref="E20" r:id="rId8" xr:uid="{77E75D5E-F948-2248-A233-77176542B4F7}"/>
+    <hyperlink ref="E26" r:id="rId9" xr:uid="{D9028AA5-E4C8-9E40-BF28-A681BB8D6B4F}"/>
+    <hyperlink ref="E30" r:id="rId10" xr:uid="{221B0995-0A38-FC4A-A9DC-9EFA0954E180}"/>
+    <hyperlink ref="E32" r:id="rId11" xr:uid="{2B53C67F-39F7-4A49-99C5-3CED9DB96DF6}"/>
+    <hyperlink ref="E35" r:id="rId12" xr:uid="{B022962F-480B-E242-A4EB-4B4743EC7105}"/>
+    <hyperlink ref="E37" r:id="rId13" xr:uid="{3503F030-FF3A-A74C-AECE-58009DA1DD3E}"/>
+    <hyperlink ref="E42" r:id="rId14" xr:uid="{CEB8BAB9-B042-A34A-B635-6BCBB758D6F8}"/>
+    <hyperlink ref="E43" r:id="rId15" xr:uid="{8D9B2120-0137-C040-A53B-A370B9044CCB}"/>
+    <hyperlink ref="E44" r:id="rId16" xr:uid="{5EAE9946-74A0-2C4C-AF2E-8CC318946DFB}"/>
+    <hyperlink ref="E45" r:id="rId17" xr:uid="{414E8F76-C9B5-D043-B8F7-66A7AC4FE7F9}"/>
+    <hyperlink ref="E46" r:id="rId18" xr:uid="{966468A2-ECAE-E547-B0CC-F5EEA43C95E6}"/>
+    <hyperlink ref="E47" r:id="rId19" xr:uid="{AFBA781B-74EA-4D43-8C5C-3770401790AE}"/>
+    <hyperlink ref="E48" r:id="rId20" xr:uid="{C8972E3C-E75C-D849-9CB4-7D042B3A8058}"/>
+    <hyperlink ref="E50" r:id="rId21" xr:uid="{E94A7644-CFDA-1B41-B9B5-14C74A38FCFD}"/>
+    <hyperlink ref="E53" r:id="rId22" xr:uid="{13FE86C5-4070-A048-A059-C6DC8EEBBBCF}"/>
+    <hyperlink ref="E54" r:id="rId23" xr:uid="{5DCB360F-CBC0-3848-977E-6DFD9444FE4F}"/>
+    <hyperlink ref="E56" r:id="rId24" xr:uid="{A6AE4BE4-E884-1F4F-B788-7A25EF443B8B}"/>
+    <hyperlink ref="E60" r:id="rId25" xr:uid="{026C17E2-2748-6C44-8FE8-0DE2C3EB30ED}"/>
+    <hyperlink ref="E67" r:id="rId26" xr:uid="{095CF6B6-9288-374C-AD52-210A596D5626}"/>
+    <hyperlink ref="E63" r:id="rId27" xr:uid="{202BDED9-0922-6A41-B69F-23FD343F7EF9}"/>
+    <hyperlink ref="E68" r:id="rId28" xr:uid="{33C97671-253E-254F-B62A-44FA310DB5B1}"/>
+    <hyperlink ref="E70" r:id="rId29" xr:uid="{00ECC68F-EE1A-1D4B-BBA5-7072FC5E7FCD}"/>
+    <hyperlink ref="E72" r:id="rId30" xr:uid="{99B3B958-BD25-0447-8385-625DDAE1EBF7}"/>
+    <hyperlink ref="E73" r:id="rId31" xr:uid="{24414099-AF95-D943-813C-2818DFD559F1}"/>
     <hyperlink ref="E3" r:id="rId32" xr:uid="{3A3CFB2D-9550-DB47-876D-1CF2172ED36B}"/>
-    <hyperlink ref="E62" r:id="rId33" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
-    <hyperlink ref="E71" r:id="rId34" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
-    <hyperlink ref="E72" r:id="rId35" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
-    <hyperlink ref="E25" r:id="rId36" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
-    <hyperlink ref="E73" r:id="rId37" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E74" r:id="rId38" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E75" r:id="rId39" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E76" r:id="rId40" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E77" r:id="rId41" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E78" r:id="rId42" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E79" r:id="rId43" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E81" r:id="rId44" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E83" r:id="rId45" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E84" r:id="rId46" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E85" r:id="rId47" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E86" r:id="rId48" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E90" r:id="rId49" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E92" r:id="rId50" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E97" r:id="rId51" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E99" r:id="rId52" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E100" r:id="rId53" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E101" r:id="rId54" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E102" r:id="rId55" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E103" r:id="rId56" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E105" r:id="rId57" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E106" r:id="rId58" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E109" r:id="rId59" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E111" r:id="rId60" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E112" r:id="rId61" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
-    <hyperlink ref="E56" r:id="rId62" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
-    <hyperlink ref="E68" r:id="rId63" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E91" r:id="rId64" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E98" r:id="rId65" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E65" r:id="rId33" xr:uid="{12E6E42C-6AD1-7B4D-9597-0E457430B2D1}"/>
+    <hyperlink ref="E74" r:id="rId34" xr:uid="{F84050AF-F022-0C4E-98B2-C03F3E8C81DA}"/>
+    <hyperlink ref="E75" r:id="rId35" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
+    <hyperlink ref="E28" r:id="rId36" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
+    <hyperlink ref="E76" r:id="rId37" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
+    <hyperlink ref="E77" r:id="rId38" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E78" r:id="rId39" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E79" r:id="rId40" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E80" r:id="rId41" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E81" r:id="rId42" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E82" r:id="rId43" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E84" r:id="rId44" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E86" r:id="rId45" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E87" r:id="rId46" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E88" r:id="rId47" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E89" r:id="rId48" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E93" r:id="rId49" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E95" r:id="rId50" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E100" r:id="rId51" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E102" r:id="rId52" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E103" r:id="rId53" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E104" r:id="rId54" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E105" r:id="rId55" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E106" r:id="rId56" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E108" r:id="rId57" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E109" r:id="rId58" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E113" r:id="rId59" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E115" r:id="rId60" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E116" r:id="rId61" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E59" r:id="rId62" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
+    <hyperlink ref="E71" r:id="rId63" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
+    <hyperlink ref="E94" r:id="rId64" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E101" r:id="rId65" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
     <hyperlink ref="E5" r:id="rId66" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
-    <hyperlink ref="E12" r:id="rId67" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
-    <hyperlink ref="E59" r:id="rId68" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
+    <hyperlink ref="E13" r:id="rId67" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
+    <hyperlink ref="E62" r:id="rId68" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
     <hyperlink ref="E7" r:id="rId69" display="mailto:isaac.arnquist@pnnl.gov" xr:uid="{308E6526-5B60-F34F-A8F5-559BEC15710C}"/>
-    <hyperlink ref="E11" r:id="rId70" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
-    <hyperlink ref="E63" r:id="rId71" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
-    <hyperlink ref="E54" r:id="rId72" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
-    <hyperlink ref="E55" r:id="rId73" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
+    <hyperlink ref="E12" r:id="rId70" display="mailto:kevin_bailey@anl.gov" xr:uid="{C7A6318C-B3D3-A24F-A8E4-7E9174A7398D}"/>
+    <hyperlink ref="E66" r:id="rId71" xr:uid="{8900F105-F9A6-2F49-9B19-4BBA98DEDE9B}"/>
+    <hyperlink ref="E57" r:id="rId72" xr:uid="{1CACE84F-E2CD-C74C-AEA1-D2928BFA4503}"/>
+    <hyperlink ref="E58" r:id="rId73" xr:uid="{3D7385AE-56EF-A342-A0D1-586DDD8AF4BE}"/>
     <hyperlink ref="E8" r:id="rId74" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
-    <hyperlink ref="E52" r:id="rId75" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
-    <hyperlink ref="E66" r:id="rId76" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E93" r:id="rId77" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E107" r:id="rId78" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E80" r:id="rId79" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E55" r:id="rId75" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
+    <hyperlink ref="E69" r:id="rId76" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
+    <hyperlink ref="E96" r:id="rId77" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E110" r:id="rId78" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E83" r:id="rId79" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId80" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E104" r:id="rId81" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
-    <hyperlink ref="E26" r:id="rId82" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E82" r:id="rId83" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E89" r:id="rId84" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E110" r:id="rId85" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
-    <hyperlink ref="E24" r:id="rId86" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
-    <hyperlink ref="E61" r:id="rId87" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
-    <hyperlink ref="E94" r:id="rId88" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
-    <hyperlink ref="E87" r:id="rId89" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
-    <hyperlink ref="E33" r:id="rId90" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
-    <hyperlink ref="E95" r:id="rId91" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
-    <hyperlink ref="E88" r:id="rId92" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
-    <hyperlink ref="E96" r:id="rId93" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
-    <hyperlink ref="E58" r:id="rId94" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
-    <hyperlink ref="E28" r:id="rId95" xr:uid="{E24B841F-2272-CA43-9614-50B7F36AD8C5}"/>
-    <hyperlink ref="E13" r:id="rId96" xr:uid="{29460556-99EB-6943-BF02-EAF45B9A2438}"/>
-    <hyperlink ref="E108" r:id="rId97" xr:uid="{31EA1686-1B20-3342-8310-E26369FFF7C2}"/>
-    <hyperlink ref="E21" r:id="rId98" xr:uid="{BFCD233B-85C4-684A-9E1F-CFD7E946453F}"/>
-    <hyperlink ref="E15" r:id="rId99" tooltip="abayo@lsc-canfranc.es" display="mailto:abayo@lsc-canfranc.es" xr:uid="{9D231E2D-796B-5044-A575-DB475A1F4009}"/>
-    <hyperlink ref="E22" r:id="rId100" tooltip="lcid@lsc-canfranc.es" display="mailto:lcid@lsc-canfranc.es" xr:uid="{2505E3E3-5341-1F45-B64F-DF1C414EDC59}"/>
-    <hyperlink ref="F89" r:id="rId101" xr:uid="{8A532988-D04F-D445-B8FD-AA64E787BB24}"/>
-    <hyperlink ref="F70" r:id="rId102" xr:uid="{D54F73F6-B34C-4044-9163-D80E3A8D31D1}"/>
-    <hyperlink ref="F30" r:id="rId103" xr:uid="{232B5F00-F258-A24E-BDEA-CF2F2635A32D}"/>
-    <hyperlink ref="F94" r:id="rId104" xr:uid="{219994FD-4BE4-D040-8000-FA1EAB97BA79}"/>
-    <hyperlink ref="E48" r:id="rId105" xr:uid="{5120D118-05B0-D540-BE4F-B9DCCD52040C}"/>
-    <hyperlink ref="F48" r:id="rId106" xr:uid="{BCA8D2A5-D5BD-AF4B-8D5E-2A79F1997BDF}"/>
-    <hyperlink ref="E49" r:id="rId107" xr:uid="{2D132A55-81FD-AD46-B0BE-C908F8D920E8}"/>
+    <hyperlink ref="E107" r:id="rId81" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E29" r:id="rId82" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
+    <hyperlink ref="E85" r:id="rId83" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E92" r:id="rId84" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E114" r:id="rId85" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E27" r:id="rId86" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
+    <hyperlink ref="E64" r:id="rId87" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
+    <hyperlink ref="E97" r:id="rId88" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E90" r:id="rId89" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E36" r:id="rId90" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
+    <hyperlink ref="E98" r:id="rId91" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
+    <hyperlink ref="E91" r:id="rId92" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
+    <hyperlink ref="E99" r:id="rId93" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
+    <hyperlink ref="E61" r:id="rId94" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
+    <hyperlink ref="E31" r:id="rId95" xr:uid="{E24B841F-2272-CA43-9614-50B7F36AD8C5}"/>
+    <hyperlink ref="E14" r:id="rId96" xr:uid="{29460556-99EB-6943-BF02-EAF45B9A2438}"/>
+    <hyperlink ref="E111" r:id="rId97" xr:uid="{31EA1686-1B20-3342-8310-E26369FFF7C2}"/>
+    <hyperlink ref="E22" r:id="rId98" xr:uid="{BFCD233B-85C4-684A-9E1F-CFD7E946453F}"/>
+    <hyperlink ref="E16" r:id="rId99" tooltip="abayo@lsc-canfranc.es" display="mailto:abayo@lsc-canfranc.es" xr:uid="{9D231E2D-796B-5044-A575-DB475A1F4009}"/>
+    <hyperlink ref="E23" r:id="rId100" tooltip="lcid@lsc-canfranc.es" display="mailto:lcid@lsc-canfranc.es" xr:uid="{2505E3E3-5341-1F45-B64F-DF1C414EDC59}"/>
+    <hyperlink ref="F92" r:id="rId101" xr:uid="{8A532988-D04F-D445-B8FD-AA64E787BB24}"/>
+    <hyperlink ref="F73" r:id="rId102" xr:uid="{D54F73F6-B34C-4044-9163-D80E3A8D31D1}"/>
+    <hyperlink ref="F33" r:id="rId103" xr:uid="{232B5F00-F258-A24E-BDEA-CF2F2635A32D}"/>
+    <hyperlink ref="F97" r:id="rId104" xr:uid="{219994FD-4BE4-D040-8000-FA1EAB97BA79}"/>
+    <hyperlink ref="E51" r:id="rId105" xr:uid="{5120D118-05B0-D540-BE4F-B9DCCD52040C}"/>
+    <hyperlink ref="F51" r:id="rId106" xr:uid="{BCA8D2A5-D5BD-AF4B-8D5E-2A79F1997BDF}"/>
+    <hyperlink ref="E52" r:id="rId107" xr:uid="{2D132A55-81FD-AD46-B0BE-C908F8D920E8}"/>
+    <hyperlink ref="E10" r:id="rId108" xr:uid="{E4C80A26-9BBE-CE4E-A398-4F9C5F4955F3}"/>
+    <hyperlink ref="F10" r:id="rId109" xr:uid="{5914BE48-1B32-6F46-B075-BC630F5D8608}"/>
+    <hyperlink ref="E25" r:id="rId110" xr:uid="{D5AF8CE0-2466-6647-B572-C377DB7C2F3F}"/>
+    <hyperlink ref="F25" r:id="rId111" xr:uid="{0DDC6C1F-4537-7C4D-A53D-0EA66E740063}"/>
+    <hyperlink ref="E24" r:id="rId112" xr:uid="{7651A9F0-0FB9-AD45-8536-6DA2DBA419D4}"/>
+    <hyperlink ref="F23" r:id="rId113" xr:uid="{EF908708-D656-CC4E-AA5B-142D3510D559}"/>
+    <hyperlink ref="F24" r:id="rId114" xr:uid="{89D30D76-781B-4C4A-9D08-40BF96ECDA97}"/>
+    <hyperlink ref="E112" r:id="rId115" xr:uid="{026E2B8D-FB9A-F942-A358-7A96EA60AAE6}"/>
+    <hyperlink ref="F112" r:id="rId116" xr:uid="{5D581E56-6F6D-CB4C-81EB-3C2041C0974B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Manchester update: add Osborne and Villar Padruno
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3B8EFF-5960-CB4C-9771-45D04DF4A562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B65F58-7CF5-854C-B147-13AB2C15A29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="2400" windowWidth="22920" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11820" yWindow="3120" windowWidth="22920" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="475">
   <si>
     <t>LastName</t>
   </si>
@@ -1442,13 +1442,28 @@
   </si>
   <si>
     <t>miryam.martinez@ific.uv.es</t>
+  </si>
+  <si>
+    <t>Osborne</t>
+  </si>
+  <si>
+    <t>ian.osborne@postgrad.manchester.ac.uk</t>
+  </si>
+  <si>
+    <t>Villar Padruno</t>
+  </si>
+  <si>
+    <t>L.M.</t>
+  </si>
+  <si>
+    <t>luismiguel.villarpadruno@postgrad.manchester.ac.uk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1590,6 +1605,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1934,10 +1955,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2294,10 +2316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K116"/>
+  <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3992,123 +4014,121 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>470</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>414</v>
-      </c>
+        <v>471</v>
+      </c>
+      <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I77" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B78" t="s">
-        <v>187</v>
+        <v>117</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I78" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B79" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F79" s="1"/>
+        <v>265</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>415</v>
+      </c>
       <c r="G79" s="1"/>
       <c r="H79" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="I79" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>416</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="I80" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="B81" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="I81" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
       <c r="B82" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="I82" t="s">
         <v>19</v>
@@ -4116,58 +4136,58 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B83" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="I83" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B84" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G84" s="1"/>
       <c r="H84" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="I84" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B85" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G85" s="1"/>
       <c r="H85" t="s">
@@ -4179,191 +4199,191 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B86" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" t="s">
-        <v>296</v>
+        <v>53</v>
       </c>
       <c r="I86" t="s">
-        <v>19</v>
-      </c>
-      <c r="J86" t="s">
-        <v>40</v>
-      </c>
-      <c r="K86" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" t="s">
-        <v>49</v>
+        <v>296</v>
       </c>
       <c r="I87" t="s">
         <v>19</v>
       </c>
+      <c r="J87" t="s">
+        <v>40</v>
+      </c>
+      <c r="K87" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
+        <v>9</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>318</v>
+        <v>273</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="G88" s="2">
-        <v>45718</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="G88" s="1"/>
       <c r="H88" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="I88" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
-        <v>187</v>
-      </c>
-      <c r="C89" t="s">
-        <v>300</v>
+        <v>176</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G89" s="2">
-        <v>45779</v>
+        <v>45718</v>
       </c>
       <c r="H89" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I89" t="s">
-        <v>19</v>
-      </c>
-      <c r="K89" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C90" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G90" s="2">
         <v>45779</v>
       </c>
       <c r="H90" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I90" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="K90" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>335</v>
+        <v>139</v>
       </c>
       <c r="B91" t="s">
-        <v>62</v>
+        <v>189</v>
+      </c>
+      <c r="C91" t="s">
+        <v>298</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="G91" s="1"/>
+        <v>426</v>
+      </c>
+      <c r="G91" s="2">
+        <v>45779</v>
+      </c>
       <c r="H91" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="I91" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>304</v>
+        <v>335</v>
       </c>
       <c r="B92" t="s">
-        <v>305</v>
+        <v>62</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I92" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>140</v>
+        <v>304</v>
       </c>
       <c r="B93" t="s">
-        <v>190</v>
+        <v>305</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>428</v>
+        <v>448</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I93" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -4371,17 +4391,17 @@
         <v>140</v>
       </c>
       <c r="B94" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G94" s="1"/>
       <c r="H94" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="I94" t="s">
         <v>58</v>
@@ -4389,71 +4409,71 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="B95" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>275</v>
+        <v>322</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="I95" t="s">
-        <v>19</v>
-      </c>
-      <c r="J95" t="s">
-        <v>297</v>
-      </c>
-      <c r="K95" t="s">
-        <v>293</v>
+        <v>58</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="B96" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" t="s">
-        <v>291</v>
+        <v>40</v>
       </c>
       <c r="I96" t="s">
-        <v>292</v>
+        <v>19</v>
+      </c>
+      <c r="J96" t="s">
+        <v>297</v>
+      </c>
+      <c r="K96" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>203</v>
+        <v>141</v>
       </c>
       <c r="B97" t="s">
-        <v>315</v>
+        <v>130</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>316</v>
+        <v>276</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" t="s">
-        <v>34</v>
+        <v>291</v>
       </c>
       <c r="I97" t="s">
-        <v>35</v>
+        <v>292</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -4461,101 +4481,101 @@
         <v>203</v>
       </c>
       <c r="B98" t="s">
-        <v>204</v>
+        <v>315</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F98" s="1"/>
+        <v>316</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="G98" s="1"/>
       <c r="H98" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="I98" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="B99" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>432</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I99" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B100" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>277</v>
+        <v>327</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I100" t="s">
-        <v>19</v>
-      </c>
-      <c r="J100" t="s">
-        <v>71</v>
-      </c>
-      <c r="K100" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B101" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="I101" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="J101" t="s">
+        <v>71</v>
+      </c>
+      <c r="K101" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B102" t="s">
-        <v>117</v>
+        <v>181</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" t="s">
@@ -4567,98 +4587,98 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B103" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F103" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>435</v>
+      </c>
       <c r="G103" s="1"/>
       <c r="H103" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I103" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="B104" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>436</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I104" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
       <c r="B105" t="s">
-        <v>193</v>
+        <v>32</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="I105" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>9</v>
+        <v>193</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G106" s="1"/>
       <c r="H106" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="I106" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>294</v>
+        <v>202</v>
       </c>
       <c r="B107" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G107" s="1"/>
       <c r="H107" t="s">
@@ -4670,16 +4690,16 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>294</v>
       </c>
       <c r="B108" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" t="s">
@@ -4688,194 +4708,234 @@
       <c r="I108" t="s">
         <v>19</v>
       </c>
-      <c r="J108" t="s">
-        <v>151</v>
-      </c>
-      <c r="K108" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>449</v>
+        <v>282</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I109" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J109" t="s">
+        <v>151</v>
+      </c>
+      <c r="K109" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="B110" t="s">
-        <v>199</v>
+        <v>41</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F110" s="1"/>
+        <v>449</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="G110" s="1"/>
       <c r="H110" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="I110" t="s">
-        <v>19</v>
-      </c>
-      <c r="J110" t="s">
-        <v>22</v>
-      </c>
-      <c r="K110" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>338</v>
+        <v>198</v>
       </c>
       <c r="B111" t="s">
-        <v>39</v>
+        <v>199</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>442</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="I111" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="J111" t="s">
+        <v>22</v>
+      </c>
+      <c r="K111" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>466</v>
+        <v>338</v>
       </c>
       <c r="B112" t="s">
-        <v>305</v>
+        <v>39</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>467</v>
+        <v>339</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>468</v>
+        <v>442</v>
       </c>
       <c r="G112" s="1"/>
       <c r="H112" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="I112" t="s">
-        <v>19</v>
-      </c>
-      <c r="J112" t="s">
-        <v>63</v>
-      </c>
-      <c r="K112" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>154</v>
+        <v>466</v>
       </c>
       <c r="B113" t="s">
-        <v>194</v>
+        <v>305</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>284</v>
+        <v>467</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>443</v>
+        <v>468</v>
       </c>
       <c r="G113" s="1"/>
       <c r="H113" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I113" t="s">
-        <v>73</v>
+        <v>19</v>
+      </c>
+      <c r="J113" t="s">
+        <v>63</v>
+      </c>
+      <c r="K113" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>306</v>
+        <v>154</v>
       </c>
       <c r="B114" t="s">
-        <v>307</v>
+        <v>194</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G114" s="1"/>
       <c r="H114" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="I114" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>155</v>
+        <v>306</v>
       </c>
       <c r="B115" t="s">
-        <v>156</v>
+        <v>307</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G115" s="1"/>
       <c r="H115" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="I115" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>207</v>
+      <c r="A116" s="3" t="s">
+        <v>472</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>473</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>446</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" t="s">
+        <v>14</v>
+      </c>
+      <c r="I116" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>155</v>
+      </c>
+      <c r="B117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G117" s="1"/>
+      <c r="H117" t="s">
+        <v>14</v>
+      </c>
+      <c r="I117" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>207</v>
+      </c>
+      <c r="B118" t="s">
+        <v>41</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G118" s="1"/>
+      <c r="H118" t="s">
         <v>40</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I118" t="s">
         <v>19</v>
       </c>
-      <c r="J116" t="s">
+      <c r="J118" t="s">
         <v>297</v>
       </c>
-      <c r="K116" t="s">
+      <c r="K118" t="s">
         <v>293</v>
       </c>
     </row>
@@ -4918,34 +4978,34 @@
     <hyperlink ref="E75" r:id="rId35" xr:uid="{BBAA4BFB-60C1-4D46-9903-5C81869B2451}"/>
     <hyperlink ref="E28" r:id="rId36" xr:uid="{403F5279-8F67-B64C-A27C-18563FED25F5}"/>
     <hyperlink ref="E76" r:id="rId37" xr:uid="{05780F23-E974-A14B-A7BD-29C752AC1269}"/>
-    <hyperlink ref="E77" r:id="rId38" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
-    <hyperlink ref="E78" r:id="rId39" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
-    <hyperlink ref="E79" r:id="rId40" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
-    <hyperlink ref="E80" r:id="rId41" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
-    <hyperlink ref="E81" r:id="rId42" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
-    <hyperlink ref="E82" r:id="rId43" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
-    <hyperlink ref="E84" r:id="rId44" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
-    <hyperlink ref="E86" r:id="rId45" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
-    <hyperlink ref="E87" r:id="rId46" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
-    <hyperlink ref="E88" r:id="rId47" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
-    <hyperlink ref="E89" r:id="rId48" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
-    <hyperlink ref="E93" r:id="rId49" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
-    <hyperlink ref="E95" r:id="rId50" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
-    <hyperlink ref="E100" r:id="rId51" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
-    <hyperlink ref="E102" r:id="rId52" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
-    <hyperlink ref="E103" r:id="rId53" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
-    <hyperlink ref="E104" r:id="rId54" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
-    <hyperlink ref="E105" r:id="rId55" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
-    <hyperlink ref="E106" r:id="rId56" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
-    <hyperlink ref="E108" r:id="rId57" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
-    <hyperlink ref="E109" r:id="rId58" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
-    <hyperlink ref="E113" r:id="rId59" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
-    <hyperlink ref="E115" r:id="rId60" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
-    <hyperlink ref="E116" r:id="rId61" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
+    <hyperlink ref="E78" r:id="rId38" xr:uid="{26B47F7D-C147-3848-B38C-2D9A9DA0C33F}"/>
+    <hyperlink ref="E79" r:id="rId39" xr:uid="{2BF14A96-4081-2E46-827F-32E4EA8D0C53}"/>
+    <hyperlink ref="E80" r:id="rId40" xr:uid="{2685C65F-39CF-6249-84E6-BC878E3BBC05}"/>
+    <hyperlink ref="E81" r:id="rId41" xr:uid="{C651F08A-4556-B04E-BEC5-BBBA98A040F7}"/>
+    <hyperlink ref="E82" r:id="rId42" xr:uid="{6EFE6D0A-2023-9A46-B153-528FD3B639BA}"/>
+    <hyperlink ref="E83" r:id="rId43" xr:uid="{E089342D-EADE-5144-85B4-5B221B6FB51B}"/>
+    <hyperlink ref="E85" r:id="rId44" xr:uid="{0FDDE15D-E614-8D41-81C5-58CDC38DE931}"/>
+    <hyperlink ref="E87" r:id="rId45" xr:uid="{474A574E-FBDA-FC4D-A145-8D4F1A4EB722}"/>
+    <hyperlink ref="E88" r:id="rId46" xr:uid="{7CA22AA8-EBC8-F64A-B96B-91E17E52D41B}"/>
+    <hyperlink ref="E89" r:id="rId47" xr:uid="{7FA7FE8F-9DD7-FF4D-84CA-598017C9D6C0}"/>
+    <hyperlink ref="E90" r:id="rId48" xr:uid="{46BBC652-4D86-A84E-878D-1AB9F86849D6}"/>
+    <hyperlink ref="E94" r:id="rId49" xr:uid="{118D17A4-70BB-814A-837E-BA9B4AF7AABC}"/>
+    <hyperlink ref="E96" r:id="rId50" xr:uid="{E6688BD5-536E-1F40-8D57-41F646FB3097}"/>
+    <hyperlink ref="E101" r:id="rId51" xr:uid="{A83786B8-4609-DB4C-B886-A0F508416DF4}"/>
+    <hyperlink ref="E103" r:id="rId52" xr:uid="{02EA66E6-2B70-4B41-BBC6-C0056CE95EF0}"/>
+    <hyperlink ref="E104" r:id="rId53" xr:uid="{D8FB3995-1FAB-FE49-921B-3834F08A9955}"/>
+    <hyperlink ref="E105" r:id="rId54" xr:uid="{8AE31660-08C0-7E4E-9CF5-75793EE4BAE8}"/>
+    <hyperlink ref="E106" r:id="rId55" xr:uid="{DB061F55-DBDE-A74E-8210-9FA1518AB3FA}"/>
+    <hyperlink ref="E107" r:id="rId56" xr:uid="{624DD26F-2C1E-7A49-BC32-8983E7AB5CE1}"/>
+    <hyperlink ref="E109" r:id="rId57" xr:uid="{F413B786-6B22-634A-AB2E-111579EA63C1}"/>
+    <hyperlink ref="E110" r:id="rId58" xr:uid="{E128C7BD-EB04-5940-B460-D15915636116}"/>
+    <hyperlink ref="E114" r:id="rId59" xr:uid="{92E5B0BF-1629-1544-9BF2-AA4DABAF3BE1}"/>
+    <hyperlink ref="E117" r:id="rId60" xr:uid="{A7ADBB2F-176B-C344-8322-5B13F2A3BDA1}"/>
+    <hyperlink ref="E118" r:id="rId61" xr:uid="{B1AB91E4-83D1-F449-AAB1-9585CE89E54D}"/>
     <hyperlink ref="E59" r:id="rId62" xr:uid="{B8360AE4-856E-0F4D-ACF5-E39471D481E7}"/>
     <hyperlink ref="E71" r:id="rId63" xr:uid="{1974D37E-5B37-7D4D-82A6-731A15D607BE}"/>
-    <hyperlink ref="E94" r:id="rId64" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
-    <hyperlink ref="E101" r:id="rId65" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
+    <hyperlink ref="E95" r:id="rId64" xr:uid="{0F240535-4B9A-0548-A68D-7A42A74ACDCC}"/>
+    <hyperlink ref="E102" r:id="rId65" xr:uid="{9E09B36A-3ADD-604B-82AD-2F401E55B19D}"/>
     <hyperlink ref="E5" r:id="rId66" xr:uid="{F868C6CA-568C-E347-BF39-833BED9A84ED}"/>
     <hyperlink ref="E13" r:id="rId67" xr:uid="{464857C2-993C-4144-9F79-68780529C7BD}"/>
     <hyperlink ref="E62" r:id="rId68" xr:uid="{2905F8A0-D72C-F846-B6E0-0A5993DFFA05}"/>
@@ -4956,34 +5016,34 @@
     <hyperlink ref="E8" r:id="rId73" xr:uid="{2D0C47D7-E74D-EA48-8223-B97B97694F84}"/>
     <hyperlink ref="E55" r:id="rId74" display="mailto:amaia.larumbe@ehu.eus" xr:uid="{6DF6911F-00F3-E547-A8E6-08C387F269CA}"/>
     <hyperlink ref="E69" r:id="rId75" xr:uid="{F661AF17-C778-0149-A0C7-3F0217DCC29E}"/>
-    <hyperlink ref="E96" r:id="rId76" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
-    <hyperlink ref="E110" r:id="rId77" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
-    <hyperlink ref="E83" r:id="rId78" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
+    <hyperlink ref="E97" r:id="rId76" xr:uid="{FFEAF516-B00C-E44B-83AC-7EED5FF2AB67}"/>
+    <hyperlink ref="E111" r:id="rId77" display="mailto:pablo.garcia@dipc.org" xr:uid="{0C4389B2-D44C-654A-B498-6115532471C9}"/>
+    <hyperlink ref="E84" r:id="rId78" xr:uid="{235A1856-CF13-5048-90E7-01FB7EBCF01C}"/>
     <hyperlink ref="E4" r:id="rId79" xr:uid="{1407FD31-5939-8E40-B9DC-A0AC164EEEA9}"/>
-    <hyperlink ref="E107" r:id="rId80" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
+    <hyperlink ref="E108" r:id="rId80" xr:uid="{4A109917-0016-FD4E-AB5E-85042C64CC96}"/>
     <hyperlink ref="E29" r:id="rId81" xr:uid="{A1BB8086-1232-764F-9321-DBAFA8F4E6BC}"/>
-    <hyperlink ref="E85" r:id="rId82" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
-    <hyperlink ref="E92" r:id="rId83" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
-    <hyperlink ref="E114" r:id="rId84" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
+    <hyperlink ref="E86" r:id="rId82" xr:uid="{720C49FB-E08F-A243-B2BF-818E9A279FFC}"/>
+    <hyperlink ref="E93" r:id="rId83" xr:uid="{E83E3204-222C-E341-B533-0F6F3E031F74}"/>
+    <hyperlink ref="E115" r:id="rId84" xr:uid="{5890E7DE-8C5A-194A-850D-5CB1D18110D7}"/>
     <hyperlink ref="E27" r:id="rId85" xr:uid="{D75012BC-D5E3-6D46-B329-96A4CB35BA96}"/>
     <hyperlink ref="E64" r:id="rId86" xr:uid="{27C23B05-0062-D141-9CB5-F38A5E2A5615}"/>
-    <hyperlink ref="E97" r:id="rId87" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
-    <hyperlink ref="E90" r:id="rId88" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
+    <hyperlink ref="E98" r:id="rId87" xr:uid="{300B6594-95C8-694A-BC49-79F88D1B7938}"/>
+    <hyperlink ref="E91" r:id="rId88" xr:uid="{A89D8FB9-300E-A44D-A6C9-40183C323D05}"/>
     <hyperlink ref="E36" r:id="rId89" xr:uid="{137601BF-06D1-F948-9D79-A5FEE0032F25}"/>
-    <hyperlink ref="E98" r:id="rId90" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
-    <hyperlink ref="E91" r:id="rId91" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
-    <hyperlink ref="E99" r:id="rId92" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
+    <hyperlink ref="E99" r:id="rId90" xr:uid="{401FA1E7-B57D-8A46-888A-7FC359B3E8BE}"/>
+    <hyperlink ref="E92" r:id="rId91" xr:uid="{0A20642F-D23C-0A40-A68A-C1EEFE73BFC5}"/>
+    <hyperlink ref="E100" r:id="rId92" xr:uid="{1EAA3F68-BBAB-EB46-A913-60F8E2C47D13}"/>
     <hyperlink ref="E61" r:id="rId93" xr:uid="{3695667B-23BA-B649-937C-EFF9527A0FD1}"/>
     <hyperlink ref="E31" r:id="rId94" xr:uid="{E24B841F-2272-CA43-9614-50B7F36AD8C5}"/>
     <hyperlink ref="E14" r:id="rId95" xr:uid="{29460556-99EB-6943-BF02-EAF45B9A2438}"/>
-    <hyperlink ref="E111" r:id="rId96" xr:uid="{31EA1686-1B20-3342-8310-E26369FFF7C2}"/>
+    <hyperlink ref="E112" r:id="rId96" xr:uid="{31EA1686-1B20-3342-8310-E26369FFF7C2}"/>
     <hyperlink ref="E22" r:id="rId97" xr:uid="{BFCD233B-85C4-684A-9E1F-CFD7E946453F}"/>
     <hyperlink ref="E16" r:id="rId98" tooltip="abayo@lsc-canfranc.es" display="mailto:abayo@lsc-canfranc.es" xr:uid="{9D231E2D-796B-5044-A575-DB475A1F4009}"/>
     <hyperlink ref="E23" r:id="rId99" tooltip="lcid@lsc-canfranc.es" display="mailto:lcid@lsc-canfranc.es" xr:uid="{2505E3E3-5341-1F45-B64F-DF1C414EDC59}"/>
-    <hyperlink ref="F92" r:id="rId100" xr:uid="{8A532988-D04F-D445-B8FD-AA64E787BB24}"/>
+    <hyperlink ref="F93" r:id="rId100" xr:uid="{8A532988-D04F-D445-B8FD-AA64E787BB24}"/>
     <hyperlink ref="F73" r:id="rId101" xr:uid="{D54F73F6-B34C-4044-9163-D80E3A8D31D1}"/>
     <hyperlink ref="F33" r:id="rId102" xr:uid="{232B5F00-F258-A24E-BDEA-CF2F2635A32D}"/>
-    <hyperlink ref="F97" r:id="rId103" xr:uid="{219994FD-4BE4-D040-8000-FA1EAB97BA79}"/>
+    <hyperlink ref="F98" r:id="rId103" xr:uid="{219994FD-4BE4-D040-8000-FA1EAB97BA79}"/>
     <hyperlink ref="E51" r:id="rId104" xr:uid="{5120D118-05B0-D540-BE4F-B9DCCD52040C}"/>
     <hyperlink ref="F51" r:id="rId105" xr:uid="{BCA8D2A5-D5BD-AF4B-8D5E-2A79F1997BDF}"/>
     <hyperlink ref="E52" r:id="rId106" xr:uid="{2D132A55-81FD-AD46-B0BE-C908F8D920E8}"/>
@@ -4994,9 +5054,11 @@
     <hyperlink ref="E24" r:id="rId111" xr:uid="{7651A9F0-0FB9-AD45-8536-6DA2DBA419D4}"/>
     <hyperlink ref="F23" r:id="rId112" xr:uid="{EF908708-D656-CC4E-AA5B-142D3510D559}"/>
     <hyperlink ref="F24" r:id="rId113" xr:uid="{89D30D76-781B-4C4A-9D08-40BF96ECDA97}"/>
-    <hyperlink ref="E112" r:id="rId114" xr:uid="{026E2B8D-FB9A-F942-A358-7A96EA60AAE6}"/>
-    <hyperlink ref="F112" r:id="rId115" xr:uid="{5D581E56-6F6D-CB4C-81EB-3C2041C0974B}"/>
+    <hyperlink ref="E113" r:id="rId114" xr:uid="{026E2B8D-FB9A-F942-A358-7A96EA60AAE6}"/>
+    <hyperlink ref="F113" r:id="rId115" xr:uid="{5D581E56-6F6D-CB4C-81EB-3C2041C0974B}"/>
     <hyperlink ref="E66" r:id="rId116" xr:uid="{6CDD9F24-D4B4-D646-8B31-5DDB7E06C54F}"/>
+    <hyperlink ref="E77" r:id="rId117" xr:uid="{A055B258-CFB3-274F-A1B8-E8DFAF801887}"/>
+    <hyperlink ref="E116" r:id="rId118" xr:uid="{24D2F24E-7FAE-D744-896E-B75BD10607F0}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>